<commit_message>
New figures for additional countries (xlsx) + modified presentation
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEB024B-F436-C84D-ADB5-90FDBF149DD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38800" yWindow="-23120" windowWidth="23120" windowHeight="14460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
     <sheet name="quotas_ID" sheetId="10" r:id="rId11"/>
     <sheet name="quotas_JP" sheetId="11" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="552">
   <si>
     <t>Country</t>
   </si>
@@ -1661,18 +1662,54 @@
   </si>
   <si>
     <t>Buhle Shibodze, 60$</t>
+  </si>
+  <si>
+    <t>R$</t>
+  </si>
+  <si>
+    <t>₩</t>
+  </si>
+  <si>
+    <t>12,480k</t>
+  </si>
+  <si>
+    <t>1,445k</t>
+  </si>
+  <si>
+    <t>815k</t>
+  </si>
+  <si>
+    <t>1,110k</t>
+  </si>
+  <si>
+    <t>3,375k</t>
+  </si>
+  <si>
+    <t>825k</t>
+  </si>
+  <si>
+    <t>550k</t>
+  </si>
+  <si>
+    <t>12.5M</t>
+  </si>
+  <si>
+    <t>800k</t>
+  </si>
+  <si>
+    <t>3.5M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1874,7 +1911,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2151,25 +2188,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45:M45"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N51" sqref="N51:Q56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.6328125" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" customWidth="1"/>
-    <col min="3" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="9.6328125" customWidth="1"/>
-    <col min="12" max="12" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.453125" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2222,7 +2259,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>458</v>
       </c>
@@ -2261,7 +2298,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
         <v>459</v>
       </c>
@@ -2300,7 +2337,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
         <v>460</v>
       </c>
@@ -2331,7 +2368,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
         <v>500</v>
       </c>
@@ -2356,7 +2393,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
         <v>461</v>
       </c>
@@ -2379,7 +2416,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
@@ -2419,8 +2456,20 @@
       <c r="M7" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" t="s">
+        <v>540</v>
+      </c>
+      <c r="P7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -2460,8 +2509,20 @@
       <c r="M8">
         <v>14.37</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N8">
+        <v>6.37</v>
+      </c>
+      <c r="O8">
+        <v>5.23</v>
+      </c>
+      <c r="P8">
+        <v>19.920000000000002</v>
+      </c>
+      <c r="Q8">
+        <v>1113.8499999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="2" t="s">
         <v>170</v>
       </c>
@@ -2501,8 +2562,20 @@
       <c r="M9" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N9" t="s">
+        <v>542</v>
+      </c>
+      <c r="O9" t="s">
+        <v>543</v>
+      </c>
+      <c r="P9" t="s">
+        <v>544</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="2" t="s">
         <v>171</v>
       </c>
@@ -2542,8 +2615,20 @@
       <c r="M10" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N10" t="s">
+        <v>546</v>
+      </c>
+      <c r="O10" t="s">
+        <v>547</v>
+      </c>
+      <c r="P10" t="s">
+        <v>548</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
         <v>182</v>
       </c>
@@ -2583,8 +2668,20 @@
       <c r="M11" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N11" t="s">
+        <v>549</v>
+      </c>
+      <c r="O11" t="s">
+        <v>179</v>
+      </c>
+      <c r="P11" t="s">
+        <v>550</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="1" t="s">
         <v>183</v>
       </c>
@@ -2624,8 +2721,20 @@
       <c r="M12" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N12" t="s">
+        <v>551</v>
+      </c>
+      <c r="O12" t="s">
+        <v>550</v>
+      </c>
+      <c r="P12" t="s">
+        <v>548</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
         <v>403</v>
       </c>
@@ -2666,7 +2775,7 @@
         <v>19653</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
         <v>404</v>
       </c>
@@ -2707,7 +2816,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
         <v>405</v>
       </c>
@@ -2748,7 +2857,7 @@
         <v>113696</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
@@ -2789,7 +2898,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>400</v>
       </c>
@@ -2830,7 +2939,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>401</v>
       </c>
@@ -2871,7 +2980,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>402</v>
       </c>
@@ -2912,7 +3021,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>207</v>
       </c>
@@ -2953,7 +3062,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>208</v>
       </c>
@@ -2994,7 +3103,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>209</v>
       </c>
@@ -3035,7 +3144,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
         <v>210</v>
       </c>
@@ -3076,7 +3185,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
         <v>440</v>
       </c>
@@ -3117,7 +3226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>441</v>
       </c>
@@ -3158,7 +3267,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>442</v>
       </c>
@@ -3199,7 +3308,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>443</v>
       </c>
@@ -3240,7 +3349,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
         <v>527</v>
       </c>
@@ -3254,7 +3363,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
         <v>74</v>
       </c>
@@ -3295,7 +3404,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>75</v>
       </c>
@@ -3336,7 +3445,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
         <v>76</v>
       </c>
@@ -3377,7 +3486,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
         <v>77</v>
       </c>
@@ -3418,7 +3527,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17">
       <c r="A33" s="1" t="s">
         <v>78</v>
       </c>
@@ -3459,7 +3568,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17">
       <c r="A34" s="1" t="s">
         <v>73</v>
       </c>
@@ -3470,7 +3579,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -3484,7 +3593,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17">
       <c r="A36" s="1" t="s">
         <v>67</v>
       </c>
@@ -3498,7 +3607,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17">
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
@@ -3539,7 +3648,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17">
       <c r="A38" s="1" t="s">
         <v>65</v>
       </c>
@@ -3580,7 +3689,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17">
       <c r="A39" s="1" t="s">
         <v>64</v>
       </c>
@@ -3591,7 +3700,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17">
       <c r="A40" s="1" t="s">
         <v>63</v>
       </c>
@@ -3632,7 +3741,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17">
       <c r="A41" s="1" t="s">
         <v>79</v>
       </c>
@@ -3673,7 +3782,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17">
       <c r="A42" s="1" t="s">
         <v>315</v>
       </c>
@@ -3714,7 +3823,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17">
       <c r="A43" s="1" t="s">
         <v>62</v>
       </c>
@@ -3755,7 +3864,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17">
       <c r="A44" s="1" t="s">
         <v>61</v>
       </c>
@@ -3786,7 +3895,7 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17">
       <c r="A45" s="1" t="s">
         <v>60</v>
       </c>
@@ -3827,7 +3936,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17">
       <c r="A46" s="1" t="s">
         <v>59</v>
       </c>
@@ -3843,27 +3952,27 @@
         <v>24.9</v>
       </c>
       <c r="E46" s="31">
-        <f>$B$46*E8</f>
+        <f t="shared" ref="E46:J46" si="1">$B$46*E8</f>
         <v>24.9</v>
       </c>
       <c r="F46" s="31">
-        <f>$B$46*F8</f>
+        <f t="shared" si="1"/>
         <v>24.9</v>
       </c>
       <c r="G46" s="31">
-        <f>$B$46*G8</f>
+        <f t="shared" si="1"/>
         <v>114.3</v>
       </c>
       <c r="H46" s="31">
-        <f>$B$46*H8</f>
+        <f t="shared" si="1"/>
         <v>24.9</v>
       </c>
       <c r="I46" s="31">
-        <f>$B$46*I8</f>
+        <f t="shared" si="1"/>
         <v>21.599999999999998</v>
       </c>
       <c r="J46" s="31">
-        <f>$B$46*J8</f>
+        <f t="shared" si="1"/>
         <v>3270</v>
       </c>
       <c r="K46" s="31">
@@ -3878,8 +3987,24 @@
         <f t="shared" si="0"/>
         <v>431.09999999999997</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N46" s="31">
+        <f>$B$46*N8</f>
+        <v>191.1</v>
+      </c>
+      <c r="O46" s="31">
+        <f t="shared" ref="O46:Q46" si="2">$B$46*O8</f>
+        <v>156.9</v>
+      </c>
+      <c r="P46" s="31">
+        <f t="shared" si="2"/>
+        <v>597.6</v>
+      </c>
+      <c r="Q46" s="31">
+        <f t="shared" si="2"/>
+        <v>33415.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
       <c r="A47" s="1" t="s">
         <v>58</v>
       </c>
@@ -3920,7 +4045,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17">
       <c r="A48" s="1" t="s">
         <v>57</v>
       </c>
@@ -3932,7 +4057,7 @@
         <v>420.92</v>
       </c>
       <c r="D48" s="31">
-        <f t="shared" ref="D48:K48" si="1">D47*D8</f>
+        <f t="shared" ref="D48:K48" si="3">D47*D8</f>
         <v>38.18</v>
       </c>
       <c r="E48" s="31">
@@ -3959,7 +4084,7 @@
         <v>6500</v>
       </c>
       <c r="K48" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>960.7</v>
       </c>
       <c r="L48" s="31">
@@ -3970,7 +4095,7 @@
         <v>718.5</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17">
       <c r="A49" s="1" t="s">
         <v>56</v>
       </c>
@@ -3997,7 +4122,7 @@
       </c>
       <c r="O49" s="1"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -4039,7 +4164,7 @@
       </c>
       <c r="O50" s="1"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17">
       <c r="A51" s="1" t="s">
         <v>308</v>
       </c>
@@ -4080,8 +4205,20 @@
       <c r="M51">
         <v>45</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N51">
+        <v>45</v>
+      </c>
+      <c r="O51">
+        <v>45</v>
+      </c>
+      <c r="P51">
+        <v>45</v>
+      </c>
+      <c r="Q51">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17">
       <c r="A52" s="1" t="s">
         <v>313</v>
       </c>
@@ -4121,8 +4258,20 @@
       <c r="M52" s="3">
         <v>433.17</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N52" s="3">
+        <v>10877</v>
+      </c>
+      <c r="O52" s="3">
+        <v>493</v>
+      </c>
+      <c r="P52" s="3">
+        <v>507</v>
+      </c>
+      <c r="Q52" s="3">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
       <c r="A53" s="1" t="s">
         <v>534</v>
       </c>
@@ -4162,8 +4311,20 @@
       <c r="M53" s="3">
         <v>35983394.399999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N53">
+        <v>1128677232</v>
+      </c>
+      <c r="O53">
+        <v>159837762.59999999</v>
+      </c>
+      <c r="P53">
+        <v>92799575.799999997</v>
+      </c>
+      <c r="Q53">
+        <v>43190072.399999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
       <c r="A54" s="1" t="s">
         <v>314</v>
       </c>
@@ -4176,47 +4337,63 @@
         <v>0.33521809369951533</v>
       </c>
       <c r="D54" s="17">
-        <f t="shared" ref="D54:M54" si="2">2.5*D51/1000</f>
+        <f t="shared" ref="D54:Q54" si="4">2.5*D51/1000</f>
         <v>0.1125</v>
       </c>
       <c r="E54" s="17">
-        <f>2.5*E51/1000</f>
+        <f t="shared" ref="E54:J54" si="5">2.5*E51/1000</f>
         <v>0.1125</v>
       </c>
       <c r="F54" s="17">
-        <f>2.5*F51/1000</f>
+        <f t="shared" si="5"/>
         <v>0.1125</v>
       </c>
       <c r="G54" s="17">
-        <f>2.5*G51/1000</f>
+        <f t="shared" si="5"/>
         <v>0.1125</v>
       </c>
       <c r="H54" s="17">
-        <f>2.5*H51/1000</f>
+        <f t="shared" si="5"/>
         <v>0.1125</v>
       </c>
       <c r="I54" s="17">
-        <f>2.5*I51/1000</f>
+        <f t="shared" si="5"/>
         <v>0.1125</v>
       </c>
       <c r="J54" s="17">
-        <f>2.5*J51/1000</f>
+        <f t="shared" si="5"/>
         <v>0.1125</v>
       </c>
       <c r="K54" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.1125</v>
       </c>
       <c r="L54" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.1125</v>
       </c>
       <c r="M54" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.1125</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N54" s="17">
+        <f t="shared" si="4"/>
+        <v>0.1125</v>
+      </c>
+      <c r="O54" s="17">
+        <f t="shared" si="4"/>
+        <v>0.1125</v>
+      </c>
+      <c r="P54" s="17">
+        <f t="shared" si="4"/>
+        <v>0.1125</v>
+      </c>
+      <c r="Q54" s="17">
+        <f t="shared" si="4"/>
+        <v>0.1125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
       <c r="A55" s="1" t="s">
         <v>316</v>
       </c>
@@ -4229,47 +4406,63 @@
         <v>2.0750000000000002</v>
       </c>
       <c r="D55" s="22">
-        <f t="shared" ref="D55:M55" si="3">D54*D8</f>
+        <f t="shared" ref="D55:Q55" si="6">D54*D8</f>
         <v>9.3375E-2</v>
       </c>
       <c r="E55" s="22">
-        <f>E54*E8</f>
+        <f t="shared" ref="E55:J55" si="7">E54*E8</f>
         <v>9.3375E-2</v>
       </c>
       <c r="F55" s="22">
-        <f>F54*F8</f>
+        <f t="shared" si="7"/>
         <v>9.3375E-2</v>
       </c>
       <c r="G55" s="22">
-        <f>G54*G8</f>
+        <f t="shared" si="7"/>
         <v>0.42862500000000003</v>
       </c>
       <c r="H55" s="22">
-        <f>H54*H8</f>
+        <f t="shared" si="7"/>
         <v>9.3375E-2</v>
       </c>
       <c r="I55" s="22">
-        <f>I54*I8</f>
+        <f t="shared" si="7"/>
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="J55" s="22">
-        <f>J54*J8</f>
+        <f t="shared" si="7"/>
         <v>12.262500000000001</v>
       </c>
       <c r="K55" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>8.3137500000000006</v>
       </c>
       <c r="L55" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1624.05</v>
       </c>
       <c r="M55" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.616625</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N55" s="22">
+        <f t="shared" si="6"/>
+        <v>0.71662500000000007</v>
+      </c>
+      <c r="O55" s="22">
+        <f t="shared" si="6"/>
+        <v>0.58837500000000009</v>
+      </c>
+      <c r="P55" s="22">
+        <f t="shared" si="6"/>
+        <v>2.2410000000000001</v>
+      </c>
+      <c r="Q55" s="22">
+        <f t="shared" si="6"/>
+        <v>125.30812499999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17">
       <c r="A56" s="1" t="s">
         <v>317</v>
       </c>
@@ -4282,47 +4475,63 @@
         <v>3703.602118170118</v>
       </c>
       <c r="D56" s="22">
-        <f>0.8*0.8*D52*D51*1000000*D8/D53</f>
+        <f t="shared" ref="D56:J56" si="8">0.8*0.8*D52*D51*1000000*D8/D53</f>
         <v>160.38911364310246</v>
       </c>
       <c r="E56" s="22">
-        <f>0.8*0.8*E52*E51*1000000*E8/E53</f>
+        <f t="shared" si="8"/>
         <v>277.84760275726222</v>
       </c>
       <c r="F56" s="22">
-        <f>0.8*0.8*F52*F51*1000000*F8/F53</f>
+        <f t="shared" si="8"/>
         <v>173.84220326169338</v>
       </c>
       <c r="G56" s="22">
-        <f>0.8*0.8*G52*G51*1000000*G8/G53</f>
+        <f t="shared" si="8"/>
         <v>1116.4280705068938</v>
       </c>
       <c r="H56" s="22">
-        <f>0.8*0.8*H52*H51*1000000*H8/H53</f>
+        <f t="shared" si="8"/>
         <v>176.58502339197312</v>
       </c>
       <c r="I56" s="22">
-        <f>0.8*0.8*I52*I51*1000000*I8/I53</f>
+        <f t="shared" si="8"/>
         <v>152.27866202672033</v>
       </c>
       <c r="J56" s="22">
-        <f>0.8*0.8*J52*J51*1000000*J8/J53</f>
+        <f t="shared" si="8"/>
         <v>38475.475811006392</v>
       </c>
       <c r="K56" s="22">
-        <f t="shared" ref="K56:M56" si="4">0.8*0.8*K52*K51*1000000*K8/K53</f>
+        <f t="shared" ref="K56:Q56" si="9">0.8*0.8*K52*K51*1000000*K8/K53</f>
         <v>6075.6933515784121</v>
       </c>
       <c r="L56" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1230718.9651813384</v>
       </c>
       <c r="M56" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>4982.0203599246888</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N56" s="22">
+        <f t="shared" si="9"/>
+        <v>1767.9553156787704</v>
+      </c>
+      <c r="O56" s="22">
+        <f t="shared" si="9"/>
+        <v>464.58127786631081</v>
+      </c>
+      <c r="P56" s="22">
+        <f t="shared" si="9"/>
+        <v>3134.3232928872949</v>
+      </c>
+      <c r="Q56" s="22">
+        <f t="shared" si="9"/>
+        <v>499862.23778592242</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
       <c r="A57" s="1" t="s">
         <v>333</v>
       </c>
@@ -4363,7 +4572,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17">
       <c r="A58" s="1" t="s">
         <v>492</v>
       </c>
@@ -4404,7 +4613,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17">
       <c r="A59" s="1" t="s">
         <v>355</v>
       </c>
@@ -4443,7 +4652,7 @@
       </c>
       <c r="M59" s="22"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17">
       <c r="A60" s="1" t="s">
         <v>387</v>
       </c>
@@ -4484,7 +4693,7 @@
         <v>0.92800000000000005</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17">
       <c r="A61" s="1" t="s">
         <v>493</v>
       </c>
@@ -4525,10 +4734,10 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17">
       <c r="K62" s="22"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17">
       <c r="A63" s="1" t="s">
         <v>102</v>
       </c>
@@ -4536,7 +4745,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17">
       <c r="A64" s="1" t="s">
         <v>103</v>
       </c>
@@ -4577,7 +4786,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13">
       <c r="A65" s="1" t="s">
         <v>104</v>
       </c>
@@ -4618,7 +4827,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13">
       <c r="A66" s="1" t="s">
         <v>105</v>
       </c>
@@ -4632,7 +4841,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13">
       <c r="A67" s="1" t="s">
         <v>112</v>
       </c>
@@ -4640,7 +4849,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13">
       <c r="A68" s="1" t="s">
         <v>106</v>
       </c>
@@ -4678,7 +4887,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13">
       <c r="A69" s="1" t="s">
         <v>107</v>
       </c>
@@ -4695,7 +4904,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13">
       <c r="A70" s="1" t="s">
         <v>205</v>
       </c>
@@ -4715,7 +4924,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13">
       <c r="A71" s="1" t="s">
         <v>108</v>
       </c>
@@ -4723,7 +4932,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13">
       <c r="A72" s="1" t="s">
         <v>113</v>
       </c>
@@ -4731,7 +4940,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13">
       <c r="A73" s="1" t="s">
         <v>115</v>
       </c>
@@ -4739,7 +4948,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13">
       <c r="A74" s="6" t="s">
         <v>116</v>
       </c>
@@ -4774,7 +4983,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13">
       <c r="A75" s="6" t="s">
         <v>117</v>
       </c>
@@ -4809,7 +5018,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13">
       <c r="A76" s="6" t="s">
         <v>118</v>
       </c>
@@ -4844,7 +5053,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13">
       <c r="A77" s="6" t="s">
         <v>119</v>
       </c>
@@ -4879,7 +5088,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13">
       <c r="A78" s="6" t="s">
         <v>120</v>
       </c>
@@ -4908,7 +5117,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13">
       <c r="A79" s="6" t="s">
         <v>121</v>
       </c>
@@ -4931,7 +5140,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13">
       <c r="A80" s="6" t="s">
         <v>122</v>
       </c>
@@ -4945,7 +5154,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13">
       <c r="A81" s="6" t="s">
         <v>123</v>
       </c>
@@ -4953,7 +5162,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13">
       <c r="A82" s="6" t="s">
         <v>124</v>
       </c>
@@ -4961,7 +5170,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13">
       <c r="A83" s="6" t="s">
         <v>125</v>
       </c>
@@ -4972,7 +5181,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13">
       <c r="A84" s="6" t="s">
         <v>189</v>
       </c>
@@ -4980,7 +5189,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13">
       <c r="A85" s="6" t="s">
         <v>190</v>
       </c>
@@ -4988,7 +5197,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13">
       <c r="A86" s="6" t="s">
         <v>194</v>
       </c>
@@ -4996,7 +5205,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13">
       <c r="A87" s="6" t="s">
         <v>200</v>
       </c>
@@ -5037,7 +5246,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13">
       <c r="A88" s="4" t="s">
         <v>192</v>
       </c>
@@ -5045,7 +5254,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13">
       <c r="A89" s="4" t="s">
         <v>196</v>
       </c>
@@ -5053,7 +5262,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13">
       <c r="A90" s="4" t="s">
         <v>198</v>
       </c>
@@ -5061,7 +5270,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13">
       <c r="A91" s="6" t="s">
         <v>271</v>
       </c>
@@ -5075,7 +5284,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13">
       <c r="A92" s="6" t="s">
         <v>272</v>
       </c>
@@ -5089,7 +5298,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13">
       <c r="A93" s="6" t="s">
         <v>273</v>
       </c>
@@ -5103,7 +5312,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13">
       <c r="A94" s="6" t="s">
         <v>274</v>
       </c>
@@ -5111,7 +5320,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13">
       <c r="A95" s="6" t="s">
         <v>275</v>
       </c>
@@ -5119,7 +5328,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13">
       <c r="A96" s="6" t="s">
         <v>276</v>
       </c>
@@ -5133,7 +5342,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:14">
       <c r="A97" s="6" t="s">
         <v>277</v>
       </c>
@@ -5141,7 +5350,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:14">
       <c r="A98" s="6" t="s">
         <v>295</v>
       </c>
@@ -5149,7 +5358,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:14">
       <c r="A99" s="6" t="s">
         <v>336</v>
       </c>
@@ -5175,7 +5384,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:14">
       <c r="A100" s="6" t="s">
         <v>491</v>
       </c>
@@ -5198,7 +5407,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:14">
       <c r="A101" s="6" t="s">
         <v>340</v>
       </c>
@@ -5206,7 +5415,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:14">
       <c r="A102" s="6" t="s">
         <v>494</v>
       </c>
@@ -5235,7 +5444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:14">
       <c r="A103" s="6" t="s">
         <v>496</v>
       </c>
@@ -5267,7 +5476,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:14">
       <c r="A104" s="6" t="s">
         <v>501</v>
       </c>
@@ -5281,7 +5490,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:14">
       <c r="A105" s="6" t="s">
         <v>502</v>
       </c>
@@ -5302,52 +5511,52 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>242</v>
       </c>
@@ -5364,7 +5573,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>247</v>
       </c>
@@ -5381,7 +5590,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>537</v>
       </c>
@@ -5398,7 +5607,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>241</v>
       </c>
@@ -5416,7 +5625,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>249</v>
       </c>
@@ -5440,7 +5649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>247</v>
       </c>
@@ -5465,7 +5674,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>537</v>
       </c>
@@ -5494,7 +5703,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>241</v>
       </c>
@@ -5518,10 +5727,10 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>250</v>
       </c>
@@ -5538,7 +5747,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>247</v>
       </c>
@@ -5559,7 +5768,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>537</v>
       </c>
@@ -5584,7 +5793,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>241</v>
       </c>
@@ -5605,13 +5814,13 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>255</v>
       </c>
@@ -5628,7 +5837,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>247</v>
       </c>
@@ -5649,7 +5858,7 @@
         <v>100.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>537</v>
       </c>
@@ -5674,7 +5883,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>241</v>
       </c>
@@ -5695,7 +5904,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>260</v>
       </c>
@@ -5709,7 +5918,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>247</v>
       </c>
@@ -5723,7 +5932,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>537</v>
       </c>
@@ -5740,7 +5949,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>241</v>
       </c>
@@ -5755,11 +5964,11 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>265</v>
       </c>
@@ -5776,7 +5985,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>247</v>
       </c>
@@ -5793,7 +6002,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>537</v>
       </c>
@@ -5814,7 +6023,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>241</v>
       </c>
@@ -5834,30 +6043,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>282</v>
       </c>
@@ -5883,7 +6092,7 @@
       <c r="K1" s="13"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>221</v>
       </c>
@@ -5916,7 +6125,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>222</v>
       </c>
@@ -5950,7 +6159,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>223</v>
       </c>
@@ -5984,7 +6193,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5" s="12" t="s">
         <v>241</v>
       </c>
@@ -6000,7 +6209,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="0.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="0.5" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -6014,14 +6223,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>225</v>
       </c>
@@ -6041,7 +6250,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>221</v>
       </c>
@@ -6064,7 +6273,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>222</v>
       </c>
@@ -6089,7 +6298,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>223</v>
       </c>
@@ -6114,7 +6323,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" s="12" t="s">
         <v>241</v>
       </c>
@@ -6130,7 +6339,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -6144,7 +6353,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>228</v>
       </c>
@@ -6170,7 +6379,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>221</v>
       </c>
@@ -6199,7 +6408,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>222</v>
       </c>
@@ -6233,7 +6442,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>223</v>
       </c>
@@ -6267,7 +6476,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" s="12" t="s">
         <v>241</v>
       </c>
@@ -6283,7 +6492,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -6297,7 +6506,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>234</v>
       </c>
@@ -6321,7 +6530,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>239</v>
       </c>
@@ -6347,7 +6556,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>222</v>
       </c>
@@ -6378,7 +6587,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>223</v>
       </c>
@@ -6409,7 +6618,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>241</v>
       </c>
@@ -6419,7 +6628,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -6427,7 +6636,7 @@
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" ht="16.5" customHeight="1" thickBot="1">
       <c r="A26" s="12" t="s">
         <v>516</v>
       </c>
@@ -6444,7 +6653,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>221</v>
       </c>
@@ -6463,7 +6672,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" ht="16" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>222</v>
       </c>
@@ -6485,7 +6694,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" ht="16" thickBot="1">
       <c r="A29" s="8" t="s">
         <v>520</v>
       </c>
@@ -6504,7 +6713,7 @@
       </c>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>519</v>
       </c>
@@ -6526,7 +6735,7 @@
       </c>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>521</v>
       </c>
@@ -6548,7 +6757,7 @@
       </c>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12">
       <c r="A32" s="12" t="s">
         <v>241</v>
       </c>
@@ -6559,12 +6768,12 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
-    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" ht="30" thickBot="1">
       <c r="A37" s="8" t="s">
         <v>212</v>
       </c>
@@ -6594,7 +6803,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="8" t="s">
         <v>221</v>
       </c>
@@ -6627,7 +6836,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="8" t="s">
         <v>222</v>
       </c>
@@ -6668,7 +6877,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="8" t="s">
         <v>223</v>
       </c>
@@ -6709,7 +6918,7 @@
         <v>2196</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10">
       <c r="A41" s="12" t="s">
         <v>241</v>
       </c>
@@ -6723,7 +6932,7 @@
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10">
       <c r="A42" s="2"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -6735,12 +6944,12 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>287</v>
       </c>
@@ -6761,7 +6970,7 @@
       </c>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="8" t="s">
         <v>221</v>
       </c>
@@ -6785,7 +6994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="8" t="s">
         <v>222</v>
       </c>
@@ -6814,7 +7023,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="8" t="s">
         <v>223</v>
       </c>
@@ -6843,7 +7052,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10">
       <c r="A48" s="12" t="s">
         <v>241</v>
       </c>
@@ -6854,7 +7063,7 @@
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7">
       <c r="A49" s="2"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -6870,22 +7079,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>225</v>
       </c>
@@ -6900,7 +7109,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>221</v>
       </c>
@@ -6918,7 +7127,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>222</v>
       </c>
@@ -6938,7 +7147,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>223</v>
       </c>
@@ -6958,7 +7167,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" s="12" t="s">
         <v>241</v>
       </c>
@@ -6969,7 +7178,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -6978,7 +7187,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>228</v>
       </c>
@@ -6999,7 +7208,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>221</v>
       </c>
@@ -7023,7 +7232,7 @@
         <v>1.0001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>222</v>
       </c>
@@ -7052,7 +7261,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>223</v>
       </c>
@@ -7081,8 +7290,8 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="16" thickBot="1"/>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>240</v>
       </c>
@@ -7100,7 +7309,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="8" t="s">
         <v>239</v>
       </c>
@@ -7120,7 +7329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>222</v>
       </c>
@@ -7145,7 +7354,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>223</v>
       </c>
@@ -7170,12 +7379,12 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" s="16" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="12" t="s">
         <v>224</v>
       </c>
@@ -7195,7 +7404,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="8" t="s">
         <v>221</v>
       </c>
@@ -7219,7 +7428,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>222</v>
       </c>
@@ -7248,7 +7457,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>223</v>
       </c>
@@ -7277,7 +7486,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
         <v>241</v>
       </c>
@@ -7286,7 +7495,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="16" t="s">
         <v>342</v>
       </c>
@@ -7297,7 +7506,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>221</v>
       </c>
@@ -7312,7 +7521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>222</v>
       </c>
@@ -7329,7 +7538,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>223</v>
       </c>
@@ -7346,7 +7555,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7">
       <c r="A28" s="12" t="s">
         <v>241</v>
       </c>
@@ -7357,60 +7566,60 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
preparation, xlsx ZU, WTP ZA
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="622">
   <si>
     <t>Country</t>
   </si>
@@ -1906,6 +1906,12 @@
   </si>
   <si>
     <t>Marcel Hallensleben, 150$</t>
+  </si>
+  <si>
+    <t>50/150/300/500/1,500/3,000/5,000</t>
+  </si>
+  <si>
+    <t>?Q_Language=ZU</t>
   </si>
 </sst>
 </file>
@@ -2412,8 +2418,8 @@
   <dimension ref="A1:Q105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E100" sqref="E100"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4177,7 +4183,9 @@
         <v>515</v>
       </c>
       <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
+      <c r="M46" s="1" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
@@ -4937,7 +4945,9 @@
       <c r="L61" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="M61" s="22"/>
+      <c r="M61" s="22" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">

</xml_diff>

<commit_message>
Added regions for IND, UK, ITA
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDEAA4C-1A4B-DE46-9964-B7365A33B7A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="14480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
     <sheet name="quotas_MX" sheetId="17" r:id="rId16"/>
     <sheet name="quotas_SK" sheetId="18" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="631">
   <si>
     <t>Country</t>
   </si>
@@ -1912,18 +1913,45 @@
   </si>
   <si>
     <t>?Q_Language=ZU</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Regions_of_Italy#Macroregions</t>
+  </si>
+  <si>
+    <t>Northern Zonal Council</t>
+  </si>
+  <si>
+    <t>Southern Zonal Council</t>
+  </si>
+  <si>
+    <t>Central Zonal Council</t>
+  </si>
+  <si>
+    <t>Eastern Zonal Council</t>
+  </si>
+  <si>
+    <t>Western Zonal Council</t>
+  </si>
+  <si>
+    <t>Rest (North Eastern)</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Zonal_Council</t>
+  </si>
+  <si>
+    <t>https://statisticstimes.com/demographics/india/indian-states-population.php</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2059,7 +2087,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2127,7 +2155,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2137,7 +2164,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2414,26 +2441,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.6328125" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" customWidth="1"/>
-    <col min="3" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="9.6328125" customWidth="1"/>
-    <col min="12" max="12" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.453125" customWidth="1"/>
-    <col min="17" max="17" width="13.6328125" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2486,7 +2513,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>455</v>
       </c>
@@ -2527,7 +2554,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
         <v>456</v>
       </c>
@@ -2566,7 +2593,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
         <v>457</v>
       </c>
@@ -2601,7 +2628,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
         <v>497</v>
       </c>
@@ -2628,7 +2655,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
         <v>458</v>
       </c>
@@ -2651,7 +2678,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
@@ -2704,7 +2731,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -2757,7 +2784,7 @@
         <v>1113.8499999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17">
       <c r="A9" s="2" t="s">
         <v>169</v>
       </c>
@@ -2810,7 +2837,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17">
       <c r="A10" s="2" t="s">
         <v>170</v>
       </c>
@@ -2863,7 +2890,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
         <v>181</v>
       </c>
@@ -2916,7 +2943,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17">
       <c r="A12" s="1" t="s">
         <v>182</v>
       </c>
@@ -2969,7 +2996,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
         <v>400</v>
       </c>
@@ -3010,7 +3037,7 @@
         <v>19653</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
         <v>401</v>
       </c>
@@ -3051,7 +3078,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
         <v>402</v>
       </c>
@@ -3092,7 +3119,7 @@
         <v>113696</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
@@ -3133,7 +3160,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>397</v>
       </c>
@@ -3174,7 +3201,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>398</v>
       </c>
@@ -3215,7 +3242,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>399</v>
       </c>
@@ -3256,7 +3283,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>205</v>
       </c>
@@ -3297,7 +3324,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>206</v>
       </c>
@@ -3338,7 +3365,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>207</v>
       </c>
@@ -3379,7 +3406,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
         <v>208</v>
       </c>
@@ -3420,7 +3447,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
         <v>437</v>
       </c>
@@ -3461,7 +3488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>438</v>
       </c>
@@ -3502,7 +3529,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>439</v>
       </c>
@@ -3543,7 +3570,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>440</v>
       </c>
@@ -3584,7 +3611,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
         <v>522</v>
       </c>
@@ -3598,7 +3625,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
         <v>566</v>
       </c>
@@ -3606,7 +3633,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>74</v>
       </c>
@@ -3647,7 +3674,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
         <v>75</v>
       </c>
@@ -3688,7 +3715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
         <v>76</v>
       </c>
@@ -3729,7 +3756,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17">
       <c r="A33" s="1" t="s">
         <v>77</v>
       </c>
@@ -3770,7 +3797,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17">
       <c r="A34" s="1" t="s">
         <v>78</v>
       </c>
@@ -3811,7 +3838,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -3822,7 +3849,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17">
       <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
@@ -3836,7 +3863,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17">
       <c r="A37" s="1" t="s">
         <v>67</v>
       </c>
@@ -3850,7 +3877,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17">
       <c r="A38" s="1" t="s">
         <v>66</v>
       </c>
@@ -3891,7 +3918,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17">
       <c r="A39" s="1" t="s">
         <v>65</v>
       </c>
@@ -3932,7 +3959,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17">
       <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
@@ -3943,7 +3970,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17">
       <c r="A41" s="1" t="s">
         <v>63</v>
       </c>
@@ -3984,7 +4011,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17">
       <c r="A42" s="1" t="s">
         <v>79</v>
       </c>
@@ -4025,7 +4052,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17">
       <c r="A43" s="1" t="s">
         <v>313</v>
       </c>
@@ -4078,7 +4105,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17">
       <c r="A44" s="1" t="s">
         <v>62</v>
       </c>
@@ -4131,7 +4158,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17">
       <c r="A45" s="1" t="s">
         <v>568</v>
       </c>
@@ -4154,7 +4181,7 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17">
       <c r="A46" s="1" t="s">
         <v>61</v>
       </c>
@@ -4187,7 +4214,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17">
       <c r="A47" s="1" t="s">
         <v>60</v>
       </c>
@@ -4232,7 +4259,7 @@
       <c r="P47" s="31"/>
       <c r="Q47" s="31"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17">
       <c r="A48" s="1" t="s">
         <v>59</v>
       </c>
@@ -4299,7 +4326,7 @@
         <v>33415.5</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17">
       <c r="A49" s="1" t="s">
         <v>58</v>
       </c>
@@ -4340,7 +4367,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17">
       <c r="A50" s="1" t="s">
         <v>57</v>
       </c>
@@ -4390,7 +4417,7 @@
         <v>718.5</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
@@ -4417,7 +4444,7 @@
       </c>
       <c r="O51" s="1"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -4459,7 +4486,7 @@
       </c>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17">
       <c r="A53" s="1" t="s">
         <v>306</v>
       </c>
@@ -4513,7 +4540,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17">
       <c r="A54" s="1" t="s">
         <v>311</v>
       </c>
@@ -4566,7 +4593,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17">
       <c r="A55" s="1" t="s">
         <v>529</v>
       </c>
@@ -4619,7 +4646,7 @@
         <v>43190072.399999999</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17">
       <c r="A56" s="1" t="s">
         <v>312</v>
       </c>
@@ -4688,7 +4715,7 @@
         <v>0.1125</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17">
       <c r="A57" s="1" t="s">
         <v>314</v>
       </c>
@@ -4757,7 +4784,7 @@
         <v>125.30812499999999</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17">
       <c r="A58" s="1" t="s">
         <v>315</v>
       </c>
@@ -4826,7 +4853,7 @@
         <v>499862.23778592242</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17">
       <c r="A59" s="1" t="s">
         <v>331</v>
       </c>
@@ -4867,7 +4894,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17">
       <c r="A60" s="1" t="s">
         <v>489</v>
       </c>
@@ -4908,7 +4935,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17">
       <c r="A61" s="1" t="s">
         <v>353</v>
       </c>
@@ -4949,7 +4976,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17">
       <c r="A62" s="1" t="s">
         <v>384</v>
       </c>
@@ -4990,7 +5017,7 @@
         <v>0.92800000000000005</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17">
       <c r="A63" s="1" t="s">
         <v>490</v>
       </c>
@@ -5031,7 +5058,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17">
       <c r="A64" s="1" t="s">
         <v>102</v>
       </c>
@@ -5072,7 +5099,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14">
       <c r="A65" s="1" t="s">
         <v>103</v>
       </c>
@@ -5113,7 +5140,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14">
       <c r="A66" s="1" t="s">
         <v>104</v>
       </c>
@@ -5127,7 +5154,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14">
       <c r="A67" s="1" t="s">
         <v>111</v>
       </c>
@@ -5135,7 +5162,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14">
       <c r="A68" s="1" t="s">
         <v>105</v>
       </c>
@@ -5173,7 +5200,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14">
       <c r="A69" s="1" t="s">
         <v>106</v>
       </c>
@@ -5190,7 +5217,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14">
       <c r="A70" s="1" t="s">
         <v>204</v>
       </c>
@@ -5210,7 +5237,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14">
       <c r="A71" s="1" t="s">
         <v>107</v>
       </c>
@@ -5218,7 +5245,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14">
       <c r="A72" s="1" t="s">
         <v>112</v>
       </c>
@@ -5226,7 +5253,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14">
       <c r="A73" s="1" t="s">
         <v>114</v>
       </c>
@@ -5234,7 +5261,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14">
       <c r="A74" s="6" t="s">
         <v>115</v>
       </c>
@@ -5272,7 +5299,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14">
       <c r="A75" s="6" t="s">
         <v>116</v>
       </c>
@@ -5310,7 +5337,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14">
       <c r="A76" s="6" t="s">
         <v>117</v>
       </c>
@@ -5348,7 +5375,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14">
       <c r="A77" s="6" t="s">
         <v>118</v>
       </c>
@@ -5386,7 +5413,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14">
       <c r="A78" s="6" t="s">
         <v>119</v>
       </c>
@@ -5418,7 +5445,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14">
       <c r="A79" s="6" t="s">
         <v>120</v>
       </c>
@@ -5444,7 +5471,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14">
       <c r="A80" s="6" t="s">
         <v>121</v>
       </c>
@@ -5461,7 +5488,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14">
       <c r="A81" s="6" t="s">
         <v>122</v>
       </c>
@@ -5472,7 +5499,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14">
       <c r="A82" s="6" t="s">
         <v>123</v>
       </c>
@@ -5480,7 +5507,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14">
       <c r="A83" s="6" t="s">
         <v>124</v>
       </c>
@@ -5491,7 +5518,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14">
       <c r="A84" s="6" t="s">
         <v>188</v>
       </c>
@@ -5499,7 +5526,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14">
       <c r="A85" s="6" t="s">
         <v>189</v>
       </c>
@@ -5507,7 +5534,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14">
       <c r="A86" s="6" t="s">
         <v>193</v>
       </c>
@@ -5515,7 +5542,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14">
       <c r="A87" s="6" t="s">
         <v>199</v>
       </c>
@@ -5556,7 +5583,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14">
       <c r="A88" s="4" t="s">
         <v>191</v>
       </c>
@@ -5564,7 +5591,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14">
       <c r="A89" s="4" t="s">
         <v>195</v>
       </c>
@@ -5572,7 +5599,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14">
       <c r="A90" s="4" t="s">
         <v>197</v>
       </c>
@@ -5580,7 +5607,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14">
       <c r="A91" s="6" t="s">
         <v>269</v>
       </c>
@@ -5594,7 +5621,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14">
       <c r="A92" s="6" t="s">
         <v>270</v>
       </c>
@@ -5608,7 +5635,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14">
       <c r="A93" s="6" t="s">
         <v>271</v>
       </c>
@@ -5622,7 +5649,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14">
       <c r="A94" s="6" t="s">
         <v>272</v>
       </c>
@@ -5630,7 +5657,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14">
       <c r="A95" s="6" t="s">
         <v>273</v>
       </c>
@@ -5638,7 +5665,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:14">
       <c r="A96" s="6" t="s">
         <v>274</v>
       </c>
@@ -5652,7 +5679,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:14">
       <c r="A97" s="6" t="s">
         <v>275</v>
       </c>
@@ -5660,7 +5687,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:14">
       <c r="A98" s="6" t="s">
         <v>293</v>
       </c>
@@ -5668,7 +5695,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:14">
       <c r="A99" s="6" t="s">
         <v>334</v>
       </c>
@@ -5703,7 +5730,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:14">
       <c r="A100" s="6" t="s">
         <v>488</v>
       </c>
@@ -5729,7 +5756,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:14">
       <c r="A101" s="6" t="s">
         <v>338</v>
       </c>
@@ -5737,7 +5764,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:14">
       <c r="A102" s="6" t="s">
         <v>491</v>
       </c>
@@ -5766,7 +5793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:14">
       <c r="A103" s="6" t="s">
         <v>493</v>
       </c>
@@ -5798,7 +5825,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:14">
       <c r="A104" s="6" t="s">
         <v>498</v>
       </c>
@@ -5812,7 +5839,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:14">
       <c r="A105" s="6" t="s">
         <v>499</v>
       </c>
@@ -5833,16 +5860,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -5856,7 +5883,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -5877,7 +5904,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -5898,7 +5925,7 @@
         <v>0.92622883301508352</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -5917,8 +5944,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -5939,7 +5966,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -5963,7 +5990,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -5992,7 +6019,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -6021,7 +6048,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -6038,19 +6065,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:F9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -6065,7 +6092,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -6087,7 +6114,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -6109,7 +6136,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -6129,7 +6156,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -6140,7 +6167,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="A6" s="35"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -6150,7 +6177,7 @@
       <c r="G6" s="36"/>
       <c r="H6" s="37"/>
     </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -6160,7 +6187,7 @@
       <c r="G7" s="36"/>
       <c r="H7" s="37"/>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>226</v>
       </c>
@@ -6182,7 +6209,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="37"/>
     </row>
-    <row r="9" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="30" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -6207,7 +6234,7 @@
       </c>
       <c r="H9" s="37"/>
     </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -6237,7 +6264,7 @@
       </c>
       <c r="H10" s="37"/>
     </row>
-    <row r="11" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="30" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>221</v>
       </c>
@@ -6267,7 +6294,7 @@
       </c>
       <c r="H11" s="37"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" s="12" t="s">
         <v>239</v>
       </c>
@@ -6279,90 +6306,173 @@
       <c r="G12" s="13"/>
       <c r="H12" s="37"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="H13" s="37"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="37"/>
+    <row r="14" spans="1:11" ht="44" thickBot="1">
+      <c r="A14" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>623</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>624</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>625</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>626</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>627</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>628</v>
+      </c>
       <c r="H14" s="37"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="16"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="37"/>
+    <row r="15" spans="1:11" ht="30" thickBot="1">
+      <c r="A15" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B15" s="32">
+        <v>0.13169073093611702</v>
+      </c>
+      <c r="C15" s="32">
+        <v>0.20145928952848952</v>
+      </c>
+      <c r="D15" s="32">
+        <v>0.26537793566411777</v>
+      </c>
+      <c r="E15" s="32">
+        <v>0.22558586499486741</v>
+      </c>
+      <c r="F15" s="33">
+        <v>0.13797875654055569</v>
+      </c>
+      <c r="G15">
+        <v>3.7907422335852557E-2</v>
+      </c>
+      <c r="H15" s="22">
+        <f>SUM(B15:G15)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16" thickBot="1">
+      <c r="A16" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B16" s="13">
+        <f>ROUND(2000*B15,0)</f>
+        <v>263</v>
+      </c>
+      <c r="C16" s="13">
+        <f>ROUND(2000*C15,0)</f>
+        <v>403</v>
+      </c>
+      <c r="D16" s="13">
+        <f>ROUND(2000*D15,0)</f>
+        <v>531</v>
+      </c>
+      <c r="E16" s="13">
+        <f>ROUND(2000*E15,0)</f>
+        <v>451</v>
+      </c>
+      <c r="F16" s="13">
+        <f>ROUND(2000*F15,0)</f>
+        <v>276</v>
+      </c>
+      <c r="G16" s="13">
+        <f>ROUND(2000*G15,0)</f>
+        <v>76</v>
+      </c>
+      <c r="H16" s="3">
+        <f>SUM(B16:G16)</f>
+        <v>2000</v>
+      </c>
+      <c r="K16" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" thickBot="1">
+      <c r="A17" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" s="2">
+        <f>ROUND(2200*B15,0)</f>
+        <v>290</v>
+      </c>
+      <c r="C17" s="2">
+        <f>ROUND(2200*C15,0)</f>
+        <v>443</v>
+      </c>
+      <c r="D17" s="2">
+        <f>ROUND(2200*D15,0)</f>
+        <v>584</v>
+      </c>
+      <c r="E17" s="2">
+        <f>ROUND(2200*E15,0)</f>
+        <v>496</v>
+      </c>
+      <c r="F17" s="2">
+        <f>ROUND(2200*F15,0)</f>
+        <v>304</v>
+      </c>
+      <c r="G17" s="2">
+        <f>ROUND(2200*G15,0)</f>
+        <v>83</v>
+      </c>
+      <c r="H17" s="3">
+        <f>SUM(B17:G17)</f>
+        <v>2200</v>
+      </c>
+      <c r="K17" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="14"/>
       <c r="H18" s="37"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="A19" s="12"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="33"/>
-      <c r="G19" s="40"/>
+      <c r="G19" s="39"/>
       <c r="H19" s="37"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11">
       <c r="A20" s="12"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
-      <c r="G20" s="41"/>
+      <c r="G20" s="40"/>
       <c r="H20" s="37"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11">
       <c r="A21" s="12"/>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
       <c r="F21" s="35"/>
-      <c r="G21" s="41"/>
+      <c r="G21" s="40"/>
       <c r="H21" s="37"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11">
       <c r="A22" s="12"/>
       <c r="B22" s="35"/>
       <c r="C22" s="35"/>
@@ -6372,7 +6482,7 @@
       <c r="G22" s="37"/>
       <c r="H22" s="37"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -6382,7 +6492,7 @@
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11">
       <c r="A24" s="16"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
@@ -6392,17 +6502,17 @@
       <c r="G24" s="37"/>
       <c r="H24" s="37"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11">
       <c r="A25" s="12"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
-      <c r="D25" s="40"/>
+      <c r="D25" s="39"/>
       <c r="E25" s="37"/>
       <c r="F25" s="37"/>
       <c r="G25" s="37"/>
       <c r="H25" s="37"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11">
       <c r="A26" s="12"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
@@ -6412,7 +6522,7 @@
       <c r="G26" s="37"/>
       <c r="H26" s="37"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11">
       <c r="A27" s="12"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -6422,7 +6532,7 @@
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11">
       <c r="A28" s="12"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
@@ -6432,7 +6542,7 @@
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -6448,16 +6558,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -6471,7 +6581,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -6492,7 +6602,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -6513,7 +6623,7 @@
         <v>0.99992877771181621</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -6532,8 +6642,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -6554,7 +6664,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -6578,7 +6688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -6607,7 +6717,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -6636,7 +6746,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -6653,16 +6763,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -6676,7 +6786,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -6697,7 +6807,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -6718,7 +6828,7 @@
         <v>0.97760081385085629</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -6737,8 +6847,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -6759,7 +6869,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -6783,7 +6893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -6812,7 +6922,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -6841,7 +6951,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -6858,16 +6968,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -6881,7 +6991,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -6902,7 +7012,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -6923,7 +7033,7 @@
         <v>1.0341140064832992</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -6942,8 +7052,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -6964,7 +7074,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -6988,7 +7098,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -7017,7 +7127,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -7046,7 +7156,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -7063,16 +7173,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -7086,7 +7196,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -7107,7 +7217,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -7128,7 +7238,7 @@
         <v>0.95217958067188335</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -7147,8 +7257,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -7169,7 +7279,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -7193,7 +7303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -7222,7 +7332,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -7251,7 +7361,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -7268,16 +7378,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -7291,7 +7401,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -7312,7 +7422,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -7333,7 +7443,7 @@
         <v>0.92970833595125124</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -7352,8 +7462,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -7374,7 +7484,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -7398,7 +7508,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -7427,7 +7537,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -7456,7 +7566,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -7473,16 +7583,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -7496,7 +7606,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -7517,7 +7627,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -7538,7 +7648,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -7557,8 +7667,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -7579,7 +7689,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -7603,7 +7713,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -7632,7 +7742,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -7661,7 +7771,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -7678,16 +7788,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>240</v>
       </c>
@@ -7704,7 +7814,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>245</v>
       </c>
@@ -7721,7 +7831,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>532</v>
       </c>
@@ -7738,7 +7848,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>239</v>
       </c>
@@ -7756,7 +7866,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -7780,7 +7890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>245</v>
       </c>
@@ -7805,7 +7915,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>532</v>
       </c>
@@ -7834,7 +7944,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -7858,10 +7968,10 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>248</v>
       </c>
@@ -7878,7 +7988,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>245</v>
       </c>
@@ -7899,7 +8009,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>532</v>
       </c>
@@ -7924,7 +8034,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>239</v>
       </c>
@@ -7945,13 +8055,13 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>253</v>
       </c>
@@ -7968,7 +8078,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>245</v>
       </c>
@@ -7989,7 +8099,7 @@
         <v>100.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>532</v>
       </c>
@@ -8014,7 +8124,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>239</v>
       </c>
@@ -8035,7 +8145,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>258</v>
       </c>
@@ -8049,7 +8159,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>245</v>
       </c>
@@ -8063,7 +8173,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>532</v>
       </c>
@@ -8080,7 +8190,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>239</v>
       </c>
@@ -8095,11 +8205,11 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>263</v>
       </c>
@@ -8116,7 +8226,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>245</v>
       </c>
@@ -8133,7 +8243,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>532</v>
       </c>
@@ -8154,7 +8264,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>239</v>
       </c>
@@ -8174,30 +8284,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="G22" sqref="A18:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -8212,7 +8322,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -8230,7 +8340,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -8250,7 +8360,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -8270,7 +8380,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -8281,7 +8391,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -8290,7 +8400,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -8311,7 +8421,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -8335,7 +8445,7 @@
         <v>1.0001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -8364,7 +8474,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -8393,8 +8503,8 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="16" thickBot="1"/>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>238</v>
       </c>
@@ -8412,7 +8522,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="8" t="s">
         <v>237</v>
       </c>
@@ -8432,7 +8542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>220</v>
       </c>
@@ -8457,7 +8567,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>221</v>
       </c>
@@ -8482,12 +8592,12 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" s="16" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="12" t="s">
         <v>222</v>
       </c>
@@ -8507,7 +8617,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="8" t="s">
         <v>219</v>
       </c>
@@ -8531,7 +8641,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>220</v>
       </c>
@@ -8560,7 +8670,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>221</v>
       </c>
@@ -8589,7 +8699,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
         <v>239</v>
       </c>
@@ -8598,7 +8708,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="16" t="s">
         <v>340</v>
       </c>
@@ -8609,7 +8719,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>219</v>
       </c>
@@ -8624,7 +8734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>220</v>
       </c>
@@ -8641,7 +8751,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>221</v>
       </c>
@@ -8658,7 +8768,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7">
       <c r="A28" s="12" t="s">
         <v>239</v>
       </c>
@@ -8669,22 +8779,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>280</v>
       </c>
@@ -8710,7 +8820,7 @@
       <c r="K1" s="13"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -8743,7 +8853,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -8777,7 +8887,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -8811,7 +8921,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -8827,7 +8937,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="0.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="0.5" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -8841,14 +8951,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>223</v>
       </c>
@@ -8868,7 +8978,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -8891,7 +9001,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -8916,7 +9026,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>221</v>
       </c>
@@ -8941,7 +9051,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" s="12" t="s">
         <v>239</v>
       </c>
@@ -8957,7 +9067,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -8971,7 +9081,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>226</v>
       </c>
@@ -8997,7 +9107,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -9026,7 +9136,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -9060,7 +9170,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -9094,7 +9204,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -9110,7 +9220,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -9124,7 +9234,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>232</v>
       </c>
@@ -9148,7 +9258,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>237</v>
       </c>
@@ -9174,7 +9284,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -9205,7 +9315,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>221</v>
       </c>
@@ -9236,7 +9346,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>239</v>
       </c>
@@ -9246,7 +9356,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -9254,7 +9364,7 @@
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" ht="16.5" customHeight="1" thickBot="1">
       <c r="A26" s="12" t="s">
         <v>513</v>
       </c>
@@ -9271,7 +9381,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>219</v>
       </c>
@@ -9290,7 +9400,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" ht="16" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>220</v>
       </c>
@@ -9312,7 +9422,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" ht="16" thickBot="1">
       <c r="A29" s="8" t="s">
         <v>517</v>
       </c>
@@ -9331,7 +9441,7 @@
       </c>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>516</v>
       </c>
@@ -9353,7 +9463,7 @@
       </c>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>518</v>
       </c>
@@ -9375,7 +9485,7 @@
       </c>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12">
       <c r="A32" s="12" t="s">
         <v>239</v>
       </c>
@@ -9386,12 +9496,12 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
-    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" ht="30" thickBot="1">
       <c r="A37" s="8" t="s">
         <v>210</v>
       </c>
@@ -9421,7 +9531,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="8" t="s">
         <v>219</v>
       </c>
@@ -9454,7 +9564,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="8" t="s">
         <v>220</v>
       </c>
@@ -9495,7 +9605,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="8" t="s">
         <v>221</v>
       </c>
@@ -9536,7 +9646,7 @@
         <v>2196</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10">
       <c r="A41" s="12" t="s">
         <v>239</v>
       </c>
@@ -9550,7 +9660,7 @@
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10">
       <c r="A42" s="2"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -9562,12 +9672,12 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>285</v>
       </c>
@@ -9588,7 +9698,7 @@
       </c>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="8" t="s">
         <v>219</v>
       </c>
@@ -9612,7 +9722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="8" t="s">
         <v>220</v>
       </c>
@@ -9641,7 +9751,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="8" t="s">
         <v>221</v>
       </c>
@@ -9670,7 +9780,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10">
       <c r="A48" s="12" t="s">
         <v>239</v>
       </c>
@@ -9681,7 +9791,7 @@
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7">
       <c r="A49" s="2"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -9697,16 +9807,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="75" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -9720,7 +9830,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -9741,7 +9851,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -9762,7 +9872,7 @@
         <v>0.95277529961698948</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -9781,8 +9891,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -9803,7 +9913,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -9827,7 +9937,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -9856,7 +9966,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -9885,7 +9995,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -9896,7 +10006,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -9922,7 +10032,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -9952,7 +10062,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -9987,7 +10097,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -10022,7 +10132,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -10043,16 +10153,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -10066,7 +10176,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -10087,7 +10197,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -10108,7 +10218,7 @@
         <v>0.90805800128462044</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -10127,8 +10237,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -10149,7 +10259,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -10173,7 +10283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -10202,7 +10312,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -10231,7 +10341,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -10242,7 +10352,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -10262,7 +10372,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -10286,7 +10396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -10315,7 +10425,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -10343,8 +10453,11 @@
         <f>SUM(B16:F16)</f>
         <v>2201</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="J16" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -10359,16 +10472,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H17" sqref="A13:H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -10382,7 +10495,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -10403,7 +10516,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -10424,7 +10537,7 @@
         <v>0.9267197256851698</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -10443,8 +10556,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="16" thickBot="1"/>
+    <row r="7" spans="1:13" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -10465,7 +10578,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -10489,7 +10602,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -10518,7 +10631,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -10547,7 +10660,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -10558,7 +10671,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -10577,7 +10690,7 @@
       <c r="F13" s="24" t="s">
         <v>593</v>
       </c>
-      <c r="G13" s="42" t="s">
+      <c r="G13" s="41" t="s">
         <v>594</v>
       </c>
       <c r="L13" t="s">
@@ -10587,7 +10700,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -10620,7 +10733,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -10659,7 +10772,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -10698,7 +10811,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -10713,7 +10826,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13">
       <c r="L18" t="s">
         <v>594</v>
       </c>
@@ -10727,16 +10840,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -10750,7 +10863,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -10771,7 +10884,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -10792,7 +10905,7 @@
         <v>0.94196267708118475</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -10811,8 +10924,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -10833,7 +10946,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -10857,7 +10970,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -10886,7 +10999,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -10915,7 +11028,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -10926,7 +11039,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="44" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -10945,11 +11058,11 @@
       <c r="F13" s="24" t="s">
         <v>605</v>
       </c>
-      <c r="G13" s="42" t="s">
+      <c r="G13" s="41" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -10976,7 +11089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -11015,7 +11128,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -11048,7 +11161,7 @@
         <v>2199</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -11063,16 +11176,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -11086,7 +11199,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -11107,7 +11220,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -11128,7 +11241,7 @@
         <v>0.98351979013457747</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -11147,8 +11260,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -11169,7 +11282,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -11193,7 +11306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -11222,7 +11335,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -11251,7 +11364,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -11262,7 +11375,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -11282,7 +11395,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -11306,7 +11419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -11335,7 +11448,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -11364,7 +11477,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>

</xml_diff>

<commit_message>
Add regions quota Spain
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34054314-1E4C-A94A-BC48-DAFBF6D3391F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
     <sheet name="quotas_MX" sheetId="17" r:id="rId16"/>
     <sheet name="quotas_SK" sheetId="18" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="660">
   <si>
     <t>Country</t>
   </si>
@@ -1990,18 +1991,54 @@
   </si>
   <si>
     <t>170k</t>
+  </si>
+  <si>
+    <t>Center:</t>
+  </si>
+  <si>
+    <t>Madrid, Castilla-la-Mancha</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>Norht-West</t>
+  </si>
+  <si>
+    <t>East:</t>
+  </si>
+  <si>
+    <t>Aragon, Navarre, La Rioja, Basque Country, Cantabria</t>
+  </si>
+  <si>
+    <t>Castille and Leon, Asturias, Galicia</t>
+  </si>
+  <si>
+    <t>Catalonia, Valencia, Balearic Islands</t>
+  </si>
+  <si>
+    <t>Extremadura, Andalusia, Murcia, Canaris Islands</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Autonomous_communities_of_Spain#Autonomous_communities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2214,7 +2251,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2491,27 +2528,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.6328125" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" customWidth="1"/>
-    <col min="3" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="9.6328125" customWidth="1"/>
-    <col min="12" max="12" width="9.6328125" customWidth="1"/>
-    <col min="13" max="13" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" customWidth="1"/>
-    <col min="17" max="17" width="13.6328125" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2564,7 +2601,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>455</v>
       </c>
@@ -2605,7 +2642,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
         <v>456</v>
       </c>
@@ -2646,7 +2683,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
         <v>457</v>
       </c>
@@ -2685,7 +2722,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
         <v>497</v>
       </c>
@@ -2712,7 +2749,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
         <v>458</v>
       </c>
@@ -2735,7 +2772,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
@@ -2788,7 +2825,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -2841,7 +2878,7 @@
         <v>1113.8499999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17">
       <c r="A9" s="2" t="s">
         <v>169</v>
       </c>
@@ -2894,7 +2931,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17">
       <c r="A10" s="2" t="s">
         <v>170</v>
       </c>
@@ -2947,7 +2984,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
         <v>181</v>
       </c>
@@ -3000,7 +3037,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17">
       <c r="A12" s="1" t="s">
         <v>182</v>
       </c>
@@ -3053,7 +3090,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
         <v>400</v>
       </c>
@@ -3094,7 +3131,7 @@
         <v>19653</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
         <v>401</v>
       </c>
@@ -3135,7 +3172,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
         <v>402</v>
       </c>
@@ -3176,7 +3213,7 @@
         <v>113696</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
@@ -3217,7 +3254,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
         <v>397</v>
       </c>
@@ -3258,7 +3295,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>398</v>
       </c>
@@ -3299,7 +3336,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>399</v>
       </c>
@@ -3340,7 +3377,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>205</v>
       </c>
@@ -3381,7 +3418,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>206</v>
       </c>
@@ -3422,7 +3459,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>207</v>
       </c>
@@ -3463,7 +3500,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>208</v>
       </c>
@@ -3504,7 +3541,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>437</v>
       </c>
@@ -3545,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>438</v>
       </c>
@@ -3586,7 +3623,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>439</v>
       </c>
@@ -3627,7 +3664,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>440</v>
       </c>
@@ -3668,7 +3705,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>522</v>
       </c>
@@ -3682,7 +3719,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
         <v>564</v>
       </c>
@@ -3690,7 +3727,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>74</v>
       </c>
@@ -3731,7 +3768,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>75</v>
       </c>
@@ -3772,7 +3809,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>76</v>
       </c>
@@ -3813,7 +3850,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17">
       <c r="A33" s="1" t="s">
         <v>77</v>
       </c>
@@ -3854,7 +3891,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17">
       <c r="A34" s="1" t="s">
         <v>78</v>
       </c>
@@ -3895,7 +3932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -3906,7 +3943,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17">
       <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
@@ -3920,7 +3957,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17">
       <c r="A37" s="1" t="s">
         <v>67</v>
       </c>
@@ -3934,7 +3971,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17">
       <c r="A38" s="1" t="s">
         <v>66</v>
       </c>
@@ -3975,7 +4012,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17">
       <c r="A39" s="1" t="s">
         <v>65</v>
       </c>
@@ -4016,7 +4053,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17">
       <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
@@ -4027,7 +4064,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17">
       <c r="A41" s="1" t="s">
         <v>63</v>
       </c>
@@ -4068,7 +4105,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17">
       <c r="A42" s="1" t="s">
         <v>79</v>
       </c>
@@ -4109,7 +4146,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17">
       <c r="A43" s="1" t="s">
         <v>313</v>
       </c>
@@ -4162,7 +4199,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17">
       <c r="A44" s="1" t="s">
         <v>62</v>
       </c>
@@ -4215,7 +4252,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17">
       <c r="A45" s="1" t="s">
         <v>566</v>
       </c>
@@ -4238,7 +4275,7 @@
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17">
       <c r="A46" s="1" t="s">
         <v>61</v>
       </c>
@@ -4273,7 +4310,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17">
       <c r="A47" s="1" t="s">
         <v>60</v>
       </c>
@@ -4320,7 +4357,7 @@
       <c r="P47" s="31"/>
       <c r="Q47" s="31"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17">
       <c r="A48" s="1" t="s">
         <v>59</v>
       </c>
@@ -4387,7 +4424,7 @@
         <v>33415.5</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17">
       <c r="A49" s="1" t="s">
         <v>58</v>
       </c>
@@ -4428,7 +4465,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17">
       <c r="A50" s="1" t="s">
         <v>57</v>
       </c>
@@ -4478,7 +4515,7 @@
         <v>718.5</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
@@ -4505,7 +4542,7 @@
       </c>
       <c r="O51" s="1"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -4547,7 +4584,7 @@
       </c>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17">
       <c r="A53" s="1" t="s">
         <v>306</v>
       </c>
@@ -4601,7 +4638,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17">
       <c r="A54" s="1" t="s">
         <v>311</v>
       </c>
@@ -4654,7 +4691,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17">
       <c r="A55" s="1" t="s">
         <v>529</v>
       </c>
@@ -4707,7 +4744,7 @@
         <v>43190072.399999999</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17">
       <c r="A56" s="1" t="s">
         <v>312</v>
       </c>
@@ -4776,7 +4813,7 @@
         <v>0.1125</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17">
       <c r="A57" s="1" t="s">
         <v>314</v>
       </c>
@@ -4845,7 +4882,7 @@
         <v>125.30812499999999</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17">
       <c r="A58" s="1" t="s">
         <v>315</v>
       </c>
@@ -4914,7 +4951,7 @@
         <v>499862.23778592242</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17">
       <c r="A59" s="1" t="s">
         <v>331</v>
       </c>
@@ -4955,7 +4992,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17">
       <c r="A60" s="1" t="s">
         <v>489</v>
       </c>
@@ -4996,7 +5033,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17">
       <c r="A61" s="1" t="s">
         <v>353</v>
       </c>
@@ -5037,7 +5074,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17">
       <c r="A62" s="1" t="s">
         <v>384</v>
       </c>
@@ -5078,7 +5115,7 @@
         <v>0.92800000000000005</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17">
       <c r="A63" s="1" t="s">
         <v>490</v>
       </c>
@@ -5119,7 +5156,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17">
       <c r="A64" s="1" t="s">
         <v>102</v>
       </c>
@@ -5160,7 +5197,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14">
       <c r="A65" s="1" t="s">
         <v>103</v>
       </c>
@@ -5201,7 +5238,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14">
       <c r="A66" s="1" t="s">
         <v>104</v>
       </c>
@@ -5215,7 +5252,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14">
       <c r="A67" s="1" t="s">
         <v>111</v>
       </c>
@@ -5223,7 +5260,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14">
       <c r="A68" s="1" t="s">
         <v>105</v>
       </c>
@@ -5261,7 +5298,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14">
       <c r="A69" s="1" t="s">
         <v>106</v>
       </c>
@@ -5278,7 +5315,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14">
       <c r="A70" s="1" t="s">
         <v>204</v>
       </c>
@@ -5298,7 +5335,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14">
       <c r="A71" s="1" t="s">
         <v>107</v>
       </c>
@@ -5306,7 +5343,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14">
       <c r="A72" s="1" t="s">
         <v>112</v>
       </c>
@@ -5314,7 +5351,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14">
       <c r="A73" s="1" t="s">
         <v>114</v>
       </c>
@@ -5322,7 +5359,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14">
       <c r="A74" s="6" t="s">
         <v>115</v>
       </c>
@@ -5363,7 +5400,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14">
       <c r="A75" s="6" t="s">
         <v>116</v>
       </c>
@@ -5404,7 +5441,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14">
       <c r="A76" s="6" t="s">
         <v>117</v>
       </c>
@@ -5445,7 +5482,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14">
       <c r="A77" s="6" t="s">
         <v>118</v>
       </c>
@@ -5486,7 +5523,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14">
       <c r="A78" s="6" t="s">
         <v>119</v>
       </c>
@@ -5521,7 +5558,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14">
       <c r="A79" s="6" t="s">
         <v>120</v>
       </c>
@@ -5550,7 +5587,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14">
       <c r="A80" s="6" t="s">
         <v>121</v>
       </c>
@@ -5570,7 +5607,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14">
       <c r="A81" s="6" t="s">
         <v>122</v>
       </c>
@@ -5584,7 +5621,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14">
       <c r="A82" s="6" t="s">
         <v>123</v>
       </c>
@@ -5595,7 +5632,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14">
       <c r="A83" s="6" t="s">
         <v>124</v>
       </c>
@@ -5609,7 +5646,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14">
       <c r="A84" s="6" t="s">
         <v>188</v>
       </c>
@@ -5617,7 +5654,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14">
       <c r="A85" s="6" t="s">
         <v>189</v>
       </c>
@@ -5625,7 +5662,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14">
       <c r="A86" s="6" t="s">
         <v>193</v>
       </c>
@@ -5633,7 +5670,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14">
       <c r="A87" s="6" t="s">
         <v>199</v>
       </c>
@@ -5674,7 +5711,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14">
       <c r="A88" s="4" t="s">
         <v>191</v>
       </c>
@@ -5682,7 +5719,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14">
       <c r="A89" s="4" t="s">
         <v>195</v>
       </c>
@@ -5690,7 +5727,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14">
       <c r="A90" s="4" t="s">
         <v>197</v>
       </c>
@@ -5698,7 +5735,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14">
       <c r="A91" s="6" t="s">
         <v>269</v>
       </c>
@@ -5712,7 +5749,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14">
       <c r="A92" s="6" t="s">
         <v>270</v>
       </c>
@@ -5726,7 +5763,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14">
       <c r="A93" s="6" t="s">
         <v>271</v>
       </c>
@@ -5740,7 +5777,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14">
       <c r="A94" s="6" t="s">
         <v>272</v>
       </c>
@@ -5748,7 +5785,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14">
       <c r="A95" s="6" t="s">
         <v>273</v>
       </c>
@@ -5756,7 +5793,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:14">
       <c r="A96" s="6" t="s">
         <v>274</v>
       </c>
@@ -5770,7 +5807,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:14">
       <c r="A97" s="6" t="s">
         <v>275</v>
       </c>
@@ -5778,7 +5815,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:14">
       <c r="A98" s="6" t="s">
         <v>293</v>
       </c>
@@ -5786,7 +5823,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:14">
       <c r="A99" s="6" t="s">
         <v>334</v>
       </c>
@@ -5824,7 +5861,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:14">
       <c r="A100" s="6" t="s">
         <v>488</v>
       </c>
@@ -5850,7 +5887,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:14">
       <c r="A101" s="6" t="s">
         <v>338</v>
       </c>
@@ -5858,7 +5895,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:14">
       <c r="A102" s="6" t="s">
         <v>491</v>
       </c>
@@ -5887,7 +5924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:14">
       <c r="A103" s="6" t="s">
         <v>493</v>
       </c>
@@ -5919,7 +5956,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:14">
       <c r="A104" s="6" t="s">
         <v>498</v>
       </c>
@@ -5933,7 +5970,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:14">
       <c r="A105" s="6" t="s">
         <v>499</v>
       </c>
@@ -5954,16 +5991,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -5977,7 +6014,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -5998,7 +6035,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -6019,7 +6056,7 @@
         <v>0.92622883301508352</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -6038,8 +6075,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -6060,7 +6097,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -6084,7 +6121,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -6113,7 +6150,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -6142,7 +6179,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -6159,19 +6196,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -6186,7 +6223,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -6208,7 +6245,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -6230,7 +6267,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -6250,7 +6287,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -6261,7 +6298,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="A6" s="35"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -6271,7 +6308,7 @@
       <c r="G6" s="36"/>
       <c r="H6" s="37"/>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -6281,7 +6318,7 @@
       <c r="G7" s="36"/>
       <c r="H7" s="37"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>226</v>
       </c>
@@ -6303,7 +6340,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="37"/>
     </row>
-    <row r="9" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="30" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -6328,7 +6365,7 @@
       </c>
       <c r="H9" s="37"/>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -6358,7 +6395,7 @@
       </c>
       <c r="H10" s="37"/>
     </row>
-    <row r="11" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="30" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>221</v>
       </c>
@@ -6388,7 +6425,7 @@
       </c>
       <c r="H11" s="37"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" s="12" t="s">
         <v>239</v>
       </c>
@@ -6400,10 +6437,10 @@
       <c r="G12" s="13"/>
       <c r="H12" s="37"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="H13" s="37"/>
     </row>
-    <row r="14" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="44" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -6427,7 +6464,7 @@
       </c>
       <c r="H14" s="37"/>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -6454,7 +6491,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -6490,7 +6527,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -6526,7 +6563,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -6536,7 +6573,7 @@
       <c r="E18" s="14"/>
       <c r="H18" s="37"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="A19" s="12"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
@@ -6546,7 +6583,7 @@
       <c r="G19" s="39"/>
       <c r="H19" s="37"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11">
       <c r="A20" s="12"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -6556,7 +6593,7 @@
       <c r="G20" s="40"/>
       <c r="H20" s="37"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11">
       <c r="A21" s="12"/>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
@@ -6566,7 +6603,7 @@
       <c r="G21" s="40"/>
       <c r="H21" s="37"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11">
       <c r="A22" s="12"/>
       <c r="B22" s="35"/>
       <c r="C22" s="35"/>
@@ -6576,7 +6613,7 @@
       <c r="G22" s="37"/>
       <c r="H22" s="37"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -6586,7 +6623,7 @@
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11">
       <c r="A24" s="16"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
@@ -6596,7 +6633,7 @@
       <c r="G24" s="37"/>
       <c r="H24" s="37"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11">
       <c r="A25" s="12"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -6606,7 +6643,7 @@
       <c r="G25" s="37"/>
       <c r="H25" s="37"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11">
       <c r="A26" s="12"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
@@ -6616,7 +6653,7 @@
       <c r="G26" s="37"/>
       <c r="H26" s="37"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11">
       <c r="A27" s="12"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -6626,7 +6663,7 @@
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11">
       <c r="A28" s="12"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
@@ -6636,7 +6673,7 @@
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -6652,16 +6689,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -6675,7 +6712,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -6696,7 +6733,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -6717,7 +6754,7 @@
         <v>0.99992877771181621</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -6736,8 +6773,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -6758,7 +6795,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -6782,7 +6819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -6811,7 +6848,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -6840,7 +6877,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -6857,16 +6894,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -6880,7 +6917,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -6901,7 +6938,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -6922,7 +6959,7 @@
         <v>0.97760081385085629</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -6941,8 +6978,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -6963,7 +7000,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -6987,7 +7024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -7016,7 +7053,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -7045,7 +7082,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -7062,16 +7099,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -7085,7 +7122,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -7106,7 +7143,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -7127,7 +7164,7 @@
         <v>1.0341140064832992</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -7146,8 +7183,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -7168,7 +7205,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -7192,7 +7229,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -7221,7 +7258,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -7250,7 +7287,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -7267,16 +7304,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -7290,7 +7327,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -7311,7 +7348,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -7332,7 +7369,7 @@
         <v>0.95217958067188335</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -7351,8 +7388,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -7373,7 +7410,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -7397,7 +7434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -7426,7 +7463,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -7455,7 +7492,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -7472,16 +7509,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -7495,7 +7532,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -7516,7 +7553,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -7537,7 +7574,7 @@
         <v>0.92970833595125124</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -7556,8 +7593,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -7578,7 +7615,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -7602,7 +7639,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -7631,7 +7668,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -7660,7 +7697,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -7677,16 +7714,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -7700,7 +7737,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -7721,7 +7758,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -7742,7 +7779,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -7761,8 +7798,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -7783,7 +7820,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -7807,7 +7844,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -7836,7 +7873,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -7865,7 +7902,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -7882,16 +7919,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>240</v>
       </c>
@@ -7908,7 +7945,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>245</v>
       </c>
@@ -7925,7 +7962,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>532</v>
       </c>
@@ -7942,7 +7979,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>239</v>
       </c>
@@ -7960,7 +7997,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -7984,7 +8021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>245</v>
       </c>
@@ -8009,7 +8046,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>532</v>
       </c>
@@ -8038,7 +8075,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -8062,10 +8099,10 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>248</v>
       </c>
@@ -8082,7 +8119,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>245</v>
       </c>
@@ -8103,7 +8140,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>532</v>
       </c>
@@ -8128,7 +8165,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>239</v>
       </c>
@@ -8149,13 +8186,13 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>253</v>
       </c>
@@ -8172,7 +8209,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>245</v>
       </c>
@@ -8193,7 +8230,7 @@
         <v>100.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>532</v>
       </c>
@@ -8218,7 +8255,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>239</v>
       </c>
@@ -8239,7 +8276,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>258</v>
       </c>
@@ -8253,7 +8290,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>245</v>
       </c>
@@ -8267,7 +8304,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>532</v>
       </c>
@@ -8284,7 +8321,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>239</v>
       </c>
@@ -8299,11 +8336,11 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>263</v>
       </c>
@@ -8320,7 +8357,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>245</v>
       </c>
@@ -8337,7 +8374,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>532</v>
       </c>
@@ -8358,7 +8395,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>239</v>
       </c>
@@ -8378,30 +8415,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D28" sqref="A24:D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -8416,7 +8453,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -8434,7 +8471,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -8454,7 +8491,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -8474,7 +8511,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -8485,7 +8522,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -8494,7 +8531,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -8515,7 +8552,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -8539,7 +8576,7 @@
         <v>1.0001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -8568,7 +8605,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -8597,8 +8634,8 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="16" thickBot="1"/>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>238</v>
       </c>
@@ -8616,7 +8653,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="8" t="s">
         <v>237</v>
       </c>
@@ -8636,7 +8673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>220</v>
       </c>
@@ -8661,7 +8698,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>221</v>
       </c>
@@ -8686,12 +8723,12 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" s="16" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="12" t="s">
         <v>222</v>
       </c>
@@ -8711,7 +8748,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="8" t="s">
         <v>219</v>
       </c>
@@ -8735,7 +8772,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>220</v>
       </c>
@@ -8764,7 +8801,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>221</v>
       </c>
@@ -8793,7 +8830,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
         <v>239</v>
       </c>
@@ -8802,7 +8839,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="16" t="s">
         <v>340</v>
       </c>
@@ -8813,7 +8850,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>219</v>
       </c>
@@ -8828,7 +8865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>220</v>
       </c>
@@ -8845,7 +8882,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>221</v>
       </c>
@@ -8862,7 +8899,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7">
       <c r="A28" s="12" t="s">
         <v>239</v>
       </c>
@@ -8873,22 +8910,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>280</v>
       </c>
@@ -8914,7 +8951,7 @@
       <c r="K1" s="13"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -8947,7 +8984,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -8981,7 +9018,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -9015,7 +9052,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -9031,7 +9068,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="0.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="0.5" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -9045,14 +9082,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>223</v>
       </c>
@@ -9072,7 +9109,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -9095,7 +9132,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -9120,7 +9157,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>221</v>
       </c>
@@ -9145,7 +9182,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" s="12" t="s">
         <v>239</v>
       </c>
@@ -9161,7 +9198,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -9175,7 +9212,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>226</v>
       </c>
@@ -9201,7 +9238,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -9230,7 +9267,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -9264,7 +9301,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -9298,7 +9335,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -9314,7 +9351,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -9328,7 +9365,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>232</v>
       </c>
@@ -9352,7 +9389,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>237</v>
       </c>
@@ -9378,7 +9415,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -9409,7 +9446,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>221</v>
       </c>
@@ -9440,7 +9477,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>239</v>
       </c>
@@ -9450,7 +9487,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -9458,7 +9495,7 @@
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" ht="16.5" customHeight="1" thickBot="1">
       <c r="A26" s="12" t="s">
         <v>513</v>
       </c>
@@ -9475,7 +9512,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>219</v>
       </c>
@@ -9494,7 +9531,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" ht="16" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>220</v>
       </c>
@@ -9516,7 +9553,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" ht="16" thickBot="1">
       <c r="A29" s="8" t="s">
         <v>517</v>
       </c>
@@ -9535,7 +9572,7 @@
       </c>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>516</v>
       </c>
@@ -9557,7 +9594,7 @@
       </c>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>518</v>
       </c>
@@ -9579,7 +9616,7 @@
       </c>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12">
       <c r="A32" s="12" t="s">
         <v>239</v>
       </c>
@@ -9590,12 +9627,12 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
-    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" ht="30" thickBot="1">
       <c r="A37" s="8" t="s">
         <v>210</v>
       </c>
@@ -9625,7 +9662,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="8" t="s">
         <v>219</v>
       </c>
@@ -9658,7 +9695,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="8" t="s">
         <v>220</v>
       </c>
@@ -9699,7 +9736,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="8" t="s">
         <v>221</v>
       </c>
@@ -9740,7 +9777,7 @@
         <v>2196</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10">
       <c r="A41" s="12" t="s">
         <v>239</v>
       </c>
@@ -9754,7 +9791,7 @@
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10">
       <c r="A42" s="2"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -9766,12 +9803,12 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>285</v>
       </c>
@@ -9792,7 +9829,7 @@
       </c>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="8" t="s">
         <v>219</v>
       </c>
@@ -9816,7 +9853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="8" t="s">
         <v>220</v>
       </c>
@@ -9845,7 +9882,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="8" t="s">
         <v>221</v>
       </c>
@@ -9874,7 +9911,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10">
       <c r="A48" s="12" t="s">
         <v>239</v>
       </c>
@@ -9885,7 +9922,7 @@
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7">
       <c r="A49" s="2"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -9901,16 +9938,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="B14" sqref="B14:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -9924,7 +9961,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -9945,7 +9982,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -9966,7 +10003,7 @@
         <v>0.95277529961698948</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -9985,8 +10022,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -10007,7 +10044,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -10031,7 +10068,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -10060,7 +10097,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -10089,7 +10126,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -10100,7 +10137,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -10126,7 +10163,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -10156,7 +10193,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -10191,7 +10228,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -10226,7 +10263,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -10247,16 +10284,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -10270,7 +10307,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -10291,7 +10328,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -10312,7 +10349,7 @@
         <v>0.90805800128462044</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -10331,8 +10368,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -10353,7 +10390,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -10377,7 +10414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -10406,7 +10443,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -10435,7 +10472,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -10446,7 +10483,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -10466,7 +10503,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -10490,7 +10527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -10519,7 +10556,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -10551,7 +10588,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -10560,7 +10597,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>340</v>
       </c>
@@ -10571,7 +10608,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="30" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>219</v>
       </c>
@@ -10586,7 +10623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>220</v>
       </c>
@@ -10603,7 +10640,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>221</v>
       </c>
@@ -10620,13 +10657,13 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8">
       <c r="A23" s="12" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="16" thickBot="1"/>
+    <row r="25" spans="1:8" ht="30" thickBot="1">
       <c r="A25" s="12" t="s">
         <v>513</v>
       </c>
@@ -10641,7 +10678,7 @@
       </c>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" ht="30" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>219</v>
       </c>
@@ -10659,7 +10696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>220</v>
       </c>
@@ -10680,7 +10717,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" ht="44" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>518</v>
       </c>
@@ -10704,7 +10741,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8">
       <c r="A29" s="12" t="s">
         <v>239</v>
       </c>
@@ -10722,16 +10759,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:G13"/>
+      <selection activeCell="A13" sqref="A13:H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -10745,7 +10782,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -10766,7 +10803,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -10787,7 +10824,7 @@
         <v>0.9267197256851698</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -10806,8 +10843,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="16" thickBot="1"/>
+    <row r="7" spans="1:13" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -10828,7 +10865,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -10852,7 +10889,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -10881,7 +10918,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -10910,7 +10947,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -10921,7 +10958,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -10950,7 +10987,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -10983,7 +11020,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -11022,7 +11059,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -11061,7 +11098,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -11076,7 +11113,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13">
       <c r="L18" t="s">
         <v>592</v>
       </c>
@@ -11090,16 +11127,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -11113,7 +11153,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -11134,7 +11174,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -11155,7 +11195,7 @@
         <v>0.97448244785232785</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -11174,8 +11214,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -11196,7 +11236,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -11220,7 +11260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -11249,7 +11289,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -11278,7 +11318,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -11289,7 +11329,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11">
       <c r="A13" s="12"/>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -11298,36 +11338,162 @@
       <c r="F13" s="24"/>
       <c r="G13" s="41"/>
     </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="8"/>
-      <c r="H14" s="22"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="8"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="8"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+    <row r="14" spans="1:11" ht="16" thickBot="1">
+      <c r="A14" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>652</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>648</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>650</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>651</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30" thickBot="1">
+      <c r="A15" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B15">
+        <v>0.29630960485488883</v>
+      </c>
+      <c r="C15">
+        <v>0.18665818857667263</v>
+      </c>
+      <c r="D15">
+        <v>0.27952064315716252</v>
+      </c>
+      <c r="E15">
+        <v>0.10816335116113814</v>
+      </c>
+      <c r="F15">
+        <v>0.12934821225013785</v>
+      </c>
+      <c r="G15">
+        <f>SUM(B15:F15)</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="22"/>
+      <c r="J15" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="K15" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16" thickBot="1">
+      <c r="A16" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B16" s="13">
+        <f t="shared" ref="B16:G16" si="2">ROUND(2000*B15,0)</f>
+        <v>593</v>
+      </c>
+      <c r="C16" s="13">
+        <f t="shared" si="2"/>
+        <v>373</v>
+      </c>
+      <c r="D16" s="13">
+        <f t="shared" si="2"/>
+        <v>559</v>
+      </c>
+      <c r="E16" s="13">
+        <f t="shared" si="2"/>
+        <v>216</v>
+      </c>
+      <c r="F16" s="13">
+        <f t="shared" si="2"/>
+        <v>259</v>
+      </c>
+      <c r="G16" s="13">
+        <f>SUM(B16:F16)</f>
+        <v>2000</v>
+      </c>
       <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="14"/>
+      <c r="J16" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="K16" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" thickBot="1">
+      <c r="A17" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" ref="B17:G17" si="3">ROUND(2200*B15,0)</f>
+        <v>652</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="3"/>
+        <v>411</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="3"/>
+        <v>615</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="3"/>
+        <v>238</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="3"/>
+        <v>285</v>
+      </c>
+      <c r="G17" s="2">
+        <f>SUM(B17:F17)</f>
+        <v>2201</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="J17" t="s">
+        <v>256</v>
+      </c>
+      <c r="K17" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="14"/>
+      <c r="J18" t="s">
+        <v>650</v>
+      </c>
+      <c r="K18" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="J19" t="s">
+        <v>585</v>
+      </c>
+      <c r="K19" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="J20" t="s">
+        <v>658</v>
+      </c>
+      <c r="K20" t="s">
+        <v>659</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11335,16 +11501,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -11358,7 +11524,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -11379,7 +11545,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -11400,7 +11566,7 @@
         <v>0.98351979013457747</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -11419,8 +11585,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -11441,7 +11607,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -11465,7 +11631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -11494,7 +11660,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -11523,7 +11689,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -11534,7 +11700,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -11554,7 +11720,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -11578,7 +11744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -11607,7 +11773,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -11636,7 +11802,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -11645,8 +11811,8 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="16" thickBot="1"/>
+    <row r="21" spans="1:8" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>513</v>
       </c>
@@ -11661,7 +11827,7 @@
       </c>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -11679,7 +11845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>220</v>
       </c>
@@ -11703,7 +11869,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="44" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>518</v>
       </c>
@@ -11727,7 +11893,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8">
       <c r="A25" s="12" t="s">
         <v>239</v>
       </c>

</xml_diff>

<commit_message>
data + quota JP (urban)
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502508E0-0A6E-B246-8A48-3157442E2335}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
     <sheet name="quotas_MX" sheetId="17" r:id="rId16"/>
     <sheet name="quotas_SK" sheetId="18" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="751">
   <si>
     <t>Country</t>
   </si>
@@ -2293,18 +2294,24 @@
   </si>
   <si>
     <t>Quotas done</t>
+  </si>
+  <si>
+    <t>town &lt;100k</t>
+  </si>
+  <si>
+    <t>town &gt;100k</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2517,7 +2524,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2794,27 +2801,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.6328125" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" customWidth="1"/>
-    <col min="3" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="9.6328125" customWidth="1"/>
-    <col min="12" max="12" width="9.6328125" customWidth="1"/>
-    <col min="13" max="13" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" customWidth="1"/>
-    <col min="17" max="17" width="13.6328125" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2870,7 +2877,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>454</v>
       </c>
@@ -2914,7 +2921,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>455</v>
       </c>
@@ -2958,7 +2965,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>456</v>
       </c>
@@ -2999,7 +3006,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>495</v>
       </c>
@@ -3043,7 +3050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
         <v>748</v>
       </c>
@@ -3077,7 +3084,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
         <v>457</v>
       </c>
@@ -3108,7 +3115,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -3161,7 +3168,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -3214,7 +3221,7 @@
         <v>1113.8499999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18">
       <c r="A10" s="2" t="s">
         <v>169</v>
       </c>
@@ -3267,7 +3274,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18">
       <c r="A11" s="2" t="s">
         <v>170</v>
       </c>
@@ -3320,7 +3327,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18">
       <c r="A12" s="1" t="s">
         <v>181</v>
       </c>
@@ -3373,7 +3380,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
         <v>182</v>
       </c>
@@ -3426,7 +3433,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18">
       <c r="A14" s="1" t="s">
         <v>399</v>
       </c>
@@ -3470,7 +3477,7 @@
         <v>19653</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18">
       <c r="A15" s="1" t="s">
         <v>400</v>
       </c>
@@ -3514,7 +3521,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18">
       <c r="A16" s="1" t="s">
         <v>401</v>
       </c>
@@ -3558,7 +3565,7 @@
         <v>113696</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14">
       <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
@@ -3602,7 +3609,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>396</v>
       </c>
@@ -3646,7 +3653,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>397</v>
       </c>
@@ -3690,7 +3697,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>398</v>
       </c>
@@ -3734,7 +3741,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>205</v>
       </c>
@@ -3778,7 +3785,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>206</v>
       </c>
@@ -3822,7 +3829,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>207</v>
       </c>
@@ -3866,7 +3873,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>208</v>
       </c>
@@ -3910,7 +3917,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>436</v>
       </c>
@@ -3954,7 +3961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>437</v>
       </c>
@@ -3998,7 +4005,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>438</v>
       </c>
@@ -4042,7 +4049,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>439</v>
       </c>
@@ -4086,7 +4093,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
         <v>520</v>
       </c>
@@ -4103,7 +4110,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>560</v>
       </c>
@@ -4111,7 +4118,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
@@ -4155,7 +4162,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>75</v>
       </c>
@@ -4199,7 +4206,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17">
       <c r="A33" s="1" t="s">
         <v>76</v>
       </c>
@@ -4243,7 +4250,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17">
       <c r="A34" s="1" t="s">
         <v>77</v>
       </c>
@@ -4287,7 +4294,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17">
       <c r="A35" s="1" t="s">
         <v>78</v>
       </c>
@@ -4331,7 +4338,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17">
       <c r="A36" s="1" t="s">
         <v>73</v>
       </c>
@@ -4345,7 +4352,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17">
       <c r="A37" s="1" t="s">
         <v>68</v>
       </c>
@@ -4359,7 +4366,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17">
       <c r="A38" s="1" t="s">
         <v>67</v>
       </c>
@@ -4373,7 +4380,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17">
       <c r="A39" s="1" t="s">
         <v>66</v>
       </c>
@@ -4417,7 +4424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17">
       <c r="A40" s="1" t="s">
         <v>65</v>
       </c>
@@ -4458,7 +4465,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17">
       <c r="A41" s="1" t="s">
         <v>64</v>
       </c>
@@ -4469,7 +4476,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17">
       <c r="A42" s="1" t="s">
         <v>63</v>
       </c>
@@ -4513,7 +4520,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17">
       <c r="A43" s="1" t="s">
         <v>79</v>
       </c>
@@ -4557,7 +4564,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17">
       <c r="A44" s="1" t="s">
         <v>313</v>
       </c>
@@ -4610,7 +4617,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17">
       <c r="A45" s="1" t="s">
         <v>62</v>
       </c>
@@ -4663,7 +4670,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17">
       <c r="A46" s="1" t="s">
         <v>562</v>
       </c>
@@ -4686,7 +4693,7 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17">
       <c r="A47" s="1" t="s">
         <v>61</v>
       </c>
@@ -4728,7 +4735,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17">
       <c r="A48" s="1" t="s">
         <v>60</v>
       </c>
@@ -4775,7 +4782,7 @@
       <c r="P48" s="31"/>
       <c r="Q48" s="31"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17">
       <c r="A49" s="1" t="s">
         <v>59</v>
       </c>
@@ -4842,7 +4849,7 @@
         <v>33415.5</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17">
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
@@ -4886,7 +4893,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17">
       <c r="A51" s="1" t="s">
         <v>57</v>
       </c>
@@ -4939,7 +4946,7 @@
         <v>718.5</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -4969,7 +4976,7 @@
       </c>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
@@ -5014,7 +5021,7 @@
       </c>
       <c r="O53" s="1"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17">
       <c r="A54" s="1" t="s">
         <v>306</v>
       </c>
@@ -5068,7 +5075,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17">
       <c r="A55" s="1" t="s">
         <v>311</v>
       </c>
@@ -5121,7 +5128,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17">
       <c r="A56" s="1" t="s">
         <v>527</v>
       </c>
@@ -5174,7 +5181,7 @@
         <v>43190072.399999999</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17">
       <c r="A57" s="1" t="s">
         <v>312</v>
       </c>
@@ -5243,7 +5250,7 @@
         <v>0.1125</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17">
       <c r="A58" s="1" t="s">
         <v>314</v>
       </c>
@@ -5312,7 +5319,7 @@
         <v>125.30812499999999</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17">
       <c r="A59" s="1" t="s">
         <v>315</v>
       </c>
@@ -5381,7 +5388,7 @@
         <v>499862.23778592242</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17">
       <c r="A60" s="1" t="s">
         <v>331</v>
       </c>
@@ -5425,7 +5432,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17">
       <c r="A61" s="1" t="s">
         <v>487</v>
       </c>
@@ -5469,7 +5476,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17">
       <c r="A62" s="1" t="s">
         <v>729</v>
       </c>
@@ -5513,7 +5520,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17">
       <c r="A63" s="1" t="s">
         <v>727</v>
       </c>
@@ -5553,7 +5560,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17">
       <c r="A64" s="1" t="s">
         <v>728</v>
       </c>
@@ -5597,7 +5604,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14">
       <c r="A65" s="1" t="s">
         <v>353</v>
       </c>
@@ -5641,7 +5648,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14">
       <c r="A66" s="1" t="s">
         <v>384</v>
       </c>
@@ -5682,7 +5689,7 @@
         <v>0.92800000000000005</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14">
       <c r="A67" s="1" t="s">
         <v>488</v>
       </c>
@@ -5726,7 +5733,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14">
       <c r="A68" s="1" t="s">
         <v>102</v>
       </c>
@@ -5770,7 +5777,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14">
       <c r="A69" s="1" t="s">
         <v>103</v>
       </c>
@@ -5814,7 +5821,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14">
       <c r="A70" s="1" t="s">
         <v>104</v>
       </c>
@@ -5828,7 +5835,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14">
       <c r="A71" s="1" t="s">
         <v>111</v>
       </c>
@@ -5836,7 +5843,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14">
       <c r="A72" s="1" t="s">
         <v>105</v>
       </c>
@@ -5877,7 +5884,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14">
       <c r="A73" s="1" t="s">
         <v>106</v>
       </c>
@@ -5894,7 +5901,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14">
       <c r="A74" s="1" t="s">
         <v>204</v>
       </c>
@@ -5914,7 +5921,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14">
       <c r="A75" s="1" t="s">
         <v>107</v>
       </c>
@@ -5922,7 +5929,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14">
       <c r="A76" s="1" t="s">
         <v>112</v>
       </c>
@@ -5930,7 +5937,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14">
       <c r="A77" s="1" t="s">
         <v>114</v>
       </c>
@@ -5938,7 +5945,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14">
       <c r="A78" s="6" t="s">
         <v>115</v>
       </c>
@@ -5979,7 +5986,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14">
       <c r="A79" s="6" t="s">
         <v>116</v>
       </c>
@@ -6020,7 +6027,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14">
       <c r="A80" s="6" t="s">
         <v>117</v>
       </c>
@@ -6061,7 +6068,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14">
       <c r="A81" s="6" t="s">
         <v>118</v>
       </c>
@@ -6102,7 +6109,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14">
       <c r="A82" s="6" t="s">
         <v>119</v>
       </c>
@@ -6137,7 +6144,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14">
       <c r="A83" s="6" t="s">
         <v>120</v>
       </c>
@@ -6166,7 +6173,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14">
       <c r="A84" s="6" t="s">
         <v>121</v>
       </c>
@@ -6186,7 +6193,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14">
       <c r="A85" s="6" t="s">
         <v>122</v>
       </c>
@@ -6200,7 +6207,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14">
       <c r="A86" s="6" t="s">
         <v>123</v>
       </c>
@@ -6211,7 +6218,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14">
       <c r="A87" s="6" t="s">
         <v>124</v>
       </c>
@@ -6225,7 +6232,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14">
       <c r="A88" s="6" t="s">
         <v>188</v>
       </c>
@@ -6233,7 +6240,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14">
       <c r="A89" s="6" t="s">
         <v>189</v>
       </c>
@@ -6241,7 +6248,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14">
       <c r="A90" s="6" t="s">
         <v>193</v>
       </c>
@@ -6249,7 +6256,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14">
       <c r="A91" s="6" t="s">
         <v>199</v>
       </c>
@@ -6290,7 +6297,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14">
       <c r="A92" s="4" t="s">
         <v>191</v>
       </c>
@@ -6298,7 +6305,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14">
       <c r="A93" s="4" t="s">
         <v>195</v>
       </c>
@@ -6306,7 +6313,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14">
       <c r="A94" s="4" t="s">
         <v>197</v>
       </c>
@@ -6314,7 +6321,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14">
       <c r="A95" s="6" t="s">
         <v>269</v>
       </c>
@@ -6328,7 +6335,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:14">
       <c r="A96" s="6" t="s">
         <v>270</v>
       </c>
@@ -6342,7 +6349,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:18">
       <c r="A97" s="6" t="s">
         <v>271</v>
       </c>
@@ -6356,7 +6363,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:18">
       <c r="A98" s="6" t="s">
         <v>272</v>
       </c>
@@ -6364,7 +6371,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:18">
       <c r="A99" s="6" t="s">
         <v>273</v>
       </c>
@@ -6372,7 +6379,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:18">
       <c r="A100" s="6" t="s">
         <v>274</v>
       </c>
@@ -6386,7 +6393,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:18">
       <c r="A101" s="6" t="s">
         <v>275</v>
       </c>
@@ -6394,7 +6401,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:18">
       <c r="A102" s="6" t="s">
         <v>293</v>
       </c>
@@ -6402,7 +6409,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:18">
       <c r="A103" s="6" t="s">
         <v>334</v>
       </c>
@@ -6443,7 +6450,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:18">
       <c r="A104" s="6" t="s">
         <v>486</v>
       </c>
@@ -6475,7 +6482,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:18">
       <c r="A105" s="6" t="s">
         <v>338</v>
       </c>
@@ -6483,7 +6490,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:18">
       <c r="A106" s="6" t="s">
         <v>489</v>
       </c>
@@ -6512,7 +6519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:18">
       <c r="A107" s="6" t="s">
         <v>491</v>
       </c>
@@ -6544,7 +6551,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:18">
       <c r="A108" s="6" t="s">
         <v>662</v>
       </c>
@@ -6579,7 +6586,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:18">
       <c r="A109" s="6" t="s">
         <v>496</v>
       </c>
@@ -6593,7 +6600,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:18">
       <c r="A110" s="6" t="s">
         <v>497</v>
       </c>
@@ -6607,7 +6614,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:18">
       <c r="A112" s="6" t="s">
         <v>719</v>
       </c>
@@ -6636,7 +6643,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:14">
       <c r="A113" s="6" t="s">
         <v>740</v>
       </c>
@@ -6644,12 +6651,12 @@
         <v>458</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:14">
       <c r="A114" s="6" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:14">
       <c r="A115" s="6" t="s">
         <v>672</v>
       </c>
@@ -6675,12 +6682,12 @@
         <v>680</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:14">
       <c r="A116" s="6" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:14">
       <c r="A117" s="6" t="s">
         <v>674</v>
       </c>
@@ -6706,7 +6713,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:14">
       <c r="A118" s="6" t="s">
         <v>675</v>
       </c>
@@ -6741,7 +6748,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:14">
       <c r="A119" s="6" t="s">
         <v>677</v>
       </c>
@@ -6776,12 +6783,12 @@
         <v>676</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:14">
       <c r="A120" s="6" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:14">
       <c r="A121" s="6" t="s">
         <v>679</v>
       </c>
@@ -6807,12 +6814,12 @@
         <v>680</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:14">
       <c r="A122" s="6" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:14">
       <c r="A123" s="6" t="s">
         <v>682</v>
       </c>
@@ -6847,7 +6854,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:14">
       <c r="A124" s="6" t="s">
         <v>683</v>
       </c>
@@ -6876,7 +6883,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:14">
       <c r="A125" s="6" t="s">
         <v>706</v>
       </c>
@@ -6887,7 +6894,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:14">
       <c r="A126" s="6" t="s">
         <v>684</v>
       </c>
@@ -6895,7 +6902,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:14">
       <c r="A127" s="6" t="s">
         <v>685</v>
       </c>
@@ -6930,7 +6937,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:14">
       <c r="A128" s="6" t="s">
         <v>686</v>
       </c>
@@ -6944,7 +6951,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:14">
       <c r="A129" s="6" t="s">
         <v>687</v>
       </c>
@@ -6973,7 +6980,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:14">
       <c r="A130" s="6" t="s">
         <v>741</v>
       </c>
@@ -7008,12 +7015,12 @@
         <v>676</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:14">
       <c r="A131" s="6" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:14">
       <c r="A132" s="6" t="s">
         <v>690</v>
       </c>
@@ -7036,7 +7043,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:14">
       <c r="A133" s="6" t="s">
         <v>692</v>
       </c>
@@ -7053,7 +7060,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:14">
       <c r="A134" s="6" t="s">
         <v>693</v>
       </c>
@@ -7070,7 +7077,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:14">
       <c r="A135" s="6" t="s">
         <v>694</v>
       </c>
@@ -7102,7 +7109,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:14">
       <c r="A136" s="1" t="s">
         <v>696</v>
       </c>
@@ -7116,7 +7123,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:14">
       <c r="A137" s="6" t="s">
         <v>695</v>
       </c>
@@ -7142,7 +7149,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:14">
       <c r="A138" s="6" t="s">
         <v>697</v>
       </c>
@@ -7168,7 +7175,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:14">
       <c r="A139" s="6" t="s">
         <v>698</v>
       </c>
@@ -7203,7 +7210,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:14">
       <c r="A140" s="6" t="s">
         <v>699</v>
       </c>
@@ -7238,7 +7245,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:14">
       <c r="A141" s="6" t="s">
         <v>700</v>
       </c>
@@ -7258,17 +7265,17 @@
         <v>701</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:14">
       <c r="A142" s="6" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:14">
       <c r="A143" s="6" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:14">
       <c r="A144" s="6" t="s">
         <v>704</v>
       </c>
@@ -7276,7 +7283,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13">
       <c r="A145" s="6" t="s">
         <v>707</v>
       </c>
@@ -7308,7 +7315,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13">
       <c r="A146" s="6" t="s">
         <v>718</v>
       </c>
@@ -7323,16 +7330,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:J18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -7346,7 +7353,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -7367,7 +7374,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -7388,7 +7395,7 @@
         <v>0.92622883301508352</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -7407,8 +7414,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -7429,7 +7436,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -7453,7 +7460,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -7482,7 +7489,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -7511,7 +7518,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -7522,7 +7529,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="16" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -7545,7 +7552,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -7575,7 +7582,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -7610,7 +7617,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -7645,7 +7652,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -7653,6 +7660,72 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
+    </row>
+    <row r="19" spans="1:5" ht="16" thickBot="1"/>
+    <row r="20" spans="1:5" ht="30" thickBot="1">
+      <c r="A20" s="12" t="s">
+        <v>511</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>749</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>750</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:5" ht="30" thickBot="1">
+      <c r="A21" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0.32701219999999998</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.67298780000000002</v>
+      </c>
+      <c r="D21" s="9">
+        <f>SUM(B21:C21)</f>
+        <v>1</v>
+      </c>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" ht="16" thickBot="1">
+      <c r="A22" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B22" s="11">
+        <f t="shared" ref="B22:C22" si="2">ROUND(2000*B21,0)</f>
+        <v>654</v>
+      </c>
+      <c r="C22" s="11">
+        <f t="shared" si="2"/>
+        <v>1346</v>
+      </c>
+      <c r="D22" s="11">
+        <f>SUM(B22:C22)</f>
+        <v>2000</v>
+      </c>
+      <c r="E22" s="29"/>
+    </row>
+    <row r="23" spans="1:5" ht="44" thickBot="1">
+      <c r="A23" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="B23" s="13">
+        <f>ROUND(2200*B21,0)</f>
+        <v>719</v>
+      </c>
+      <c r="C23" s="13">
+        <f t="shared" ref="C23" si="3">ROUND(2200*C21,0)</f>
+        <v>1481</v>
+      </c>
+      <c r="D23" s="13">
+        <f>SUM(B23:C23)</f>
+        <v>2200</v>
+      </c>
+      <c r="E23" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7660,19 +7733,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A20" sqref="A20:L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -7687,7 +7760,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -7709,7 +7782,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -7731,7 +7804,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -7751,7 +7824,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -7762,7 +7835,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="A6" s="35"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -7772,7 +7845,7 @@
       <c r="G6" s="36"/>
       <c r="H6" s="37"/>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -7782,7 +7855,7 @@
       <c r="G7" s="36"/>
       <c r="H7" s="37"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>226</v>
       </c>
@@ -7804,7 +7877,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="37"/>
     </row>
-    <row r="9" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="30" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -7829,7 +7902,7 @@
       </c>
       <c r="H9" s="37"/>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -7859,7 +7932,7 @@
       </c>
       <c r="H10" s="37"/>
     </row>
-    <row r="11" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="30" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>221</v>
       </c>
@@ -7889,7 +7962,7 @@
       </c>
       <c r="H11" s="37"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" s="12" t="s">
         <v>239</v>
       </c>
@@ -7901,10 +7974,10 @@
       <c r="G12" s="13"/>
       <c r="H12" s="37"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="H13" s="37"/>
     </row>
-    <row r="14" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="44" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -7928,7 +8001,7 @@
       </c>
       <c r="H14" s="37"/>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -7955,7 +8028,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -7991,7 +8064,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -8027,7 +8100,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -8037,7 +8110,7 @@
       <c r="E18" s="14"/>
       <c r="H18" s="37"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12">
       <c r="A19" s="12"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
@@ -8047,7 +8120,7 @@
       <c r="G19" s="39"/>
       <c r="H19" s="37"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12">
       <c r="A20" s="12"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -8063,7 +8136,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>222</v>
       </c>
@@ -8087,7 +8160,7 @@
       </c>
       <c r="H21" s="37"/>
     </row>
-    <row r="22" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -8114,7 +8187,7 @@
         <v>0.99989215000000009</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>220</v>
       </c>
@@ -8147,7 +8220,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>221</v>
       </c>
@@ -8180,7 +8253,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12">
       <c r="A25" s="12" t="s">
         <v>239</v>
       </c>
@@ -8190,7 +8263,7 @@
       <c r="E25" s="14"/>
       <c r="H25" s="37"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12">
       <c r="A26" s="12"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
@@ -8200,7 +8273,7 @@
       <c r="G26" s="37"/>
       <c r="H26" s="37"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12">
       <c r="A27" s="12"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -8210,7 +8283,7 @@
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12">
       <c r="A28" s="12"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
@@ -8220,7 +8293,7 @@
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -8236,16 +8309,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -8259,7 +8332,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -8280,7 +8353,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -8301,7 +8374,7 @@
         <v>0.99992877771181621</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -8320,8 +8393,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -8342,7 +8415,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -8366,7 +8439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -8395,7 +8468,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -8424,7 +8497,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -8441,16 +8514,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -8464,7 +8537,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -8485,7 +8558,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -8506,7 +8579,7 @@
         <v>0.97760081385085629</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -8525,8 +8598,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -8547,7 +8620,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -8571,7 +8644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -8600,7 +8673,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -8629,7 +8702,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -8646,16 +8719,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -8669,7 +8742,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -8690,7 +8763,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -8711,7 +8784,7 @@
         <v>1.0341140064832992</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -8730,8 +8803,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -8752,7 +8825,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -8776,7 +8849,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -8805,7 +8878,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -8834,7 +8907,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -8851,16 +8924,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -8874,7 +8947,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -8895,7 +8968,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -8916,7 +8989,7 @@
         <v>0.95217958067188335</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -8935,8 +9008,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -8957,7 +9030,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -8981,7 +9054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -9010,7 +9083,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -9039,7 +9112,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -9056,16 +9129,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -9079,7 +9152,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -9100,7 +9173,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -9121,7 +9194,7 @@
         <v>0.92970833595125124</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -9140,8 +9213,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -9162,7 +9235,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -9186,7 +9259,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -9215,7 +9288,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -9244,7 +9317,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -9261,16 +9334,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -9284,7 +9357,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -9305,7 +9378,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -9326,7 +9399,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -9345,8 +9418,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -9367,7 +9440,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -9391,7 +9464,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -9420,7 +9493,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -9449,7 +9522,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -9466,16 +9539,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>240</v>
       </c>
@@ -9492,7 +9565,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>245</v>
       </c>
@@ -9509,7 +9582,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>530</v>
       </c>
@@ -9526,7 +9599,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>239</v>
       </c>
@@ -9544,7 +9617,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -9568,7 +9641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>245</v>
       </c>
@@ -9593,7 +9666,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>530</v>
       </c>
@@ -9622,7 +9695,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -9646,10 +9719,10 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>248</v>
       </c>
@@ -9666,7 +9739,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>245</v>
       </c>
@@ -9687,7 +9760,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>530</v>
       </c>
@@ -9712,7 +9785,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>239</v>
       </c>
@@ -9733,13 +9806,13 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>253</v>
       </c>
@@ -9756,7 +9829,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>245</v>
       </c>
@@ -9777,7 +9850,7 @@
         <v>100.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>530</v>
       </c>
@@ -9802,7 +9875,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>239</v>
       </c>
@@ -9823,7 +9896,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>258</v>
       </c>
@@ -9837,7 +9910,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>245</v>
       </c>
@@ -9851,7 +9924,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>530</v>
       </c>
@@ -9868,7 +9941,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>239</v>
       </c>
@@ -9883,11 +9956,11 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>263</v>
       </c>
@@ -9904,7 +9977,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>245</v>
       </c>
@@ -9921,7 +9994,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>530</v>
       </c>
@@ -9942,7 +10015,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>239</v>
       </c>
@@ -9962,30 +10035,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D28" sqref="A24:D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -10000,7 +10073,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -10018,7 +10091,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -10038,7 +10111,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -10058,7 +10131,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -10069,7 +10142,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -10078,7 +10151,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -10099,7 +10172,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -10123,7 +10196,7 @@
         <v>1.0001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -10152,7 +10225,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -10181,8 +10254,8 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="16" thickBot="1"/>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>238</v>
       </c>
@@ -10200,7 +10273,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="8" t="s">
         <v>237</v>
       </c>
@@ -10220,7 +10293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>220</v>
       </c>
@@ -10245,7 +10318,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>221</v>
       </c>
@@ -10270,12 +10343,12 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" s="16" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="12" t="s">
         <v>222</v>
       </c>
@@ -10295,7 +10368,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="8" t="s">
         <v>219</v>
       </c>
@@ -10319,7 +10392,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>220</v>
       </c>
@@ -10348,7 +10421,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>221</v>
       </c>
@@ -10377,7 +10450,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
         <v>239</v>
       </c>
@@ -10386,7 +10459,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="16" t="s">
         <v>340</v>
       </c>
@@ -10397,7 +10470,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>219</v>
       </c>
@@ -10412,7 +10485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>220</v>
       </c>
@@ -10429,7 +10502,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>221</v>
       </c>
@@ -10446,7 +10519,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7">
       <c r="A28" s="12" t="s">
         <v>239</v>
       </c>
@@ -10457,22 +10530,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>280</v>
       </c>
@@ -10498,7 +10571,7 @@
       <c r="K1" s="13"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -10531,7 +10604,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -10565,7 +10638,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -10599,7 +10672,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -10615,7 +10688,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="0.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="0.5" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -10629,14 +10702,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>223</v>
       </c>
@@ -10656,7 +10729,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -10679,7 +10752,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -10704,7 +10777,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>221</v>
       </c>
@@ -10729,7 +10802,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" s="12" t="s">
         <v>239</v>
       </c>
@@ -10745,7 +10818,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -10759,7 +10832,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>226</v>
       </c>
@@ -10785,7 +10858,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -10814,7 +10887,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -10848,7 +10921,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -10882,7 +10955,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -10898,7 +10971,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -10912,7 +10985,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>232</v>
       </c>
@@ -10936,7 +11009,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>237</v>
       </c>
@@ -10962,7 +11035,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -10993,7 +11066,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>221</v>
       </c>
@@ -11024,7 +11097,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>239</v>
       </c>
@@ -11034,7 +11107,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -11042,7 +11115,7 @@
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" ht="16.5" customHeight="1" thickBot="1">
       <c r="A26" s="12" t="s">
         <v>511</v>
       </c>
@@ -11059,7 +11132,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>219</v>
       </c>
@@ -11078,7 +11151,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" ht="16" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>220</v>
       </c>
@@ -11100,7 +11173,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" ht="16" thickBot="1">
       <c r="A29" s="8" t="s">
         <v>515</v>
       </c>
@@ -11119,7 +11192,7 @@
       </c>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>514</v>
       </c>
@@ -11141,7 +11214,7 @@
       </c>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>516</v>
       </c>
@@ -11163,7 +11236,7 @@
       </c>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12">
       <c r="A32" s="12" t="s">
         <v>239</v>
       </c>
@@ -11174,12 +11247,12 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
-    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" ht="30" thickBot="1">
       <c r="A37" s="8" t="s">
         <v>210</v>
       </c>
@@ -11209,7 +11282,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="8" t="s">
         <v>219</v>
       </c>
@@ -11242,7 +11315,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="8" t="s">
         <v>220</v>
       </c>
@@ -11283,7 +11356,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="8" t="s">
         <v>221</v>
       </c>
@@ -11324,7 +11397,7 @@
         <v>2196</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10">
       <c r="A41" s="12" t="s">
         <v>239</v>
       </c>
@@ -11338,7 +11411,7 @@
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10">
       <c r="A42" s="2"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -11350,12 +11423,12 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>285</v>
       </c>
@@ -11376,7 +11449,7 @@
       </c>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="8" t="s">
         <v>219</v>
       </c>
@@ -11400,7 +11473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="8" t="s">
         <v>220</v>
       </c>
@@ -11429,7 +11502,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="8" t="s">
         <v>221</v>
       </c>
@@ -11458,7 +11531,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10">
       <c r="A48" s="12" t="s">
         <v>239</v>
       </c>
@@ -11469,7 +11542,7 @@
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7">
       <c r="A49" s="2"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -11485,16 +11558,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -11508,7 +11581,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -11529,7 +11602,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -11550,7 +11623,7 @@
         <v>0.95277529961698948</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -11569,8 +11642,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -11591,7 +11664,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -11615,7 +11688,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -11644,7 +11717,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -11673,7 +11746,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -11684,7 +11757,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -11710,7 +11783,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -11740,7 +11813,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -11775,7 +11848,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -11810,7 +11883,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -11831,16 +11904,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="E30" sqref="A25:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -11854,7 +11927,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -11875,7 +11948,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -11896,7 +11969,7 @@
         <v>0.90805800128462044</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -11915,8 +11988,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -11937,7 +12010,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -11961,7 +12034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -11990,7 +12063,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -12019,7 +12092,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -12030,7 +12103,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -12050,7 +12123,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -12074,7 +12147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -12103,7 +12176,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -12135,7 +12208,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -12144,7 +12217,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>340</v>
       </c>
@@ -12155,7 +12228,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="30" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>219</v>
       </c>
@@ -12170,7 +12243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>220</v>
       </c>
@@ -12187,7 +12260,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>221</v>
       </c>
@@ -12204,13 +12277,13 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8">
       <c r="A23" s="12" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="16" thickBot="1"/>
+    <row r="25" spans="1:8" ht="30" thickBot="1">
       <c r="A25" s="12" t="s">
         <v>511</v>
       </c>
@@ -12225,7 +12298,7 @@
       </c>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" ht="30" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>219</v>
       </c>
@@ -12243,7 +12316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>220</v>
       </c>
@@ -12264,7 +12337,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" ht="44" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>516</v>
       </c>
@@ -12288,7 +12361,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8">
       <c r="A29" s="12" t="s">
         <v>239</v>
       </c>
@@ -12306,16 +12379,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E23" sqref="A20:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -12329,7 +12402,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -12350,7 +12423,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -12371,7 +12444,7 @@
         <v>0.9267197256851698</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -12390,8 +12463,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="16" thickBot="1"/>
+    <row r="7" spans="1:13" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -12412,7 +12485,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -12436,7 +12509,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -12465,7 +12538,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -12494,7 +12567,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -12505,7 +12578,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -12534,7 +12607,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -12567,7 +12640,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -12606,7 +12679,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -12645,7 +12718,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -12660,7 +12733,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13">
       <c r="L18" t="s">
         <v>588</v>
       </c>
@@ -12668,8 +12741,8 @@
         <v>594</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" ht="16" thickBot="1"/>
+    <row r="20" spans="1:13" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>511</v>
       </c>
@@ -12682,7 +12755,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:13" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>219</v>
       </c>
@@ -12698,7 +12771,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:13" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -12716,7 +12789,7 @@
       </c>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:13" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>516</v>
       </c>
@@ -12734,7 +12807,7 @@
       </c>
       <c r="E23" s="29"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13">
       <c r="A24" s="12" t="s">
         <v>239</v>
       </c>
@@ -12749,19 +12822,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -12775,7 +12848,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -12796,7 +12869,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -12817,7 +12890,7 @@
         <v>0.97448244785232785</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -12836,8 +12909,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -12858,7 +12931,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -12882,7 +12955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -12911,7 +12984,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -12940,7 +13013,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -12951,7 +13024,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="A13" s="12"/>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -12960,7 +13033,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="41"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -12983,7 +13056,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -13014,7 +13087,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -13050,7 +13123,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -13086,7 +13159,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -13101,7 +13174,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="J19" t="s">
         <v>581</v>
       </c>
@@ -13109,7 +13182,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11">
       <c r="J20" t="s">
         <v>649</v>
       </c>
@@ -13117,7 +13190,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" ht="16" thickBot="1">
       <c r="A21" s="16" t="s">
         <v>340</v>
       </c>
@@ -13128,7 +13201,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -13143,7 +13216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>220</v>
       </c>
@@ -13160,7 +13233,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>221</v>
       </c>
@@ -13177,7 +13250,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11">
       <c r="A25" s="12" t="s">
         <v>239</v>
       </c>
@@ -13188,16 +13261,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -13211,7 +13284,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -13232,7 +13305,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -13253,7 +13326,7 @@
         <v>0.98351979013457747</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -13272,8 +13345,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -13294,7 +13367,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -13318,7 +13391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -13347,7 +13420,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -13376,7 +13449,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -13387,7 +13460,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -13407,7 +13480,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -13431,7 +13504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -13460,7 +13533,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -13489,7 +13562,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -13498,8 +13571,8 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="16" thickBot="1"/>
+    <row r="21" spans="1:8" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>511</v>
       </c>
@@ -13514,7 +13587,7 @@
       </c>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -13532,7 +13605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>220</v>
       </c>
@@ -13556,7 +13629,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="44" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>516</v>
       </c>
@@ -13580,7 +13653,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8">
       <c r="A25" s="12" t="s">
         <v>239</v>
       </c>

</xml_diff>

<commit_message>
China update quota urban
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C7654E-F300-B642-A7E6-C9FB7E2863B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375477DC-A089-BC48-9F12-1FE7B53624F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1688" uniqueCount="788">
   <si>
     <t>Country</t>
   </si>
@@ -2407,10 +2407,10 @@
     <t>https://en.wikipedia.org/wiki/List_of_regions_of_China</t>
   </si>
   <si>
-    <t>town &lt;50k</t>
-  </si>
-  <si>
-    <t>town &gt;50k</t>
+    <t>Rural:</t>
+  </si>
+  <si>
+    <t>Rural Township + semi-urban Area + town &lt; 50k</t>
   </si>
 </sst>
 </file>
@@ -9128,8 +9128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -9441,7 +9441,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:7">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -9450,67 +9450,73 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:5" ht="16" thickBot="1">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>340</v>
       </c>
       <c r="B19" t="s">
-        <v>786</v>
+        <v>260</v>
       </c>
       <c r="C19" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16" thickBot="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>219</v>
       </c>
       <c r="B20">
-        <v>0.53894249999999999</v>
+        <v>0.4437874</v>
       </c>
       <c r="C20">
-        <v>0.46102019999999999</v>
+        <v>0.55621259999999995</v>
       </c>
       <c r="D20" s="22">
         <f>SUM(B20:C20)</f>
-        <v>0.99996269999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="16" thickBot="1">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>786</v>
+      </c>
+      <c r="G20" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>220</v>
       </c>
       <c r="B21">
         <f>ROUND(2000*B20,0)</f>
-        <v>1078</v>
+        <v>888</v>
       </c>
       <c r="C21">
         <f>ROUND(2000*C20,0)</f>
-        <v>922</v>
+        <v>1112</v>
       </c>
       <c r="D21">
         <f>SUM(B21:C21)</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" thickBot="1">
+    <row r="22" spans="1:7" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>221</v>
       </c>
       <c r="B22">
         <f>ROUND(2200*B20,0)</f>
-        <v>1186</v>
+        <v>976</v>
       </c>
       <c r="C22">
         <f>ROUND(2200*C20,0)</f>
-        <v>1014</v>
+        <v>1224</v>
       </c>
       <c r="D22">
         <f>SUM(B22:C22)</f>
         <v>2200</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:7">
       <c r="A23" s="12" t="s">
         <v>239</v>
       </c>

</xml_diff>

<commit_message>
Update CH categories label
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375477DC-A089-BC48-9F12-1FE7B53624F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53250293-B736-B648-964C-8EB346F155F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1688" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="807">
   <si>
     <t>Country</t>
   </si>
@@ -2411,6 +2411,63 @@
   </si>
   <si>
     <t>Rural Township + semi-urban Area + town &lt; 50k</t>
+  </si>
+  <si>
+    <t>Town</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Zhèn</t>
+  </si>
+  <si>
+    <t>Jiēdào</t>
+  </si>
+  <si>
+    <t>Urban Subdistrict</t>
+  </si>
+  <si>
+    <t>Xiāng</t>
+  </si>
+  <si>
+    <t>Rural Township</t>
+  </si>
+  <si>
+    <t>Dìqū</t>
+  </si>
+  <si>
+    <t>Semi-Urban Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chăng </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jùqū </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xiàn </t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>Sūmù</t>
+  </si>
+  <si>
+    <t>Township</t>
+  </si>
+  <si>
+    <t>Zìzhìxiàn</t>
+  </si>
+  <si>
+    <t>Autonomous County</t>
+  </si>
+  <si>
+    <t>Most important</t>
   </si>
 </sst>
 </file>
@@ -2521,12 +2578,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2558,7 +2621,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2631,6 +2694,7 @@
     <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9126,10 +9190,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -9441,7 +9505,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:9">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -9450,7 +9514,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:7" ht="16" thickBot="1">
+    <row r="19" spans="1:9" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>340</v>
       </c>
@@ -9461,7 +9525,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16" thickBot="1">
+    <row r="20" spans="1:9" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>219</v>
       </c>
@@ -9482,7 +9546,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" thickBot="1">
+    <row r="21" spans="1:9" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>220</v>
       </c>
@@ -9499,7 +9563,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" thickBot="1">
+    <row r="22" spans="1:9" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>221</v>
       </c>
@@ -9515,10 +9579,110 @@
         <f>SUM(B22:C22)</f>
         <v>2200</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="G22" t="s">
+        <v>789</v>
+      </c>
+      <c r="H22" t="s">
+        <v>790</v>
+      </c>
+      <c r="I22" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="12" t="s">
         <v>239</v>
+      </c>
+      <c r="G23" s="42" t="s">
+        <v>791</v>
+      </c>
+      <c r="H23" s="42" t="s">
+        <v>788</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="G24" s="42" t="s">
+        <v>792</v>
+      </c>
+      <c r="H24" s="42" t="s">
+        <v>793</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="G25" s="42" t="s">
+        <v>794</v>
+      </c>
+      <c r="H25" s="42" t="s">
+        <v>795</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="G26" t="s">
+        <v>796</v>
+      </c>
+      <c r="H26" t="s">
+        <v>797</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="G27" t="s">
+        <v>798</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="G28" t="s">
+        <v>799</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="G29" t="s">
+        <v>800</v>
+      </c>
+      <c r="H29" t="s">
+        <v>801</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="G30" t="s">
+        <v>802</v>
+      </c>
+      <c r="H30" t="s">
+        <v>803</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="G31" t="s">
+        <v>804</v>
+      </c>
+      <c r="H31" t="s">
+        <v>805</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add GE urban quota + csv zip
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53250293-B736-B648-964C-8EB346F155F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7645B704-F0F0-1841-BA2E-0EAA63861624}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="809">
   <si>
     <t>Country</t>
   </si>
@@ -2468,6 +2468,12 @@
   </si>
   <si>
     <t>Most important</t>
+  </si>
+  <si>
+    <t>https://www.destatis.de/DE/Themen/Laender-Regionen/Regionales/Gemeindeverzeichnis/Administrativ/Archiv/GVAuszugJ/31122019_Auszug_GV.html</t>
+  </si>
+  <si>
+    <t>category 3 https://ec.europa.eu/eurostat/ramon/miscellaneous/index.cfm?TargetUrl=DSP_DEGURBA</t>
   </si>
 </sst>
 </file>
@@ -9192,8 +9198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -12326,10 +12332,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:F14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -12663,6 +12669,83 @@
       </c>
       <c r="K17" t="s">
         <v>580</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16" thickBot="1">
+      <c r="A20" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="B20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C20" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" thickBot="1">
+      <c r="A21" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B21">
+        <v>0.2020653</v>
+      </c>
+      <c r="C21">
+        <v>0.7979347</v>
+      </c>
+      <c r="D21" s="22">
+        <f>SUM(B21:C21)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="16" thickBot="1">
+      <c r="A22" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B22">
+        <f>ROUND(2000*B21,0)</f>
+        <v>404</v>
+      </c>
+      <c r="C22">
+        <f>ROUND(2000*C21,0)</f>
+        <v>1596</v>
+      </c>
+      <c r="D22">
+        <f>SUM(B22:C22)</f>
+        <v>2000</v>
+      </c>
+      <c r="F22" t="s">
+        <v>649</v>
+      </c>
+      <c r="G22" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" thickBot="1">
+      <c r="A23" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B23">
+        <f>ROUND(2200*B21,0)</f>
+        <v>445</v>
+      </c>
+      <c r="C23">
+        <f>ROUND(2200*C21,0)</f>
+        <v>1755</v>
+      </c>
+      <c r="D23">
+        <f>SUM(B23:C23)</f>
+        <v>2200</v>
+      </c>
+      <c r="F23" t="s">
+        <v>786</v>
+      </c>
+      <c r="G23" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="12" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update rural quota DE
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7645B704-F0F0-1841-BA2E-0EAA63861624}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6401C1A-52DC-684A-B209-2E994265A4CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="811">
   <si>
     <t>Country</t>
   </si>
@@ -2473,7 +2473,13 @@
     <t>https://www.destatis.de/DE/Themen/Laender-Regionen/Regionales/Gemeindeverzeichnis/Administrativ/Archiv/GVAuszugJ/31122019_Auszug_GV.html</t>
   </si>
   <si>
-    <t>category 3 https://ec.europa.eu/eurostat/ramon/miscellaneous/index.cfm?TargetUrl=DSP_DEGURBA</t>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>https://ec.europa.eu/eurostat/ramon/miscellaneous/index.cfm?TargetUrl=DSP_DEGURBA</t>
+  </si>
+  <si>
+    <t>Town and Suburbs</t>
   </si>
 </sst>
 </file>
@@ -12335,7 +12341,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -12679,7 +12685,10 @@
         <v>260</v>
       </c>
       <c r="C20" t="s">
-        <v>259</v>
+        <v>810</v>
+      </c>
+      <c r="D20" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" thickBot="1">
@@ -12690,10 +12699,13 @@
         <v>0.2020653</v>
       </c>
       <c r="C21">
-        <v>0.7979347</v>
+        <v>0.40323310000000001</v>
       </c>
       <c r="D21" s="22">
-        <f>SUM(B21:C21)</f>
+        <v>0.39470159999999999</v>
+      </c>
+      <c r="E21" s="22">
+        <f>SUM(B21:D21)</f>
         <v>1</v>
       </c>
     </row>
@@ -12707,11 +12719,15 @@
       </c>
       <c r="C22">
         <f>ROUND(2000*C21,0)</f>
-        <v>1596</v>
+        <v>806</v>
       </c>
       <c r="D22">
-        <f>SUM(B22:C22)</f>
-        <v>2000</v>
+        <f>ROUND(2000*D21,0)</f>
+        <v>789</v>
+      </c>
+      <c r="E22">
+        <f>SUM(B22:D22)</f>
+        <v>1999</v>
       </c>
       <c r="F22" t="s">
         <v>649</v>
@@ -12730,17 +12746,21 @@
       </c>
       <c r="C23">
         <f>ROUND(2200*C21,0)</f>
-        <v>1755</v>
+        <v>887</v>
       </c>
       <c r="D23">
-        <f>SUM(B23:C23)</f>
+        <f>ROUND(2200*D21,0)</f>
+        <v>868</v>
+      </c>
+      <c r="E23">
+        <f>SUM(B23:D23)</f>
         <v>2200</v>
       </c>
       <c r="F23" t="s">
-        <v>786</v>
-      </c>
-      <c r="G23" t="s">
         <v>808</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>809</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -12749,6 +12769,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G23" r:id="rId1" xr:uid="{7C1243EF-E3B4-BD47-9600-2E92878D6D36}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
quota SA + zip csv
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800D4B4A-806F-954F-BF06-8275C33A45D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
     <sheet name="quotas_MX" sheetId="17" r:id="rId16"/>
     <sheet name="quotas_SK" sheetId="18" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="820">
   <si>
     <t>Country</t>
   </si>
@@ -2494,18 +2495,30 @@
   </si>
   <si>
     <t>a,t</t>
+  </si>
+  <si>
+    <t>Urban:</t>
+  </si>
+  <si>
+    <t>Live in metropolitan municipality or in capital of a District municipality</t>
+  </si>
+  <si>
+    <t>Census 2011</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Districts_of_South_Africa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2725,7 +2738,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3002,27 +3015,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.6328125" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" customWidth="1"/>
-    <col min="3" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="9.6328125" customWidth="1"/>
-    <col min="12" max="12" width="9.6328125" customWidth="1"/>
-    <col min="13" max="13" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" customWidth="1"/>
-    <col min="17" max="17" width="13.6328125" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3084,7 +3097,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
         <v>454</v>
       </c>
@@ -3128,7 +3141,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
         <v>455</v>
       </c>
@@ -3172,7 +3185,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20">
       <c r="A4" s="1" t="s">
         <v>456</v>
       </c>
@@ -3213,7 +3226,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
         <v>495</v>
       </c>
@@ -3257,7 +3270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20">
       <c r="A6" s="1" t="s">
         <v>747</v>
       </c>
@@ -3297,7 +3310,7 @@
       </c>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20">
       <c r="A7" s="1" t="s">
         <v>457</v>
       </c>
@@ -3328,7 +3341,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -3381,7 +3394,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -3434,7 +3447,7 @@
         <v>1113.8499999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20">
       <c r="A10" s="2" t="s">
         <v>169</v>
       </c>
@@ -3487,7 +3500,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20">
       <c r="A11" s="2" t="s">
         <v>170</v>
       </c>
@@ -3540,7 +3553,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20">
       <c r="A12" s="1" t="s">
         <v>181</v>
       </c>
@@ -3593,7 +3606,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20">
       <c r="A13" s="1" t="s">
         <v>182</v>
       </c>
@@ -3646,7 +3659,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20">
       <c r="A14" s="1" t="s">
         <v>399</v>
       </c>
@@ -3690,7 +3703,7 @@
         <v>19653</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20">
       <c r="A15" s="1" t="s">
         <v>400</v>
       </c>
@@ -3734,7 +3747,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20">
       <c r="A16" s="1" t="s">
         <v>401</v>
       </c>
@@ -3778,7 +3791,7 @@
         <v>113696</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14">
       <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
@@ -3822,7 +3835,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>396</v>
       </c>
@@ -3866,7 +3879,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>397</v>
       </c>
@@ -3910,7 +3923,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>398</v>
       </c>
@@ -3954,7 +3967,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>205</v>
       </c>
@@ -3998,7 +4011,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>206</v>
       </c>
@@ -4042,7 +4055,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>207</v>
       </c>
@@ -4086,7 +4099,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>208</v>
       </c>
@@ -4130,7 +4143,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>436</v>
       </c>
@@ -4174,7 +4187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>437</v>
       </c>
@@ -4218,7 +4231,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>438</v>
       </c>
@@ -4262,7 +4275,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>439</v>
       </c>
@@ -4306,7 +4319,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
         <v>520</v>
       </c>
@@ -4323,7 +4336,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>560</v>
       </c>
@@ -4331,7 +4344,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
@@ -4375,7 +4388,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>75</v>
       </c>
@@ -4419,7 +4432,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17">
       <c r="A33" s="1" t="s">
         <v>76</v>
       </c>
@@ -4463,7 +4476,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17">
       <c r="A34" s="1" t="s">
         <v>77</v>
       </c>
@@ -4507,7 +4520,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17">
       <c r="A35" s="1" t="s">
         <v>78</v>
       </c>
@@ -4551,7 +4564,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17">
       <c r="A36" s="1" t="s">
         <v>73</v>
       </c>
@@ -4565,7 +4578,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17">
       <c r="A37" s="1" t="s">
         <v>68</v>
       </c>
@@ -4579,7 +4592,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17">
       <c r="A38" s="1" t="s">
         <v>67</v>
       </c>
@@ -4593,7 +4606,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17">
       <c r="A39" s="1" t="s">
         <v>66</v>
       </c>
@@ -4637,7 +4650,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17">
       <c r="A40" s="1" t="s">
         <v>65</v>
       </c>
@@ -4678,7 +4691,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17">
       <c r="A41" s="1" t="s">
         <v>64</v>
       </c>
@@ -4689,7 +4702,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17">
       <c r="A42" s="1" t="s">
         <v>63</v>
       </c>
@@ -4733,7 +4746,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17">
       <c r="A43" s="1" t="s">
         <v>79</v>
       </c>
@@ -4777,7 +4790,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17">
       <c r="A44" s="1" t="s">
         <v>313</v>
       </c>
@@ -4830,7 +4843,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17">
       <c r="A45" s="1" t="s">
         <v>62</v>
       </c>
@@ -4883,7 +4896,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17">
       <c r="A46" s="1" t="s">
         <v>562</v>
       </c>
@@ -4906,7 +4919,7 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17">
       <c r="A47" s="1" t="s">
         <v>61</v>
       </c>
@@ -4948,7 +4961,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17">
       <c r="A48" s="1" t="s">
         <v>60</v>
       </c>
@@ -4995,7 +5008,7 @@
       <c r="P48" s="31"/>
       <c r="Q48" s="31"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17">
       <c r="A49" s="1" t="s">
         <v>59</v>
       </c>
@@ -5062,7 +5075,7 @@
         <v>33415.5</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17">
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
@@ -5106,7 +5119,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17">
       <c r="A51" s="1" t="s">
         <v>57</v>
       </c>
@@ -5159,7 +5172,7 @@
         <v>718.5</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -5189,7 +5202,7 @@
       </c>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
@@ -5234,7 +5247,7 @@
       </c>
       <c r="O53" s="1"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17">
       <c r="A54" s="1" t="s">
         <v>306</v>
       </c>
@@ -5288,7 +5301,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17">
       <c r="A55" s="1" t="s">
         <v>311</v>
       </c>
@@ -5341,7 +5354,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17">
       <c r="A56" s="1" t="s">
         <v>527</v>
       </c>
@@ -5394,7 +5407,7 @@
         <v>43190072.399999999</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17">
       <c r="A57" s="1" t="s">
         <v>312</v>
       </c>
@@ -5463,7 +5476,7 @@
         <v>0.1125</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17">
       <c r="A58" s="1" t="s">
         <v>314</v>
       </c>
@@ -5532,7 +5545,7 @@
         <v>125.30812499999999</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17">
       <c r="A59" s="1" t="s">
         <v>315</v>
       </c>
@@ -5601,7 +5614,7 @@
         <v>499862.23778592242</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17">
       <c r="A60" s="1" t="s">
         <v>331</v>
       </c>
@@ -5645,7 +5658,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17">
       <c r="A61" s="1" t="s">
         <v>487</v>
       </c>
@@ -5689,7 +5702,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17">
       <c r="A62" s="1" t="s">
         <v>728</v>
       </c>
@@ -5733,7 +5746,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17">
       <c r="A63" s="1" t="s">
         <v>726</v>
       </c>
@@ -5773,7 +5786,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17">
       <c r="A64" s="1" t="s">
         <v>727</v>
       </c>
@@ -5817,7 +5830,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14">
       <c r="A65" s="1" t="s">
         <v>353</v>
       </c>
@@ -5861,7 +5874,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14">
       <c r="A66" s="1" t="s">
         <v>384</v>
       </c>
@@ -5902,7 +5915,7 @@
         <v>0.92800000000000005</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14">
       <c r="A67" s="1" t="s">
         <v>488</v>
       </c>
@@ -5946,7 +5959,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14">
       <c r="A68" s="1" t="s">
         <v>102</v>
       </c>
@@ -5990,7 +6003,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14">
       <c r="A69" s="1" t="s">
         <v>103</v>
       </c>
@@ -6034,7 +6047,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14">
       <c r="A70" s="1" t="s">
         <v>104</v>
       </c>
@@ -6048,7 +6061,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14">
       <c r="A71" s="1" t="s">
         <v>111</v>
       </c>
@@ -6056,7 +6069,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14">
       <c r="A72" s="1" t="s">
         <v>105</v>
       </c>
@@ -6097,7 +6110,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14">
       <c r="A73" s="1" t="s">
         <v>106</v>
       </c>
@@ -6114,7 +6127,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14">
       <c r="A74" s="1" t="s">
         <v>204</v>
       </c>
@@ -6134,7 +6147,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14">
       <c r="A75" s="1" t="s">
         <v>107</v>
       </c>
@@ -6142,7 +6155,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14">
       <c r="A76" s="1" t="s">
         <v>112</v>
       </c>
@@ -6150,7 +6163,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14">
       <c r="A77" s="1" t="s">
         <v>114</v>
       </c>
@@ -6158,7 +6171,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14">
       <c r="A78" s="6" t="s">
         <v>115</v>
       </c>
@@ -6199,7 +6212,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14">
       <c r="A79" s="6" t="s">
         <v>116</v>
       </c>
@@ -6240,7 +6253,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14">
       <c r="A80" s="6" t="s">
         <v>117</v>
       </c>
@@ -6281,7 +6294,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14">
       <c r="A81" s="6" t="s">
         <v>118</v>
       </c>
@@ -6322,7 +6335,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14">
       <c r="A82" s="6" t="s">
         <v>119</v>
       </c>
@@ -6357,7 +6370,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14">
       <c r="A83" s="6" t="s">
         <v>120</v>
       </c>
@@ -6386,7 +6399,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14">
       <c r="A84" s="6" t="s">
         <v>121</v>
       </c>
@@ -6406,7 +6419,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14">
       <c r="A85" s="6" t="s">
         <v>122</v>
       </c>
@@ -6420,7 +6433,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14">
       <c r="A86" s="6" t="s">
         <v>123</v>
       </c>
@@ -6431,7 +6444,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14">
       <c r="A87" s="6" t="s">
         <v>124</v>
       </c>
@@ -6445,7 +6458,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14">
       <c r="A88" s="6" t="s">
         <v>188</v>
       </c>
@@ -6453,7 +6466,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14">
       <c r="A89" s="6" t="s">
         <v>189</v>
       </c>
@@ -6461,7 +6474,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14">
       <c r="A90" s="6" t="s">
         <v>193</v>
       </c>
@@ -6469,7 +6482,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14">
       <c r="A91" s="6" t="s">
         <v>199</v>
       </c>
@@ -6510,7 +6523,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14">
       <c r="A92" s="4" t="s">
         <v>191</v>
       </c>
@@ -6518,7 +6531,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14">
       <c r="A93" s="4" t="s">
         <v>195</v>
       </c>
@@ -6526,7 +6539,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14">
       <c r="A94" s="4" t="s">
         <v>197</v>
       </c>
@@ -6534,7 +6547,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14">
       <c r="A95" s="6" t="s">
         <v>269</v>
       </c>
@@ -6548,7 +6561,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:14">
       <c r="A96" s="6" t="s">
         <v>270</v>
       </c>
@@ -6562,7 +6575,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:18">
       <c r="A97" s="6" t="s">
         <v>271</v>
       </c>
@@ -6576,7 +6589,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:18">
       <c r="A98" s="6" t="s">
         <v>272</v>
       </c>
@@ -6584,7 +6597,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:18">
       <c r="A99" s="6" t="s">
         <v>273</v>
       </c>
@@ -6592,7 +6605,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:18">
       <c r="A100" s="6" t="s">
         <v>274</v>
       </c>
@@ -6606,7 +6619,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:18">
       <c r="A101" s="6" t="s">
         <v>275</v>
       </c>
@@ -6614,7 +6627,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:18">
       <c r="A102" s="6" t="s">
         <v>293</v>
       </c>
@@ -6622,7 +6635,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:18">
       <c r="A103" s="6" t="s">
         <v>334</v>
       </c>
@@ -6663,7 +6676,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:18">
       <c r="A104" s="6" t="s">
         <v>486</v>
       </c>
@@ -6695,7 +6708,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:18">
       <c r="A105" s="6" t="s">
         <v>338</v>
       </c>
@@ -6703,7 +6716,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:18">
       <c r="A106" s="6" t="s">
         <v>489</v>
       </c>
@@ -6732,7 +6745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:18">
       <c r="A107" s="6" t="s">
         <v>491</v>
       </c>
@@ -6764,7 +6777,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:18">
       <c r="A108" s="6" t="s">
         <v>661</v>
       </c>
@@ -6799,7 +6812,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:18">
       <c r="A109" s="6" t="s">
         <v>496</v>
       </c>
@@ -6813,7 +6826,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:18">
       <c r="A110" s="6" t="s">
         <v>497</v>
       </c>
@@ -6827,7 +6840,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:18">
       <c r="A112" s="6" t="s">
         <v>718</v>
       </c>
@@ -6856,7 +6869,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:14">
       <c r="A113" s="6" t="s">
         <v>739</v>
       </c>
@@ -6864,12 +6877,12 @@
         <v>458</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:14">
       <c r="A114" s="6" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:14">
       <c r="A115" s="6" t="s">
         <v>671</v>
       </c>
@@ -6895,12 +6908,12 @@
         <v>679</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:14">
       <c r="A116" s="6" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:14">
       <c r="A117" s="6" t="s">
         <v>673</v>
       </c>
@@ -6926,7 +6939,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:14">
       <c r="A118" s="6" t="s">
         <v>674</v>
       </c>
@@ -6961,7 +6974,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:14">
       <c r="A119" s="6" t="s">
         <v>676</v>
       </c>
@@ -6996,12 +7009,12 @@
         <v>675</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:14">
       <c r="A120" s="6" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:14">
       <c r="A121" s="6" t="s">
         <v>678</v>
       </c>
@@ -7027,12 +7040,12 @@
         <v>679</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:14">
       <c r="A122" s="6" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:14">
       <c r="A123" s="6" t="s">
         <v>681</v>
       </c>
@@ -7067,7 +7080,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:14">
       <c r="A124" s="6" t="s">
         <v>682</v>
       </c>
@@ -7096,7 +7109,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:14">
       <c r="A125" s="6" t="s">
         <v>705</v>
       </c>
@@ -7107,7 +7120,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:14">
       <c r="A126" s="6" t="s">
         <v>683</v>
       </c>
@@ -7115,7 +7128,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:14">
       <c r="A127" s="6" t="s">
         <v>684</v>
       </c>
@@ -7150,7 +7163,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:14">
       <c r="A128" s="6" t="s">
         <v>685</v>
       </c>
@@ -7164,7 +7177,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:14">
       <c r="A129" s="6" t="s">
         <v>686</v>
       </c>
@@ -7193,7 +7206,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:14">
       <c r="A130" s="6" t="s">
         <v>740</v>
       </c>
@@ -7228,12 +7241,12 @@
         <v>675</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:14">
       <c r="A131" s="6" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:14">
       <c r="A132" s="6" t="s">
         <v>689</v>
       </c>
@@ -7256,7 +7269,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:14">
       <c r="A133" s="6" t="s">
         <v>691</v>
       </c>
@@ -7273,7 +7286,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:14">
       <c r="A134" s="6" t="s">
         <v>692</v>
       </c>
@@ -7290,7 +7303,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:14">
       <c r="A135" s="6" t="s">
         <v>693</v>
       </c>
@@ -7322,7 +7335,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:14">
       <c r="A136" s="1" t="s">
         <v>695</v>
       </c>
@@ -7336,7 +7349,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:14">
       <c r="A137" s="6" t="s">
         <v>694</v>
       </c>
@@ -7362,7 +7375,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:14">
       <c r="A138" s="6" t="s">
         <v>696</v>
       </c>
@@ -7388,7 +7401,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:14">
       <c r="A139" s="6" t="s">
         <v>697</v>
       </c>
@@ -7423,7 +7436,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:14">
       <c r="A140" s="6" t="s">
         <v>698</v>
       </c>
@@ -7458,7 +7471,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:14">
       <c r="A141" s="6" t="s">
         <v>699</v>
       </c>
@@ -7478,17 +7491,17 @@
         <v>700</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:14">
       <c r="A142" s="6" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:14">
       <c r="A143" s="6" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:14">
       <c r="A144" s="6" t="s">
         <v>703</v>
       </c>
@@ -7496,7 +7509,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13">
       <c r="A145" s="6" t="s">
         <v>706</v>
       </c>
@@ -7528,7 +7541,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13">
       <c r="A146" s="6" t="s">
         <v>717</v>
       </c>
@@ -7536,7 +7549,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
         <v>814</v>
       </c>
@@ -7560,16 +7573,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A20" sqref="A20:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -7583,7 +7596,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -7604,7 +7617,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -7625,7 +7638,7 @@
         <v>0.92622883301508352</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -7644,8 +7657,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -7666,7 +7679,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -7690,7 +7703,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -7719,7 +7732,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -7748,7 +7761,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -7759,7 +7772,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="16" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -7782,7 +7795,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -7812,7 +7825,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -7847,7 +7860,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -7882,7 +7895,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -7891,8 +7904,8 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" ht="16" thickBot="1"/>
+    <row r="20" spans="1:5" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>511</v>
       </c>
@@ -7905,7 +7918,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>219</v>
       </c>
@@ -7921,7 +7934,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -7939,7 +7952,7 @@
       </c>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>516</v>
       </c>
@@ -7963,19 +7976,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A20" sqref="A20:L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -7990,7 +8003,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -8012,7 +8025,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -8034,7 +8047,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -8054,7 +8067,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -8065,7 +8078,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="A6" s="35"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -8075,7 +8088,7 @@
       <c r="G6" s="36"/>
       <c r="H6" s="37"/>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -8085,7 +8098,7 @@
       <c r="G7" s="36"/>
       <c r="H7" s="37"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>226</v>
       </c>
@@ -8107,7 +8120,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="37"/>
     </row>
-    <row r="9" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="30" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -8132,7 +8145,7 @@
       </c>
       <c r="H9" s="37"/>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -8162,7 +8175,7 @@
       </c>
       <c r="H10" s="37"/>
     </row>
-    <row r="11" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="30" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>221</v>
       </c>
@@ -8192,7 +8205,7 @@
       </c>
       <c r="H11" s="37"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" s="12" t="s">
         <v>239</v>
       </c>
@@ -8204,10 +8217,10 @@
       <c r="G12" s="13"/>
       <c r="H12" s="37"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="H13" s="37"/>
     </row>
-    <row r="14" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="44" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -8231,7 +8244,7 @@
       </c>
       <c r="H14" s="37"/>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -8258,7 +8271,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -8294,7 +8307,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -8330,7 +8343,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -8340,7 +8353,7 @@
       <c r="E18" s="14"/>
       <c r="H18" s="37"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12">
       <c r="A19" s="12"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
@@ -8350,7 +8363,7 @@
       <c r="G19" s="39"/>
       <c r="H19" s="37"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12">
       <c r="A20" s="12"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -8366,7 +8379,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>222</v>
       </c>
@@ -8390,7 +8403,7 @@
       </c>
       <c r="H21" s="37"/>
     </row>
-    <row r="22" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -8417,7 +8430,7 @@
         <v>0.99989215000000009</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>220</v>
       </c>
@@ -8450,7 +8463,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>221</v>
       </c>
@@ -8483,7 +8496,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12">
       <c r="A25" s="12" t="s">
         <v>239</v>
       </c>
@@ -8493,7 +8506,7 @@
       <c r="E25" s="14"/>
       <c r="H25" s="37"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12">
       <c r="A26" s="12"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
@@ -8503,7 +8516,7 @@
       <c r="G26" s="37"/>
       <c r="H26" s="37"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12">
       <c r="A27" s="12"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -8513,7 +8526,7 @@
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12">
       <c r="A28" s="12"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
@@ -8523,7 +8536,7 @@
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -8539,16 +8552,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="B23" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -8562,7 +8575,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -8583,7 +8596,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -8604,7 +8617,7 @@
         <v>0.99992877771181621</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -8623,8 +8636,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -8645,7 +8658,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -8669,7 +8682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -8698,7 +8711,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -8727,7 +8740,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -8738,7 +8751,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -8767,7 +8780,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -8797,7 +8810,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -8832,7 +8845,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -8867,7 +8880,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -8882,13 +8895,13 @@
         <v>767</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="K19" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" ht="16" thickBot="1"/>
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="12" t="s">
         <v>511</v>
       </c>
@@ -8901,7 +8914,7 @@
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>219</v>
       </c>
@@ -8923,7 +8936,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>220</v>
       </c>
@@ -8947,7 +8960,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" ht="44" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>516</v>
       </c>
@@ -8972,16 +8985,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -8995,7 +9008,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -9016,7 +9029,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -9037,7 +9050,7 @@
         <v>0.97760081385085629</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -9056,8 +9069,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -9078,7 +9091,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -9102,7 +9115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -9131,7 +9144,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -9160,7 +9173,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -9171,7 +9184,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -9194,7 +9207,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -9224,7 +9237,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -9259,7 +9272,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -9294,7 +9307,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -9309,22 +9322,103 @@
         <v>777</v>
       </c>
     </row>
+    <row r="21" spans="1:11" ht="16" thickBot="1"/>
+    <row r="22" spans="1:11" ht="30" thickBot="1">
+      <c r="A22" s="12" t="s">
+        <v>511</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:11" ht="16" thickBot="1">
+      <c r="A23" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B23" s="9">
+        <v>0.5109049</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.4890951</v>
+      </c>
+      <c r="D23" s="9">
+        <f>SUM(B23:C23)</f>
+        <v>1</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" t="s">
+        <v>816</v>
+      </c>
+      <c r="G23" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16" thickBot="1">
+      <c r="A24" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B24" s="11">
+        <f>ROUND(2000*B23,0)</f>
+        <v>1022</v>
+      </c>
+      <c r="C24" s="11">
+        <f>ROUND(2000*C23,0)</f>
+        <v>978</v>
+      </c>
+      <c r="D24" s="11">
+        <f>SUM(B24:C24)</f>
+        <v>2000</v>
+      </c>
+      <c r="E24" s="29"/>
+      <c r="F24" t="s">
+        <v>766</v>
+      </c>
+      <c r="G24" t="s">
+        <v>818</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="44" thickBot="1">
+      <c r="A25" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="B25" s="13">
+        <f>ROUND(2200*B23,0)</f>
+        <v>1124</v>
+      </c>
+      <c r="C25" s="13">
+        <f>ROUND(2200*C23,0)</f>
+        <v>1076</v>
+      </c>
+      <c r="D25" s="13">
+        <f>SUM(B25:C25)</f>
+        <v>2200</v>
+      </c>
+      <c r="E25" s="29"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -9338,7 +9432,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -9359,7 +9453,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -9380,7 +9474,7 @@
         <v>1.0341140064832992</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -9399,8 +9493,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -9421,7 +9515,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -9445,7 +9539,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -9474,7 +9568,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -9503,7 +9597,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -9514,7 +9608,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="44" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -9537,7 +9631,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -9567,7 +9661,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -9602,7 +9696,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -9631,7 +9725,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -9640,7 +9734,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>340</v>
       </c>
@@ -9651,7 +9745,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>219</v>
       </c>
@@ -9672,7 +9766,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>220</v>
       </c>
@@ -9689,7 +9783,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>221</v>
       </c>
@@ -9715,7 +9809,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9">
       <c r="A23" s="12" t="s">
         <v>239</v>
       </c>
@@ -9729,7 +9823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9">
       <c r="G24" s="42" t="s">
         <v>792</v>
       </c>
@@ -9740,7 +9834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9">
       <c r="G25" s="42" t="s">
         <v>794</v>
       </c>
@@ -9751,7 +9845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9">
       <c r="G26" t="s">
         <v>796</v>
       </c>
@@ -9762,7 +9856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9">
       <c r="G27" t="s">
         <v>798</v>
       </c>
@@ -9770,7 +9864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9">
       <c r="G28" t="s">
         <v>799</v>
       </c>
@@ -9778,7 +9872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9">
       <c r="G29" t="s">
         <v>800</v>
       </c>
@@ -9789,7 +9883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9">
       <c r="G30" t="s">
         <v>802</v>
       </c>
@@ -9800,7 +9894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9">
       <c r="G31" t="s">
         <v>804</v>
       </c>
@@ -9817,16 +9911,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -9840,7 +9934,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -9861,7 +9955,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -9882,7 +9976,7 @@
         <v>0.95217958067188335</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -9901,8 +9995,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -9923,7 +10017,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -9947,7 +10041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -9976,7 +10070,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -10005,7 +10099,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -10022,16 +10116,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -10045,7 +10139,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -10066,7 +10160,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -10087,7 +10181,7 @@
         <v>0.92970833595125124</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -10106,8 +10200,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -10128,7 +10222,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -10152,7 +10246,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -10181,7 +10275,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -10210,7 +10304,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -10227,16 +10321,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -10250,7 +10344,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -10271,7 +10365,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -10292,7 +10386,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -10311,8 +10405,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -10333,7 +10427,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -10357,7 +10451,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -10386,7 +10480,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -10415,7 +10509,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -10432,16 +10526,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>240</v>
       </c>
@@ -10458,7 +10552,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>245</v>
       </c>
@@ -10475,7 +10569,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>530</v>
       </c>
@@ -10492,7 +10586,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>239</v>
       </c>
@@ -10510,7 +10604,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -10534,7 +10628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>245</v>
       </c>
@@ -10559,7 +10653,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>530</v>
       </c>
@@ -10588,7 +10682,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -10612,10 +10706,10 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>248</v>
       </c>
@@ -10632,7 +10726,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>245</v>
       </c>
@@ -10653,7 +10747,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>530</v>
       </c>
@@ -10678,7 +10772,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>239</v>
       </c>
@@ -10699,13 +10793,13 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>253</v>
       </c>
@@ -10722,7 +10816,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>245</v>
       </c>
@@ -10743,7 +10837,7 @@
         <v>100.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>530</v>
       </c>
@@ -10768,7 +10862,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>239</v>
       </c>
@@ -10789,7 +10883,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>258</v>
       </c>
@@ -10803,7 +10897,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>245</v>
       </c>
@@ -10817,7 +10911,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>530</v>
       </c>
@@ -10834,7 +10928,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>239</v>
       </c>
@@ -10849,11 +10943,11 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>263</v>
       </c>
@@ -10870,7 +10964,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>245</v>
       </c>
@@ -10887,7 +10981,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>530</v>
       </c>
@@ -10908,7 +11002,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>239</v>
       </c>
@@ -10928,30 +11022,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D28" sqref="A24:D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -10966,7 +11060,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -10984,7 +11078,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -11004,7 +11098,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -11024,7 +11118,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -11035,7 +11129,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -11044,7 +11138,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -11065,7 +11159,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -11089,7 +11183,7 @@
         <v>1.0001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -11118,7 +11212,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -11147,8 +11241,8 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="16" thickBot="1"/>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>238</v>
       </c>
@@ -11166,7 +11260,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="8" t="s">
         <v>237</v>
       </c>
@@ -11186,7 +11280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>220</v>
       </c>
@@ -11211,7 +11305,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>221</v>
       </c>
@@ -11236,12 +11330,12 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" s="16" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="12" t="s">
         <v>222</v>
       </c>
@@ -11261,7 +11355,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="8" t="s">
         <v>219</v>
       </c>
@@ -11285,7 +11379,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>220</v>
       </c>
@@ -11314,7 +11408,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>221</v>
       </c>
@@ -11343,7 +11437,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
         <v>239</v>
       </c>
@@ -11352,7 +11446,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="16" t="s">
         <v>340</v>
       </c>
@@ -11363,7 +11457,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>219</v>
       </c>
@@ -11378,7 +11472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>220</v>
       </c>
@@ -11395,7 +11489,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>221</v>
       </c>
@@ -11412,7 +11506,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7">
       <c r="A28" s="12" t="s">
         <v>239</v>
       </c>
@@ -11423,22 +11517,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>280</v>
       </c>
@@ -11464,7 +11558,7 @@
       <c r="K1" s="13"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -11497,7 +11591,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -11531,7 +11625,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -11565,7 +11659,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -11581,7 +11675,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="0.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="0.5" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -11595,14 +11689,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>223</v>
       </c>
@@ -11622,7 +11716,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -11645,7 +11739,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -11670,7 +11764,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>221</v>
       </c>
@@ -11695,7 +11789,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" s="12" t="s">
         <v>239</v>
       </c>
@@ -11711,7 +11805,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -11725,7 +11819,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>226</v>
       </c>
@@ -11751,7 +11845,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -11780,7 +11874,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -11814,7 +11908,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -11848,7 +11942,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -11864,7 +11958,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -11878,7 +11972,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>232</v>
       </c>
@@ -11902,7 +11996,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>237</v>
       </c>
@@ -11928,7 +12022,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -11959,7 +12053,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>221</v>
       </c>
@@ -11990,7 +12084,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>239</v>
       </c>
@@ -12000,7 +12094,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -12008,7 +12102,7 @@
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" ht="16.5" customHeight="1" thickBot="1">
       <c r="A26" s="12" t="s">
         <v>511</v>
       </c>
@@ -12025,7 +12119,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>219</v>
       </c>
@@ -12044,7 +12138,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" ht="16" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>220</v>
       </c>
@@ -12066,7 +12160,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" ht="16" thickBot="1">
       <c r="A29" s="8" t="s">
         <v>515</v>
       </c>
@@ -12085,7 +12179,7 @@
       </c>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>514</v>
       </c>
@@ -12107,7 +12201,7 @@
       </c>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>516</v>
       </c>
@@ -12129,7 +12223,7 @@
       </c>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12">
       <c r="A32" s="12" t="s">
         <v>239</v>
       </c>
@@ -12140,12 +12234,12 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
-    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" ht="30" thickBot="1">
       <c r="A37" s="8" t="s">
         <v>210</v>
       </c>
@@ -12175,7 +12269,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="8" t="s">
         <v>219</v>
       </c>
@@ -12208,7 +12302,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="8" t="s">
         <v>220</v>
       </c>
@@ -12249,7 +12343,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="8" t="s">
         <v>221</v>
       </c>
@@ -12290,7 +12384,7 @@
         <v>2196</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10">
       <c r="A41" s="12" t="s">
         <v>239</v>
       </c>
@@ -12304,7 +12398,7 @@
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10">
       <c r="A42" s="2"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -12316,12 +12410,12 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>285</v>
       </c>
@@ -12342,7 +12436,7 @@
       </c>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="8" t="s">
         <v>219</v>
       </c>
@@ -12366,7 +12460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="8" t="s">
         <v>220</v>
       </c>
@@ -12395,7 +12489,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="8" t="s">
         <v>221</v>
       </c>
@@ -12424,7 +12518,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10">
       <c r="A48" s="12" t="s">
         <v>239</v>
       </c>
@@ -12435,7 +12529,7 @@
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7">
       <c r="A49" s="2"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -12451,16 +12545,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -12474,7 +12568,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -12495,7 +12589,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -12516,7 +12610,7 @@
         <v>0.95277529961698948</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -12535,8 +12629,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -12557,7 +12651,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -12581,7 +12675,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -12610,7 +12704,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -12639,7 +12733,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -12650,7 +12744,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -12676,7 +12770,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -12706,7 +12800,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -12741,7 +12835,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -12776,7 +12870,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -12791,7 +12885,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" ht="16" thickBot="1">
       <c r="A20" s="16" t="s">
         <v>340</v>
       </c>
@@ -12805,7 +12899,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>219</v>
       </c>
@@ -12823,7 +12917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -12850,7 +12944,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>221</v>
       </c>
@@ -12877,30 +12971,30 @@
         <v>809</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11">
       <c r="A24" s="12" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G23" r:id="rId1"/>
+    <hyperlink ref="G23" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="E30" sqref="A25:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -12914,7 +13008,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -12935,7 +13029,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -12956,7 +13050,7 @@
         <v>0.90805800128462044</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -12975,8 +13069,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -12997,7 +13091,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -13021,7 +13115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -13050,7 +13144,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -13079,7 +13173,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -13090,7 +13184,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -13110,7 +13204,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -13134,7 +13228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -13163,7 +13257,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -13195,7 +13289,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -13204,7 +13298,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>340</v>
       </c>
@@ -13215,7 +13309,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="30" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>219</v>
       </c>
@@ -13230,7 +13324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>220</v>
       </c>
@@ -13247,7 +13341,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>221</v>
       </c>
@@ -13264,13 +13358,13 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8">
       <c r="A23" s="12" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="16" thickBot="1"/>
+    <row r="25" spans="1:8" ht="30" thickBot="1">
       <c r="A25" s="12" t="s">
         <v>511</v>
       </c>
@@ -13285,7 +13379,7 @@
       </c>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" ht="30" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>219</v>
       </c>
@@ -13303,7 +13397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>220</v>
       </c>
@@ -13324,7 +13418,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" ht="44" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>516</v>
       </c>
@@ -13348,7 +13442,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8">
       <c r="A29" s="12" t="s">
         <v>239</v>
       </c>
@@ -13366,16 +13460,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="E23" sqref="A20:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -13389,7 +13483,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -13410,7 +13504,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -13431,7 +13525,7 @@
         <v>0.9267197256851698</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -13450,8 +13544,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="16" thickBot="1"/>
+    <row r="7" spans="1:13" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -13472,7 +13566,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -13496,7 +13590,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -13525,7 +13619,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -13554,7 +13648,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -13565,7 +13659,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -13594,7 +13688,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -13627,7 +13721,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -13666,7 +13760,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -13705,7 +13799,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -13720,7 +13814,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13">
       <c r="L18" t="s">
         <v>588</v>
       </c>
@@ -13728,8 +13822,8 @@
         <v>594</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" ht="16" thickBot="1"/>
+    <row r="20" spans="1:13" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>511</v>
       </c>
@@ -13742,7 +13836,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:13" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>219</v>
       </c>
@@ -13758,7 +13852,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:13" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -13776,7 +13870,7 @@
       </c>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:13" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>516</v>
       </c>
@@ -13794,7 +13888,7 @@
       </c>
       <c r="E23" s="29"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13">
       <c r="A24" s="12" t="s">
         <v>239</v>
       </c>
@@ -13809,19 +13903,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -13835,7 +13929,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -13856,7 +13950,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -13877,7 +13971,7 @@
         <v>0.97448244785232785</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -13896,8 +13990,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -13918,7 +14012,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -13942,7 +14036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -13971,7 +14065,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -14000,7 +14094,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -14011,7 +14105,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="A13" s="12"/>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -14020,7 +14114,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="41"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -14043,7 +14137,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -14074,7 +14168,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -14110,7 +14204,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -14146,7 +14240,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -14161,7 +14255,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="J19" t="s">
         <v>581</v>
       </c>
@@ -14169,7 +14263,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11">
       <c r="J20" t="s">
         <v>649</v>
       </c>
@@ -14177,7 +14271,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" ht="16" thickBot="1">
       <c r="A21" s="16" t="s">
         <v>340</v>
       </c>
@@ -14188,7 +14282,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -14203,7 +14297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>220</v>
       </c>
@@ -14220,7 +14314,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>221</v>
       </c>
@@ -14237,7 +14331,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11">
       <c r="A25" s="12" t="s">
         <v>239</v>
       </c>
@@ -14248,16 +14342,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -14271,7 +14365,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -14292,7 +14386,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -14313,7 +14407,7 @@
         <v>0.98351979013457747</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -14332,8 +14426,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -14354,7 +14448,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -14378,7 +14472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -14407,7 +14501,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -14436,7 +14530,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -14447,7 +14541,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -14467,7 +14561,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -14491,7 +14585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -14520,7 +14614,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -14549,7 +14643,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -14558,8 +14652,8 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="16" thickBot="1"/>
+    <row r="21" spans="1:8" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>511</v>
       </c>
@@ -14574,7 +14668,7 @@
       </c>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -14592,7 +14686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>220</v>
       </c>
@@ -14616,7 +14710,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="44" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>516</v>
       </c>
@@ -14640,7 +14734,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8">
       <c r="A25" s="12" t="s">
         <v>239</v>
       </c>

</xml_diff>

<commit_message>
Coal prices SA + PL
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACD699B-0BC7-9947-87E1-86F509A47C0C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA648F0-F630-BC4D-93E6-310DBB44918C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1773" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1777" uniqueCount="834">
   <si>
     <t>Country</t>
   </si>
@@ -2537,6 +2537,18 @@
   </si>
   <si>
     <t>https://www.globalpetrolprices.com/heating_oil_prices/</t>
+  </si>
+  <si>
+    <t>Source price coal</t>
+  </si>
+  <si>
+    <t>http://gpi.tge.pl/en/web/wegiel/51;jsessionid=FE151D8133A5227E9CF83DD1E59C757A.gpi-app1</t>
+  </si>
+  <si>
+    <t>Price coal (bituminous) USD/t</t>
+  </si>
+  <si>
+    <t>Table 4.1(Jan 2017) http://www.energy.gov.za/files/media/explained/Energy-Price-Report-2018.pdf</t>
   </si>
 </sst>
 </file>
@@ -3046,11 +3058,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T152"/>
+  <dimension ref="A1:T154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T98" sqref="T98"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N102" sqref="N102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6154,1105 +6166,1098 @@
       </c>
     </row>
     <row r="72" spans="1:20">
-      <c r="A72" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="E72" t="s">
-        <v>426</v>
-      </c>
-      <c r="F72" t="s">
-        <v>426</v>
-      </c>
-      <c r="G72" t="s">
-        <v>426</v>
-      </c>
-      <c r="H72" t="s">
-        <v>426</v>
-      </c>
-      <c r="I72" t="s">
-        <v>425</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="M72" t="s">
-        <v>427</v>
-      </c>
-      <c r="N72" s="2" t="s">
-        <v>404</v>
+      <c r="A72" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="G72">
+        <f>240.49/G9</f>
+        <v>63.120734908136484</v>
+      </c>
+      <c r="O72">
+        <f>374/O9</f>
+        <v>71.510516252390047</v>
       </c>
     </row>
     <row r="73" spans="1:20">
       <c r="A73" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B73" t="s">
-        <v>208</v>
-      </c>
-      <c r="C73" t="s">
-        <v>443</v>
-      </c>
-      <c r="D73" t="s">
-        <v>442</v>
+        <v>102</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>423</v>
       </c>
       <c r="E73" t="s">
-        <v>445</v>
+        <v>426</v>
       </c>
       <c r="F73" t="s">
-        <v>447</v>
+        <v>426</v>
       </c>
       <c r="G73" t="s">
-        <v>450</v>
+        <v>426</v>
       </c>
       <c r="H73" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="I73" t="s">
-        <v>445</v>
-      </c>
-      <c r="J73" t="s">
-        <v>448</v>
-      </c>
-      <c r="K73" t="s">
-        <v>707</v>
-      </c>
-      <c r="L73" t="s">
-        <v>444</v>
+        <v>425</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>402</v>
       </c>
       <c r="M73" t="s">
-        <v>449</v>
-      </c>
-      <c r="N73" t="s">
-        <v>451</v>
+        <v>427</v>
+      </c>
+      <c r="N73" s="2" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="74" spans="1:20">
       <c r="A74" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B74" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="C74" t="s">
-        <v>202</v>
+        <v>443</v>
       </c>
       <c r="D74" t="s">
-        <v>201</v>
+        <v>442</v>
+      </c>
+      <c r="E74" t="s">
+        <v>445</v>
+      </c>
+      <c r="F74" t="s">
+        <v>447</v>
+      </c>
+      <c r="G74" t="s">
+        <v>450</v>
+      </c>
+      <c r="H74" t="s">
+        <v>446</v>
+      </c>
+      <c r="I74" t="s">
+        <v>445</v>
+      </c>
+      <c r="J74" t="s">
+        <v>448</v>
+      </c>
+      <c r="K74" t="s">
+        <v>707</v>
+      </c>
+      <c r="L74" t="s">
+        <v>444</v>
+      </c>
+      <c r="M74" t="s">
+        <v>449</v>
+      </c>
+      <c r="N74" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="75" spans="1:20">
       <c r="A75" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
+      </c>
+      <c r="B75" t="s">
+        <v>200</v>
+      </c>
+      <c r="C75" t="s">
+        <v>202</v>
+      </c>
+      <c r="D75" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="76" spans="1:20">
       <c r="A76" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B76" t="s">
-        <v>186</v>
-      </c>
-      <c r="C76" t="s">
-        <v>185</v>
-      </c>
-      <c r="D76" t="s">
-        <v>185</v>
-      </c>
-      <c r="E76" t="s">
-        <v>185</v>
-      </c>
-      <c r="F76" t="s">
-        <v>185</v>
-      </c>
-      <c r="G76" t="s">
-        <v>185</v>
-      </c>
-      <c r="H76" t="s">
-        <v>185</v>
-      </c>
-      <c r="I76" t="s">
-        <v>185</v>
-      </c>
-      <c r="J76" t="s">
-        <v>385</v>
-      </c>
-      <c r="K76" t="s">
-        <v>711</v>
-      </c>
-      <c r="L76" t="s">
-        <v>392</v>
-      </c>
-      <c r="M76" t="s">
-        <v>388</v>
+        <v>111</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="77" spans="1:20">
       <c r="A77" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B77" t="s">
-        <v>306</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>308</v>
+        <v>186</v>
+      </c>
+      <c r="C77" t="s">
+        <v>185</v>
       </c>
       <c r="D77" t="s">
-        <v>109</v>
-      </c>
-      <c r="L77" s="2" t="s">
-        <v>315</v>
+        <v>185</v>
+      </c>
+      <c r="E77" t="s">
+        <v>185</v>
+      </c>
+      <c r="F77" t="s">
+        <v>185</v>
+      </c>
+      <c r="G77" t="s">
+        <v>185</v>
+      </c>
+      <c r="H77" t="s">
+        <v>185</v>
+      </c>
+      <c r="I77" t="s">
+        <v>185</v>
+      </c>
+      <c r="J77" t="s">
+        <v>385</v>
+      </c>
+      <c r="K77" t="s">
+        <v>711</v>
+      </c>
+      <c r="L77" t="s">
+        <v>392</v>
+      </c>
+      <c r="M77" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="78" spans="1:20">
       <c r="A78" s="1" t="s">
-        <v>203</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="D78" t="s">
         <v>109</v>
       </c>
-      <c r="I78" t="s">
-        <v>328</v>
-      </c>
-      <c r="L78" t="s">
-        <v>110</v>
+      <c r="L78" s="2" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="79" spans="1:20">
       <c r="A79" s="1" t="s">
-        <v>107</v>
+        <v>203</v>
       </c>
       <c r="B79" t="s">
-        <v>184</v>
+        <v>307</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D79" t="s">
+        <v>109</v>
+      </c>
+      <c r="I79" t="s">
+        <v>328</v>
+      </c>
+      <c r="L79" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:20">
       <c r="A80" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B80" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14">
+      <c r="A81" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B81" s="5" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="81" spans="1:20">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:14">
+      <c r="A82" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:20">
-      <c r="A82" s="6" t="s">
+    <row r="83" spans="1:14">
+      <c r="A83" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>125</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>135</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D83" t="s">
         <v>129</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F83" t="s">
         <v>491</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G83" t="s">
         <v>475</v>
       </c>
-      <c r="H82" t="s">
+      <c r="H83" t="s">
         <v>625</v>
       </c>
-      <c r="I82" t="s">
+      <c r="I83" t="s">
         <v>147</v>
       </c>
-      <c r="J82" t="s">
+      <c r="J83" t="s">
         <v>470</v>
       </c>
-      <c r="K82" t="s">
+      <c r="K83" t="s">
         <v>564</v>
       </c>
-      <c r="L82" t="s">
+      <c r="L83" t="s">
         <v>138</v>
       </c>
-      <c r="M82" t="s">
+      <c r="M83" t="s">
         <v>460</v>
       </c>
-      <c r="N82" t="s">
+      <c r="N83" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="83" spans="1:20">
-      <c r="A83" s="6" t="s">
+    <row r="84" spans="1:14">
+      <c r="A84" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>126</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C84" t="s">
         <v>136</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D84" t="s">
         <v>134</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F84" t="s">
         <v>347</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G84" t="s">
         <v>476</v>
       </c>
-      <c r="H83" t="s">
+      <c r="H84" t="s">
         <v>626</v>
       </c>
-      <c r="I83" t="s">
+      <c r="I84" t="s">
         <v>148</v>
       </c>
-      <c r="J83" t="s">
+      <c r="J84" t="s">
         <v>471</v>
       </c>
-      <c r="K83" t="s">
+      <c r="K84" t="s">
         <v>549</v>
       </c>
-      <c r="L83" t="s">
+      <c r="L84" t="s">
         <v>139</v>
       </c>
-      <c r="M83" t="s">
+      <c r="M84" t="s">
         <v>462</v>
       </c>
-      <c r="N83" t="s">
+      <c r="N84" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="84" spans="1:20">
-      <c r="A84" s="6" t="s">
+    <row r="85" spans="1:14">
+      <c r="A85" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>127</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>137</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D85" t="s">
         <v>130</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F85" t="s">
         <v>348</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G85" t="s">
         <v>477</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H85" t="s">
         <v>627</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I85" t="s">
         <v>149</v>
       </c>
-      <c r="J84" t="s">
+      <c r="J85" t="s">
         <v>472</v>
       </c>
-      <c r="K84" t="s">
+      <c r="K85" t="s">
         <v>544</v>
       </c>
-      <c r="L84" t="s">
+      <c r="L85" t="s">
         <v>140</v>
       </c>
-      <c r="M84" t="s">
+      <c r="M85" t="s">
         <v>464</v>
       </c>
-      <c r="N84" t="s">
+      <c r="N85" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="85" spans="1:20">
-      <c r="A85" s="6" t="s">
+    <row r="86" spans="1:14">
+      <c r="A86" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B85" s="7" t="s">
+      <c r="B86" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>309</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D86" t="s">
         <v>131</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F86" t="s">
         <v>349</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G86" t="s">
         <v>478</v>
       </c>
-      <c r="H85" t="s">
+      <c r="H86" t="s">
         <v>628</v>
       </c>
-      <c r="I85" t="s">
+      <c r="I86" t="s">
         <v>150</v>
       </c>
-      <c r="J85" t="s">
+      <c r="J86" t="s">
         <v>473</v>
       </c>
-      <c r="K85" t="s">
+      <c r="K86" t="s">
         <v>483</v>
       </c>
-      <c r="L85" t="s">
+      <c r="L86" t="s">
         <v>141</v>
       </c>
-      <c r="M85" t="s">
+      <c r="M86" t="s">
         <v>466</v>
       </c>
-      <c r="N85" t="s">
+      <c r="N86" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="86" spans="1:20">
-      <c r="A86" s="6" t="s">
+    <row r="87" spans="1:14">
+      <c r="A87" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D87" t="s">
         <v>132</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F87" t="s">
         <v>350</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G87" t="s">
         <v>479</v>
       </c>
-      <c r="H86" t="s">
+      <c r="H87" t="s">
         <v>629</v>
       </c>
-      <c r="I86" t="s">
+      <c r="I87" t="s">
         <v>151</v>
       </c>
-      <c r="J86" t="s">
+      <c r="J87" t="s">
         <v>474</v>
       </c>
-      <c r="K86" t="s">
+      <c r="K87" t="s">
         <v>545</v>
       </c>
-      <c r="L86" t="s">
+      <c r="L87" t="s">
         <v>142</v>
       </c>
-      <c r="M86" t="s">
+      <c r="M87" t="s">
         <v>468</v>
       </c>
-      <c r="N86" t="s">
+      <c r="N87" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="87" spans="1:20">
-      <c r="A87" s="6" t="s">
+    <row r="88" spans="1:14">
+      <c r="A88" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D88" t="s">
         <v>133</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F88" t="s">
         <v>351</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G88" t="s">
         <v>480</v>
       </c>
-      <c r="H87" t="s">
+      <c r="H88" t="s">
         <v>630</v>
       </c>
-      <c r="I87" t="s">
+      <c r="I88" t="s">
         <v>152</v>
       </c>
-      <c r="K87" t="s">
+      <c r="K88" t="s">
         <v>546</v>
       </c>
-      <c r="L87" t="s">
+      <c r="L88" t="s">
         <v>143</v>
       </c>
-      <c r="M87" t="s">
+      <c r="M88" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="88" spans="1:20">
-      <c r="A88" s="6" t="s">
+    <row r="89" spans="1:14">
+      <c r="A89" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F89" t="s">
         <v>459</v>
       </c>
-      <c r="H88" t="s">
+      <c r="H89" t="s">
         <v>631</v>
       </c>
-      <c r="K88" t="s">
+      <c r="K89" t="s">
         <v>547</v>
       </c>
-      <c r="L88" t="s">
+      <c r="L89" t="s">
         <v>144</v>
       </c>
-      <c r="M88" t="s">
+      <c r="M89" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="89" spans="1:20">
-      <c r="A89" s="6" t="s">
+    <row r="90" spans="1:14">
+      <c r="A90" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H89" t="s">
+      <c r="H90" t="s">
         <v>632</v>
       </c>
-      <c r="K89" t="s">
+      <c r="K90" t="s">
         <v>548</v>
       </c>
-      <c r="L89" t="s">
+      <c r="L90" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="90" spans="1:20">
-      <c r="A90" s="6" t="s">
+    <row r="91" spans="1:14">
+      <c r="A91" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H90" t="s">
+      <c r="H91" t="s">
         <v>633</v>
       </c>
-      <c r="L90" t="s">
+      <c r="L91" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="91" spans="1:20">
-      <c r="A91" s="6" t="s">
+    <row r="92" spans="1:14">
+      <c r="A92" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H92" t="s">
         <v>634</v>
       </c>
-      <c r="L91" t="s">
+      <c r="L92" t="s">
         <v>483</v>
       </c>
-      <c r="M91" t="s">
+      <c r="M92" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="92" spans="1:20">
-      <c r="A92" s="6" t="s">
+    <row r="93" spans="1:14">
+      <c r="A93" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="93" spans="1:20">
-      <c r="A93" s="6" t="s">
+    <row r="94" spans="1:14">
+      <c r="A94" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="94" spans="1:20">
-      <c r="A94" s="6" t="s">
+    <row r="95" spans="1:14">
+      <c r="A95" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="95" spans="1:20">
-      <c r="A95" s="6" t="s">
+    <row r="96" spans="1:14">
+      <c r="A96" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>199</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>382</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D96" t="s">
         <v>382</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E96" t="s">
         <v>382</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F96" t="s">
         <v>382</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G96" t="s">
         <v>382</v>
       </c>
-      <c r="H95" t="s">
+      <c r="H96" t="s">
         <v>382</v>
       </c>
-      <c r="I95" t="s">
+      <c r="I96" t="s">
         <v>382</v>
       </c>
-      <c r="J95" t="s">
+      <c r="J96" t="s">
         <v>382</v>
       </c>
-      <c r="L95" t="s">
+      <c r="L96" t="s">
         <v>382</v>
       </c>
-      <c r="M95" t="s">
+      <c r="M96" t="s">
         <v>382</v>
       </c>
-      <c r="N95" t="s">
+      <c r="N96" t="s">
         <v>382</v>
-      </c>
-    </row>
-    <row r="96" spans="1:20">
-      <c r="A96" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="B96" t="s">
-        <v>192</v>
-      </c>
-      <c r="C96" t="s">
-        <v>821</v>
-      </c>
-      <c r="D96" t="s">
-        <v>821</v>
-      </c>
-      <c r="E96" t="s">
-        <v>821</v>
-      </c>
-      <c r="F96" t="s">
-        <v>821</v>
-      </c>
-      <c r="G96" t="s">
-        <v>821</v>
-      </c>
-      <c r="H96" t="s">
-        <v>821</v>
-      </c>
-      <c r="I96" t="s">
-        <v>821</v>
-      </c>
-      <c r="J96" t="s">
-        <v>821</v>
-      </c>
-      <c r="K96" t="s">
-        <v>821</v>
-      </c>
-      <c r="L96" t="s">
-        <v>821</v>
-      </c>
-      <c r="M96" t="s">
-        <v>821</v>
-      </c>
-      <c r="N96" t="s">
-        <v>821</v>
-      </c>
-      <c r="O96" t="s">
-        <v>821</v>
-      </c>
-      <c r="P96" t="s">
-        <v>821</v>
-      </c>
-      <c r="T96" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="97" spans="1:20">
       <c r="A97" s="4" t="s">
-        <v>827</v>
+        <v>191</v>
       </c>
       <c r="B97" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="G97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="H97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="I97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="J97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="K97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="L97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="M97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="N97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="O97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="P97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="T97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="98" spans="1:20">
       <c r="A98" s="4" t="s">
-        <v>828</v>
+        <v>827</v>
+      </c>
+      <c r="B98" t="s">
+        <v>194</v>
       </c>
       <c r="C98" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
       <c r="D98" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
       <c r="E98" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
       <c r="F98" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
       <c r="G98" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
       <c r="H98" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
       <c r="I98" t="s">
-        <v>829</v>
+        <v>822</v>
+      </c>
+      <c r="J98" t="s">
+        <v>822</v>
+      </c>
+      <c r="K98" t="s">
+        <v>822</v>
+      </c>
+      <c r="L98" t="s">
+        <v>822</v>
+      </c>
+      <c r="M98" t="s">
+        <v>822</v>
+      </c>
+      <c r="N98" t="s">
+        <v>822</v>
+      </c>
+      <c r="O98" t="s">
+        <v>822</v>
+      </c>
+      <c r="P98" t="s">
+        <v>822</v>
       </c>
       <c r="T98" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
     </row>
     <row r="99" spans="1:20">
       <c r="A99" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="C99" t="s">
+        <v>829</v>
+      </c>
+      <c r="D99" t="s">
+        <v>829</v>
+      </c>
+      <c r="E99" t="s">
+        <v>829</v>
+      </c>
+      <c r="F99" t="s">
+        <v>829</v>
+      </c>
+      <c r="G99" t="s">
+        <v>829</v>
+      </c>
+      <c r="H99" t="s">
+        <v>829</v>
+      </c>
+      <c r="I99" t="s">
+        <v>829</v>
+      </c>
+      <c r="T99" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20">
+      <c r="A100" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>197</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>823</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D100" t="s">
         <v>823</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E100" t="s">
         <v>823</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F100" t="s">
         <v>823</v>
       </c>
-      <c r="H99" t="s">
+      <c r="H100" t="s">
         <v>823</v>
       </c>
-      <c r="I99" t="s">
+      <c r="I100" t="s">
         <v>823</v>
       </c>
-      <c r="P99" t="s">
+      <c r="P100" t="s">
         <v>823</v>
       </c>
-      <c r="T99" t="s">
+      <c r="T100" t="s">
         <v>823</v>
       </c>
     </row>
-    <row r="100" spans="1:20">
-      <c r="A100" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="B100" t="s">
-        <v>298</v>
-      </c>
-      <c r="C100" t="s">
-        <v>277</v>
-      </c>
-      <c r="D100" t="s">
-        <v>290</v>
-      </c>
-    </row>
     <row r="101" spans="1:20">
-      <c r="A101" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="B101" t="s">
-        <v>297</v>
-      </c>
-      <c r="C101" t="s">
-        <v>278</v>
-      </c>
-      <c r="D101" t="s">
-        <v>291</v>
+      <c r="A101" s="4" t="s">
+        <v>830</v>
+      </c>
+      <c r="G101" t="s">
+        <v>831</v>
+      </c>
+      <c r="N101" t="s">
+        <v>833</v>
       </c>
     </row>
     <row r="102" spans="1:20">
       <c r="A102" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B102" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C102" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D102" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="103" spans="1:20">
       <c r="A103" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
+      </c>
+      <c r="B103" t="s">
+        <v>297</v>
+      </c>
+      <c r="C103" t="s">
+        <v>278</v>
       </c>
       <c r="D103" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="104" spans="1:20">
       <c r="A104" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B104" t="s">
-        <v>294</v>
+        <v>296</v>
+      </c>
+      <c r="C104" t="s">
+        <v>276</v>
+      </c>
+      <c r="D104" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="105" spans="1:20">
       <c r="A105" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="B105" t="s">
-        <v>295</v>
-      </c>
-      <c r="C105" s="19" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D105" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="106" spans="1:20">
       <c r="A106" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B106" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
     </row>
     <row r="107" spans="1:20">
       <c r="A107" s="6" t="s">
-        <v>292</v>
+        <v>273</v>
+      </c>
+      <c r="B107" t="s">
+        <v>295</v>
+      </c>
+      <c r="C107" s="19" t="s">
+        <v>267</v>
       </c>
       <c r="D107" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="108" spans="1:20">
       <c r="A108" s="6" t="s">
-        <v>333</v>
+        <v>274</v>
       </c>
       <c r="B108" t="s">
-        <v>334</v>
-      </c>
-      <c r="C108" t="s">
-        <v>336</v>
-      </c>
-      <c r="D108" t="s">
-        <v>458</v>
-      </c>
-      <c r="E108" t="s">
-        <v>602</v>
-      </c>
-      <c r="F108" t="s">
-        <v>517</v>
-      </c>
-      <c r="G108" t="s">
-        <v>635</v>
-      </c>
-      <c r="H108" t="s">
-        <v>599</v>
-      </c>
-      <c r="I108" t="s">
-        <v>530</v>
-      </c>
-      <c r="J108" t="s">
-        <v>600</v>
-      </c>
-      <c r="L108" t="s">
-        <v>516</v>
-      </c>
-      <c r="M108" t="s">
-        <v>657</v>
-      </c>
-      <c r="N108" s="34" t="s">
-        <v>531</v>
+        <v>275</v>
       </c>
     </row>
     <row r="109" spans="1:20">
       <c r="A109" s="6" t="s">
-        <v>485</v>
-      </c>
-      <c r="C109" t="s">
-        <v>335</v>
-      </c>
-      <c r="F109" t="s">
-        <v>718</v>
-      </c>
-      <c r="G109" t="s">
-        <v>528</v>
-      </c>
-      <c r="H109" t="s">
-        <v>601</v>
-      </c>
-      <c r="J109" t="s">
-        <v>493</v>
-      </c>
-      <c r="K109" t="s">
-        <v>654</v>
-      </c>
-      <c r="L109" t="s">
-        <v>484</v>
-      </c>
-      <c r="M109" t="s">
-        <v>492</v>
-      </c>
-      <c r="N109" t="s">
-        <v>527</v>
+        <v>292</v>
+      </c>
+      <c r="D109" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="110" spans="1:20">
       <c r="A110" s="6" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B110" t="s">
-        <v>338</v>
+        <v>334</v>
+      </c>
+      <c r="C110" t="s">
+        <v>336</v>
+      </c>
+      <c r="D110" t="s">
+        <v>458</v>
+      </c>
+      <c r="E110" t="s">
+        <v>602</v>
+      </c>
+      <c r="F110" t="s">
+        <v>517</v>
+      </c>
+      <c r="G110" t="s">
+        <v>635</v>
+      </c>
+      <c r="H110" t="s">
+        <v>599</v>
+      </c>
+      <c r="I110" t="s">
+        <v>530</v>
+      </c>
+      <c r="J110" t="s">
+        <v>600</v>
+      </c>
+      <c r="L110" t="s">
+        <v>516</v>
+      </c>
+      <c r="M110" t="s">
+        <v>657</v>
+      </c>
+      <c r="N110" s="34" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="111" spans="1:20">
       <c r="A111" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="E111">
-        <v>7</v>
-      </c>
-      <c r="F111">
-        <v>10</v>
-      </c>
-      <c r="G111">
-        <v>10</v>
-      </c>
-      <c r="H111">
-        <v>10</v>
-      </c>
-      <c r="I111">
-        <v>7</v>
-      </c>
-      <c r="J111">
-        <v>7</v>
-      </c>
-      <c r="M111">
-        <v>7</v>
-      </c>
-      <c r="N111">
-        <v>10</v>
+        <v>485</v>
+      </c>
+      <c r="C111" t="s">
+        <v>335</v>
+      </c>
+      <c r="F111" t="s">
+        <v>718</v>
+      </c>
+      <c r="G111" t="s">
+        <v>528</v>
+      </c>
+      <c r="H111" t="s">
+        <v>601</v>
+      </c>
+      <c r="J111" t="s">
+        <v>493</v>
+      </c>
+      <c r="K111" t="s">
+        <v>654</v>
+      </c>
+      <c r="L111" t="s">
+        <v>484</v>
+      </c>
+      <c r="M111" t="s">
+        <v>492</v>
+      </c>
+      <c r="N111" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="112" spans="1:20">
       <c r="A112" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="E112">
-        <v>6300</v>
-      </c>
-      <c r="F112">
-        <v>6300</v>
-      </c>
-      <c r="G112">
-        <v>6300</v>
-      </c>
-      <c r="H112">
-        <v>6300</v>
-      </c>
-      <c r="I112">
-        <v>6300</v>
-      </c>
-      <c r="J112">
-        <v>6300</v>
-      </c>
-      <c r="K112">
-        <v>6000</v>
-      </c>
-      <c r="M112">
-        <v>6300</v>
-      </c>
-      <c r="N112">
-        <v>6300</v>
+        <v>337</v>
+      </c>
+      <c r="B112" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="113" spans="1:18">
       <c r="A113" s="6" t="s">
-        <v>660</v>
+        <v>488</v>
       </c>
       <c r="E113">
-        <v>6500</v>
+        <v>7</v>
       </c>
       <c r="F113">
-        <v>6500</v>
+        <v>10</v>
       </c>
       <c r="G113">
-        <v>8000</v>
+        <v>10</v>
       </c>
       <c r="H113">
-        <v>6500</v>
+        <v>10</v>
       </c>
       <c r="I113">
-        <v>6500</v>
+        <v>7</v>
       </c>
       <c r="J113">
-        <v>9000</v>
-      </c>
-      <c r="K113">
-        <v>7900</v>
+        <v>7</v>
       </c>
       <c r="M113">
-        <v>8000</v>
+        <v>7</v>
       </c>
       <c r="N113">
-        <v>9000</v>
-      </c>
-      <c r="R113">
-        <v>9000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:18">
       <c r="A114" s="6" t="s">
-        <v>495</v>
-      </c>
-      <c r="B114" t="s">
-        <v>501</v>
-      </c>
-      <c r="C114" t="s">
-        <v>497</v>
-      </c>
-      <c r="D114" t="s">
-        <v>499</v>
+        <v>490</v>
+      </c>
+      <c r="E114">
+        <v>6300</v>
+      </c>
+      <c r="F114">
+        <v>6300</v>
+      </c>
+      <c r="G114">
+        <v>6300</v>
+      </c>
+      <c r="H114">
+        <v>6300</v>
+      </c>
+      <c r="I114">
+        <v>6300</v>
+      </c>
+      <c r="J114">
+        <v>6300</v>
+      </c>
+      <c r="K114">
+        <v>6000</v>
+      </c>
+      <c r="M114">
+        <v>6300</v>
+      </c>
+      <c r="N114">
+        <v>6300</v>
       </c>
     </row>
     <row r="115" spans="1:18">
       <c r="A115" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="B115" t="s">
-        <v>502</v>
-      </c>
-      <c r="C115" t="s">
-        <v>498</v>
-      </c>
-      <c r="D115" t="s">
-        <v>500</v>
+        <v>660</v>
+      </c>
+      <c r="E115">
+        <v>6500</v>
+      </c>
+      <c r="F115">
+        <v>6500</v>
+      </c>
+      <c r="G115">
+        <v>8000</v>
+      </c>
+      <c r="H115">
+        <v>6500</v>
+      </c>
+      <c r="I115">
+        <v>6500</v>
+      </c>
+      <c r="J115">
+        <v>9000</v>
+      </c>
+      <c r="K115">
+        <v>7900</v>
+      </c>
+      <c r="M115">
+        <v>8000</v>
+      </c>
+      <c r="N115">
+        <v>9000</v>
+      </c>
+      <c r="R115">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18">
+      <c r="A116" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="B116" t="s">
+        <v>501</v>
+      </c>
+      <c r="C116" t="s">
+        <v>497</v>
+      </c>
+      <c r="D116" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="117" spans="1:18">
       <c r="A117" s="6" t="s">
-        <v>717</v>
-      </c>
-      <c r="F117" t="s">
-        <v>457</v>
-      </c>
-      <c r="G117" t="s">
-        <v>457</v>
-      </c>
-      <c r="H117" t="s">
-        <v>457</v>
-      </c>
-      <c r="J117" t="s">
-        <v>457</v>
-      </c>
-      <c r="K117" t="s">
-        <v>457</v>
-      </c>
-      <c r="L117" t="s">
-        <v>457</v>
-      </c>
-      <c r="M117" t="s">
-        <v>457</v>
-      </c>
-      <c r="N117" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="118" spans="1:18">
-      <c r="A118" s="6" t="s">
-        <v>738</v>
-      </c>
-      <c r="F118" t="s">
-        <v>457</v>
+        <v>496</v>
+      </c>
+      <c r="B117" t="s">
+        <v>502</v>
+      </c>
+      <c r="C117" t="s">
+        <v>498</v>
+      </c>
+      <c r="D117" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="119" spans="1:18">
       <c r="A119" s="6" t="s">
-        <v>669</v>
+        <v>717</v>
+      </c>
+      <c r="F119" t="s">
+        <v>457</v>
+      </c>
+      <c r="G119" t="s">
+        <v>457</v>
+      </c>
+      <c r="H119" t="s">
+        <v>457</v>
+      </c>
+      <c r="J119" t="s">
+        <v>457</v>
+      </c>
+      <c r="K119" t="s">
+        <v>457</v>
+      </c>
+      <c r="L119" t="s">
+        <v>457</v>
+      </c>
+      <c r="M119" t="s">
+        <v>457</v>
+      </c>
+      <c r="N119" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="120" spans="1:18">
       <c r="A120" s="6" t="s">
-        <v>670</v>
-      </c>
-      <c r="M120" t="s">
-        <v>678</v>
-      </c>
-      <c r="N120" t="s">
-        <v>678</v>
+        <v>738</v>
+      </c>
+      <c r="F120" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="121" spans="1:18">
       <c r="A121" s="6" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="122" spans="1:18">
       <c r="A122" s="6" t="s">
-        <v>672</v>
-      </c>
-      <c r="F122" t="s">
-        <v>678</v>
-      </c>
-      <c r="G122" t="s">
-        <v>678</v>
-      </c>
-      <c r="H122" t="s">
-        <v>678</v>
-      </c>
-      <c r="J122" t="s">
-        <v>678</v>
-      </c>
-      <c r="L122" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="M122" t="s">
         <v>678</v>
@@ -7263,205 +7268,196 @@
     </row>
     <row r="123" spans="1:18">
       <c r="A123" s="6" t="s">
-        <v>673</v>
-      </c>
-      <c r="E123" t="s">
-        <v>674</v>
-      </c>
-      <c r="F123" t="s">
-        <v>674</v>
-      </c>
-      <c r="G123" t="s">
-        <v>674</v>
-      </c>
-      <c r="H123" t="s">
-        <v>674</v>
-      </c>
-      <c r="I123" t="s">
-        <v>674</v>
-      </c>
-      <c r="J123" t="s">
-        <v>674</v>
-      </c>
-      <c r="K123" t="s">
-        <v>674</v>
-      </c>
-      <c r="L123" t="s">
-        <v>674</v>
-      </c>
-      <c r="M123" t="s">
-        <v>674</v>
-      </c>
-      <c r="N123" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="124" spans="1:18">
       <c r="A124" s="6" t="s">
-        <v>675</v>
-      </c>
-      <c r="E124" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="F124" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="G124" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="H124" t="s">
-        <v>674</v>
-      </c>
-      <c r="I124" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="J124" t="s">
-        <v>674</v>
-      </c>
-      <c r="K124" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="L124" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="M124" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="N124" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
     </row>
     <row r="125" spans="1:18">
       <c r="A125" s="6" t="s">
-        <v>676</v>
+        <v>673</v>
+      </c>
+      <c r="E125" t="s">
+        <v>674</v>
+      </c>
+      <c r="F125" t="s">
+        <v>674</v>
+      </c>
+      <c r="G125" t="s">
+        <v>674</v>
+      </c>
+      <c r="H125" t="s">
+        <v>674</v>
+      </c>
+      <c r="I125" t="s">
+        <v>674</v>
+      </c>
+      <c r="J125" t="s">
+        <v>674</v>
+      </c>
+      <c r="K125" t="s">
+        <v>674</v>
+      </c>
+      <c r="L125" t="s">
+        <v>674</v>
+      </c>
+      <c r="M125" t="s">
+        <v>674</v>
+      </c>
+      <c r="N125" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="126" spans="1:18">
       <c r="A126" s="6" t="s">
-        <v>677</v>
+        <v>675</v>
+      </c>
+      <c r="E126" t="s">
+        <v>674</v>
+      </c>
+      <c r="F126" t="s">
+        <v>674</v>
+      </c>
+      <c r="G126" t="s">
+        <v>674</v>
+      </c>
+      <c r="H126" t="s">
+        <v>674</v>
+      </c>
+      <c r="I126" t="s">
+        <v>674</v>
+      </c>
+      <c r="J126" t="s">
+        <v>674</v>
+      </c>
+      <c r="K126" t="s">
+        <v>674</v>
       </c>
       <c r="L126" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="M126" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="N126" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="127" spans="1:18">
       <c r="A127" s="6" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="128" spans="1:18">
       <c r="A128" s="6" t="s">
-        <v>680</v>
-      </c>
-      <c r="E128" t="s">
-        <v>300</v>
-      </c>
-      <c r="F128" t="s">
-        <v>300</v>
-      </c>
-      <c r="G128" t="s">
-        <v>300</v>
-      </c>
-      <c r="H128" t="s">
-        <v>300</v>
-      </c>
-      <c r="I128" t="s">
-        <v>300</v>
-      </c>
-      <c r="J128" t="s">
-        <v>300</v>
-      </c>
-      <c r="K128" t="s">
-        <v>300</v>
+        <v>677</v>
       </c>
       <c r="L128" t="s">
-        <v>300</v>
+        <v>678</v>
       </c>
       <c r="M128" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="N128" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
     </row>
     <row r="129" spans="1:14">
       <c r="A129" s="6" t="s">
-        <v>681</v>
-      </c>
-      <c r="E129" t="s">
-        <v>300</v>
-      </c>
-      <c r="F129" t="s">
-        <v>300</v>
-      </c>
-      <c r="G129" t="s">
-        <v>300</v>
-      </c>
-      <c r="H129" t="s">
-        <v>300</v>
-      </c>
-      <c r="I129" t="s">
-        <v>300</v>
-      </c>
-      <c r="J129" t="s">
-        <v>300</v>
-      </c>
-      <c r="K129" t="s">
-        <v>300</v>
-      </c>
-      <c r="N129" t="s">
-        <v>300</v>
+        <v>679</v>
       </c>
     </row>
     <row r="130" spans="1:14">
       <c r="A130" s="6" t="s">
-        <v>704</v>
+        <v>680</v>
+      </c>
+      <c r="E130" t="s">
+        <v>300</v>
+      </c>
+      <c r="F130" t="s">
+        <v>300</v>
+      </c>
+      <c r="G130" t="s">
+        <v>300</v>
+      </c>
+      <c r="H130" t="s">
+        <v>300</v>
+      </c>
+      <c r="I130" t="s">
+        <v>300</v>
+      </c>
+      <c r="J130" t="s">
+        <v>300</v>
+      </c>
+      <c r="K130" t="s">
+        <v>300</v>
       </c>
       <c r="L130" t="s">
-        <v>674</v>
+        <v>300</v>
       </c>
       <c r="M130" t="s">
-        <v>674</v>
+        <v>686</v>
+      </c>
+      <c r="N130" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="131" spans="1:14">
       <c r="A131" s="6" t="s">
-        <v>682</v>
-      </c>
-      <c r="L131" t="s">
-        <v>674</v>
+        <v>681</v>
+      </c>
+      <c r="E131" t="s">
+        <v>300</v>
+      </c>
+      <c r="F131" t="s">
+        <v>300</v>
+      </c>
+      <c r="G131" t="s">
+        <v>300</v>
+      </c>
+      <c r="H131" t="s">
+        <v>300</v>
+      </c>
+      <c r="I131" t="s">
+        <v>300</v>
+      </c>
+      <c r="J131" t="s">
+        <v>300</v>
+      </c>
+      <c r="K131" t="s">
+        <v>300</v>
+      </c>
+      <c r="N131" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="132" spans="1:14">
       <c r="A132" s="6" t="s">
-        <v>683</v>
-      </c>
-      <c r="E132" t="s">
-        <v>674</v>
-      </c>
-      <c r="F132" t="s">
-        <v>674</v>
-      </c>
-      <c r="G132" t="s">
-        <v>674</v>
-      </c>
-      <c r="H132" t="s">
-        <v>674</v>
-      </c>
-      <c r="I132" t="s">
-        <v>674</v>
-      </c>
-      <c r="J132" t="s">
-        <v>674</v>
-      </c>
-      <c r="K132" t="s">
-        <v>674</v>
+        <v>704</v>
       </c>
       <c r="L132" t="s">
         <v>674</v>
@@ -7469,78 +7465,84 @@
       <c r="M132" t="s">
         <v>674</v>
       </c>
-      <c r="N132" t="s">
-        <v>674</v>
-      </c>
     </row>
     <row r="133" spans="1:14">
       <c r="A133" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
+      </c>
+      <c r="L133" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="134" spans="1:14">
       <c r="A134" s="6" t="s">
-        <v>685</v>
+        <v>683</v>
+      </c>
+      <c r="E134" t="s">
+        <v>674</v>
+      </c>
+      <c r="F134" t="s">
+        <v>674</v>
+      </c>
+      <c r="G134" t="s">
+        <v>674</v>
+      </c>
+      <c r="H134" t="s">
+        <v>674</v>
+      </c>
+      <c r="I134" t="s">
+        <v>674</v>
+      </c>
+      <c r="J134" t="s">
+        <v>674</v>
+      </c>
+      <c r="K134" t="s">
+        <v>674</v>
       </c>
       <c r="L134" t="s">
-        <v>678</v>
+        <v>674</v>
+      </c>
+      <c r="M134" t="s">
+        <v>674</v>
+      </c>
+      <c r="N134" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="6" t="s">
-        <v>739</v>
-      </c>
-      <c r="E135" t="s">
-        <v>674</v>
-      </c>
-      <c r="F135" t="s">
-        <v>674</v>
-      </c>
-      <c r="G135" t="s">
-        <v>674</v>
-      </c>
-      <c r="H135" t="s">
-        <v>674</v>
-      </c>
-      <c r="I135" t="s">
-        <v>674</v>
-      </c>
-      <c r="J135" t="s">
-        <v>674</v>
-      </c>
-      <c r="K135" t="s">
-        <v>674</v>
-      </c>
-      <c r="L135" t="s">
-        <v>674</v>
-      </c>
-      <c r="M135" t="s">
-        <v>674</v>
-      </c>
-      <c r="N135" t="s">
-        <v>674</v>
+        <v>684</v>
       </c>
     </row>
     <row r="136" spans="1:14">
       <c r="A136" s="6" t="s">
-        <v>687</v>
+        <v>685</v>
+      </c>
+      <c r="L136" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="137" spans="1:14">
       <c r="A137" s="6" t="s">
-        <v>688</v>
+        <v>739</v>
       </c>
       <c r="E137" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="F137" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="G137" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="H137" t="s">
-        <v>689</v>
+        <v>674</v>
+      </c>
+      <c r="I137" t="s">
+        <v>674</v>
+      </c>
+      <c r="J137" t="s">
+        <v>674</v>
       </c>
       <c r="K137" t="s">
         <v>674</v>
@@ -7548,76 +7550,64 @@
       <c r="L137" t="s">
         <v>674</v>
       </c>
+      <c r="M137" t="s">
+        <v>674</v>
+      </c>
+      <c r="N137" t="s">
+        <v>674</v>
+      </c>
     </row>
     <row r="138" spans="1:14">
       <c r="A138" s="6" t="s">
-        <v>690</v>
-      </c>
-      <c r="K138" t="s">
-        <v>678</v>
-      </c>
-      <c r="L138" t="s">
-        <v>678</v>
-      </c>
-      <c r="M138" t="s">
-        <v>678</v>
-      </c>
-      <c r="N138" t="s">
-        <v>678</v>
+        <v>687</v>
       </c>
     </row>
     <row r="139" spans="1:14">
       <c r="A139" s="6" t="s">
-        <v>691</v>
+        <v>688</v>
+      </c>
+      <c r="E139" t="s">
+        <v>689</v>
+      </c>
+      <c r="F139" t="s">
+        <v>689</v>
+      </c>
+      <c r="G139" t="s">
+        <v>689</v>
+      </c>
+      <c r="H139" t="s">
+        <v>689</v>
       </c>
       <c r="K139" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="L139" t="s">
-        <v>678</v>
-      </c>
-      <c r="M139" t="s">
-        <v>678</v>
-      </c>
-      <c r="N139" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="140" spans="1:14">
       <c r="A140" s="6" t="s">
-        <v>692</v>
-      </c>
-      <c r="E140" t="s">
-        <v>300</v>
-      </c>
-      <c r="F140" t="s">
-        <v>300</v>
-      </c>
-      <c r="G140" t="s">
-        <v>300</v>
-      </c>
-      <c r="H140" t="s">
-        <v>300</v>
-      </c>
-      <c r="I140" t="s">
-        <v>300</v>
-      </c>
-      <c r="J140" t="s">
-        <v>300</v>
+        <v>690</v>
+      </c>
+      <c r="K140" t="s">
+        <v>678</v>
       </c>
       <c r="L140" t="s">
-        <v>300</v>
+        <v>678</v>
       </c>
       <c r="M140" t="s">
-        <v>300</v>
+        <v>678</v>
       </c>
       <c r="N140" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
     </row>
     <row r="141" spans="1:14">
-      <c r="A141" s="1" t="s">
-        <v>694</v>
+      <c r="A141" s="6" t="s">
+        <v>691</v>
+      </c>
+      <c r="K141" t="s">
+        <v>678</v>
       </c>
       <c r="L141" t="s">
         <v>678</v>
@@ -7631,33 +7621,45 @@
     </row>
     <row r="142" spans="1:14">
       <c r="A142" s="6" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E142" t="s">
-        <v>674</v>
+        <v>300</v>
       </c>
       <c r="F142" t="s">
-        <v>674</v>
+        <v>300</v>
       </c>
       <c r="G142" t="s">
-        <v>674</v>
+        <v>300</v>
       </c>
       <c r="H142" t="s">
-        <v>674</v>
+        <v>300</v>
       </c>
       <c r="I142" t="s">
-        <v>674</v>
+        <v>300</v>
       </c>
       <c r="J142" t="s">
-        <v>674</v>
-      </c>
-      <c r="K142" t="s">
-        <v>674</v>
+        <v>300</v>
+      </c>
+      <c r="L142" t="s">
+        <v>300</v>
+      </c>
+      <c r="M142" t="s">
+        <v>300</v>
+      </c>
+      <c r="N142" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="143" spans="1:14">
-      <c r="A143" s="6" t="s">
-        <v>695</v>
+      <c r="A143" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="L143" t="s">
+        <v>678</v>
+      </c>
+      <c r="M143" t="s">
+        <v>678</v>
       </c>
       <c r="N143" t="s">
         <v>678</v>
@@ -7665,166 +7667,200 @@
     </row>
     <row r="144" spans="1:14">
       <c r="A144" s="6" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E144" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="F144" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="G144" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="H144" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="I144" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="J144" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="K144" t="s">
-        <v>689</v>
-      </c>
-      <c r="L144" t="s">
-        <v>689</v>
-      </c>
-      <c r="M144" t="s">
-        <v>689</v>
-      </c>
-      <c r="N144" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
     </row>
     <row r="145" spans="1:14">
       <c r="A145" s="6" t="s">
-        <v>697</v>
-      </c>
-      <c r="E145" t="s">
-        <v>52</v>
-      </c>
-      <c r="F145" t="s">
-        <v>706</v>
-      </c>
-      <c r="G145" t="s">
-        <v>706</v>
-      </c>
-      <c r="H145" t="s">
-        <v>706</v>
-      </c>
-      <c r="I145" t="s">
-        <v>52</v>
-      </c>
-      <c r="J145" t="s">
-        <v>706</v>
-      </c>
-      <c r="K145" t="s">
-        <v>706</v>
-      </c>
-      <c r="L145" t="s">
-        <v>706</v>
-      </c>
-      <c r="M145" t="s">
-        <v>706</v>
+        <v>695</v>
       </c>
       <c r="N145" t="s">
-        <v>706</v>
+        <v>678</v>
       </c>
     </row>
     <row r="146" spans="1:14">
       <c r="A146" s="6" t="s">
-        <v>698</v>
+        <v>696</v>
+      </c>
+      <c r="E146" t="s">
+        <v>689</v>
+      </c>
+      <c r="F146" t="s">
+        <v>689</v>
+      </c>
+      <c r="G146" t="s">
+        <v>689</v>
+      </c>
+      <c r="H146" t="s">
+        <v>689</v>
+      </c>
+      <c r="I146" t="s">
+        <v>689</v>
       </c>
       <c r="J146" t="s">
-        <v>674</v>
+        <v>689</v>
       </c>
       <c r="K146" t="s">
-        <v>674</v>
+        <v>689</v>
       </c>
       <c r="L146" t="s">
-        <v>300</v>
+        <v>689</v>
       </c>
       <c r="M146" t="s">
-        <v>674</v>
+        <v>689</v>
       </c>
       <c r="N146" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
     </row>
     <row r="147" spans="1:14">
       <c r="A147" s="6" t="s">
-        <v>700</v>
+        <v>697</v>
+      </c>
+      <c r="E147" t="s">
+        <v>52</v>
+      </c>
+      <c r="F147" t="s">
+        <v>706</v>
+      </c>
+      <c r="G147" t="s">
+        <v>706</v>
+      </c>
+      <c r="H147" t="s">
+        <v>706</v>
+      </c>
+      <c r="I147" t="s">
+        <v>52</v>
+      </c>
+      <c r="J147" t="s">
+        <v>706</v>
+      </c>
+      <c r="K147" t="s">
+        <v>706</v>
+      </c>
+      <c r="L147" t="s">
+        <v>706</v>
+      </c>
+      <c r="M147" t="s">
+        <v>706</v>
+      </c>
+      <c r="N147" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="148" spans="1:14">
       <c r="A148" s="6" t="s">
-        <v>701</v>
+        <v>698</v>
+      </c>
+      <c r="J148" t="s">
+        <v>674</v>
+      </c>
+      <c r="K148" t="s">
+        <v>674</v>
+      </c>
+      <c r="L148" t="s">
+        <v>300</v>
+      </c>
+      <c r="M148" t="s">
+        <v>674</v>
+      </c>
+      <c r="N148" t="s">
+        <v>699</v>
       </c>
     </row>
     <row r="149" spans="1:14">
       <c r="A149" s="6" t="s">
-        <v>702</v>
-      </c>
-      <c r="H149" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="150" spans="1:14">
       <c r="A150" s="6" t="s">
-        <v>705</v>
-      </c>
-      <c r="E150" t="s">
-        <v>674</v>
-      </c>
-      <c r="F150" t="s">
-        <v>674</v>
-      </c>
-      <c r="G150" t="s">
-        <v>674</v>
-      </c>
-      <c r="H150" t="s">
-        <v>674</v>
-      </c>
-      <c r="I150" t="s">
-        <v>674</v>
-      </c>
-      <c r="J150" t="s">
-        <v>674</v>
-      </c>
-      <c r="K150" t="s">
-        <v>674</v>
-      </c>
-      <c r="L150" t="s">
-        <v>674</v>
-      </c>
-      <c r="M150" t="s">
-        <v>674</v>
+        <v>701</v>
       </c>
     </row>
     <row r="151" spans="1:14">
       <c r="A151" s="6" t="s">
+        <v>702</v>
+      </c>
+      <c r="H151" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14">
+      <c r="A152" s="6" t="s">
+        <v>705</v>
+      </c>
+      <c r="E152" t="s">
+        <v>674</v>
+      </c>
+      <c r="F152" t="s">
+        <v>674</v>
+      </c>
+      <c r="G152" t="s">
+        <v>674</v>
+      </c>
+      <c r="H152" t="s">
+        <v>674</v>
+      </c>
+      <c r="I152" t="s">
+        <v>674</v>
+      </c>
+      <c r="J152" t="s">
+        <v>674</v>
+      </c>
+      <c r="K152" t="s">
+        <v>674</v>
+      </c>
+      <c r="L152" t="s">
+        <v>674</v>
+      </c>
+      <c r="M152" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14">
+      <c r="A153" s="6" t="s">
         <v>716</v>
       </c>
-      <c r="K151" t="s">
+      <c r="K153" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="152" spans="1:14">
-      <c r="A152" s="1" t="s">
+    <row r="154" spans="1:14">
+      <c r="A154" s="1" t="s">
         <v>813</v>
       </c>
-      <c r="J152" s="1" t="s">
+      <c r="J154" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="K152" s="1" t="s">
+      <c r="K154" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="L152" s="1" t="s">
+      <c r="L154" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="M152" s="1" t="s">
+      <c r="M154" s="1" t="s">
         <v>814</v>
       </c>
     </row>

</xml_diff>

<commit_message>
JP region 2020 census
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE382B22-0149-C241-B761-D7378F8D47B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E743980E-CAB3-5A4B-8B0D-5A888E9D82CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -3060,7 +3060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N101" sqref="N101"/>
     </sheetView>
@@ -7874,8 +7874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8098,19 +8098,19 @@
         <v>218</v>
       </c>
       <c r="B14">
-        <v>0.34067663257277736</v>
+        <v>0.34599740763411402</v>
       </c>
       <c r="C14">
-        <v>0.17702596380802518</v>
+        <v>0.176839093907908</v>
       </c>
       <c r="D14">
-        <v>0.11250983477576712</v>
+        <v>0.109666596260914</v>
       </c>
       <c r="E14">
-        <v>0.16837136113296616</v>
+        <v>0.167605083516045</v>
       </c>
       <c r="F14">
-        <v>0.20141620771046423</v>
+        <v>0.19989181868101899</v>
       </c>
       <c r="G14">
         <f>SUM(B14:F14)</f>
@@ -8129,7 +8129,7 @@
       </c>
       <c r="B15" s="13">
         <f>ROUND(2000*B14,0)</f>
-        <v>681</v>
+        <v>692</v>
       </c>
       <c r="C15" s="13">
         <f>ROUND(2000*C14,0)</f>
@@ -8137,15 +8137,15 @@
       </c>
       <c r="D15" s="13">
         <f>ROUND(2000*D14,0)</f>
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E15" s="13">
         <f>ROUND(2000*E14,0)</f>
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F15" s="13">
         <f>ROUND(2000*F14,0)</f>
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G15" s="13">
         <f>SUM(B15:F15)</f>
@@ -8164,7 +8164,7 @@
       </c>
       <c r="B16" s="2">
         <f>ROUND(2200*B14,0)</f>
-        <v>749</v>
+        <v>761</v>
       </c>
       <c r="C16" s="2">
         <f>ROUND(2200*C14,0)</f>
@@ -8172,19 +8172,19 @@
       </c>
       <c r="D16" s="2">
         <f>ROUND(2200*D14,0)</f>
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="E16" s="2">
         <f>ROUND(2200*E14,0)</f>
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F16" s="2">
         <f>ROUND(2200*F14,0)</f>
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G16" s="2">
         <f>SUM(B16:F16)</f>
-        <v>2199</v>
+        <v>2200</v>
       </c>
       <c r="I16" t="s">
         <v>648</v>
@@ -14205,7 +14205,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
update jp census 2020
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A931BE90-9845-B944-A8E8-A25CF4CC3DD4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
     <sheet name="quotas_MX" sheetId="17" r:id="rId16"/>
     <sheet name="quotas_SK" sheetId="18" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="833">
   <si>
     <t>Country</t>
   </si>
@@ -2542,18 +2543,21 @@
   </si>
   <si>
     <t>equiv, year (pre-tax)</t>
+  </si>
+  <si>
+    <t>https://www.citypopulation.de/en/japan/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2774,7 +2778,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3051,39 +3055,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.6328125" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" customWidth="1"/>
-    <col min="4" max="4" width="6.54296875" customWidth="1"/>
-    <col min="5" max="5" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.36328125" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="6.5" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" customWidth="1"/>
-    <col min="9" max="9" width="6.54296875" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" customWidth="1"/>
-    <col min="11" max="11" width="7.7265625" customWidth="1"/>
-    <col min="12" max="12" width="8.36328125" customWidth="1"/>
-    <col min="13" max="13" width="8.90625" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" customWidth="1"/>
-    <col min="15" max="15" width="6.81640625" customWidth="1"/>
-    <col min="16" max="16" width="7.36328125" customWidth="1"/>
-    <col min="17" max="17" width="8.54296875" customWidth="1"/>
-    <col min="18" max="18" width="11.6328125" customWidth="1"/>
+    <col min="8" max="8" width="8.5" customWidth="1"/>
+    <col min="9" max="9" width="6.5" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" customWidth="1"/>
+    <col min="14" max="14" width="9.5" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" customWidth="1"/>
+    <col min="17" max="17" width="8.5" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" customWidth="1"/>
     <col min="19" max="20" width="10" customWidth="1"/>
-    <col min="21" max="21" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3154,7 +3158,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
         <v>451</v>
       </c>
@@ -3198,7 +3202,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23">
       <c r="A3" s="1" t="s">
         <v>452</v>
       </c>
@@ -3242,7 +3246,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
         <v>453</v>
       </c>
@@ -3283,7 +3287,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23">
       <c r="A5" s="1" t="s">
         <v>492</v>
       </c>
@@ -3327,7 +3331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23">
       <c r="A6" s="1" t="s">
         <v>742</v>
       </c>
@@ -3369,7 +3373,7 @@
       </c>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23">
       <c r="A7" s="1" t="s">
         <v>454</v>
       </c>
@@ -3396,7 +3400,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -3449,7 +3453,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -3502,7 +3506,7 @@
         <v>1113.8499999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23">
       <c r="A10" s="2" t="s">
         <v>169</v>
       </c>
@@ -3555,7 +3559,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23">
       <c r="A11" s="2" t="s">
         <v>170</v>
       </c>
@@ -3608,7 +3612,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23">
       <c r="A12" s="1" t="s">
         <v>181</v>
       </c>
@@ -3661,7 +3665,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23">
       <c r="A13" s="1" t="s">
         <v>182</v>
       </c>
@@ -3714,7 +3718,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23">
       <c r="A14" s="1" t="s">
         <v>396</v>
       </c>
@@ -3758,7 +3762,7 @@
         <v>19653</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23">
       <c r="A15" s="1" t="s">
         <v>397</v>
       </c>
@@ -3802,7 +3806,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23">
       <c r="A16" s="1" t="s">
         <v>398</v>
       </c>
@@ -3846,7 +3850,7 @@
         <v>113696</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14">
       <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
@@ -3890,7 +3894,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>393</v>
       </c>
@@ -3934,7 +3938,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>394</v>
       </c>
@@ -3978,7 +3982,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>395</v>
       </c>
@@ -4022,7 +4026,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>205</v>
       </c>
@@ -4066,7 +4070,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>206</v>
       </c>
@@ -4110,7 +4114,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>207</v>
       </c>
@@ -4154,7 +4158,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>208</v>
       </c>
@@ -4198,7 +4202,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>433</v>
       </c>
@@ -4242,7 +4246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>434</v>
       </c>
@@ -4286,7 +4290,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>435</v>
       </c>
@@ -4330,7 +4334,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>436</v>
       </c>
@@ -4374,7 +4378,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
         <v>517</v>
       </c>
@@ -4391,7 +4395,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>557</v>
       </c>
@@ -4399,7 +4403,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
@@ -4443,7 +4447,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>75</v>
       </c>
@@ -4487,7 +4491,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20">
       <c r="A33" s="1" t="s">
         <v>76</v>
       </c>
@@ -4531,7 +4535,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20">
       <c r="A34" s="1" t="s">
         <v>77</v>
       </c>
@@ -4575,7 +4579,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20">
       <c r="A35" s="1" t="s">
         <v>78</v>
       </c>
@@ -4619,7 +4623,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20">
       <c r="A36" s="1" t="s">
         <v>73</v>
       </c>
@@ -4633,7 +4637,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20">
       <c r="A37" s="1" t="s">
         <v>68</v>
       </c>
@@ -4647,7 +4651,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20">
       <c r="A38" s="1" t="s">
         <v>67</v>
       </c>
@@ -4661,7 +4665,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20">
       <c r="A39" s="1" t="s">
         <v>66</v>
       </c>
@@ -4705,7 +4709,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20">
       <c r="A40" s="1" t="s">
         <v>65</v>
       </c>
@@ -4746,7 +4750,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20">
       <c r="A41" s="1" t="s">
         <v>64</v>
       </c>
@@ -4757,7 +4761,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20">
       <c r="A42" s="1" t="s">
         <v>63</v>
       </c>
@@ -4801,7 +4805,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20">
       <c r="A43" s="1" t="s">
         <v>79</v>
       </c>
@@ -4845,7 +4849,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20">
       <c r="A44" s="1" t="s">
         <v>313</v>
       </c>
@@ -4901,7 +4905,7 @@
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20">
       <c r="A45" s="1" t="s">
         <v>62</v>
       </c>
@@ -4957,7 +4961,7 @@
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20">
       <c r="A46" s="1" t="s">
         <v>559</v>
       </c>
@@ -4980,7 +4984,7 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20">
       <c r="A47" s="1" t="s">
         <v>61</v>
       </c>
@@ -5022,7 +5026,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20">
       <c r="A48" s="1" t="s">
         <v>60</v>
       </c>
@@ -5072,7 +5076,7 @@
       <c r="S48" s="31"/>
       <c r="T48" s="31"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:21">
       <c r="A49" s="1" t="s">
         <v>59</v>
       </c>
@@ -5142,7 +5146,7 @@
       <c r="S49" s="31"/>
       <c r="T49" s="31"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:21">
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
@@ -5186,7 +5190,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21">
       <c r="A51" s="1" t="s">
         <v>57</v>
       </c>
@@ -5239,7 +5243,7 @@
         <v>718.5</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:21">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -5269,7 +5273,7 @@
       </c>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:21">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
@@ -5314,7 +5318,7 @@
       </c>
       <c r="O53" s="1"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:21">
       <c r="A54" s="1" t="s">
         <v>821</v>
       </c>
@@ -5377,7 +5381,7 @@
       </c>
       <c r="U54" s="2"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:21">
       <c r="A55" s="1" t="s">
         <v>820</v>
       </c>
@@ -5431,7 +5435,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:21">
       <c r="A56" s="1" t="s">
         <v>823</v>
       </c>
@@ -5516,7 +5520,7 @@
         <v>6.8095238095238093</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:21">
       <c r="A57" s="1" t="s">
         <v>306</v>
       </c>
@@ -5570,7 +5574,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:21">
       <c r="A58" s="1" t="s">
         <v>311</v>
       </c>
@@ -5626,7 +5630,7 @@
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:21">
       <c r="A59" s="1" t="s">
         <v>524</v>
       </c>
@@ -5679,7 +5683,7 @@
         <v>43190072.399999999</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21">
       <c r="A60" s="1" t="s">
         <v>822</v>
       </c>
@@ -5744,7 +5748,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:21">
       <c r="A61" s="1" t="s">
         <v>312</v>
       </c>
@@ -5816,7 +5820,7 @@
       <c r="S61" s="17"/>
       <c r="T61" s="17"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:21">
       <c r="A62" s="1" t="s">
         <v>314</v>
       </c>
@@ -5888,7 +5892,7 @@
       <c r="S62" s="22"/>
       <c r="T62" s="22"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:21">
       <c r="A63" s="1" t="s">
         <v>315</v>
       </c>
@@ -5960,7 +5964,7 @@
       <c r="S63" s="22"/>
       <c r="T63" s="22"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:21">
       <c r="A64" s="1" t="s">
         <v>331</v>
       </c>
@@ -6004,7 +6008,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14">
       <c r="A65" s="1" t="s">
         <v>484</v>
       </c>
@@ -6048,7 +6052,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14">
       <c r="A66" s="1" t="s">
         <v>723</v>
       </c>
@@ -6092,7 +6096,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14">
       <c r="A67" s="1" t="s">
         <v>721</v>
       </c>
@@ -6132,7 +6136,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14">
       <c r="A68" s="1" t="s">
         <v>722</v>
       </c>
@@ -6176,7 +6180,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14">
       <c r="A69" s="1" t="s">
         <v>353</v>
       </c>
@@ -6220,7 +6224,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14">
       <c r="A70" s="1" t="s">
         <v>381</v>
       </c>
@@ -6261,7 +6265,7 @@
         <v>0.92800000000000005</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14">
       <c r="A71" s="1" t="s">
         <v>485</v>
       </c>
@@ -6305,7 +6309,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14">
       <c r="A72" s="1" t="s">
         <v>102</v>
       </c>
@@ -6349,7 +6353,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14">
       <c r="A73" s="1" t="s">
         <v>103</v>
       </c>
@@ -6393,7 +6397,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14">
       <c r="A74" s="1" t="s">
         <v>104</v>
       </c>
@@ -6407,7 +6411,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14">
       <c r="A75" s="1" t="s">
         <v>111</v>
       </c>
@@ -6415,7 +6419,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14">
       <c r="A76" s="1" t="s">
         <v>105</v>
       </c>
@@ -6456,7 +6460,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14">
       <c r="A77" s="1" t="s">
         <v>106</v>
       </c>
@@ -6473,7 +6477,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14">
       <c r="A78" s="1" t="s">
         <v>204</v>
       </c>
@@ -6493,7 +6497,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14">
       <c r="A79" s="1" t="s">
         <v>107</v>
       </c>
@@ -6501,7 +6505,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14">
       <c r="A80" s="1" t="s">
         <v>112</v>
       </c>
@@ -6509,7 +6513,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14">
       <c r="A81" s="1" t="s">
         <v>114</v>
       </c>
@@ -6517,7 +6521,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14">
       <c r="A82" s="6" t="s">
         <v>115</v>
       </c>
@@ -6558,7 +6562,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14">
       <c r="A83" s="6" t="s">
         <v>116</v>
       </c>
@@ -6599,7 +6603,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14">
       <c r="A84" s="6" t="s">
         <v>117</v>
       </c>
@@ -6640,7 +6644,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14">
       <c r="A85" s="6" t="s">
         <v>118</v>
       </c>
@@ -6681,7 +6685,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14">
       <c r="A86" s="6" t="s">
         <v>119</v>
       </c>
@@ -6716,7 +6720,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14">
       <c r="A87" s="6" t="s">
         <v>120</v>
       </c>
@@ -6745,7 +6749,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14">
       <c r="A88" s="6" t="s">
         <v>121</v>
       </c>
@@ -6765,7 +6769,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14">
       <c r="A89" s="6" t="s">
         <v>122</v>
       </c>
@@ -6779,7 +6783,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14">
       <c r="A90" s="6" t="s">
         <v>123</v>
       </c>
@@ -6790,7 +6794,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14">
       <c r="A91" s="6" t="s">
         <v>124</v>
       </c>
@@ -6804,7 +6808,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14">
       <c r="A92" s="6" t="s">
         <v>188</v>
       </c>
@@ -6812,7 +6816,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14">
       <c r="A93" s="6" t="s">
         <v>189</v>
       </c>
@@ -6820,7 +6824,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14">
       <c r="A94" s="6" t="s">
         <v>193</v>
       </c>
@@ -6828,7 +6832,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14">
       <c r="A95" s="6" t="s">
         <v>199</v>
       </c>
@@ -6869,7 +6873,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:14">
       <c r="A96" s="4" t="s">
         <v>191</v>
       </c>
@@ -6877,7 +6881,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:21">
       <c r="A97" s="4" t="s">
         <v>195</v>
       </c>
@@ -6885,7 +6889,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:21">
       <c r="A98" s="4" t="s">
         <v>197</v>
       </c>
@@ -6893,7 +6897,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:21">
       <c r="A99" s="6" t="s">
         <v>269</v>
       </c>
@@ -6907,7 +6911,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:21">
       <c r="A100" s="6" t="s">
         <v>270</v>
       </c>
@@ -6921,7 +6925,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:21">
       <c r="A101" s="6" t="s">
         <v>271</v>
       </c>
@@ -6935,7 +6939,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:21">
       <c r="A102" s="6" t="s">
         <v>272</v>
       </c>
@@ -6943,7 +6947,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:21">
       <c r="A103" s="6" t="s">
         <v>273</v>
       </c>
@@ -6951,7 +6955,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:21">
       <c r="A104" s="6" t="s">
         <v>274</v>
       </c>
@@ -6965,7 +6969,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:21">
       <c r="A105" s="6" t="s">
         <v>275</v>
       </c>
@@ -6973,7 +6977,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:21">
       <c r="A106" s="6" t="s">
         <v>293</v>
       </c>
@@ -6981,7 +6985,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:21">
       <c r="A107" s="6" t="s">
         <v>334</v>
       </c>
@@ -7022,7 +7026,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:21">
       <c r="A108" s="6" t="s">
         <v>483</v>
       </c>
@@ -7054,7 +7058,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:21">
       <c r="A109" s="6" t="s">
         <v>338</v>
       </c>
@@ -7062,7 +7066,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:21">
       <c r="A110" s="6" t="s">
         <v>486</v>
       </c>
@@ -7091,7 +7095,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:21">
       <c r="A111" s="6" t="s">
         <v>488</v>
       </c>
@@ -7123,7 +7127,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:21">
       <c r="A112" s="6" t="s">
         <v>658</v>
       </c>
@@ -7158,7 +7162,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:14">
       <c r="A113" s="6" t="s">
         <v>493</v>
       </c>
@@ -7172,7 +7176,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:14">
       <c r="A114" s="6" t="s">
         <v>494</v>
       </c>
@@ -7186,7 +7190,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:14">
       <c r="A116" s="6" t="s">
         <v>713</v>
       </c>
@@ -7215,7 +7219,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:14">
       <c r="A117" s="6" t="s">
         <v>734</v>
       </c>
@@ -7226,7 +7230,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:14">
       <c r="A118" s="6" t="s">
         <v>826</v>
       </c>
@@ -7240,7 +7244,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:14">
       <c r="A119" s="6" t="s">
         <v>825</v>
       </c>
@@ -7248,7 +7252,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:14">
       <c r="A120" s="6" t="s">
         <v>667</v>
       </c>
@@ -7259,7 +7263,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:14">
       <c r="A121" s="6" t="s">
         <v>668</v>
       </c>
@@ -7294,7 +7298,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:14">
       <c r="A122" s="6" t="s">
         <v>669</v>
       </c>
@@ -7314,7 +7318,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:14">
       <c r="A123" s="6" t="s">
         <v>670</v>
       </c>
@@ -7343,7 +7347,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:14">
       <c r="A124" s="6" t="s">
         <v>672</v>
       </c>
@@ -7354,7 +7358,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:14">
       <c r="A125" s="6" t="s">
         <v>673</v>
       </c>
@@ -7380,7 +7384,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:14">
       <c r="A126" s="6" t="s">
         <v>674</v>
       </c>
@@ -7394,7 +7398,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:14">
       <c r="A127" s="6" t="s">
         <v>676</v>
       </c>
@@ -7429,7 +7433,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:14">
       <c r="A128" s="6" t="s">
         <v>677</v>
       </c>
@@ -7464,7 +7468,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:14">
       <c r="A129" s="6" t="s">
         <v>678</v>
       </c>
@@ -7493,7 +7497,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:14">
       <c r="A130" s="6" t="s">
         <v>700</v>
       </c>
@@ -7504,7 +7508,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:14">
       <c r="A131" s="6" t="s">
         <v>679</v>
       </c>
@@ -7512,7 +7516,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:14">
       <c r="A132" s="6" t="s">
         <v>680</v>
       </c>
@@ -7523,12 +7527,12 @@
         <v>671</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:14">
       <c r="A133" s="6" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:14">
       <c r="A134" s="6" t="s">
         <v>682</v>
       </c>
@@ -7536,7 +7540,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:14">
       <c r="A135" s="6" t="s">
         <v>735</v>
       </c>
@@ -7544,12 +7548,12 @@
         <v>671</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:14">
       <c r="A136" s="6" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:14">
       <c r="A137" s="6" t="s">
         <v>685</v>
       </c>
@@ -7566,7 +7570,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:14">
       <c r="A138" s="6" t="s">
         <v>687</v>
       </c>
@@ -7583,7 +7587,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:14">
       <c r="A139" s="6" t="s">
         <v>688</v>
       </c>
@@ -7600,7 +7604,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:14">
       <c r="A140" s="6" t="s">
         <v>689</v>
       </c>
@@ -7632,7 +7636,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:14">
       <c r="A141" s="1" t="s">
         <v>691</v>
       </c>
@@ -7646,7 +7650,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:14">
       <c r="A142" s="6" t="s">
         <v>690</v>
       </c>
@@ -7663,7 +7667,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:14">
       <c r="A143" s="6" t="s">
         <v>692</v>
       </c>
@@ -7671,7 +7675,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:14">
       <c r="A144" s="6" t="s">
         <v>693</v>
       </c>
@@ -7694,7 +7698,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:14">
       <c r="A145" s="6" t="s">
         <v>694</v>
       </c>
@@ -7702,7 +7706,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:14">
       <c r="A146" s="6" t="s">
         <v>695</v>
       </c>
@@ -7722,22 +7726,22 @@
         <v>696</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:14">
       <c r="A147" s="6" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:14">
       <c r="A148" s="6" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:14">
       <c r="A149" s="6" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:14">
       <c r="A150" s="6" t="s">
         <v>701</v>
       </c>
@@ -7760,7 +7764,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:14">
       <c r="A151" s="6" t="s">
         <v>712</v>
       </c>
@@ -7768,7 +7772,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:14">
       <c r="A152" s="1" t="s">
         <v>809</v>
       </c>
@@ -7787,7 +7791,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I69" r:id="rId1"/>
+    <hyperlink ref="I69" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -7795,16 +7799,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:E23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -7818,7 +7822,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -7839,7 +7843,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -7860,7 +7864,7 @@
         <v>0.92622883301508352</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -7879,8 +7883,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -7901,7 +7905,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -7925,7 +7929,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -7954,7 +7958,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -7983,7 +7987,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -7994,7 +7998,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="16" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -8017,24 +8021,24 @@
         <v>645</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
       <c r="B14">
-        <v>0.34067663257277736</v>
+        <v>0.34599740763411402</v>
       </c>
       <c r="C14">
-        <v>0.17702596380802518</v>
+        <v>0.176839093907908</v>
       </c>
       <c r="D14">
-        <v>0.11250983477576712</v>
+        <v>0.109666596260914</v>
       </c>
       <c r="E14">
-        <v>0.16837136113296616</v>
+        <v>0.167605083516045</v>
       </c>
       <c r="F14">
-        <v>0.20141620771046423</v>
+        <v>0.19989181868101899</v>
       </c>
       <c r="G14">
         <f>SUM(B14:F14)</f>
@@ -8047,13 +8051,13 @@
         <v>738</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
       <c r="B15" s="13">
         <f>ROUND(2000*B14,0)</f>
-        <v>681</v>
+        <v>692</v>
       </c>
       <c r="C15" s="13">
         <f>ROUND(2000*C14,0)</f>
@@ -8061,15 +8065,15 @@
       </c>
       <c r="D15" s="13">
         <f>ROUND(2000*D14,0)</f>
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E15" s="13">
         <f>ROUND(2000*E14,0)</f>
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F15" s="13">
         <f>ROUND(2000*F14,0)</f>
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G15" s="13">
         <f>SUM(B15:F15)</f>
@@ -8082,13 +8086,13 @@
         <v>737</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
       <c r="B16" s="2">
         <f>ROUND(2200*B14,0)</f>
-        <v>749</v>
+        <v>761</v>
       </c>
       <c r="C16" s="2">
         <f>ROUND(2200*C14,0)</f>
@@ -8096,19 +8100,19 @@
       </c>
       <c r="D16" s="2">
         <f>ROUND(2200*D14,0)</f>
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="E16" s="2">
         <f>ROUND(2200*E14,0)</f>
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F16" s="2">
         <f>ROUND(2200*F14,0)</f>
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G16" s="2">
         <f>SUM(B16:F16)</f>
-        <v>2199</v>
+        <v>2200</v>
       </c>
       <c r="I16" t="s">
         <v>646</v>
@@ -8117,7 +8121,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -8125,9 +8129,12 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J17" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="16" thickBot="1"/>
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>508</v>
       </c>
@@ -8140,7 +8147,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>219</v>
       </c>
@@ -8156,7 +8163,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -8174,7 +8181,7 @@
       </c>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>513</v>
       </c>
@@ -8198,19 +8205,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -8225,7 +8232,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -8247,7 +8254,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -8269,7 +8276,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -8289,7 +8296,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -8300,7 +8307,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="A6" s="35"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -8310,7 +8317,7 @@
       <c r="G6" s="36"/>
       <c r="H6" s="37"/>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -8320,7 +8327,7 @@
       <c r="G7" s="36"/>
       <c r="H7" s="37"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>226</v>
       </c>
@@ -8342,7 +8349,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="37"/>
     </row>
-    <row r="9" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="30" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -8367,7 +8374,7 @@
       </c>
       <c r="H9" s="37"/>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -8397,7 +8404,7 @@
       </c>
       <c r="H10" s="37"/>
     </row>
-    <row r="11" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="30" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>221</v>
       </c>
@@ -8427,7 +8434,7 @@
       </c>
       <c r="H11" s="37"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" s="12" t="s">
         <v>239</v>
       </c>
@@ -8439,10 +8446,10 @@
       <c r="G12" s="13"/>
       <c r="H12" s="37"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="H13" s="37"/>
     </row>
-    <row r="14" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="44" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -8466,7 +8473,7 @@
       </c>
       <c r="H14" s="37"/>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -8493,7 +8500,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -8529,7 +8536,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -8565,7 +8572,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -8575,7 +8582,7 @@
       <c r="E18" s="14"/>
       <c r="H18" s="37"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12">
       <c r="A19" s="12"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
@@ -8585,7 +8592,7 @@
       <c r="G19" s="39"/>
       <c r="H19" s="37"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12">
       <c r="A20" s="12"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -8601,7 +8608,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>815</v>
       </c>
@@ -8625,7 +8632,7 @@
       </c>
       <c r="H21" s="37"/>
     </row>
-    <row r="22" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -8652,7 +8659,7 @@
         <v>0.99989215000000009</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>220</v>
       </c>
@@ -8685,7 +8692,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>221</v>
       </c>
@@ -8718,7 +8725,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12">
       <c r="A25" s="12" t="s">
         <v>239</v>
       </c>
@@ -8728,7 +8735,7 @@
       <c r="E25" s="14"/>
       <c r="H25" s="37"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12">
       <c r="A26" s="12"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
@@ -8738,7 +8745,7 @@
       <c r="G26" s="37"/>
       <c r="H26" s="37"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12">
       <c r="A27" s="12"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -8748,7 +8755,7 @@
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12">
       <c r="A28" s="12"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
@@ -8758,7 +8765,7 @@
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -8774,16 +8781,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -8797,7 +8804,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -8818,7 +8825,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -8839,7 +8846,7 @@
         <v>0.99992877771181621</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -8858,8 +8865,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -8880,7 +8887,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -8904,7 +8911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -8933,7 +8940,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -8962,7 +8969,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -8973,7 +8980,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -9002,7 +9009,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -9032,7 +9039,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -9067,7 +9074,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -9102,7 +9109,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -9117,13 +9124,13 @@
         <v>762</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="K19" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" ht="16" thickBot="1"/>
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="12" t="s">
         <v>508</v>
       </c>
@@ -9136,7 +9143,7 @@
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>219</v>
       </c>
@@ -9158,7 +9165,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>220</v>
       </c>
@@ -9182,7 +9189,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" ht="44" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>513</v>
       </c>
@@ -9207,16 +9214,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22:H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -9230,7 +9237,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -9251,7 +9258,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -9272,7 +9279,7 @@
         <v>0.97760081385085629</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -9291,8 +9298,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -9313,7 +9320,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -9337,7 +9344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -9366,7 +9373,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -9395,7 +9402,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -9406,7 +9413,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -9429,7 +9436,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -9459,7 +9466,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -9494,7 +9501,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -9529,7 +9536,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -9544,8 +9551,8 @@
         <v>772</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" ht="16" thickBot="1"/>
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="12" t="s">
         <v>508</v>
       </c>
@@ -9558,7 +9565,7 @@
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>219</v>
       </c>
@@ -9580,7 +9587,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" ht="16" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>220</v>
       </c>
@@ -9607,7 +9614,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" ht="44" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>513</v>
       </c>
@@ -9631,16 +9638,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -9654,7 +9661,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -9675,7 +9682,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -9696,7 +9703,7 @@
         <v>1.0341140064832992</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -9715,8 +9722,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -9737,7 +9744,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -9761,7 +9768,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -9790,7 +9797,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -9819,7 +9826,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -9830,7 +9837,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="44" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -9853,7 +9860,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -9883,7 +9890,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -9918,7 +9925,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -9947,7 +9954,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -9956,7 +9963,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>340</v>
       </c>
@@ -9967,7 +9974,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>219</v>
       </c>
@@ -9988,7 +9995,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>220</v>
       </c>
@@ -10005,7 +10012,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>221</v>
       </c>
@@ -10031,7 +10038,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9">
       <c r="A23" s="12" t="s">
         <v>239</v>
       </c>
@@ -10045,7 +10052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9">
       <c r="G24" s="42" t="s">
         <v>787</v>
       </c>
@@ -10056,7 +10063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9">
       <c r="G25" s="42" t="s">
         <v>789</v>
       </c>
@@ -10067,7 +10074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9">
       <c r="G26" t="s">
         <v>791</v>
       </c>
@@ -10078,7 +10085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9">
       <c r="G27" t="s">
         <v>793</v>
       </c>
@@ -10086,7 +10093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9">
       <c r="G28" t="s">
         <v>794</v>
       </c>
@@ -10094,7 +10101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9">
       <c r="G29" t="s">
         <v>795</v>
       </c>
@@ -10105,7 +10112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9">
       <c r="G30" t="s">
         <v>797</v>
       </c>
@@ -10116,7 +10123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9">
       <c r="G31" t="s">
         <v>799</v>
       </c>
@@ -10133,16 +10140,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -10156,7 +10163,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -10177,7 +10184,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -10198,7 +10205,7 @@
         <v>0.95217958067188335</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -10217,8 +10224,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -10239,7 +10246,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -10263,7 +10270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -10292,7 +10299,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -10321,7 +10328,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -10338,16 +10345,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -10361,7 +10368,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -10382,7 +10389,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -10403,7 +10410,7 @@
         <v>0.92970833595125124</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -10422,8 +10429,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -10444,7 +10451,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -10468,7 +10475,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -10497,7 +10504,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -10526,7 +10533,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -10543,16 +10550,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -10566,7 +10573,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -10587,7 +10594,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -10608,7 +10615,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -10627,8 +10634,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -10649,7 +10656,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -10673,7 +10680,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -10702,7 +10709,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -10731,7 +10738,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -10748,16 +10755,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>240</v>
       </c>
@@ -10774,7 +10781,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>245</v>
       </c>
@@ -10791,7 +10798,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>527</v>
       </c>
@@ -10808,7 +10815,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>239</v>
       </c>
@@ -10826,7 +10833,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -10850,7 +10857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>245</v>
       </c>
@@ -10875,7 +10882,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>527</v>
       </c>
@@ -10904,7 +10911,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -10928,10 +10935,10 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>248</v>
       </c>
@@ -10948,7 +10955,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>245</v>
       </c>
@@ -10969,7 +10976,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>527</v>
       </c>
@@ -10994,7 +11001,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>239</v>
       </c>
@@ -11015,13 +11022,13 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>253</v>
       </c>
@@ -11038,7 +11045,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>245</v>
       </c>
@@ -11059,7 +11066,7 @@
         <v>100.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>527</v>
       </c>
@@ -11084,7 +11091,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>239</v>
       </c>
@@ -11105,7 +11112,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>258</v>
       </c>
@@ -11119,7 +11126,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>245</v>
       </c>
@@ -11133,7 +11140,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>527</v>
       </c>
@@ -11150,7 +11157,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>239</v>
       </c>
@@ -11165,11 +11172,11 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>263</v>
       </c>
@@ -11186,7 +11193,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>245</v>
       </c>
@@ -11203,7 +11210,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>527</v>
       </c>
@@ -11224,7 +11231,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>239</v>
       </c>
@@ -11244,30 +11251,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D28" sqref="A24:D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -11282,7 +11289,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -11300,7 +11307,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -11320,7 +11327,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -11340,7 +11347,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -11351,7 +11358,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -11360,7 +11367,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -11381,7 +11388,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -11405,7 +11412,7 @@
         <v>1.0001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -11434,7 +11441,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -11463,8 +11470,8 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="16" thickBot="1"/>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>238</v>
       </c>
@@ -11482,7 +11489,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="8" t="s">
         <v>237</v>
       </c>
@@ -11502,7 +11509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>220</v>
       </c>
@@ -11527,7 +11534,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>221</v>
       </c>
@@ -11552,12 +11559,12 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" s="16" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="12" t="s">
         <v>222</v>
       </c>
@@ -11577,7 +11584,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="8" t="s">
         <v>219</v>
       </c>
@@ -11601,7 +11608,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>220</v>
       </c>
@@ -11630,7 +11637,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>221</v>
       </c>
@@ -11659,7 +11666,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
         <v>239</v>
       </c>
@@ -11668,7 +11675,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="16" t="s">
         <v>340</v>
       </c>
@@ -11679,7 +11686,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>219</v>
       </c>
@@ -11694,7 +11701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>220</v>
       </c>
@@ -11711,7 +11718,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>221</v>
       </c>
@@ -11728,7 +11735,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7">
       <c r="A28" s="12" t="s">
         <v>239</v>
       </c>
@@ -11739,22 +11746,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>280</v>
       </c>
@@ -11780,7 +11787,7 @@
       <c r="K1" s="13"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -11813,7 +11820,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -11847,7 +11854,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -11881,7 +11888,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5" s="12" t="s">
         <v>239</v>
       </c>
@@ -11897,7 +11904,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="0.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="0.5" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -11911,14 +11918,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>223</v>
       </c>
@@ -11938,7 +11945,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -11961,7 +11968,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -11986,7 +11993,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>221</v>
       </c>
@@ -12011,7 +12018,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" s="12" t="s">
         <v>239</v>
       </c>
@@ -12027,7 +12034,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -12041,7 +12048,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>226</v>
       </c>
@@ -12067,7 +12074,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -12096,7 +12103,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -12130,7 +12137,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -12164,7 +12171,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -12180,7 +12187,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -12194,7 +12201,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>232</v>
       </c>
@@ -12218,7 +12225,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>237</v>
       </c>
@@ -12244,7 +12251,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -12275,7 +12282,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>221</v>
       </c>
@@ -12306,7 +12313,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>239</v>
       </c>
@@ -12316,7 +12323,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -12324,7 +12331,7 @@
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" ht="16.5" customHeight="1" thickBot="1">
       <c r="A26" s="12" t="s">
         <v>508</v>
       </c>
@@ -12341,7 +12348,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>219</v>
       </c>
@@ -12360,7 +12367,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" ht="16" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>220</v>
       </c>
@@ -12382,7 +12389,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" ht="16" thickBot="1">
       <c r="A29" s="8" t="s">
         <v>512</v>
       </c>
@@ -12401,7 +12408,7 @@
       </c>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>511</v>
       </c>
@@ -12423,7 +12430,7 @@
       </c>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>513</v>
       </c>
@@ -12445,7 +12452,7 @@
       </c>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12">
       <c r="A32" s="12" t="s">
         <v>239</v>
       </c>
@@ -12456,12 +12463,12 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
-    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" ht="30" thickBot="1">
       <c r="A37" s="8" t="s">
         <v>210</v>
       </c>
@@ -12491,7 +12498,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="8" t="s">
         <v>219</v>
       </c>
@@ -12524,7 +12531,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="8" t="s">
         <v>220</v>
       </c>
@@ -12565,7 +12572,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="8" t="s">
         <v>221</v>
       </c>
@@ -12606,7 +12613,7 @@
         <v>2196</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10">
       <c r="A41" s="12" t="s">
         <v>239</v>
       </c>
@@ -12620,7 +12627,7 @@
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10">
       <c r="A42" s="2"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -12632,12 +12639,12 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>285</v>
       </c>
@@ -12658,7 +12665,7 @@
       </c>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="8" t="s">
         <v>219</v>
       </c>
@@ -12682,7 +12689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="8" t="s">
         <v>220</v>
       </c>
@@ -12711,7 +12718,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="8" t="s">
         <v>221</v>
       </c>
@@ -12740,7 +12747,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10">
       <c r="A48" s="12" t="s">
         <v>239</v>
       </c>
@@ -12751,7 +12758,7 @@
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7">
       <c r="A49" s="2"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -12767,16 +12774,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -12790,7 +12797,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -12811,7 +12818,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -12832,7 +12839,7 @@
         <v>0.95277529961698948</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -12851,8 +12858,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -12873,7 +12880,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -12897,7 +12904,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -12926,7 +12933,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -12955,7 +12962,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -12966,7 +12973,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -12992,7 +12999,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -13022,7 +13029,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -13057,7 +13064,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -13092,7 +13099,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -13107,7 +13114,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" ht="16" thickBot="1">
       <c r="A20" s="16" t="s">
         <v>340</v>
       </c>
@@ -13121,7 +13128,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>219</v>
       </c>
@@ -13139,7 +13146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -13166,7 +13173,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>221</v>
       </c>
@@ -13193,30 +13200,30 @@
         <v>804</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11">
       <c r="A24" s="12" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G23" r:id="rId1"/>
+    <hyperlink ref="G23" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -13230,7 +13237,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -13251,7 +13258,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -13272,7 +13279,7 @@
         <v>0.90805800128462044</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -13291,8 +13298,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -13313,7 +13320,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -13337,7 +13344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -13366,7 +13373,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -13395,7 +13402,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -13406,7 +13413,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -13426,7 +13433,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -13450,7 +13457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -13479,7 +13486,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -13511,7 +13518,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -13520,7 +13527,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>340</v>
       </c>
@@ -13531,7 +13538,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="30" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>219</v>
       </c>
@@ -13546,7 +13553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>220</v>
       </c>
@@ -13563,7 +13570,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>221</v>
       </c>
@@ -13580,13 +13587,13 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8">
       <c r="A23" s="12" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="16" thickBot="1"/>
+    <row r="25" spans="1:8" ht="30" thickBot="1">
       <c r="A25" s="12" t="s">
         <v>508</v>
       </c>
@@ -13601,7 +13608,7 @@
       </c>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" ht="30" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>219</v>
       </c>
@@ -13619,7 +13626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>220</v>
       </c>
@@ -13640,7 +13647,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" ht="44" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>513</v>
       </c>
@@ -13664,7 +13671,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8">
       <c r="A29" s="12" t="s">
         <v>239</v>
       </c>
@@ -13682,16 +13689,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="E23" sqref="A20:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -13705,7 +13712,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -13726,7 +13733,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -13747,7 +13754,7 @@
         <v>0.9267197256851698</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -13766,8 +13773,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="16" thickBot="1"/>
+    <row r="7" spans="1:13" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -13788,7 +13795,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -13812,7 +13819,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -13841,7 +13848,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -13870,7 +13877,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -13881,7 +13888,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>222</v>
       </c>
@@ -13910,7 +13917,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -13943,7 +13950,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -13982,7 +13989,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>221</v>
       </c>
@@ -14021,7 +14028,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13">
       <c r="A17" s="12" t="s">
         <v>239</v>
       </c>
@@ -14036,7 +14043,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13">
       <c r="L18" t="s">
         <v>585</v>
       </c>
@@ -14044,8 +14051,8 @@
         <v>591</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" ht="16" thickBot="1"/>
+    <row r="20" spans="1:13" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>508</v>
       </c>
@@ -14058,7 +14065,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:13" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>219</v>
       </c>
@@ -14074,7 +14081,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:13" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -14092,7 +14099,7 @@
       </c>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:13" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>513</v>
       </c>
@@ -14110,7 +14117,7 @@
       </c>
       <c r="E23" s="29"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13">
       <c r="A24" s="12" t="s">
         <v>239</v>
       </c>
@@ -14125,19 +14132,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -14151,7 +14158,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -14172,7 +14179,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -14193,7 +14200,7 @@
         <v>0.97448244785232785</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -14212,8 +14219,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -14234,7 +14241,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -14258,7 +14265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -14287,7 +14294,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -14316,7 +14323,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -14327,7 +14334,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="A13" s="12"/>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -14336,7 +14343,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="41"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -14359,7 +14366,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -14390,7 +14397,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -14426,7 +14433,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -14462,7 +14469,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -14477,7 +14484,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="J19" t="s">
         <v>578</v>
       </c>
@@ -14485,7 +14492,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11">
       <c r="J20" t="s">
         <v>646</v>
       </c>
@@ -14493,7 +14500,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" ht="16" thickBot="1">
       <c r="A21" s="16" t="s">
         <v>340</v>
       </c>
@@ -14504,7 +14511,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -14519,7 +14526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>220</v>
       </c>
@@ -14536,7 +14543,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>221</v>
       </c>
@@ -14553,7 +14560,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11">
       <c r="A25" s="12" t="s">
         <v>239</v>
       </c>
@@ -14564,16 +14571,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>223</v>
       </c>
@@ -14587,7 +14594,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>219</v>
       </c>
@@ -14608,7 +14615,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>220</v>
       </c>
@@ -14629,7 +14636,7 @@
         <v>0.98351979013457747</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>221</v>
       </c>
@@ -14648,8 +14655,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>226</v>
       </c>
@@ -14670,7 +14677,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>219</v>
       </c>
@@ -14694,7 +14701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>220</v>
       </c>
@@ -14723,7 +14730,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>221</v>
       </c>
@@ -14752,7 +14759,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
         <v>239</v>
       </c>
@@ -14763,7 +14770,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>222</v>
       </c>
@@ -14783,7 +14790,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -14807,7 +14814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -14836,7 +14843,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>221</v>
       </c>
@@ -14865,7 +14872,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8">
       <c r="A18" s="12" t="s">
         <v>239</v>
       </c>
@@ -14874,8 +14881,8 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="16" thickBot="1"/>
+    <row r="21" spans="1:8" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>508</v>
       </c>
@@ -14890,7 +14897,7 @@
       </c>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -14908,7 +14915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>220</v>
       </c>
@@ -14932,7 +14939,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="44" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>513</v>
       </c>
@@ -14956,7 +14963,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8">
       <c r="A25" s="12" t="s">
         <v>239</v>
       </c>

</xml_diff>

<commit_message>
Update ES region quotas
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A931BE90-9845-B944-A8E8-A25CF4CC3DD4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88488D03-D32F-2D45-A36E-E3A701A7DEB4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -1981,9 +1981,6 @@
     <t>Catalonia, Valencia, Balearic Islands</t>
   </si>
   <si>
-    <t>Extremadura, Andalusia, Murcia, Canaris Islands</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -2546,6 +2543,9 @@
   </si>
   <si>
     <t>https://www.citypopulation.de/en/japan/</t>
+  </si>
+  <si>
+    <t>Extremadura, Andalusia, Murcia, Canaris Islands, Melillla, Ceuta</t>
   </si>
 </sst>
 </file>
@@ -2557,7 +2557,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2655,6 +2655,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2699,7 +2705,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2774,6 +2780,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3140,22 +3147,22 @@
         <v>523</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>818</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>819</v>
-      </c>
       <c r="U1" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>746</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -3222,7 +3229,7 @@
         <v>455</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>455</v>
@@ -3234,13 +3241,13 @@
         <v>455</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>516</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>455</v>
@@ -3325,7 +3332,7 @@
         <v>455</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="N5" s="1">
         <v>2</v>
@@ -3333,7 +3340,7 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>455</v>
@@ -3391,11 +3398,11 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -3864,19 +3871,19 @@
         <v>399</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>392</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>392</v>
@@ -3885,13 +3892,13 @@
         <v>52</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>304</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -4392,7 +4399,7 @@
         <v>519</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -4634,7 +4641,7 @@
         <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="37" spans="1:20">
@@ -4793,7 +4800,7 @@
         <v>389</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>391</v>
@@ -5011,7 +5018,7 @@
       </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>45</v>
@@ -5020,7 +5027,7 @@
         <v>510</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="N47" s="1" t="s">
         <v>601</v>
@@ -5269,7 +5276,7 @@
         <v>51</v>
       </c>
       <c r="L52" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="O52" s="1"/>
     </row>
@@ -5305,7 +5312,7 @@
         <v>377</v>
       </c>
       <c r="K53" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="L53" t="s">
         <v>54</v>
@@ -5320,7 +5327,7 @@
     </row>
     <row r="54" spans="1:21">
       <c r="A54" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B54">
         <v>18</v>
@@ -5383,7 +5390,7 @@
     </row>
     <row r="55" spans="1:21">
       <c r="A55" s="1" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B55">
         <v>5716</v>
@@ -5437,7 +5444,7 @@
     </row>
     <row r="56" spans="1:21">
       <c r="A56" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B56" s="28">
         <f>B55/B60</f>
@@ -5685,7 +5692,7 @@
     </row>
     <row r="60" spans="1:21">
       <c r="A60" s="1" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B60" s="3">
         <v>331</v>
@@ -6054,130 +6061,130 @@
     </row>
     <row r="66" spans="1:14">
       <c r="A66" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B66" s="22" t="s">
         <v>723</v>
       </c>
-      <c r="B66" s="22" t="s">
+      <c r="C66" s="22" t="s">
+        <v>723</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>723</v>
+      </c>
+      <c r="E66" s="22" t="s">
         <v>724</v>
       </c>
-      <c r="C66" s="22" t="s">
+      <c r="F66" s="22" t="s">
         <v>724</v>
       </c>
-      <c r="D66" s="22" t="s">
+      <c r="G66" s="22" t="s">
         <v>724</v>
       </c>
-      <c r="E66" s="22" t="s">
+      <c r="H66" s="22" t="s">
+        <v>724</v>
+      </c>
+      <c r="I66" s="22" t="s">
+        <v>724</v>
+      </c>
+      <c r="J66" s="22" t="s">
+        <v>724</v>
+      </c>
+      <c r="K66" s="22" t="s">
+        <v>724</v>
+      </c>
+      <c r="L66" s="22" t="s">
         <v>725</v>
       </c>
-      <c r="F66" s="22" t="s">
+      <c r="M66" s="22" t="s">
         <v>725</v>
       </c>
-      <c r="G66" s="22" t="s">
-        <v>725</v>
-      </c>
-      <c r="H66" s="22" t="s">
-        <v>725</v>
-      </c>
-      <c r="I66" s="22" t="s">
-        <v>725</v>
-      </c>
-      <c r="J66" s="22" t="s">
-        <v>725</v>
-      </c>
-      <c r="K66" s="22" t="s">
-        <v>725</v>
-      </c>
-      <c r="L66" s="22" t="s">
-        <v>726</v>
-      </c>
-      <c r="M66" s="22" t="s">
-        <v>726</v>
-      </c>
       <c r="N66" s="22" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="67" spans="1:14">
       <c r="A67" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E67" s="22" t="s">
+        <v>726</v>
+      </c>
+      <c r="F67" s="22" t="s">
+        <v>726</v>
+      </c>
+      <c r="G67" s="22" t="s">
         <v>727</v>
       </c>
-      <c r="F67" s="22" t="s">
-        <v>727</v>
-      </c>
-      <c r="G67" s="22" t="s">
+      <c r="H67" s="22" t="s">
+        <v>726</v>
+      </c>
+      <c r="I67" s="22" t="s">
+        <v>726</v>
+      </c>
+      <c r="J67" s="22" t="s">
         <v>728</v>
       </c>
-      <c r="H67" s="22" t="s">
-        <v>727</v>
-      </c>
-      <c r="I67" s="22" t="s">
-        <v>727</v>
-      </c>
-      <c r="J67" s="22" t="s">
-        <v>729</v>
-      </c>
       <c r="K67" s="22" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="L67" s="22"/>
       <c r="M67" s="22"/>
       <c r="N67" s="22" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="68" spans="1:14">
       <c r="A68" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B68" s="22" t="s">
+        <v>715</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>715</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>715</v>
+      </c>
+      <c r="E68" s="22" t="s">
         <v>716</v>
       </c>
-      <c r="C68" s="22" t="s">
+      <c r="F68" s="22" t="s">
         <v>716</v>
       </c>
-      <c r="D68" s="22" t="s">
+      <c r="G68" s="22" t="s">
+        <v>717</v>
+      </c>
+      <c r="H68" s="22" t="s">
         <v>716</v>
       </c>
-      <c r="E68" s="22" t="s">
+      <c r="I68" s="22" t="s">
+        <v>716</v>
+      </c>
+      <c r="J68" s="22" t="s">
+        <v>731</v>
+      </c>
+      <c r="K68" s="22" t="s">
         <v>717</v>
       </c>
-      <c r="F68" s="22" t="s">
-        <v>717</v>
-      </c>
-      <c r="G68" s="22" t="s">
-        <v>718</v>
-      </c>
-      <c r="H68" s="22" t="s">
-        <v>717</v>
-      </c>
-      <c r="I68" s="22" t="s">
-        <v>717</v>
-      </c>
-      <c r="J68" s="22" t="s">
+      <c r="L68" s="22" t="s">
+        <v>719</v>
+      </c>
+      <c r="M68" s="22" t="s">
         <v>732</v>
       </c>
-      <c r="K68" s="22" t="s">
-        <v>718</v>
-      </c>
-      <c r="L68" s="22" t="s">
-        <v>720</v>
-      </c>
-      <c r="M68" s="22" t="s">
-        <v>733</v>
-      </c>
       <c r="N68" s="22" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="69" spans="1:14">
@@ -6197,22 +6204,22 @@
         <v>355</v>
       </c>
       <c r="F69" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="G69" s="22" t="s">
         <v>358</v>
       </c>
       <c r="H69" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I69" s="43" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="J69" s="22" t="s">
         <v>356</v>
       </c>
       <c r="K69" s="22" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="L69" s="22" t="s">
         <v>354</v>
@@ -6385,7 +6392,7 @@
         <v>446</v>
       </c>
       <c r="K73" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="L73" t="s">
         <v>442</v>
@@ -6451,7 +6458,7 @@
         <v>383</v>
       </c>
       <c r="K76" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="L76" t="s">
         <v>390</v>
@@ -7020,7 +7027,7 @@
         <v>514</v>
       </c>
       <c r="M107" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="N107" s="34" t="s">
         <v>529</v>
@@ -7034,7 +7041,7 @@
         <v>336</v>
       </c>
       <c r="F108" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="G108" t="s">
         <v>526</v>
@@ -7046,7 +7053,7 @@
         <v>491</v>
       </c>
       <c r="K108" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="L108" t="s">
         <v>482</v>
@@ -7129,7 +7136,7 @@
     </row>
     <row r="112" spans="1:21">
       <c r="A112" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E112">
         <v>6500</v>
@@ -7192,7 +7199,7 @@
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="6" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F116" t="s">
         <v>455</v>
@@ -7221,7 +7228,7 @@
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="6" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="F117" t="s">
         <v>455</v>
@@ -7232,7 +7239,7 @@
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="6" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B118" t="s">
         <v>455</v>
@@ -7246,196 +7253,196 @@
     </row>
     <row r="119" spans="1:14">
       <c r="A119" s="6" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="H119" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="120" spans="1:14">
       <c r="A120" s="6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="M120" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N120" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="121" spans="1:14">
       <c r="A121" s="6" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E121" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F121" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="G121" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="H121" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I121" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J121" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K121" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="L121" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M121" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N121" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="122" spans="1:14">
       <c r="A122" s="6" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G122" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J122" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L122" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="M122" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N122" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="123" spans="1:14">
       <c r="A123" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="E123" t="s">
         <v>670</v>
       </c>
-      <c r="E123" t="s">
-        <v>671</v>
-      </c>
       <c r="G123" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I123" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J123" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K123" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="L123" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M123" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N123" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="124" spans="1:14">
       <c r="A124" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="K124" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="L124" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="125" spans="1:14">
       <c r="A125" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E125" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G125" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J125" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K125" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="L125" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M125" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N125" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="126" spans="1:14">
       <c r="A126" s="6" t="s">
+        <v>673</v>
+      </c>
+      <c r="L126" t="s">
         <v>674</v>
       </c>
-      <c r="L126" t="s">
-        <v>675</v>
-      </c>
       <c r="M126" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N126" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="127" spans="1:14">
       <c r="A127" s="6" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E127" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F127" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G127" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="H127" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I127" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J127" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K127" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="L127" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M127" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N127" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="128" spans="1:14">
       <c r="A128" s="6" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E128" t="s">
         <v>301</v>
@@ -7462,15 +7469,15 @@
         <v>301</v>
       </c>
       <c r="M128" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="N128" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="129" spans="1:14">
       <c r="A129" s="6" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E129" t="s">
         <v>301</v>
@@ -7499,114 +7506,114 @@
     </row>
     <row r="130" spans="1:14">
       <c r="A130" s="6" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="L130" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M130" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="131" spans="1:14">
       <c r="A131" s="6" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="L131" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="132" spans="1:14">
       <c r="A132" s="6" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="L132" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M132" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="133" spans="1:14">
       <c r="A133" s="6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="134" spans="1:14">
       <c r="A134" s="6" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="L134" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="6" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="K135" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="136" spans="1:14">
       <c r="A136" s="6" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="137" spans="1:14">
       <c r="A137" s="6" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E137" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G137" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K137" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="L137" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="138" spans="1:14">
       <c r="A138" s="6" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="K138" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L138" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="M138" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N138" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="139" spans="1:14">
       <c r="A139" s="6" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="K139" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L139" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="M139" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N139" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="140" spans="1:14">
       <c r="A140" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E140" t="s">
         <v>301</v>
@@ -7633,160 +7640,160 @@
         <v>301</v>
       </c>
       <c r="N140" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="141" spans="1:14">
       <c r="A141" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="L141" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="M141" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N141" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="142" spans="1:14">
       <c r="A142" s="6" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E142" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G142" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J142" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K142" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="143" spans="1:14">
       <c r="A143" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="N143" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="144" spans="1:14">
       <c r="A144" s="6" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G144" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="J144" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="K144" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="L144" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="M144" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="N144" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="145" spans="1:14">
       <c r="A145" s="6" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="L145" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="146" spans="1:14">
       <c r="A146" s="6" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="J146" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K146" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="L146" t="s">
         <v>301</v>
       </c>
       <c r="M146" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N146" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="147" spans="1:14">
       <c r="A147" s="6" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="148" spans="1:14">
       <c r="A148" s="6" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="149" spans="1:14">
       <c r="A149" s="6" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="150" spans="1:14">
       <c r="A150" s="6" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E150" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G150" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J150" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K150" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="L150" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M150" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="151" spans="1:14">
       <c r="A151" s="6" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="K151" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="152" spans="1:14">
       <c r="A152" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="J152" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="J152" s="1" t="s">
-        <v>810</v>
-      </c>
       <c r="K152" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="L152" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="M152" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
   </sheetData>
@@ -7802,7 +7809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -8003,22 +8010,22 @@
         <v>222</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>638</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>256</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" thickBot="1">
@@ -8048,7 +8055,7 @@
         <v>638</v>
       </c>
       <c r="J14" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -8083,7 +8090,7 @@
         <v>256</v>
       </c>
       <c r="J15" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" thickBot="1">
@@ -8115,10 +8122,10 @@
         <v>2200</v>
       </c>
       <c r="I16" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J16" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -8130,7 +8137,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
       <c r="J17" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" thickBot="1"/>
@@ -8139,10 +8146,10 @@
         <v>508</v>
       </c>
       <c r="B20" s="15" t="s">
+        <v>742</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>743</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>744</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
@@ -8602,33 +8609,33 @@
       <c r="G20" s="40"/>
       <c r="H20" s="37"/>
       <c r="K20" t="s">
+        <v>658</v>
+      </c>
+      <c r="L20" t="s">
         <v>659</v>
-      </c>
-      <c r="L20" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B21" s="23" t="s">
+        <v>660</v>
+      </c>
+      <c r="C21" s="23" t="s">
         <v>661</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="D21" s="23" t="s">
         <v>662</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="E21" s="23" t="s">
         <v>663</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="F21" s="24" t="s">
         <v>664</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="G21" s="41" t="s">
         <v>665</v>
-      </c>
-      <c r="G21" s="41" t="s">
-        <v>666</v>
       </c>
       <c r="H21" s="37"/>
     </row>
@@ -8985,28 +8992,28 @@
         <v>222</v>
       </c>
       <c r="B14" s="23" t="s">
+        <v>747</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>748</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="D14" s="23" t="s">
         <v>749</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="E14" s="23" t="s">
         <v>750</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="F14" s="24" t="s">
         <v>751</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="G14" s="41" t="s">
+        <v>644</v>
+      </c>
+      <c r="J14" t="s">
         <v>752</v>
       </c>
-      <c r="G14" s="41" t="s">
-        <v>645</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>753</v>
-      </c>
-      <c r="K14" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" thickBot="1">
@@ -9033,10 +9040,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
+        <v>754</v>
+      </c>
+      <c r="K15" t="s">
         <v>755</v>
-      </c>
-      <c r="K15" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -9068,10 +9075,10 @@
         <v>2001</v>
       </c>
       <c r="J16" t="s">
+        <v>756</v>
+      </c>
+      <c r="K16" t="s">
         <v>757</v>
-      </c>
-      <c r="K16" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -9103,10 +9110,10 @@
         <v>2200</v>
       </c>
       <c r="J17" t="s">
+        <v>758</v>
+      </c>
+      <c r="K17" t="s">
         <v>759</v>
-      </c>
-      <c r="K17" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -9118,15 +9125,15 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
       <c r="J18" t="s">
+        <v>760</v>
+      </c>
+      <c r="K18" t="s">
         <v>761</v>
-      </c>
-      <c r="K18" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="K19" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16" thickBot="1"/>
@@ -9159,10 +9166,10 @@
       </c>
       <c r="E24" s="10"/>
       <c r="F24" t="s">
+        <v>805</v>
+      </c>
+      <c r="G24" t="s">
         <v>806</v>
-      </c>
-      <c r="G24" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="16" thickBot="1">
@@ -9183,10 +9190,10 @@
       </c>
       <c r="E25" s="29"/>
       <c r="F25" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G25" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="44" thickBot="1">
@@ -9418,13 +9425,13 @@
         <v>222</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C14" s="23" t="s">
         <v>257</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>579</v>
@@ -9433,7 +9440,7 @@
         <v>585</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="16" thickBot="1">
@@ -9460,10 +9467,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
+        <v>765</v>
+      </c>
+      <c r="K15" t="s">
         <v>766</v>
-      </c>
-      <c r="K15" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -9498,7 +9505,7 @@
         <v>636</v>
       </c>
       <c r="K16" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -9530,10 +9537,10 @@
         <v>2200</v>
       </c>
       <c r="J17" t="s">
+        <v>768</v>
+      </c>
+      <c r="K17" t="s">
         <v>769</v>
-      </c>
-      <c r="K17" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -9545,10 +9552,10 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
       <c r="J18" t="s">
+        <v>770</v>
+      </c>
+      <c r="K18" t="s">
         <v>771</v>
-      </c>
-      <c r="K18" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16" thickBot="1"/>
@@ -9581,10 +9588,10 @@
       </c>
       <c r="E23" s="10"/>
       <c r="F23" t="s">
+        <v>810</v>
+      </c>
+      <c r="G23" t="s">
         <v>811</v>
-      </c>
-      <c r="G23" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="16" thickBot="1">
@@ -9605,13 +9612,13 @@
       </c>
       <c r="E24" s="29"/>
       <c r="F24" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="G24" t="s">
+        <v>812</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>813</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="44" thickBot="1">
@@ -9842,22 +9849,22 @@
         <v>222</v>
       </c>
       <c r="B13" s="23" t="s">
+        <v>772</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>773</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="D13" s="23" t="s">
         <v>774</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="E13" s="23" t="s">
         <v>775</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="F13" s="24" t="s">
         <v>776</v>
       </c>
-      <c r="F13" s="24" t="s">
-        <v>777</v>
-      </c>
       <c r="G13" s="41" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16" thickBot="1">
@@ -9884,10 +9891,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
+        <v>777</v>
+      </c>
+      <c r="J14" t="s">
         <v>778</v>
-      </c>
-      <c r="J14" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -9919,10 +9926,10 @@
         <v>2000</v>
       </c>
       <c r="I15" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" thickBot="1">
@@ -9989,10 +9996,10 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
+        <v>780</v>
+      </c>
+      <c r="G20" t="s">
         <v>781</v>
-      </c>
-      <c r="G20" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="16" thickBot="1">
@@ -10029,13 +10036,13 @@
         <v>2200</v>
       </c>
       <c r="G22" t="s">
+        <v>783</v>
+      </c>
+      <c r="H22" t="s">
         <v>784</v>
       </c>
-      <c r="H22" t="s">
-        <v>785</v>
-      </c>
       <c r="I22" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -10043,10 +10050,10 @@
         <v>239</v>
       </c>
       <c r="G23" s="42" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H23" s="42" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -10054,10 +10061,10 @@
     </row>
     <row r="24" spans="1:9">
       <c r="G24" s="42" t="s">
+        <v>786</v>
+      </c>
+      <c r="H24" s="42" t="s">
         <v>787</v>
-      </c>
-      <c r="H24" s="42" t="s">
-        <v>788</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -10065,10 +10072,10 @@
     </row>
     <row r="25" spans="1:9">
       <c r="G25" s="42" t="s">
+        <v>788</v>
+      </c>
+      <c r="H25" s="42" t="s">
         <v>789</v>
-      </c>
-      <c r="H25" s="42" t="s">
-        <v>790</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -10076,10 +10083,10 @@
     </row>
     <row r="26" spans="1:9">
       <c r="G26" t="s">
+        <v>790</v>
+      </c>
+      <c r="H26" t="s">
         <v>791</v>
-      </c>
-      <c r="H26" t="s">
-        <v>792</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -10087,7 +10094,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="G27" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -10095,7 +10102,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="G28" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -10103,10 +10110,10 @@
     </row>
     <row r="29" spans="1:9">
       <c r="G29" t="s">
+        <v>794</v>
+      </c>
+      <c r="H29" t="s">
         <v>795</v>
-      </c>
-      <c r="H29" t="s">
-        <v>796</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -10114,10 +10121,10 @@
     </row>
     <row r="30" spans="1:9">
       <c r="G30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H30" t="s">
         <v>797</v>
-      </c>
-      <c r="H30" t="s">
-        <v>798</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -10125,10 +10132,10 @@
     </row>
     <row r="31" spans="1:9">
       <c r="G31" t="s">
+        <v>798</v>
+      </c>
+      <c r="H31" t="s">
         <v>799</v>
-      </c>
-      <c r="H31" t="s">
-        <v>800</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -13122,7 +13129,7 @@
         <v>260</v>
       </c>
       <c r="C20" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D20" t="s">
         <v>616</v>
@@ -13167,10 +13174,10 @@
         <v>1999</v>
       </c>
       <c r="F22" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G22" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" thickBot="1">
@@ -13194,10 +13201,10 @@
         <v>2200</v>
       </c>
       <c r="F23" t="s">
+        <v>802</v>
+      </c>
+      <c r="G23" s="18" t="s">
         <v>803</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -14135,8 +14142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14363,31 +14370,31 @@
         <v>639</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="B15">
-        <v>0.29630960485488883</v>
-      </c>
-      <c r="C15">
-        <v>0.18665818857667263</v>
-      </c>
-      <c r="D15">
-        <v>0.27952064315716252</v>
-      </c>
-      <c r="E15">
-        <v>0.10816335116113814</v>
-      </c>
-      <c r="F15">
-        <v>0.12934821225013785</v>
+      <c r="B15" s="44">
+        <v>0.29524004813828703</v>
+      </c>
+      <c r="C15" s="44">
+        <v>0.18598442871189</v>
+      </c>
+      <c r="D15" s="44">
+        <v>0.282121279527561</v>
+      </c>
+      <c r="E15" s="44">
+        <v>0.107772925616947</v>
+      </c>
+      <c r="F15" s="44">
+        <v>0.12888131800531499</v>
       </c>
       <c r="G15">
         <f>SUM(B15:F15)</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="H15" s="22"/>
       <c r="J15" s="3" t="s">
@@ -14403,15 +14410,15 @@
       </c>
       <c r="B16" s="13">
         <f t="shared" ref="B16:F16" si="2">ROUND(2000*B15,0)</f>
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C16" s="13">
         <f t="shared" si="2"/>
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D16" s="13">
         <f t="shared" si="2"/>
-        <v>559</v>
+        <v>564</v>
       </c>
       <c r="E16" s="13">
         <f t="shared" si="2"/>
@@ -14419,7 +14426,7 @@
       </c>
       <c r="F16" s="13">
         <f t="shared" si="2"/>
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G16" s="13">
         <f>SUM(B16:F16)</f>
@@ -14439,23 +14446,23 @@
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17:F17" si="3">ROUND(2200*B15,0)</f>
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="3"/>
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="3"/>
-        <v>615</v>
+        <v>621</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="3"/>
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="3"/>
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G17" s="2">
         <f>SUM(B17:F17)</f>
@@ -14466,7 +14473,7 @@
         <v>256</v>
       </c>
       <c r="K17" t="s">
-        <v>644</v>
+        <v>832</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -14494,10 +14501,10 @@
     </row>
     <row r="20" spans="1:11">
       <c r="J20" t="s">
+        <v>645</v>
+      </c>
+      <c r="K20" t="s">
         <v>646</v>
-      </c>
-      <c r="K20" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16" thickBot="1">
@@ -14567,6 +14574,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add price elec, coal, etc.
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0AC5D0-4076-7B45-A882-60B99598440D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF690970-EC06-5D40-B7C7-79959B66AB80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8140" yWindow="480" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3106,7 +3106,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N76" sqref="N76"/>
+      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Update coal price CH
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9757490D-2661-934E-9F25-1E98204C5F1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
     <sheet name="quotas_MX" sheetId="17" r:id="rId16"/>
     <sheet name="quotas_SK" sheetId="18" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1776" uniqueCount="853">
   <si>
     <t>Country</t>
   </si>
@@ -2602,12 +2603,15 @@
   </si>
   <si>
     <t>fossil CO2 emissions (2017, MtCO2) global: 37.1 Gt source: https://publications.jrc.ec.europa.eu/repository/handle/JRC113738 https://en.wikipedia.org/wiki/List_of_countries_by_carbon_dioxide_emissions</t>
+  </si>
+  <si>
+    <t>https://www.argusmedia.com/ja/news/2166902-chinas-ndrc-keeps-base-coal-price-unchanged-for-2021#.X9AriLw3LDc.twitter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2840,7 +2844,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3117,36 +3121,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U59" sqref="U59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K105" sqref="K105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.6328125" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" customWidth="1"/>
-    <col min="3" max="3" width="8.36328125" customWidth="1"/>
-    <col min="4" max="4" width="6.453125" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.36328125" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="6.5" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" customWidth="1"/>
-    <col min="9" max="9" width="6.453125" customWidth="1"/>
-    <col min="10" max="10" width="8.6328125" customWidth="1"/>
-    <col min="11" max="11" width="7.6328125" customWidth="1"/>
-    <col min="12" max="12" width="8.36328125" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" customWidth="1"/>
-    <col min="15" max="15" width="6.81640625" customWidth="1"/>
-    <col min="16" max="16" width="7.36328125" customWidth="1"/>
-    <col min="17" max="17" width="8.453125" customWidth="1"/>
-    <col min="18" max="18" width="11.6328125" customWidth="1"/>
+    <col min="8" max="8" width="8.5" customWidth="1"/>
+    <col min="9" max="9" width="6.5" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" customWidth="1"/>
+    <col min="14" max="14" width="9.5" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" customWidth="1"/>
+    <col min="17" max="17" width="8.5" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" customWidth="1"/>
     <col min="19" max="20" width="10" customWidth="1"/>
-    <col min="21" max="21" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -6552,6 +6556,10 @@
         <f>240.49/G9</f>
         <v>63.120734908136484</v>
       </c>
+      <c r="K76">
+        <f>535/K9</f>
+        <v>83.987441130298265</v>
+      </c>
       <c r="N76">
         <f>374/O9</f>
         <v>71.510516252390047</v>
@@ -7294,6 +7302,9 @@
       </c>
       <c r="G105" t="s">
         <v>831</v>
+      </c>
+      <c r="K105" t="s">
+        <v>852</v>
       </c>
       <c r="N105" t="s">
         <v>832</v>
@@ -8198,16 +8209,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -8221,7 +8232,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -8242,7 +8253,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -8263,7 +8274,7 @@
         <v>0.92622883301508352</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -8282,8 +8293,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>225</v>
       </c>
@@ -8304,7 +8315,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>218</v>
       </c>
@@ -8328,7 +8339,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -8357,7 +8368,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -8397,7 +8408,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1">
+    <row r="13" spans="1:10" ht="16" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>221</v>
       </c>
@@ -8420,7 +8431,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>218</v>
       </c>
@@ -8450,7 +8461,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -8485,7 +8496,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -8532,8 +8543,8 @@
         <v>822</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1"/>
-    <row r="20" spans="1:10" ht="26.5" thickBot="1">
+    <row r="19" spans="1:10" ht="16" thickBot="1"/>
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>505</v>
       </c>
@@ -8546,7 +8557,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:10" ht="26.5" thickBot="1">
+    <row r="21" spans="1:10" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>218</v>
       </c>
@@ -8562,7 +8573,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -8580,7 +8591,7 @@
       </c>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:10" ht="39" thickBot="1">
+    <row r="23" spans="1:10" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>510</v>
       </c>
@@ -8604,19 +8615,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -8631,7 +8642,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -8653,7 +8664,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -8675,7 +8686,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -8716,7 +8727,7 @@
       <c r="G6" s="36"/>
       <c r="H6" s="37"/>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -8726,7 +8737,7 @@
       <c r="G7" s="36"/>
       <c r="H7" s="37"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>225</v>
       </c>
@@ -8748,7 +8759,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="37"/>
     </row>
-    <row r="9" spans="1:11" ht="26.5" thickBot="1">
+    <row r="9" spans="1:11" ht="30" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>218</v>
       </c>
@@ -8773,7 +8784,7 @@
       </c>
       <c r="H9" s="37"/>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1">
+    <row r="10" spans="1:11" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>219</v>
       </c>
@@ -8803,7 +8814,7 @@
       </c>
       <c r="H10" s="37"/>
     </row>
-    <row r="11" spans="1:11" ht="26.5" thickBot="1">
+    <row r="11" spans="1:11" ht="30" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>220</v>
       </c>
@@ -8848,7 +8859,7 @@
     <row r="13" spans="1:11">
       <c r="H13" s="37"/>
     </row>
-    <row r="14" spans="1:11" ht="39" thickBot="1">
+    <row r="14" spans="1:11" ht="44" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>221</v>
       </c>
@@ -8872,7 +8883,7 @@
       </c>
       <c r="H14" s="37"/>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>218</v>
       </c>
@@ -8899,7 +8910,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>219</v>
       </c>
@@ -8935,7 +8946,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="26.5" thickBot="1">
+    <row r="17" spans="1:12" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>220</v>
       </c>
@@ -9007,7 +9018,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="26.5" thickBot="1">
+    <row r="21" spans="1:12" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>805</v>
       </c>
@@ -9031,7 +9042,7 @@
       </c>
       <c r="H21" s="37"/>
     </row>
-    <row r="22" spans="1:12" ht="26.5" thickBot="1">
+    <row r="22" spans="1:12" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>218</v>
       </c>
@@ -9058,7 +9069,7 @@
         <v>0.99989215000000009</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>219</v>
       </c>
@@ -9091,7 +9102,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="26.5" thickBot="1">
+    <row r="24" spans="1:12" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>220</v>
       </c>
@@ -9180,16 +9191,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -9203,7 +9214,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -9224,7 +9235,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -9245,7 +9256,7 @@
         <v>0.99992877771181621</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -9264,8 +9275,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>225</v>
       </c>
@@ -9286,7 +9297,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>218</v>
       </c>
@@ -9310,7 +9321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -9339,7 +9350,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -9379,7 +9390,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>221</v>
       </c>
@@ -9408,7 +9419,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>218</v>
       </c>
@@ -9438,7 +9449,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>219</v>
       </c>
@@ -9473,7 +9484,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>220</v>
       </c>
@@ -9528,8 +9539,8 @@
         <v>753</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1"/>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1"/>
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="12" t="s">
         <v>505</v>
       </c>
@@ -9542,7 +9553,7 @@
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>218</v>
       </c>
@@ -9564,7 +9575,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1">
+    <row r="25" spans="1:11" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>219</v>
       </c>
@@ -9588,7 +9599,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="39" thickBot="1">
+    <row r="26" spans="1:11" ht="44" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>510</v>
       </c>
@@ -9613,16 +9624,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22:H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -9636,7 +9647,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1">
+    <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -9657,7 +9668,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -9678,7 +9689,7 @@
         <v>0.97760081385085629</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -9697,8 +9708,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>225</v>
       </c>
@@ -9719,7 +9730,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>218</v>
       </c>
@@ -9743,7 +9754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -9772,7 +9783,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -9812,7 +9823,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>221</v>
       </c>
@@ -9835,7 +9846,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>218</v>
       </c>
@@ -9865,7 +9876,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>219</v>
       </c>
@@ -9900,7 +9911,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>220</v>
       </c>
@@ -9950,8 +9961,8 @@
         <v>762</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1"/>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1"/>
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="12" t="s">
         <v>505</v>
       </c>
@@ -9964,7 +9975,7 @@
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>218</v>
       </c>
@@ -9986,7 +9997,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1">
+    <row r="24" spans="1:11" ht="16" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>219</v>
       </c>
@@ -10013,7 +10024,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="39" thickBot="1">
+    <row r="25" spans="1:11" ht="44" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>510</v>
       </c>
@@ -10037,16 +10048,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -10060,7 +10071,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -10081,7 +10092,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -10102,7 +10113,7 @@
         <v>1.0341140064832992</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -10121,8 +10132,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>225</v>
       </c>
@@ -10143,7 +10154,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>218</v>
       </c>
@@ -10167,7 +10178,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -10196,7 +10207,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -10236,7 +10247,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="39" thickBot="1">
+    <row r="13" spans="1:10" ht="44" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>221</v>
       </c>
@@ -10259,7 +10270,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>218</v>
       </c>
@@ -10289,7 +10300,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -10324,7 +10335,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -10362,7 +10373,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1">
+    <row r="19" spans="1:9" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>337</v>
       </c>
@@ -10373,7 +10384,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1">
+    <row r="20" spans="1:9" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>218</v>
       </c>
@@ -10394,7 +10405,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1">
+    <row r="21" spans="1:9" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>219</v>
       </c>
@@ -10411,7 +10422,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="26.5" thickBot="1">
+    <row r="22" spans="1:9" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -10539,16 +10550,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -10562,7 +10573,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -10583,7 +10594,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -10604,7 +10615,7 @@
         <v>0.95217958067188335</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -10623,8 +10634,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>225</v>
       </c>
@@ -10645,7 +10656,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>218</v>
       </c>
@@ -10669,7 +10680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -10698,7 +10709,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -10744,16 +10755,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -10767,7 +10778,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -10788,7 +10799,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -10809,7 +10820,7 @@
         <v>0.92970833595125124</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -10828,8 +10839,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>225</v>
       </c>
@@ -10850,7 +10861,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>218</v>
       </c>
@@ -10874,7 +10885,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -10903,7 +10914,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -10949,16 +10960,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -10972,7 +10983,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -10993,7 +11004,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -11014,7 +11025,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -11033,8 +11044,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>225</v>
       </c>
@@ -11055,7 +11066,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>218</v>
       </c>
@@ -11079,7 +11090,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -11108,7 +11119,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -11154,14 +11165,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -11650,30 +11661,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D28" sqref="A24:D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -11688,7 +11699,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -11706,7 +11717,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -11726,7 +11737,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -11757,7 +11768,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -11766,7 +11777,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>225</v>
       </c>
@@ -11787,7 +11798,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>218</v>
       </c>
@@ -11811,7 +11822,7 @@
         <v>1.0001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -11840,7 +11851,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -11869,8 +11880,8 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1"/>
-    <row r="12" spans="1:7" ht="15" thickBot="1">
+    <row r="11" spans="1:7" ht="16" thickBot="1"/>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>237</v>
       </c>
@@ -11888,7 +11899,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="8" t="s">
         <v>236</v>
       </c>
@@ -11908,7 +11919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
@@ -11933,7 +11944,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>220</v>
       </c>
@@ -11963,7 +11974,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="12" t="s">
         <v>221</v>
       </c>
@@ -11983,7 +11994,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="8" t="s">
         <v>218</v>
       </c>
@@ -12007,7 +12018,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>219</v>
       </c>
@@ -12036,7 +12047,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>220</v>
       </c>
@@ -12074,7 +12085,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="16" t="s">
         <v>337</v>
       </c>
@@ -12085,7 +12096,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>218</v>
       </c>
@@ -12100,7 +12111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>219</v>
       </c>
@@ -12117,7 +12128,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>220</v>
       </c>
@@ -12145,22 +12156,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:E32"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>279</v>
       </c>
@@ -12186,7 +12197,7 @@
       <c r="K1" s="13"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -12219,7 +12230,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -12253,7 +12264,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1">
+    <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -12317,14 +12328,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>222</v>
       </c>
@@ -12344,7 +12355,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>218</v>
       </c>
@@ -12367,7 +12378,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>219</v>
       </c>
@@ -12392,7 +12403,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>220</v>
       </c>
@@ -12433,7 +12444,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -12447,7 +12458,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>225</v>
       </c>
@@ -12473,7 +12484,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>218</v>
       </c>
@@ -12502,7 +12513,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>219</v>
       </c>
@@ -12536,7 +12547,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>220</v>
       </c>
@@ -12586,7 +12597,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -12600,7 +12611,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="26.5" thickBot="1">
+    <row r="20" spans="1:12" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>231</v>
       </c>
@@ -12624,7 +12635,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>236</v>
       </c>
@@ -12650,7 +12661,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -12681,7 +12692,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>220</v>
       </c>
@@ -12712,7 +12723,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>238</v>
       </c>
@@ -12722,7 +12733,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -12747,7 +12758,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1">
+    <row r="27" spans="1:12" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>218</v>
       </c>
@@ -12766,7 +12777,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1">
+    <row r="28" spans="1:12" ht="16" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>219</v>
       </c>
@@ -12788,7 +12799,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1">
+    <row r="29" spans="1:12" ht="16" thickBot="1">
       <c r="A29" s="8" t="s">
         <v>509</v>
       </c>
@@ -12807,7 +12818,7 @@
       </c>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>508</v>
       </c>
@@ -12829,7 +12840,7 @@
       </c>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:12" ht="26.5" thickBot="1">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>510</v>
       </c>
@@ -12862,12 +12873,12 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
-    <row r="36" spans="1:10" ht="15" thickBot="1">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26.5" thickBot="1">
+    <row r="37" spans="1:10" ht="30" thickBot="1">
       <c r="A37" s="8" t="s">
         <v>209</v>
       </c>
@@ -12897,7 +12908,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="8" t="s">
         <v>218</v>
       </c>
@@ -12930,7 +12941,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="8" t="s">
         <v>219</v>
       </c>
@@ -12971,7 +12982,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" thickBot="1">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="8" t="s">
         <v>220</v>
       </c>
@@ -13038,12 +13049,12 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="15" thickBot="1">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" thickBot="1">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>284</v>
       </c>
@@ -13064,7 +13075,7 @@
       </c>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="15" thickBot="1">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="8" t="s">
         <v>218</v>
       </c>
@@ -13088,7 +13099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" thickBot="1">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="8" t="s">
         <v>219</v>
       </c>
@@ -13117,7 +13128,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="8" t="s">
         <v>220</v>
       </c>
@@ -13173,16 +13184,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -13196,7 +13207,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -13217,7 +13228,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -13238,7 +13249,7 @@
         <v>0.95277529961698948</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -13257,8 +13268,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>225</v>
       </c>
@@ -13279,7 +13290,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>218</v>
       </c>
@@ -13303,7 +13314,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -13332,7 +13343,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -13372,7 +13383,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="26.5" thickBot="1">
+    <row r="13" spans="1:11" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>221</v>
       </c>
@@ -13398,7 +13409,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>218</v>
       </c>
@@ -13428,7 +13439,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -13463,7 +13474,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.5" thickBot="1">
+    <row r="16" spans="1:11" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -13513,7 +13524,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1">
+    <row r="20" spans="1:11" ht="16" thickBot="1">
       <c r="A20" s="16" t="s">
         <v>337</v>
       </c>
@@ -13527,7 +13538,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="26.5" thickBot="1">
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>218</v>
       </c>
@@ -13545,7 +13556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -13572,7 +13583,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1">
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>220</v>
       </c>
@@ -13606,23 +13617,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G23" r:id="rId1"/>
+    <hyperlink ref="G23" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -13636,7 +13647,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -13657,7 +13668,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -13678,7 +13689,7 @@
         <v>0.90805800128462044</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -13697,8 +13708,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>225</v>
       </c>
@@ -13719,7 +13730,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>218</v>
       </c>
@@ -13743,7 +13754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -13772,7 +13783,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -13812,7 +13823,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="26.5" thickBot="1">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>221</v>
       </c>
@@ -13832,7 +13843,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>218</v>
       </c>
@@ -13856,7 +13867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -13885,7 +13896,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -13926,7 +13937,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1">
+    <row r="19" spans="1:8" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>337</v>
       </c>
@@ -13937,7 +13948,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="26.5" thickBot="1">
+    <row r="20" spans="1:8" ht="30" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>218</v>
       </c>
@@ -13952,7 +13963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1">
+    <row r="21" spans="1:8" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>219</v>
       </c>
@@ -13969,7 +13980,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="26.5" thickBot="1">
+    <row r="22" spans="1:8" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>220</v>
       </c>
@@ -13991,8 +14002,8 @@
         <v>238</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1"/>
-    <row r="25" spans="1:8" ht="26.5" thickBot="1">
+    <row r="24" spans="1:8" ht="16" thickBot="1"/>
+    <row r="25" spans="1:8" ht="30" thickBot="1">
       <c r="A25" s="12" t="s">
         <v>505</v>
       </c>
@@ -14007,7 +14018,7 @@
       </c>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:8" ht="26.5" thickBot="1">
+    <row r="26" spans="1:8" ht="30" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>218</v>
       </c>
@@ -14025,7 +14036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1">
+    <row r="27" spans="1:8" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>219</v>
       </c>
@@ -14046,7 +14057,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="39" thickBot="1">
+    <row r="28" spans="1:8" ht="44" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>510</v>
       </c>
@@ -14088,16 +14099,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="E23" sqref="A20:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1">
+    <row r="1" spans="1:13" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -14111,7 +14122,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:13" ht="26.5" thickBot="1">
+    <row r="2" spans="1:13" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -14132,7 +14143,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -14153,7 +14164,7 @@
         <v>0.9267197256851698</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="26.5" thickBot="1">
+    <row r="4" spans="1:13" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -14172,8 +14183,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1"/>
-    <row r="7" spans="1:13" ht="15" thickBot="1">
+    <row r="6" spans="1:13" ht="16" thickBot="1"/>
+    <row r="7" spans="1:13" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>225</v>
       </c>
@@ -14194,7 +14205,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="26.5" thickBot="1">
+    <row r="8" spans="1:13" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>218</v>
       </c>
@@ -14218,7 +14229,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1">
+    <row r="9" spans="1:13" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -14247,7 +14258,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.5" thickBot="1">
+    <row r="10" spans="1:13" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -14287,7 +14298,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:13" ht="26.5" thickBot="1">
+    <row r="13" spans="1:13" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>221</v>
       </c>
@@ -14316,7 +14327,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="26.5" thickBot="1">
+    <row r="14" spans="1:13" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>218</v>
       </c>
@@ -14349,7 +14360,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1">
+    <row r="15" spans="1:13" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>219</v>
       </c>
@@ -14388,7 +14399,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="26.5" thickBot="1">
+    <row r="16" spans="1:13" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>220</v>
       </c>
@@ -14450,8 +14461,8 @@
         <v>588</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" thickBot="1"/>
-    <row r="20" spans="1:13" ht="26.5" thickBot="1">
+    <row r="19" spans="1:13" ht="16" thickBot="1"/>
+    <row r="20" spans="1:13" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>505</v>
       </c>
@@ -14464,7 +14475,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:13" ht="26.5" thickBot="1">
+    <row r="21" spans="1:13" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>218</v>
       </c>
@@ -14480,7 +14491,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:13" ht="15" thickBot="1">
+    <row r="22" spans="1:13" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>219</v>
       </c>
@@ -14498,7 +14509,7 @@
       </c>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:13" ht="39" thickBot="1">
+    <row r="23" spans="1:13" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>510</v>
       </c>
@@ -14531,19 +14542,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -14557,7 +14568,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -14578,7 +14589,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -14599,7 +14610,7 @@
         <v>0.97448244785232785</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -14618,8 +14629,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>225</v>
       </c>
@@ -14640,7 +14651,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>218</v>
       </c>
@@ -14664,7 +14675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -14693,7 +14704,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -14742,7 +14753,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="41"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>221</v>
       </c>
@@ -14765,7 +14776,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>218</v>
       </c>
@@ -14796,7 +14807,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>219</v>
       </c>
@@ -14832,7 +14843,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>220</v>
       </c>
@@ -14899,7 +14910,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1">
       <c r="A21" s="16" t="s">
         <v>337</v>
       </c>
@@ -14910,7 +14921,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1">
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>218</v>
       </c>
@@ -14925,7 +14936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>219</v>
       </c>
@@ -14942,7 +14953,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>220</v>
       </c>
@@ -14971,16 +14982,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>222</v>
       </c>
@@ -14994,7 +15005,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>218</v>
       </c>
@@ -15015,7 +15026,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>219</v>
       </c>
@@ -15036,7 +15047,7 @@
         <v>0.98351979013457747</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>220</v>
       </c>
@@ -15055,8 +15066,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>225</v>
       </c>
@@ -15077,7 +15088,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>218</v>
       </c>
@@ -15101,7 +15112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>219</v>
       </c>
@@ -15130,7 +15141,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>220</v>
       </c>
@@ -15170,7 +15181,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>221</v>
       </c>
@@ -15196,7 +15207,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>218</v>
       </c>
@@ -15226,7 +15237,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>219</v>
       </c>
@@ -15258,7 +15269,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="26.5" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>220</v>
       </c>
@@ -15302,8 +15313,8 @@
         <v>850</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1"/>
-    <row r="21" spans="1:10" ht="26.5" thickBot="1">
+    <row r="20" spans="1:10" ht="16" thickBot="1"/>
+    <row r="21" spans="1:10" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>505</v>
       </c>
@@ -15318,7 +15329,7 @@
       </c>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:10" ht="26.5" thickBot="1">
+    <row r="22" spans="1:10" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>218</v>
       </c>
@@ -15336,7 +15347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1">
+    <row r="23" spans="1:10" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>219</v>
       </c>
@@ -15360,7 +15371,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="39" thickBot="1">
+    <row r="24" spans="1:10" ht="44" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>510</v>
       </c>

</xml_diff>

<commit_message>
ES + quota UK
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60914BC8-24CF-0C42-B06C-AF3F963F8506}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480"/>
+    <workbookView xWindow="0" yWindow="2420" windowWidth="25600" windowHeight="14480" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
     <sheet name="quotas_MX" sheetId="17" r:id="rId16"/>
     <sheet name="quotas_SK" sheetId="18" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2796,7 +2797,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -3040,7 +3041,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3317,42 +3318,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A73" sqref="A73:A77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" customWidth="1"/>
-    <col min="6" max="6" width="6.453125" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" customWidth="1"/>
-    <col min="9" max="9" width="8.36328125" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" customWidth="1"/>
-    <col min="12" max="12" width="7.36328125" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="6.5" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" customWidth="1"/>
+    <col min="11" max="11" width="9.5" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" customWidth="1"/>
     <col min="13" max="14" width="8" customWidth="1"/>
-    <col min="15" max="15" width="8.453125" customWidth="1"/>
-    <col min="16" max="16" width="8.81640625" customWidth="1"/>
-    <col min="17" max="17" width="6.81640625" customWidth="1"/>
-    <col min="18" max="18" width="8.26953125" customWidth="1"/>
-    <col min="19" max="19" width="7.453125" customWidth="1"/>
-    <col min="20" max="20" width="8.36328125" customWidth="1"/>
-    <col min="21" max="21" width="6.453125" customWidth="1"/>
-    <col min="22" max="22" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" customWidth="1"/>
+    <col min="17" max="17" width="6.83203125" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" customWidth="1"/>
+    <col min="19" max="19" width="7.5" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" customWidth="1"/>
+    <col min="21" max="21" width="6.5" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -5628,7 +5629,7 @@
         <v>600</v>
       </c>
       <c r="M50" s="30">
-        <f t="shared" ref="M50:AA50" si="0">$S$50*M9</f>
+        <f t="shared" ref="M50:P50" si="0">$S$50*M9</f>
         <v>38.1</v>
       </c>
       <c r="N50" s="30">
@@ -6142,7 +6143,7 @@
         <v>798</v>
       </c>
       <c r="B57" s="27">
-        <f t="shared" ref="B57:X57" si="5">B56/B61</f>
+        <f t="shared" ref="B57:P57" si="5">B56/B61</f>
         <v>10.55952380952381</v>
       </c>
       <c r="C57" s="27">
@@ -6202,47 +6203,47 @@
         <v>5.3571428571428568</v>
       </c>
       <c r="Q57" s="27">
-        <f>Q56/Q61</f>
+        <f t="shared" ref="Q57:V57" si="6">Q56/Q61</f>
         <v>2.460093896713615</v>
       </c>
       <c r="R57" s="27">
-        <f>R56/R61</f>
+        <f t="shared" si="6"/>
         <v>14.823529411764707</v>
       </c>
       <c r="S57" s="27">
-        <f>S56/S61</f>
+        <f t="shared" si="6"/>
         <v>17.268882175226587</v>
       </c>
       <c r="T57" s="27">
-        <f>T56/T61</f>
+        <f t="shared" si="6"/>
         <v>9.6551724137931032</v>
       </c>
       <c r="U57" s="27">
-        <f>U56/U61</f>
+        <f t="shared" si="6"/>
         <v>6.8769230769230774</v>
       </c>
       <c r="V57" s="27">
-        <f>V56/V61</f>
+        <f t="shared" si="6"/>
         <v>1.733009708737864</v>
       </c>
       <c r="W57" s="27">
-        <f t="shared" ref="V57:AA57" si="6">W56/W61</f>
+        <f t="shared" ref="W57:AA57" si="7">W56/W61</f>
         <v>3.2254901960784315</v>
       </c>
       <c r="X57" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.8095238095238093</v>
       </c>
       <c r="Y57" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.4589041095890405</v>
       </c>
       <c r="Z57" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>17.8</v>
       </c>
       <c r="AA57" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.2325581395348841</v>
       </c>
     </row>
@@ -6584,27 +6585,27 @@
         <v>302</v>
       </c>
       <c r="B62" s="17">
-        <f t="shared" ref="B62:P62" si="7">2.5*B58/1000</f>
+        <f t="shared" ref="B62:P62" si="8">2.5*B58/1000</f>
         <v>0.1125</v>
       </c>
       <c r="C62" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1125</v>
       </c>
       <c r="D62" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1125</v>
       </c>
       <c r="E62" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1125</v>
       </c>
       <c r="F62" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1125</v>
       </c>
       <c r="G62" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1125</v>
       </c>
       <c r="H62" s="17">
@@ -6612,15 +6613,15 @@
         <v>0.1125</v>
       </c>
       <c r="I62" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1125</v>
       </c>
       <c r="J62" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1125</v>
       </c>
       <c r="K62" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1125</v>
       </c>
       <c r="L62" s="17">
@@ -6636,11 +6637,11 @@
         <v>0.1125</v>
       </c>
       <c r="O62" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1125</v>
       </c>
       <c r="P62" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1125</v>
       </c>
       <c r="Q62" s="17">
@@ -6664,27 +6665,27 @@
         <v>0.1125</v>
       </c>
       <c r="V62" s="17">
-        <f t="shared" ref="V62:AA62" si="8">2.5*V58/1000</f>
+        <f t="shared" ref="V62:AA62" si="9">2.5*V58/1000</f>
         <v>0.1125</v>
       </c>
       <c r="W62" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.1125</v>
       </c>
       <c r="X62" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.1125</v>
       </c>
       <c r="Y62" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.1125</v>
       </c>
       <c r="Z62" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.1125</v>
       </c>
       <c r="AA62" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.1125</v>
       </c>
     </row>
@@ -6693,27 +6694,27 @@
         <v>304</v>
       </c>
       <c r="B63" s="22">
-        <f t="shared" ref="B63:O63" si="9">B62*B9</f>
+        <f t="shared" ref="B63:K63" si="10">B62*B9</f>
         <v>9.5625000000000002E-2</v>
       </c>
       <c r="C63" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9.5625000000000002E-2</v>
       </c>
       <c r="D63" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.43762500000000004</v>
       </c>
       <c r="E63" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9.5625000000000002E-2</v>
       </c>
       <c r="F63" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.2125000000000004E-2</v>
       </c>
       <c r="G63" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.262500000000001</v>
       </c>
       <c r="H63" s="22">
@@ -6721,15 +6722,15 @@
         <v>0.73012500000000002</v>
       </c>
       <c r="I63" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.4375</v>
       </c>
       <c r="J63" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1636.2</v>
       </c>
       <c r="K63" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.6312500000000001</v>
       </c>
       <c r="L63" s="22">
@@ -6737,27 +6738,27 @@
         <v>2.25</v>
       </c>
       <c r="M63" s="22">
-        <f t="shared" ref="M63:R63" si="10">M62*M9</f>
+        <f t="shared" ref="M63:R63" si="11">M62*M9</f>
         <v>0.142875</v>
       </c>
       <c r="N63" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.07125</v>
       </c>
       <c r="O63" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>129.6</v>
       </c>
       <c r="P63" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.96525000000000005</v>
       </c>
       <c r="Q63" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.58274999999999999</v>
       </c>
       <c r="R63" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.15300000000000002</v>
       </c>
       <c r="S63" s="22">
@@ -6765,35 +6766,35 @@
         <v>0.42585862500000005</v>
       </c>
       <c r="T63" s="22">
-        <f t="shared" ref="T63" si="11">T62*T9</f>
+        <f t="shared" ref="T63" si="12">T62*T9</f>
         <v>2.0750000000000002</v>
       </c>
       <c r="U63" s="22">
-        <f t="shared" ref="U63" si="12">U62*U9</f>
+        <f t="shared" ref="U63" si="13">U62*U9</f>
         <v>9.5625000000000002E-2</v>
       </c>
       <c r="V63" s="22">
-        <f t="shared" ref="V63" si="13">V62*V9</f>
+        <f t="shared" ref="V63" si="14">V62*V9</f>
         <v>46.237500000000004</v>
       </c>
       <c r="W63" s="22">
-        <f t="shared" ref="W63" si="14">W62*W9</f>
+        <f t="shared" ref="W63" si="15">W62*W9</f>
         <v>1.762875</v>
       </c>
       <c r="X63" s="22">
-        <f t="shared" ref="X63" si="15">X62*X9</f>
+        <f t="shared" ref="X63" si="16">X62*X9</f>
         <v>4727.8125</v>
       </c>
       <c r="Y63" s="22">
-        <f t="shared" ref="Y63" si="16">Y62*Y9</f>
+        <f t="shared" ref="Y63" si="17">Y62*Y9</f>
         <v>8.3970000000000002</v>
       </c>
       <c r="Z63" s="22">
-        <f t="shared" ref="Z63" si="17">Z62*Z9</f>
+        <f t="shared" ref="Z63" si="18">Z62*Z9</f>
         <v>0.421875</v>
       </c>
       <c r="AA63" s="22">
-        <f t="shared" ref="AA63" si="18">AA62*AA9</f>
+        <f t="shared" ref="AA63" si="19">AA62*AA9</f>
         <v>0.10350000000000001</v>
       </c>
     </row>
@@ -6802,27 +6803,27 @@
         <v>305</v>
       </c>
       <c r="B64" s="3">
-        <f t="shared" ref="B64:R64" si="19">0.8*0.8*B59*B58*1000000*B9/B60</f>
+        <f t="shared" ref="B64:R64" si="20">0.8*0.8*B59*B58*1000000*B9/B60</f>
         <v>284.54272571526855</v>
       </c>
       <c r="C64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>178.03117201498719</v>
       </c>
       <c r="D64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1139.8701297301359</v>
       </c>
       <c r="E64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>180.84008419659901</v>
       </c>
       <c r="F64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>154.39364344375809</v>
       </c>
       <c r="G64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>38475.475811006392</v>
       </c>
       <c r="H64" s="3">
@@ -6830,43 +6831,43 @@
         <v>1801.2605963508981</v>
       </c>
       <c r="I64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>6166.1299237940575</v>
       </c>
       <c r="J64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1239926.3389856876</v>
       </c>
       <c r="K64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5027.0908294299234</v>
       </c>
       <c r="L64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>3146.9109366338298</v>
       </c>
       <c r="M64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>744.01624764457154</v>
       </c>
       <c r="N64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>4573.2807681056329</v>
       </c>
       <c r="O64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>516982.80552083551</v>
       </c>
       <c r="P64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1777.2420087868363</v>
       </c>
       <c r="Q64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>460.13977425382205</v>
       </c>
       <c r="R64" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>803.97497584214091</v>
       </c>
       <c r="S64" s="3">
@@ -6882,27 +6883,27 @@
         <v>164.25391156221337</v>
       </c>
       <c r="V64" s="3">
-        <f t="shared" ref="V64:AA64" si="20">0.8*0.8*V59*V58*1000000*V9/V60</f>
+        <f t="shared" ref="V64:AA64" si="21">0.8*0.8*V59*V58*1000000*V9/V60</f>
         <v>10857.316205167268</v>
       </c>
       <c r="W64" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1838.6871158022327</v>
       </c>
       <c r="X64" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>13363296.990635848</v>
       </c>
       <c r="Y64" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33457.4054407687</v>
       </c>
       <c r="Z64" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2765.8745991050655</v>
       </c>
       <c r="AA64" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>147.96508326729767</v>
       </c>
     </row>
@@ -9292,16 +9293,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -9315,7 +9316,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -9336,7 +9337,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -9357,7 +9358,7 @@
         <v>0.92622883301508352</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -9376,8 +9377,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -9398,7 +9399,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -9422,7 +9423,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -9451,7 +9452,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -9491,7 +9492,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1">
+    <row r="13" spans="1:10" ht="16" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -9514,7 +9515,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -9544,7 +9545,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -9579,7 +9580,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -9626,8 +9627,8 @@
         <v>807</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1"/>
-    <row r="20" spans="1:10" ht="26.5" thickBot="1">
+    <row r="19" spans="1:10" ht="16" thickBot="1"/>
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>496</v>
       </c>
@@ -9640,7 +9641,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:10" ht="26.5" thickBot="1">
+    <row r="21" spans="1:10" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>211</v>
       </c>
@@ -9656,7 +9657,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -9674,7 +9675,7 @@
       </c>
       <c r="E22" s="28"/>
     </row>
-    <row r="23" spans="1:10" ht="39" thickBot="1">
+    <row r="23" spans="1:10" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>501</v>
       </c>
@@ -9698,19 +9699,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -9725,7 +9726,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -9747,7 +9748,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -9769,7 +9770,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -9810,7 +9811,7 @@
       <c r="G6" s="35"/>
       <c r="H6" s="36"/>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -9820,7 +9821,7 @@
       <c r="G7" s="35"/>
       <c r="H7" s="36"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>218</v>
       </c>
@@ -9842,7 +9843,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="36"/>
     </row>
-    <row r="9" spans="1:11" ht="26.5" thickBot="1">
+    <row r="9" spans="1:11" ht="30" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -9867,7 +9868,7 @@
       </c>
       <c r="H9" s="36"/>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1">
+    <row r="10" spans="1:11" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -9897,7 +9898,7 @@
       </c>
       <c r="H10" s="36"/>
     </row>
-    <row r="11" spans="1:11" ht="26.5" thickBot="1">
+    <row r="11" spans="1:11" ht="30" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>213</v>
       </c>
@@ -9942,7 +9943,7 @@
     <row r="13" spans="1:11">
       <c r="H13" s="36"/>
     </row>
-    <row r="14" spans="1:11" ht="39" thickBot="1">
+    <row r="14" spans="1:11" ht="44" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -9966,7 +9967,7 @@
       </c>
       <c r="H14" s="36"/>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -9993,7 +9994,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -10029,7 +10030,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="26.5" thickBot="1">
+    <row r="17" spans="1:12" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -10101,7 +10102,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="26.5" thickBot="1">
+    <row r="21" spans="1:12" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>792</v>
       </c>
@@ -10125,7 +10126,7 @@
       </c>
       <c r="H21" s="36"/>
     </row>
-    <row r="22" spans="1:12" ht="26.5" thickBot="1">
+    <row r="22" spans="1:12" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>211</v>
       </c>
@@ -10152,7 +10153,7 @@
         <v>0.99989215000000009</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>212</v>
       </c>
@@ -10185,7 +10186,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="26.5" thickBot="1">
+    <row r="24" spans="1:12" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>213</v>
       </c>
@@ -10274,16 +10275,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -10297,7 +10298,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -10318,7 +10319,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -10339,7 +10340,7 @@
         <v>0.99992877771181621</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -10358,8 +10359,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -10380,7 +10381,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -10404,7 +10405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -10433,7 +10434,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -10473,7 +10474,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -10502,7 +10503,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -10532,7 +10533,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -10567,7 +10568,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -10622,8 +10623,8 @@
         <v>740</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1"/>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1"/>
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="12" t="s">
         <v>496</v>
       </c>
@@ -10636,7 +10637,7 @@
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>211</v>
       </c>
@@ -10658,7 +10659,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1">
+    <row r="25" spans="1:11" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>212</v>
       </c>
@@ -10682,7 +10683,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="39" thickBot="1">
+    <row r="26" spans="1:11" ht="44" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>501</v>
       </c>
@@ -10707,16 +10708,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22:H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -10730,7 +10731,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1">
+    <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -10751,7 +10752,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -10772,7 +10773,7 @@
         <v>0.97760081385085629</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -10791,8 +10792,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -10813,7 +10814,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -10837,7 +10838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -10866,7 +10867,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -10906,7 +10907,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -10929,7 +10930,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -10959,7 +10960,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -10994,7 +10995,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -11044,8 +11045,8 @@
         <v>749</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1"/>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1"/>
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="12" t="s">
         <v>496</v>
       </c>
@@ -11058,7 +11059,7 @@
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>211</v>
       </c>
@@ -11080,7 +11081,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1">
+    <row r="24" spans="1:11" ht="16" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>212</v>
       </c>
@@ -11107,7 +11108,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="39" thickBot="1">
+    <row r="25" spans="1:11" ht="44" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>501</v>
       </c>
@@ -11131,16 +11132,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -11154,7 +11155,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -11175,7 +11176,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -11196,7 +11197,7 @@
         <v>1.0341140064832992</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -11215,8 +11216,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -11237,7 +11238,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -11261,7 +11262,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -11290,7 +11291,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -11330,7 +11331,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="39" thickBot="1">
+    <row r="13" spans="1:10" ht="44" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -11353,7 +11354,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -11383,7 +11384,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -11418,7 +11419,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -11456,7 +11457,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1">
+    <row r="19" spans="1:9" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>330</v>
       </c>
@@ -11467,7 +11468,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1">
+    <row r="20" spans="1:9" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>211</v>
       </c>
@@ -11488,7 +11489,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1">
+    <row r="21" spans="1:9" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>212</v>
       </c>
@@ -11505,7 +11506,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="26.5" thickBot="1">
+    <row r="22" spans="1:9" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>213</v>
       </c>
@@ -11633,16 +11634,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -11656,7 +11657,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -11677,7 +11678,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -11698,7 +11699,7 @@
         <v>0.95217958067188335</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -11717,8 +11718,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -11739,7 +11740,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -11763,7 +11764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -11792,7 +11793,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -11838,16 +11839,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -11861,7 +11862,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -11882,7 +11883,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -11903,7 +11904,7 @@
         <v>0.92970833595125124</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -11922,8 +11923,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -11944,7 +11945,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -11968,7 +11969,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -11997,7 +11998,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -12043,16 +12044,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -12066,7 +12067,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -12087,7 +12088,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -12108,7 +12109,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -12127,8 +12128,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -12149,7 +12150,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -12173,7 +12174,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -12202,7 +12203,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -12248,14 +12249,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -12744,30 +12745,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D28" sqref="A24:D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -12782,7 +12783,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -12800,7 +12801,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -12820,7 +12821,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -12851,7 +12852,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -12860,7 +12861,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -12881,7 +12882,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -12905,7 +12906,7 @@
         <v>1.0001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -12934,7 +12935,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -12963,8 +12964,8 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1"/>
-    <row r="12" spans="1:7" ht="15" thickBot="1">
+    <row r="11" spans="1:7" ht="16" thickBot="1"/>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>230</v>
       </c>
@@ -12982,7 +12983,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="8" t="s">
         <v>229</v>
       </c>
@@ -13002,7 +13003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>212</v>
       </c>
@@ -13027,7 +13028,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>213</v>
       </c>
@@ -13057,7 +13058,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="12" t="s">
         <v>214</v>
       </c>
@@ -13077,7 +13078,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="8" t="s">
         <v>211</v>
       </c>
@@ -13101,7 +13102,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>212</v>
       </c>
@@ -13130,7 +13131,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>213</v>
       </c>
@@ -13168,7 +13169,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="16" t="s">
         <v>330</v>
       </c>
@@ -13179,7 +13180,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>211</v>
       </c>
@@ -13194,7 +13195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>212</v>
       </c>
@@ -13211,7 +13212,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>213</v>
       </c>
@@ -13239,22 +13240,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>272</v>
       </c>
@@ -13280,7 +13281,7 @@
       <c r="K1" s="13"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -13313,7 +13314,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -13347,7 +13348,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1">
+    <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -13411,14 +13412,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>215</v>
       </c>
@@ -13438,7 +13439,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -13461,7 +13462,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -13486,7 +13487,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>213</v>
       </c>
@@ -13527,7 +13528,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -13541,7 +13542,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>218</v>
       </c>
@@ -13567,7 +13568,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -13596,7 +13597,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -13630,7 +13631,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -13680,7 +13681,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -13694,7 +13695,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="26.5" thickBot="1">
+    <row r="20" spans="1:12" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>224</v>
       </c>
@@ -13718,7 +13719,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>229</v>
       </c>
@@ -13744,7 +13745,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -13775,7 +13776,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>213</v>
       </c>
@@ -13806,7 +13807,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>231</v>
       </c>
@@ -13816,7 +13817,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -13841,7 +13842,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1">
+    <row r="27" spans="1:12" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>211</v>
       </c>
@@ -13860,7 +13861,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1">
+    <row r="28" spans="1:12" ht="16" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>212</v>
       </c>
@@ -13882,7 +13883,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1">
+    <row r="29" spans="1:12" ht="16" thickBot="1">
       <c r="A29" s="8" t="s">
         <v>500</v>
       </c>
@@ -13901,7 +13902,7 @@
       </c>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>499</v>
       </c>
@@ -13923,7 +13924,7 @@
       </c>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:12" ht="26.5" thickBot="1">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>501</v>
       </c>
@@ -13956,12 +13957,12 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
-    <row r="36" spans="1:10" ht="15" thickBot="1">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26.5" thickBot="1">
+    <row r="37" spans="1:10" ht="30" thickBot="1">
       <c r="A37" s="8" t="s">
         <v>202</v>
       </c>
@@ -13991,7 +13992,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="8" t="s">
         <v>211</v>
       </c>
@@ -14024,7 +14025,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="8" t="s">
         <v>212</v>
       </c>
@@ -14065,7 +14066,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" thickBot="1">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="8" t="s">
         <v>213</v>
       </c>
@@ -14132,12 +14133,12 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="15" thickBot="1">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" thickBot="1">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>277</v>
       </c>
@@ -14158,7 +14159,7 @@
       </c>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="15" thickBot="1">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="8" t="s">
         <v>211</v>
       </c>
@@ -14182,7 +14183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" thickBot="1">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="8" t="s">
         <v>212</v>
       </c>
@@ -14211,7 +14212,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="8" t="s">
         <v>213</v>
       </c>
@@ -14267,16 +14268,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -14290,7 +14291,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -14311,7 +14312,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -14332,7 +14333,7 @@
         <v>0.95277529961698948</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -14351,8 +14352,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -14373,7 +14374,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -14397,7 +14398,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -14426,7 +14427,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -14466,7 +14467,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="26.5" thickBot="1">
+    <row r="13" spans="1:11" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -14492,7 +14493,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -14522,7 +14523,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -14557,7 +14558,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.5" thickBot="1">
+    <row r="16" spans="1:11" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -14607,7 +14608,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1">
+    <row r="20" spans="1:11" ht="16" thickBot="1">
       <c r="A20" s="16" t="s">
         <v>330</v>
       </c>
@@ -14621,7 +14622,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="26.5" thickBot="1">
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>211</v>
       </c>
@@ -14639,7 +14640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -14666,7 +14667,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1">
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>213</v>
       </c>
@@ -14700,23 +14701,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G23" r:id="rId1"/>
+    <hyperlink ref="G23" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -14730,7 +14731,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -14751,7 +14752,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -14772,7 +14773,7 @@
         <v>0.90805800128462044</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -14791,8 +14792,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -14813,7 +14814,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -14837,7 +14838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -14866,7 +14867,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -14906,7 +14907,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="26.5" thickBot="1">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -14926,7 +14927,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -14950,7 +14951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -14979,7 +14980,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -15020,7 +15021,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1">
+    <row r="19" spans="1:8" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>330</v>
       </c>
@@ -15031,7 +15032,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="26.5" thickBot="1">
+    <row r="20" spans="1:8" ht="30" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>211</v>
       </c>
@@ -15046,7 +15047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1">
+    <row r="21" spans="1:8" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>212</v>
       </c>
@@ -15063,7 +15064,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="26.5" thickBot="1">
+    <row r="22" spans="1:8" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>213</v>
       </c>
@@ -15085,8 +15086,8 @@
         <v>231</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1"/>
-    <row r="25" spans="1:8" ht="26.5" thickBot="1">
+    <row r="24" spans="1:8" ht="16" thickBot="1"/>
+    <row r="25" spans="1:8" ht="30" thickBot="1">
       <c r="A25" s="12" t="s">
         <v>496</v>
       </c>
@@ -15101,7 +15102,7 @@
       </c>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:8" ht="26.5" thickBot="1">
+    <row r="26" spans="1:8" ht="30" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>211</v>
       </c>
@@ -15119,7 +15120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1">
+    <row r="27" spans="1:8" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>212</v>
       </c>
@@ -15140,7 +15141,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="39" thickBot="1">
+    <row r="28" spans="1:8" ht="44" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>501</v>
       </c>
@@ -15182,16 +15183,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="E23" sqref="A20:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1">
+    <row r="1" spans="1:13" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -15205,7 +15206,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:13" ht="26.5" thickBot="1">
+    <row r="2" spans="1:13" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -15226,7 +15227,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -15247,7 +15248,7 @@
         <v>0.9267197256851698</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="26.5" thickBot="1">
+    <row r="4" spans="1:13" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -15266,8 +15267,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1"/>
-    <row r="7" spans="1:13" ht="15" thickBot="1">
+    <row r="6" spans="1:13" ht="16" thickBot="1"/>
+    <row r="7" spans="1:13" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -15288,7 +15289,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="26.5" thickBot="1">
+    <row r="8" spans="1:13" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -15312,7 +15313,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1">
+    <row r="9" spans="1:13" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -15341,7 +15342,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.5" thickBot="1">
+    <row r="10" spans="1:13" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -15381,7 +15382,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:13" ht="26.5" thickBot="1">
+    <row r="13" spans="1:13" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -15410,7 +15411,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="26.5" thickBot="1">
+    <row r="14" spans="1:13" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -15443,7 +15444,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1">
+    <row r="15" spans="1:13" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -15482,7 +15483,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="26.5" thickBot="1">
+    <row r="16" spans="1:13" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -15544,8 +15545,8 @@
         <v>579</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" thickBot="1"/>
-    <row r="20" spans="1:13" ht="26.5" thickBot="1">
+    <row r="19" spans="1:13" ht="16" thickBot="1"/>
+    <row r="20" spans="1:13" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>496</v>
       </c>
@@ -15558,7 +15559,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:13" ht="26.5" thickBot="1">
+    <row r="21" spans="1:13" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>211</v>
       </c>
@@ -15574,7 +15575,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:13" ht="15" thickBot="1">
+    <row r="22" spans="1:13" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -15592,7 +15593,7 @@
       </c>
       <c r="E22" s="28"/>
     </row>
-    <row r="23" spans="1:13" ht="39" thickBot="1">
+    <row r="23" spans="1:13" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>501</v>
       </c>
@@ -15625,19 +15626,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -15651,7 +15652,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -15672,7 +15673,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -15693,7 +15694,7 @@
         <v>0.97448244785232785</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -15712,8 +15713,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -15734,7 +15735,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -15758,7 +15759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -15787,7 +15788,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -15836,7 +15837,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="40"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -15859,7 +15860,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -15890,7 +15891,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -15926,7 +15927,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -15993,7 +15994,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1">
       <c r="A21" s="16" t="s">
         <v>330</v>
       </c>
@@ -16004,7 +16005,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1">
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>211</v>
       </c>
@@ -16019,7 +16020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>212</v>
       </c>
@@ -16036,7 +16037,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>213</v>
       </c>
@@ -16065,16 +16066,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:J18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -16088,7 +16089,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -16109,7 +16110,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -16130,7 +16131,7 @@
         <v>0.98351979013457747</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -16149,8 +16150,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -16171,7 +16172,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -16195,7 +16196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -16224,7 +16225,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -16264,7 +16265,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -16290,24 +16291,24 @@
         <v>826</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
       <c r="B15" s="31">
-        <v>0.12942909999999999</v>
+        <v>0.12971460000000001</v>
       </c>
       <c r="C15" s="31">
-        <v>0.31305650000000002</v>
+        <v>0.31223600000000001</v>
       </c>
       <c r="D15" s="31">
-        <v>0.20899190000000001</v>
+        <v>0.20946770000000001</v>
       </c>
       <c r="E15" s="31">
-        <v>0.23645070000000001</v>
+        <v>0.2365054</v>
       </c>
       <c r="F15" s="32">
-        <v>0.1120718</v>
+        <v>0.1120763</v>
       </c>
       <c r="G15" s="22">
         <f>SUM(B15:F15)</f>
@@ -16320,7 +16321,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -16330,11 +16331,11 @@
       </c>
       <c r="C16" s="13">
         <f>ROUND(2000*C15,0)</f>
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D16" s="13">
         <f>ROUND(2000*D15,0)</f>
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E16" s="13">
         <f>ROUND(2000*E15,0)</f>
@@ -16346,13 +16347,13 @@
       </c>
       <c r="G16" s="3">
         <f>SUM(B16:F16)</f>
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="J16" t="s">
         <v>833</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="26.5" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -16362,11 +16363,11 @@
       </c>
       <c r="C17" s="2">
         <f>ROUND(2200*C15,0)</f>
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D17" s="2">
         <f>ROUND(2200*D15,0)</f>
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="E17" s="2">
         <f>ROUND(2200*E15,0)</f>
@@ -16378,7 +16379,7 @@
       </c>
       <c r="G17" s="3">
         <f>SUM(B17:F17)</f>
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="J17" t="s">
         <v>834</v>
@@ -16396,8 +16397,8 @@
         <v>835</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1"/>
-    <row r="21" spans="1:10" ht="26.5" thickBot="1">
+    <row r="20" spans="1:10" ht="16" thickBot="1"/>
+    <row r="21" spans="1:10" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>496</v>
       </c>
@@ -16412,63 +16413,63 @@
       </c>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:10" ht="26.5" thickBot="1">
+    <row r="22" spans="1:10" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>211</v>
       </c>
       <c r="B22" s="9">
-        <v>0.21759990000000001</v>
+        <v>0.17558260000000001</v>
       </c>
       <c r="C22" s="9">
-        <v>0.38593549999999999</v>
+        <v>0.40122160000000001</v>
       </c>
       <c r="D22" s="9">
-        <v>0.3964646</v>
+        <v>0.42319580000000001</v>
       </c>
       <c r="E22" s="10">
         <f>SUM(B22:D22)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1">
+    <row r="23" spans="1:10" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>212</v>
       </c>
       <c r="B23" s="11">
         <f t="shared" ref="B23:D23" si="2">ROUND(2000*B22,0)</f>
-        <v>435</v>
+        <v>351</v>
       </c>
       <c r="C23" s="11">
         <f t="shared" si="2"/>
-        <v>772</v>
+        <v>802</v>
       </c>
       <c r="D23" s="11">
         <f t="shared" si="2"/>
-        <v>793</v>
+        <v>846</v>
       </c>
       <c r="E23" s="28">
         <f t="shared" ref="E23" si="3">SUM(B23:D23)</f>
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="H23" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="39" thickBot="1">
+    <row r="24" spans="1:10" ht="44" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>501</v>
       </c>
       <c r="B24" s="13">
         <f>ROUND(2200*B22,0)</f>
-        <v>479</v>
+        <v>386</v>
       </c>
       <c r="C24" s="13">
         <f t="shared" ref="C24:D24" si="4">ROUND(2200*C22,0)</f>
-        <v>849</v>
+        <v>883</v>
       </c>
       <c r="D24" s="13">
         <f t="shared" si="4"/>
-        <v>872</v>
+        <v>931</v>
       </c>
       <c r="E24" s="28">
         <f>SUM(B24:D24)</f>

</xml_diff>

<commit_message>
Update ITA quota + zip csv
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60914BC8-24CF-0C42-B06C-AF3F963F8506}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87267931-5CE2-AA4C-A1BB-E2801DA37770}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2420" windowWidth="25600" windowHeight="14480" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -14711,8 +14711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14932,19 +14932,19 @@
         <v>211</v>
       </c>
       <c r="B14" s="31">
-        <v>0.2666</v>
+        <v>0.26589170000000001</v>
       </c>
       <c r="C14" s="31">
-        <v>0.19309999999999999</v>
+        <v>0.1920481</v>
       </c>
       <c r="D14" s="31">
-        <v>0.1991</v>
+        <v>0.19711400000000001</v>
       </c>
       <c r="E14" s="31">
-        <v>0.23119999999999999</v>
+        <v>0.2339965</v>
       </c>
       <c r="F14" s="32">
-        <v>0.11</v>
+        <v>0.1109497</v>
       </c>
       <c r="G14" s="22">
         <f>SUM(B14:F14)</f>
@@ -14957,27 +14957,27 @@
       </c>
       <c r="B15" s="13">
         <f>ROUND(2000*B14,0)</f>
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C15" s="13">
         <f>ROUND(2000*C14,0)</f>
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D15" s="13">
         <f>ROUND(2000*D14,0)</f>
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E15" s="13">
         <f>ROUND(2000*E14,0)</f>
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="F15" s="13">
         <f>ROUND(2000*F14,0)</f>
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="G15" s="3">
         <f>SUM(B15:F15)</f>
-        <v>1999</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" thickBot="1">
@@ -14986,23 +14986,23 @@
       </c>
       <c r="B16" s="2">
         <f>ROUND(2200*B14,0)</f>
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C16" s="2">
         <f>ROUND(2200*C14,0)</f>
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D16" s="2">
         <f>ROUND(2200*D14,0)</f>
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E16" s="2">
         <f>ROUND(2200*E14,0)</f>
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="F16" s="2">
         <f>ROUND(2200*F14,0)</f>
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="G16" s="3">
         <f>SUM(B16:F16)</f>
@@ -15107,13 +15107,13 @@
         <v>211</v>
       </c>
       <c r="B26" s="9">
-        <v>0.3560815</v>
+        <v>0.34949580000000002</v>
       </c>
       <c r="C26" s="9">
-        <v>0.4741165</v>
+        <v>0.48005009999999998</v>
       </c>
       <c r="D26" s="9">
-        <v>0.16980200000000001</v>
+        <v>0.1704541</v>
       </c>
       <c r="E26" s="10">
         <f>SUM(B26:D26)</f>
@@ -15126,15 +15126,15 @@
       </c>
       <c r="B27" s="11">
         <f t="shared" ref="B27:D27" si="2">ROUND(2000*B26,0)</f>
-        <v>712</v>
+        <v>699</v>
       </c>
       <c r="C27" s="11">
         <f t="shared" si="2"/>
-        <v>948</v>
+        <v>960</v>
       </c>
       <c r="D27" s="11">
         <f t="shared" si="2"/>
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E27" s="28">
         <f t="shared" ref="E27" si="3">SUM(B27:D27)</f>
@@ -15147,15 +15147,15 @@
       </c>
       <c r="B28" s="13">
         <f>ROUND(2200*B26,0)</f>
-        <v>783</v>
+        <v>769</v>
       </c>
       <c r="C28" s="13">
         <f t="shared" ref="C28:D28" si="4">ROUND(2200*C26,0)</f>
-        <v>1043</v>
+        <v>1056</v>
       </c>
       <c r="D28" s="13">
         <f t="shared" si="4"/>
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E28" s="28">
         <f>SUM(B28:D28)</f>
@@ -16069,8 +16069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Merge 2 regions for PL
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E143D9DF-79B4-9A49-BDBF-44CC65F6AD7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1295E184-FDEF-5E4F-8A59-837AD47E5A41}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5220" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1931" uniqueCount="939">
   <si>
     <t>Country</t>
   </si>
@@ -1771,9 +1771,6 @@
     <t>South-East</t>
   </si>
   <si>
-    <t>Warman-Masurian, Podlaskie</t>
-  </si>
-  <si>
     <t>Lodz, Masovian, Lubin, Holy Cross</t>
   </si>
   <si>
@@ -2845,9 +2842,6 @@
     <t>Seoul - Busan, 350km</t>
   </si>
   <si>
-    <t>Pomeranian, West Pomeranian, Kuyavian-Pomeranian</t>
-  </si>
-  <si>
     <t>Lubusz, Greater Poland</t>
   </si>
   <si>
@@ -2861,6 +2855,27 @@
   </si>
   <si>
     <t>https://stat.gov.pl/obszary-tematyczne/ludnosc/ludnosc/ludnosc-stan-i-struktura-ludnosci-oraz-ruch-naturalny-w-przekroju-terytorialnym-stan-w-dniu-30-06-2020,6,28.html</t>
+  </si>
+  <si>
+    <r>
+      <t>https://www.destatis.de/EN/Themes/Society-Environment/Population/Current-Population/Tables/population-by-laender.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>http://demo.istat.it/bilmens/index.php?anno=2019&amp;lingua=ita</t>
+  </si>
+  <si>
+    <t>Pomeranian, West Pomeranian, Kuyavian-Pomeranian, Warman-Masurian, Podlaskie</t>
   </si>
 </sst>
 </file>
@@ -2872,7 +2887,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2985,6 +3000,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3029,7 +3057,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3106,6 +3134,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3390,8 +3419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA160"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
@@ -3463,22 +3492,22 @@
         <v>510</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>511</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>509</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>1</v>
@@ -3490,22 +3519,22 @@
         <v>2</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="Y1" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>839</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>840</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="2" spans="1:27">
@@ -3557,7 +3586,7 @@
         <v>441</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>444</v>
@@ -3575,13 +3604,13 @@
         <v>444</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>504</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>444</v>
@@ -3628,7 +3657,7 @@
         <v>444</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>444</v>
@@ -3669,7 +3698,7 @@
         <v>444</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="K5" s="1">
         <v>2</v>
@@ -3686,7 +3715,7 @@
     </row>
     <row r="6" spans="1:27">
       <c r="A6" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>444</v>
@@ -3732,22 +3761,22 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -3802,13 +3831,13 @@
         <v>11</v>
       </c>
       <c r="N8" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="O8" t="s">
         <v>519</v>
       </c>
       <c r="P8" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="Q8" t="s">
         <v>518</v>
@@ -3828,7 +3857,7 @@
     </row>
     <row r="9" spans="1:27">
       <c r="A9" s="1" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B9">
         <v>0.85</v>
@@ -3911,85 +3940,85 @@
     </row>
     <row r="10" spans="1:27">
       <c r="A10" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>844</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>845</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>846</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>847</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>848</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="K10" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>850</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>849</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>865</v>
-      </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>851</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>852</v>
-      </c>
       <c r="N10" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>860</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>862</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>861</v>
-      </c>
       <c r="Q10" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="R10" s="2" t="s">
         <v>854</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>855</v>
       </c>
       <c r="S10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="T10" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="U10" s="2" t="s">
         <v>842</v>
       </c>
-      <c r="U10" s="2" t="s">
-        <v>843</v>
-      </c>
       <c r="V10" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="W10" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="X10" s="2" t="s">
         <v>857</v>
       </c>
-      <c r="X10" s="2" t="s">
+      <c r="Y10" s="2" t="s">
         <v>858</v>
       </c>
-      <c r="Y10" s="2" t="s">
-        <v>859</v>
-      </c>
       <c r="Z10" s="2" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -4030,22 +4059,22 @@
         <v>522</v>
       </c>
       <c r="M11" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="N11" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="O11" t="s">
         <v>523</v>
       </c>
       <c r="P11" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="Q11" t="s">
         <v>521</v>
       </c>
       <c r="R11" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="S11" t="s">
         <v>161</v>
@@ -4057,22 +4086,22 @@
         <v>147</v>
       </c>
       <c r="V11" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="W11" t="s">
+        <v>896</v>
+      </c>
+      <c r="X11" t="s">
         <v>897</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>898</v>
       </c>
-      <c r="Y11" t="s">
-        <v>899</v>
-      </c>
       <c r="Z11" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="AA11" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -4113,10 +4142,10 @@
         <v>526</v>
       </c>
       <c r="M12" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="N12" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="O12" t="s">
         <v>148</v>
@@ -4128,7 +4157,7 @@
         <v>525</v>
       </c>
       <c r="R12" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="S12" t="s">
         <v>162</v>
@@ -4140,7 +4169,7 @@
         <v>148</v>
       </c>
       <c r="V12" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="W12" t="s">
         <v>159</v>
@@ -4149,10 +4178,10 @@
         <v>528</v>
       </c>
       <c r="Y12" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="Z12" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="AA12" t="s">
         <v>333</v>
@@ -4205,7 +4234,7 @@
         <v>169</v>
       </c>
       <c r="P13" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="Q13" t="s">
         <v>172</v>
@@ -4232,7 +4261,7 @@
         <v>169</v>
       </c>
       <c r="Y13" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="Z13" t="s">
         <v>294</v>
@@ -4315,7 +4344,7 @@
         <v>528</v>
       </c>
       <c r="Y14" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="Z14" t="s">
         <v>169</v>
@@ -4461,19 +4490,19 @@
         <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>381</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>381</v>
@@ -4482,13 +4511,13 @@
         <v>49</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="S18" t="s">
         <v>31</v>
@@ -4866,7 +4895,7 @@
         <v>166</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F27" t="s">
         <v>416</v>
@@ -4910,7 +4939,7 @@
         <v>89</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F28" t="s">
         <v>23</v>
@@ -4989,7 +5018,7 @@
         <v>505</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="S30" t="s">
         <v>506</v>
@@ -5240,7 +5269,7 @@
         <v>29</v>
       </c>
       <c r="U37" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="38" spans="1:23">
@@ -5273,7 +5302,7 @@
     </row>
     <row r="40" spans="1:23">
       <c r="A40" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="S40" t="s">
         <v>34</v>
@@ -5281,7 +5310,7 @@
     </row>
     <row r="41" spans="1:23">
       <c r="A41" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="S41" t="s">
         <v>45</v>
@@ -5321,7 +5350,7 @@
         <v>378</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>380</v>
@@ -5333,25 +5362,25 @@
         <v>374</v>
       </c>
       <c r="L43" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="Q43" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="M43" s="1" t="s">
-        <v>928</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>929</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>931</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>930</v>
-      </c>
-      <c r="Q43" s="1" t="s">
+      <c r="R43" s="1" t="s">
         <v>925</v>
-      </c>
-      <c r="R43" s="1" t="s">
-        <v>926</v>
       </c>
       <c r="S43" s="1" t="s">
         <v>37</v>
@@ -5404,7 +5433,7 @@
         <v>373</v>
       </c>
       <c r="Q44" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="S44" t="s">
         <v>74</v>
@@ -5454,22 +5483,22 @@
         <v>538</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="O45" s="1" t="s">
         <v>539</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="Q45" s="1" t="s">
         <v>537</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="S45" s="1" t="s">
         <v>38</v>
@@ -5520,22 +5549,22 @@
         <v>542</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="O46" s="1" t="s">
         <v>543</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="Q46" s="1" t="s">
         <v>541</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="S46" s="1" t="s">
         <v>41</v>
@@ -5582,14 +5611,14 @@
         <v>44</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>43</v>
@@ -5598,28 +5627,28 @@
         <v>498</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="M48" s="1" t="s">
         <v>44</v>
       </c>
       <c r="N48" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="O48" s="1" t="s">
         <v>920</v>
       </c>
-      <c r="O48" s="1" t="s">
+      <c r="P48" s="1" t="s">
         <v>921</v>
       </c>
-      <c r="P48" s="1" t="s">
+      <c r="Q48" s="1" t="s">
         <v>922</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>923</v>
       </c>
       <c r="R48" s="1" t="s">
         <v>44</v>
@@ -5826,7 +5855,7 @@
     </row>
     <row r="51" spans="1:27">
       <c r="A51" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="B51">
         <v>61</v>
@@ -6029,7 +6058,7 @@
         <v>48</v>
       </c>
       <c r="I53" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
@@ -6066,7 +6095,7 @@
         <v>367</v>
       </c>
       <c r="H54" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="I54" t="s">
         <v>51</v>
@@ -6128,7 +6157,7 @@
     </row>
     <row r="55" spans="1:27">
       <c r="A55" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B55">
         <v>10</v>
@@ -6193,7 +6222,7 @@
     </row>
     <row r="56" spans="1:27">
       <c r="A56" s="1" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B56">
         <v>887</v>
@@ -6276,7 +6305,7 @@
     </row>
     <row r="57" spans="1:27">
       <c r="A57" s="1" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B57" s="27">
         <f t="shared" ref="B57:P57" si="5">B56/B61</f>
@@ -6469,7 +6498,7 @@
     </row>
     <row r="59" spans="1:27">
       <c r="A59" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B59" s="3">
         <v>796.529</v>
@@ -6635,7 +6664,7 @@
     </row>
     <row r="61" spans="1:27">
       <c r="A61" s="1" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B61" s="3">
         <v>84</v>
@@ -7125,7 +7154,7 @@
         <v>333</v>
       </c>
       <c r="M66" s="22" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="N66" s="22" t="s">
         <v>22</v>
@@ -7140,7 +7169,7 @@
         <v>336</v>
       </c>
       <c r="R66" s="22" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="S66" s="22" t="s">
         <v>166</v>
@@ -7152,7 +7181,7 @@
         <v>333</v>
       </c>
       <c r="V66" s="22" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="W66" s="22" t="s">
         <v>21</v>
@@ -7172,169 +7201,169 @@
     </row>
     <row r="67" spans="1:27">
       <c r="A67" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="F67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="G67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="H67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="I67" s="22" t="s">
+        <v>699</v>
+      </c>
+      <c r="J67" s="22" t="s">
+        <v>699</v>
+      </c>
+      <c r="K67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="L67" s="22" t="s">
+        <v>699</v>
+      </c>
+      <c r="M67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="N67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="O67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="P67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="Q67" s="22" t="s">
+        <v>699</v>
+      </c>
+      <c r="R67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="S67" s="22" t="s">
         <v>697</v>
       </c>
-      <c r="B67" s="22" t="s">
+      <c r="T67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="U67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="V67" s="22" t="s">
         <v>699</v>
       </c>
-      <c r="C67" s="22" t="s">
+      <c r="W67" s="22" t="s">
         <v>699</v>
       </c>
-      <c r="D67" s="22" t="s">
+      <c r="X67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="Z67" s="22" t="s">
         <v>699</v>
       </c>
-      <c r="E67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="F67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="G67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="H67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="I67" s="22" t="s">
-        <v>700</v>
-      </c>
-      <c r="J67" s="22" t="s">
-        <v>700</v>
-      </c>
-      <c r="K67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="L67" s="22" t="s">
-        <v>700</v>
-      </c>
-      <c r="M67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="N67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="O67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="P67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="Q67" s="22" t="s">
-        <v>700</v>
-      </c>
-      <c r="R67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="S67" s="22" t="s">
+      <c r="AA67" t="s">
         <v>698</v>
-      </c>
-      <c r="T67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="U67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="V67" s="22" t="s">
-        <v>700</v>
-      </c>
-      <c r="W67" s="22" t="s">
-        <v>700</v>
-      </c>
-      <c r="X67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="Y67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="Z67" s="22" t="s">
-        <v>700</v>
-      </c>
-      <c r="AA67" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="68" spans="1:27">
       <c r="A68" s="2" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B68" s="22" t="s">
+        <v>700</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>700</v>
+      </c>
+      <c r="D68" s="22" t="s">
         <v>701</v>
       </c>
-      <c r="C68" s="22" t="s">
-        <v>701</v>
-      </c>
-      <c r="D68" s="22" t="s">
+      <c r="E68" s="22" t="s">
+        <v>700</v>
+      </c>
+      <c r="F68" s="22" t="s">
+        <v>700</v>
+      </c>
+      <c r="G68" s="22" t="s">
         <v>702</v>
       </c>
-      <c r="E68" s="22" t="s">
-        <v>701</v>
-      </c>
-      <c r="F68" s="22" t="s">
-        <v>701</v>
-      </c>
-      <c r="G68" s="22" t="s">
-        <v>703</v>
-      </c>
       <c r="H68" s="22" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="I68" s="22"/>
       <c r="J68" s="22"/>
       <c r="K68" s="22" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="S68" s="22" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="T68" s="22" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="U68" s="22" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="69" spans="1:27">
       <c r="A69" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B69" s="22" t="s">
+        <v>690</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>690</v>
+      </c>
+      <c r="D69" s="22" t="s">
         <v>691</v>
       </c>
-      <c r="C69" s="22" t="s">
+      <c r="E69" s="22" t="s">
+        <v>690</v>
+      </c>
+      <c r="F69" s="22" t="s">
+        <v>690</v>
+      </c>
+      <c r="G69" s="22" t="s">
+        <v>705</v>
+      </c>
+      <c r="H69" s="22" t="s">
         <v>691</v>
       </c>
-      <c r="D69" s="22" t="s">
-        <v>692</v>
-      </c>
-      <c r="E69" s="22" t="s">
-        <v>691</v>
-      </c>
-      <c r="F69" s="22" t="s">
-        <v>691</v>
-      </c>
-      <c r="G69" s="22" t="s">
+      <c r="I69" s="22" t="s">
+        <v>693</v>
+      </c>
+      <c r="J69" s="22" t="s">
         <v>706</v>
       </c>
-      <c r="H69" s="22" t="s">
-        <v>692</v>
-      </c>
-      <c r="I69" s="22" t="s">
-        <v>694</v>
-      </c>
-      <c r="J69" s="22" t="s">
-        <v>707</v>
-      </c>
       <c r="K69" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="S69" s="22" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="T69" s="22" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="U69" s="22" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="70" spans="1:27">
@@ -7345,22 +7374,22 @@
         <v>345</v>
       </c>
       <c r="C70" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D70" s="22" t="s">
         <v>348</v>
       </c>
       <c r="E70" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="F70" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="G70" s="22" t="s">
         <v>346</v>
       </c>
       <c r="H70" s="22" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="I70" s="22" t="s">
         <v>344</v>
@@ -7369,25 +7398,25 @@
         <v>347</v>
       </c>
       <c r="K70" s="22" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="L70" t="s">
+        <v>874</v>
+      </c>
+      <c r="M70" s="22" t="s">
+        <v>879</v>
+      </c>
+      <c r="N70" s="22" t="s">
         <v>875</v>
       </c>
-      <c r="M70" s="22" t="s">
+      <c r="O70" s="22" t="s">
         <v>880</v>
       </c>
-      <c r="N70" s="22" t="s">
+      <c r="P70" t="s">
         <v>876</v>
       </c>
-      <c r="O70" s="22" t="s">
-        <v>881</v>
-      </c>
-      <c r="P70" t="s">
+      <c r="Q70" t="s">
         <v>877</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>878</v>
       </c>
       <c r="S70" s="22" t="s">
         <v>349</v>
@@ -7399,21 +7428,21 @@
         <v>492</v>
       </c>
       <c r="W70" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="X70" t="s">
+        <v>881</v>
+      </c>
+      <c r="Y70" t="s">
+        <v>878</v>
+      </c>
+      <c r="Z70" t="s">
         <v>882</v>
-      </c>
-      <c r="Y70" t="s">
-        <v>879</v>
-      </c>
-      <c r="Z70" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="71" spans="1:27">
       <c r="A71" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B71">
         <v>0.37862000000000001</v>
@@ -7487,7 +7516,7 @@
     </row>
     <row r="72" spans="1:27">
       <c r="A72" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B72">
         <v>1.5</v>
@@ -7570,7 +7599,7 @@
     </row>
     <row r="73" spans="1:27">
       <c r="A73" s="2" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B73">
         <v>1.804</v>
@@ -7623,7 +7652,7 @@
     </row>
     <row r="74" spans="1:27">
       <c r="A74" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B74">
         <v>0.36799999999999999</v>
@@ -7676,7 +7705,7 @@
     </row>
     <row r="75" spans="1:27">
       <c r="A75" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B75">
         <v>6.6000000000000003E-2</v>
@@ -7705,7 +7734,7 @@
     </row>
     <row r="76" spans="1:27">
       <c r="A76" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B76">
         <v>0.90300000000000002</v>
@@ -7734,7 +7763,7 @@
     </row>
     <row r="77" spans="1:27">
       <c r="A77" s="2" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D77">
         <f>240.49/D9</f>
@@ -7816,7 +7845,7 @@
         <v>435</v>
       </c>
       <c r="H79" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="I79" t="s">
         <v>431</v>
@@ -7882,7 +7911,7 @@
         <v>372</v>
       </c>
       <c r="H82" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I82" t="s">
         <v>379</v>
@@ -7972,7 +8001,7 @@
         <v>462</v>
       </c>
       <c r="E88" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F88" t="s">
         <v>141</v>
@@ -8013,7 +8042,7 @@
         <v>463</v>
       </c>
       <c r="E89" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F89" t="s">
         <v>142</v>
@@ -8054,7 +8083,7 @@
         <v>464</v>
       </c>
       <c r="E90" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F90" t="s">
         <v>143</v>
@@ -8095,7 +8124,7 @@
         <v>465</v>
       </c>
       <c r="E91" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F91" t="s">
         <v>144</v>
@@ -8136,7 +8165,7 @@
         <v>466</v>
       </c>
       <c r="E92" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F92" t="s">
         <v>145</v>
@@ -8171,7 +8200,7 @@
         <v>467</v>
       </c>
       <c r="E93" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F93" t="s">
         <v>146</v>
@@ -8197,7 +8226,7 @@
         <v>446</v>
       </c>
       <c r="E94" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="H94" t="s">
         <v>533</v>
@@ -8214,7 +8243,7 @@
         <v>116</v>
       </c>
       <c r="E95" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="H95" t="s">
         <v>534</v>
@@ -8228,7 +8257,7 @@
         <v>117</v>
       </c>
       <c r="E96" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I96" t="s">
         <v>140</v>
@@ -8239,7 +8268,7 @@
         <v>118</v>
       </c>
       <c r="E97" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I97" t="s">
         <v>470</v>
@@ -8274,7 +8303,7 @@
     </row>
     <row r="101" spans="1:23">
       <c r="A101" s="6" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B101" t="s">
         <v>370</v>
@@ -8304,7 +8333,7 @@
         <v>370</v>
       </c>
       <c r="N101" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="S101" t="s">
         <v>192</v>
@@ -8321,134 +8350,134 @@
         <v>185</v>
       </c>
       <c r="B102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="F102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="G102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="I102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="J102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="L102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="Q102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="S102" t="s">
         <v>186</v>
       </c>
       <c r="T102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="U102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="W102" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="103" spans="1:23">
       <c r="A103" s="4" t="s">
+        <v>805</v>
+      </c>
+      <c r="B103" t="s">
         <v>806</v>
       </c>
-      <c r="B103" t="s">
-        <v>807</v>
-      </c>
       <c r="C103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="G103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="H103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="J103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="K103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="L103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="Q103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="S103" t="s">
         <v>188</v>
       </c>
       <c r="T103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="U103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="W103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="104" spans="1:23">
       <c r="A104" s="4" t="s">
+        <v>807</v>
+      </c>
+      <c r="B104" t="s">
         <v>808</v>
       </c>
-      <c r="B104" t="s">
-        <v>809</v>
-      </c>
       <c r="C104" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D104" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E104" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F104" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="T104" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="U104" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="W104" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="105" spans="1:23">
@@ -8456,45 +8485,45 @@
         <v>190</v>
       </c>
       <c r="B105" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C105" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E105" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F105" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="L105" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="S105" t="s">
         <v>191</v>
       </c>
       <c r="T105" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="U105" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="W105" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="106" spans="1:23">
       <c r="A106" s="4" t="s">
+        <v>810</v>
+      </c>
+      <c r="D106" t="s">
         <v>811</v>
       </c>
-      <c r="D106" t="s">
+      <c r="H106" t="s">
+        <v>831</v>
+      </c>
+      <c r="K106" t="s">
         <v>812</v>
-      </c>
-      <c r="H106" t="s">
-        <v>832</v>
-      </c>
-      <c r="K106" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="107" spans="1:23">
@@ -8590,28 +8619,28 @@
         <v>324</v>
       </c>
       <c r="B115" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C115" t="s">
         <v>503</v>
       </c>
       <c r="D115" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E115" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F115" t="s">
         <v>516</v>
       </c>
       <c r="G115" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I115" t="s">
         <v>502</v>
       </c>
       <c r="J115" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="K115" s="33" t="s">
         <v>517</v>
@@ -8631,19 +8660,19 @@
         <v>472</v>
       </c>
       <c r="C116" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D116" t="s">
         <v>514</v>
       </c>
       <c r="E116" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G116" t="s">
         <v>479</v>
       </c>
       <c r="H116" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I116" t="s">
         <v>471</v>
@@ -8729,7 +8758,7 @@
     </row>
     <row r="120" spans="1:24">
       <c r="A120" s="6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B120">
         <v>6500</v>
@@ -8792,7 +8821,7 @@
     </row>
     <row r="124" spans="1:24">
       <c r="A124" s="6" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C124" t="s">
         <v>444</v>
@@ -8824,7 +8853,7 @@
     </row>
     <row r="125" spans="1:24">
       <c r="A125" s="6" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C125" t="s">
         <v>444</v>
@@ -8835,7 +8864,7 @@
     </row>
     <row r="126" spans="1:24">
       <c r="A126" s="6" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="S126" t="s">
         <v>444</v>
@@ -8849,223 +8878,223 @@
     </row>
     <row r="127" spans="1:24">
       <c r="A127" s="6" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B127" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C127" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D127" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E127" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F127" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G127" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H127" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I127" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J127" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="K127" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="128" spans="1:24">
       <c r="A128" s="6" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="J128" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="K128" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="129" spans="1:11">
       <c r="A129" s="6" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B129" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C129" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D129" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E129" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F129" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G129" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H129" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I129" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J129" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="K129" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="130" spans="1:11">
       <c r="A130" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D130" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G130" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I130" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J130" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="K130" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="131" spans="1:11">
       <c r="A131" s="6" t="s">
+        <v>646</v>
+      </c>
+      <c r="B131" t="s">
         <v>647</v>
       </c>
-      <c r="B131" t="s">
-        <v>648</v>
-      </c>
       <c r="D131" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F131" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G131" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H131" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I131" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J131" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="K131" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="132" spans="1:11">
       <c r="A132" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="H132" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I132" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="133" spans="1:11">
       <c r="A133" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B133" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D133" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G133" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H133" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I133" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J133" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="K133" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="134" spans="1:11">
       <c r="A134" s="6" t="s">
+        <v>650</v>
+      </c>
+      <c r="I134" t="s">
         <v>651</v>
       </c>
-      <c r="I134" t="s">
-        <v>652</v>
-      </c>
       <c r="J134" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="K134" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="135" spans="1:11">
       <c r="A135" s="6" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B135" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C135" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D135" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E135" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F135" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G135" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H135" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I135" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J135" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="K135" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="136" spans="1:11">
       <c r="A136" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B136" t="s">
         <v>293</v>
@@ -9092,15 +9121,15 @@
         <v>293</v>
       </c>
       <c r="J136" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="K136" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="137" spans="1:11">
       <c r="A137" s="6" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B137" t="s">
         <v>293</v>
@@ -9129,297 +9158,297 @@
     </row>
     <row r="138" spans="1:11">
       <c r="A138" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="I138" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J138" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="139" spans="1:11">
       <c r="A139" s="6" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I139" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="140" spans="1:11">
       <c r="A140" s="6" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I140" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J140" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="141" spans="1:11">
       <c r="A141" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="142" spans="1:11">
       <c r="A142" s="6" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I142" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="143" spans="1:11">
       <c r="A143" s="6" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="H143" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="144" spans="1:11">
       <c r="A144" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="145" spans="1:11">
       <c r="A145" s="6" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B145" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D145" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H145" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I145" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="146" spans="1:11">
       <c r="A146" s="6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H146" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I146" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J146" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="K146" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="147" spans="1:11">
       <c r="A147" s="6" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="H147" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I147" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J147" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="K147" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="148" spans="1:11">
       <c r="A148" s="6" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B148" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C148" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D148" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E148" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F148" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G148" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H148" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I148" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J148" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="K148" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="149" spans="1:11">
       <c r="A149" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I149" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J149" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="K149" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="150" spans="1:11">
       <c r="A150" s="6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B150" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D150" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G150" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H150" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="151" spans="1:11">
       <c r="A151" s="6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="K151" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="152" spans="1:11">
       <c r="A152" s="6" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D152" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G152" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H152" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I152" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J152" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="K152" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="153" spans="1:11">
       <c r="A153" s="6" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I153" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="154" spans="1:11">
       <c r="A154" s="6" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G154" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H154" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I154" t="s">
         <v>293</v>
       </c>
       <c r="J154" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="K154" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="155" spans="1:11">
       <c r="A155" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="156" spans="1:11">
       <c r="A156" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="157" spans="1:11">
       <c r="A157" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="158" spans="1:11">
       <c r="A158" s="6" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B158" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D158" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G158" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H158" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I158" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J158" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="159" spans="1:11">
       <c r="A159" s="6" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H159" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="160" spans="1:11">
       <c r="A160" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="G160" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="G160" s="1" t="s">
-        <v>783</v>
-      </c>
       <c r="H160" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I160" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
   </sheetData>
@@ -9633,22 +9662,22 @@
         <v>214</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>248</v>
       </c>
       <c r="G13" s="40" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" thickBot="1">
@@ -9675,10 +9704,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="J14" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -9713,7 +9742,7 @@
         <v>248</v>
       </c>
       <c r="J15" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" thickBot="1">
@@ -9745,10 +9774,10 @@
         <v>2200</v>
       </c>
       <c r="I16" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J16" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -9760,7 +9789,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
       <c r="J17" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" thickBot="1"/>
@@ -9769,10 +9798,10 @@
         <v>496</v>
       </c>
       <c r="B20" s="15" t="s">
+        <v>716</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>717</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>718</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
@@ -10084,22 +10113,22 @@
         <v>214</v>
       </c>
       <c r="B14" s="23" t="s">
+        <v>582</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="D14" s="23" t="s">
         <v>584</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="E14" s="23" t="s">
         <v>585</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="F14" s="24" t="s">
         <v>586</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="G14" s="40" t="s">
         <v>587</v>
-      </c>
-      <c r="G14" s="40" t="s">
-        <v>588</v>
       </c>
       <c r="H14" s="36"/>
     </row>
@@ -10163,7 +10192,7 @@
         <v>2000</v>
       </c>
       <c r="K16" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" thickBot="1">
@@ -10199,7 +10228,7 @@
         <v>2200</v>
       </c>
       <c r="K17" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -10232,33 +10261,33 @@
       <c r="G20" s="39"/>
       <c r="H20" s="36"/>
       <c r="K20" t="s">
+        <v>635</v>
+      </c>
+      <c r="L20" t="s">
         <v>636</v>
-      </c>
-      <c r="L20" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B21" s="23" t="s">
+        <v>637</v>
+      </c>
+      <c r="C21" s="23" t="s">
         <v>638</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="D21" s="23" t="s">
         <v>639</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="E21" s="23" t="s">
         <v>640</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="F21" s="24" t="s">
         <v>641</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="G21" s="40" t="s">
         <v>642</v>
-      </c>
-      <c r="G21" s="40" t="s">
-        <v>643</v>
       </c>
       <c r="H21" s="36"/>
     </row>
@@ -10615,28 +10644,28 @@
         <v>214</v>
       </c>
       <c r="B14" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>721</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="D14" s="23" t="s">
         <v>722</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="E14" s="23" t="s">
         <v>723</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="F14" s="24" t="s">
         <v>724</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="G14" s="40" t="s">
+        <v>622</v>
+      </c>
+      <c r="J14" t="s">
         <v>725</v>
       </c>
-      <c r="G14" s="40" t="s">
-        <v>623</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>726</v>
-      </c>
-      <c r="K14" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" thickBot="1">
@@ -10663,10 +10692,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
+        <v>727</v>
+      </c>
+      <c r="K15" t="s">
         <v>728</v>
-      </c>
-      <c r="K15" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -10698,10 +10727,10 @@
         <v>2001</v>
       </c>
       <c r="J16" t="s">
+        <v>729</v>
+      </c>
+      <c r="K16" t="s">
         <v>730</v>
-      </c>
-      <c r="K16" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -10733,10 +10762,10 @@
         <v>2200</v>
       </c>
       <c r="J17" t="s">
+        <v>731</v>
+      </c>
+      <c r="K17" t="s">
         <v>732</v>
-      </c>
-      <c r="K17" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -10748,15 +10777,15 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
       <c r="J18" t="s">
+        <v>733</v>
+      </c>
+      <c r="K18" t="s">
         <v>734</v>
-      </c>
-      <c r="K18" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="K19" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16" thickBot="1"/>
@@ -10789,10 +10818,10 @@
       </c>
       <c r="E24" s="10"/>
       <c r="F24" t="s">
+        <v>778</v>
+      </c>
+      <c r="G24" t="s">
         <v>779</v>
-      </c>
-      <c r="G24" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="16" thickBot="1">
@@ -10813,10 +10842,10 @@
       </c>
       <c r="E25" s="28"/>
       <c r="F25" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="G25" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="44" thickBot="1">
@@ -11048,13 +11077,13 @@
         <v>214</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C14" s="23" t="s">
         <v>249</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>567</v>
@@ -11063,7 +11092,7 @@
         <v>573</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="16" thickBot="1">
@@ -11090,10 +11119,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
+        <v>738</v>
+      </c>
+      <c r="K15" t="s">
         <v>739</v>
-      </c>
-      <c r="K15" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -11125,10 +11154,10 @@
         <v>2000</v>
       </c>
       <c r="J16" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K16" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -11160,10 +11189,10 @@
         <v>2200</v>
       </c>
       <c r="J17" t="s">
+        <v>741</v>
+      </c>
+      <c r="K17" t="s">
         <v>742</v>
-      </c>
-      <c r="K17" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -11175,10 +11204,10 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
       <c r="J18" t="s">
+        <v>743</v>
+      </c>
+      <c r="K18" t="s">
         <v>744</v>
-      </c>
-      <c r="K18" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16" thickBot="1"/>
@@ -11211,10 +11240,10 @@
       </c>
       <c r="E23" s="10"/>
       <c r="F23" t="s">
+        <v>783</v>
+      </c>
+      <c r="G23" t="s">
         <v>784</v>
-      </c>
-      <c r="G23" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="16" thickBot="1">
@@ -11235,13 +11264,13 @@
       </c>
       <c r="E24" s="28"/>
       <c r="F24" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G24" t="s">
+        <v>785</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>786</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="44" thickBot="1">
@@ -11472,22 +11501,22 @@
         <v>214</v>
       </c>
       <c r="B13" s="23" t="s">
+        <v>745</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>746</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="D13" s="23" t="s">
         <v>747</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="E13" s="23" t="s">
         <v>748</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="F13" s="24" t="s">
         <v>749</v>
       </c>
-      <c r="F13" s="24" t="s">
-        <v>750</v>
-      </c>
       <c r="G13" s="40" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16" thickBot="1">
@@ -11514,10 +11543,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
+        <v>750</v>
+      </c>
+      <c r="J14" t="s">
         <v>751</v>
-      </c>
-      <c r="J14" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -11549,10 +11578,10 @@
         <v>2000</v>
       </c>
       <c r="I15" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J15" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" thickBot="1">
@@ -11619,10 +11648,10 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
+        <v>753</v>
+      </c>
+      <c r="G20" t="s">
         <v>754</v>
-      </c>
-      <c r="G20" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="16" thickBot="1">
@@ -11659,13 +11688,13 @@
         <v>2200</v>
       </c>
       <c r="G22" t="s">
+        <v>756</v>
+      </c>
+      <c r="H22" t="s">
         <v>757</v>
       </c>
-      <c r="H22" t="s">
-        <v>758</v>
-      </c>
       <c r="I22" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -11673,10 +11702,10 @@
         <v>231</v>
       </c>
       <c r="G23" s="41" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="H23" s="41" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -11684,10 +11713,10 @@
     </row>
     <row r="24" spans="1:9">
       <c r="G24" s="41" t="s">
+        <v>759</v>
+      </c>
+      <c r="H24" s="41" t="s">
         <v>760</v>
-      </c>
-      <c r="H24" s="41" t="s">
-        <v>761</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -11695,10 +11724,10 @@
     </row>
     <row r="25" spans="1:9">
       <c r="G25" s="41" t="s">
+        <v>761</v>
+      </c>
+      <c r="H25" s="41" t="s">
         <v>762</v>
-      </c>
-      <c r="H25" s="41" t="s">
-        <v>763</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -11706,10 +11735,10 @@
     </row>
     <row r="26" spans="1:9">
       <c r="G26" t="s">
+        <v>763</v>
+      </c>
+      <c r="H26" t="s">
         <v>764</v>
-      </c>
-      <c r="H26" t="s">
-        <v>765</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -11717,7 +11746,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="G27" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -11725,7 +11754,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="G28" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -11733,10 +11762,10 @@
     </row>
     <row r="29" spans="1:9">
       <c r="G29" t="s">
+        <v>767</v>
+      </c>
+      <c r="H29" t="s">
         <v>768</v>
-      </c>
-      <c r="H29" t="s">
-        <v>769</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -11744,10 +11773,10 @@
     </row>
     <row r="30" spans="1:9">
       <c r="G30" t="s">
+        <v>769</v>
+      </c>
+      <c r="H30" t="s">
         <v>770</v>
-      </c>
-      <c r="H30" t="s">
-        <v>771</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -11755,10 +11784,10 @@
     </row>
     <row r="31" spans="1:9">
       <c r="G31" t="s">
+        <v>771</v>
+      </c>
+      <c r="H31" t="s">
         <v>772</v>
-      </c>
-      <c r="H31" t="s">
-        <v>773</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -12389,7 +12418,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -12892,8 +12921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D28" sqref="A24:D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13379,7 +13408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -14407,8 +14436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14744,6 +14773,14 @@
         <v>565</v>
       </c>
     </row>
+    <row r="19" spans="1:11" ht="16">
+      <c r="J19" t="s">
+        <v>934</v>
+      </c>
+      <c r="K19" s="46" t="s">
+        <v>936</v>
+      </c>
+    </row>
     <row r="20" spans="1:11" ht="16" thickBot="1">
       <c r="A20" s="16" t="s">
         <v>330</v>
@@ -14752,10 +14789,10 @@
         <v>252</v>
       </c>
       <c r="C20" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D20" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" thickBot="1">
@@ -14797,10 +14834,10 @@
         <v>1999</v>
       </c>
       <c r="F22" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="G22" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" thickBot="1">
@@ -14824,10 +14861,10 @@
         <v>2200</v>
       </c>
       <c r="F23" t="s">
+        <v>775</v>
+      </c>
+      <c r="G23" s="18" t="s">
         <v>776</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -14847,8 +14884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -15145,10 +15182,10 @@
         <v>2201</v>
       </c>
       <c r="J16" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="12" t="s">
         <v>231</v>
       </c>
@@ -15156,8 +15193,11 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
-    </row>
-    <row r="19" spans="1:8" ht="16" thickBot="1">
+      <c r="J17" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>330</v>
       </c>
@@ -15168,7 +15208,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30" thickBot="1">
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>211</v>
       </c>
@@ -15183,7 +15223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="16" thickBot="1">
+    <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>212</v>
       </c>
@@ -15200,7 +15240,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" thickBot="1">
+    <row r="22" spans="1:10" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>213</v>
       </c>
@@ -15217,28 +15257,28 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:10">
       <c r="A23" s="12" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="16" thickBot="1"/>
-    <row r="25" spans="1:8" ht="30" thickBot="1">
+    <row r="24" spans="1:10" ht="16" thickBot="1"/>
+    <row r="25" spans="1:10" ht="30" thickBot="1">
       <c r="A25" s="12" t="s">
         <v>496</v>
       </c>
       <c r="B25" s="15" t="s">
+        <v>594</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>595</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>596</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>252</v>
       </c>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:8" ht="30" thickBot="1">
+    <row r="26" spans="1:10" ht="30" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>211</v>
       </c>
@@ -15256,7 +15296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="16" thickBot="1">
+    <row r="27" spans="1:10" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>212</v>
       </c>
@@ -15277,7 +15317,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="44" thickBot="1">
+    <row r="28" spans="1:10" ht="44" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>501</v>
       </c>
@@ -15298,10 +15338,10 @@
         <v>2200</v>
       </c>
       <c r="H28" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="12" t="s">
         <v>231</v>
       </c>
@@ -15310,7 +15350,7 @@
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="H29" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
   </sheetData>
@@ -15322,8 +15362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -15523,28 +15563,28 @@
         <v>214</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>566</v>
+        <v>616</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>570</v>
-      </c>
-      <c r="E13" s="23" t="s">
         <v>571</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="E13" s="24" t="s">
         <v>572</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>573</v>
       </c>
       <c r="G13" s="40" t="s">
         <v>573</v>
       </c>
       <c r="L13" t="s">
-        <v>566</v>
+        <v>616</v>
       </c>
       <c r="M13" t="s">
-        <v>932</v>
+        <v>938</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" thickBot="1">
@@ -15552,32 +15592,30 @@
         <v>211</v>
       </c>
       <c r="B14">
-        <v>0.1592840758162091</v>
+        <v>0.22699743780161807</v>
       </c>
       <c r="C14">
-        <v>6.771336198540899E-2</v>
+        <v>0.11760227498582748</v>
       </c>
       <c r="D14">
-        <v>0.11760227498582748</v>
+        <v>0.21868217573091719</v>
       </c>
       <c r="E14">
-        <v>0.21868217573091719</v>
+        <v>0.14443883329201232</v>
       </c>
       <c r="F14">
-        <v>0.14443883329201232</v>
+        <v>0.2922792781896249</v>
       </c>
       <c r="G14">
-        <v>0.2922792781896249</v>
-      </c>
-      <c r="H14" s="22">
-        <f>SUM(B14:G14)</f>
+        <f>SUM(B14:F14)</f>
         <v>1</v>
       </c>
+      <c r="H14" s="22"/>
       <c r="L14" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="M14" t="s">
-        <v>574</v>
+        <v>931</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="16" thickBot="1">
@@ -15586,37 +15624,34 @@
       </c>
       <c r="B15" s="13">
         <f t="shared" ref="B15:G15" si="2">ROUND(2000*B14,0)</f>
-        <v>319</v>
+        <v>454</v>
       </c>
       <c r="C15" s="13">
         <f t="shared" si="2"/>
-        <v>135</v>
+        <v>235</v>
       </c>
       <c r="D15" s="13">
         <f t="shared" si="2"/>
-        <v>235</v>
+        <v>437</v>
       </c>
       <c r="E15" s="13">
         <f t="shared" si="2"/>
-        <v>437</v>
+        <v>289</v>
       </c>
       <c r="F15" s="13">
         <f t="shared" si="2"/>
-        <v>289</v>
+        <v>585</v>
       </c>
       <c r="G15" s="13">
-        <f t="shared" si="2"/>
-        <v>585</v>
-      </c>
-      <c r="H15" s="3">
-        <f>SUM(B15:G15)</f>
+        <f>SUM(B15:F15)</f>
         <v>2000</v>
       </c>
+      <c r="H15" s="3"/>
       <c r="L15" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="M15" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" thickBot="1">
@@ -15625,37 +15660,34 @@
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16:G16" si="3">ROUND(2200*B14,0)</f>
-        <v>350</v>
+        <v>499</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="3"/>
-        <v>149</v>
+        <v>259</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="3"/>
-        <v>259</v>
+        <v>481</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="3"/>
-        <v>481</v>
+        <v>318</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="3"/>
-        <v>318</v>
+        <v>643</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="3"/>
-        <v>643</v>
-      </c>
-      <c r="H16" s="3">
-        <f>SUM(B16:G16)</f>
+        <f>SUM(B16:F16)</f>
         <v>2200</v>
       </c>
+      <c r="H16" s="3"/>
       <c r="L16" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="M16" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -15667,28 +15699,21 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
       <c r="L17" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="M17" t="s">
-        <v>935</v>
+        <v>574</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="L18" t="s">
-        <v>573</v>
+        <v>934</v>
       </c>
       <c r="M18" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="16" thickBot="1">
-      <c r="L19" t="s">
-        <v>936</v>
-      </c>
-      <c r="M19" t="s">
-        <v>937</v>
-      </c>
-    </row>
+        <v>935</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="16" thickBot="1"/>
     <row r="20" spans="1:13" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>496</v>
@@ -16059,22 +16084,22 @@
         <v>214</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>248</v>
       </c>
       <c r="E14" s="23" t="s">
+        <v>616</v>
+      </c>
+      <c r="F14" s="24" t="s">
         <v>617</v>
       </c>
-      <c r="F14" s="24" t="s">
-        <v>618</v>
-      </c>
       <c r="G14" s="40" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" thickBot="1">
@@ -16102,10 +16127,10 @@
       </c>
       <c r="H15" s="22"/>
       <c r="J15" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="K15" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -16138,10 +16163,10 @@
       </c>
       <c r="H16" s="3"/>
       <c r="J16" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="K16" t="s">
         <v>615</v>
-      </c>
-      <c r="K16" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -16177,7 +16202,7 @@
         <v>248</v>
       </c>
       <c r="K17" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -16189,10 +16214,10 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
       <c r="J18" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="K18" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -16200,15 +16225,15 @@
         <v>566</v>
       </c>
       <c r="K19" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="J20" t="s">
+        <v>623</v>
+      </c>
+      <c r="K20" t="s">
         <v>624</v>
-      </c>
-      <c r="K20" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16" thickBot="1">
@@ -16487,25 +16512,25 @@
         <v>214</v>
       </c>
       <c r="B14" s="23" t="s">
+        <v>823</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>819</v>
+      </c>
+      <c r="D14" s="23" t="s">
         <v>824</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="E14" s="23" t="s">
         <v>820</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="F14" s="24" t="s">
         <v>825</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="J14" t="s">
+        <v>826</v>
+      </c>
+      <c r="K14" t="s">
         <v>821</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>826</v>
-      </c>
-      <c r="J14" t="s">
-        <v>827</v>
-      </c>
-      <c r="K14" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" thickBot="1">
@@ -16532,10 +16557,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="K15" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -16567,7 +16592,7 @@
         <v>1999</v>
       </c>
       <c r="J16" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" thickBot="1">
@@ -16599,7 +16624,7 @@
         <v>2200</v>
       </c>
       <c r="J17" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -16611,7 +16636,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
       <c r="J18" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="16" thickBot="1"/>
@@ -16620,13 +16645,13 @@
         <v>496</v>
       </c>
       <c r="B21" s="15" t="s">
+        <v>592</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>593</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>594</v>
-      </c>
       <c r="D21" s="15" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E21" s="15"/>
     </row>
@@ -16669,7 +16694,7 @@
         <v>1999</v>
       </c>
       <c r="H23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="44" thickBot="1">
@@ -16693,7 +16718,7 @@
         <v>2200</v>
       </c>
       <c r="H24" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="25" spans="1:10">

</xml_diff>

<commit_message>
Appendix rural and region
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9656BDD-7C44-EF40-9621-E2A252C34E44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F5BDD6-C02A-6748-A3A6-A61554073BDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="38400" windowHeight="14480" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5220" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -1834,9 +1834,6 @@
     <t>Cities</t>
   </si>
   <si>
-    <t>Small Cities</t>
-  </si>
-  <si>
     <t>https://www.istat.it/it/archivio/156224</t>
   </si>
   <si>
@@ -2882,6 +2879,9 @@
   </si>
   <si>
     <t>Scotland, Northern Ireland</t>
+  </si>
+  <si>
+    <t>Towns and Suburbs</t>
   </si>
 </sst>
 </file>
@@ -3498,22 +3498,22 @@
         <v>510</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>511</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>509</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>1</v>
@@ -3525,22 +3525,22 @@
         <v>2</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="Y1" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>836</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>837</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="2" spans="1:27">
@@ -3592,7 +3592,7 @@
         <v>441</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>444</v>
@@ -3610,13 +3610,13 @@
         <v>444</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>504</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>444</v>
@@ -3663,7 +3663,7 @@
         <v>444</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>444</v>
@@ -3704,7 +3704,7 @@
         <v>444</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="K5" s="1">
         <v>2</v>
@@ -3721,7 +3721,7 @@
     </row>
     <row r="6" spans="1:27">
       <c r="A6" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>444</v>
@@ -3767,22 +3767,22 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -3837,13 +3837,13 @@
         <v>11</v>
       </c>
       <c r="N8" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="O8" t="s">
         <v>519</v>
       </c>
       <c r="P8" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="Q8" t="s">
         <v>518</v>
@@ -3863,7 +3863,7 @@
     </row>
     <row r="9" spans="1:27">
       <c r="A9" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B9">
         <v>0.85</v>
@@ -3946,85 +3946,85 @@
     </row>
     <row r="10" spans="1:27">
       <c r="A10" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>841</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>842</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>843</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>844</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>845</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="K10" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>847</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>862</v>
-      </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>848</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>849</v>
-      </c>
       <c r="N10" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>857</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>859</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>858</v>
-      </c>
       <c r="Q10" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="R10" s="2" t="s">
         <v>851</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>852</v>
       </c>
       <c r="S10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="T10" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="U10" s="2" t="s">
         <v>839</v>
       </c>
-      <c r="U10" s="2" t="s">
-        <v>840</v>
-      </c>
       <c r="V10" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="W10" s="2" t="s">
         <v>853</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="X10" s="2" t="s">
         <v>854</v>
       </c>
-      <c r="X10" s="2" t="s">
+      <c r="Y10" s="2" t="s">
         <v>855</v>
       </c>
-      <c r="Y10" s="2" t="s">
-        <v>856</v>
-      </c>
       <c r="Z10" s="2" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -4065,22 +4065,22 @@
         <v>522</v>
       </c>
       <c r="M11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="N11" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="O11" t="s">
         <v>523</v>
       </c>
       <c r="P11" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="Q11" t="s">
         <v>521</v>
       </c>
       <c r="R11" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="S11" t="s">
         <v>161</v>
@@ -4092,22 +4092,22 @@
         <v>147</v>
       </c>
       <c r="V11" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="W11" t="s">
+        <v>893</v>
+      </c>
+      <c r="X11" t="s">
         <v>894</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>895</v>
       </c>
-      <c r="Y11" t="s">
-        <v>896</v>
-      </c>
       <c r="Z11" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="AA11" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -4148,10 +4148,10 @@
         <v>526</v>
       </c>
       <c r="M12" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="N12" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="O12" t="s">
         <v>148</v>
@@ -4163,7 +4163,7 @@
         <v>525</v>
       </c>
       <c r="R12" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="S12" t="s">
         <v>162</v>
@@ -4175,7 +4175,7 @@
         <v>148</v>
       </c>
       <c r="V12" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="W12" t="s">
         <v>159</v>
@@ -4184,10 +4184,10 @@
         <v>528</v>
       </c>
       <c r="Y12" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="Z12" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="AA12" t="s">
         <v>333</v>
@@ -4240,7 +4240,7 @@
         <v>169</v>
       </c>
       <c r="P13" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="Q13" t="s">
         <v>172</v>
@@ -4267,7 +4267,7 @@
         <v>169</v>
       </c>
       <c r="Y13" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="Z13" t="s">
         <v>294</v>
@@ -4350,7 +4350,7 @@
         <v>528</v>
       </c>
       <c r="Y14" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="Z14" t="s">
         <v>169</v>
@@ -4496,19 +4496,19 @@
         <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>381</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>381</v>
@@ -4517,13 +4517,13 @@
         <v>49</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="S18" t="s">
         <v>31</v>
@@ -4901,7 +4901,7 @@
         <v>166</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F27" t="s">
         <v>416</v>
@@ -4945,7 +4945,7 @@
         <v>89</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F28" t="s">
         <v>23</v>
@@ -5024,7 +5024,7 @@
         <v>505</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="S30" t="s">
         <v>506</v>
@@ -5275,7 +5275,7 @@
         <v>29</v>
       </c>
       <c r="U37" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="38" spans="1:23">
@@ -5308,7 +5308,7 @@
     </row>
     <row r="40" spans="1:23">
       <c r="A40" s="1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="S40" t="s">
         <v>34</v>
@@ -5316,7 +5316,7 @@
     </row>
     <row r="41" spans="1:23">
       <c r="A41" s="1" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="S41" t="s">
         <v>45</v>
@@ -5356,7 +5356,7 @@
         <v>378</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>380</v>
@@ -5368,25 +5368,25 @@
         <v>374</v>
       </c>
       <c r="L43" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="Q43" s="1" t="s">
         <v>921</v>
       </c>
-      <c r="M43" s="1" t="s">
-        <v>925</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>928</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="Q43" s="1" t="s">
+      <c r="R43" s="1" t="s">
         <v>922</v>
-      </c>
-      <c r="R43" s="1" t="s">
-        <v>923</v>
       </c>
       <c r="S43" s="1" t="s">
         <v>37</v>
@@ -5439,7 +5439,7 @@
         <v>373</v>
       </c>
       <c r="Q44" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="S44" t="s">
         <v>74</v>
@@ -5489,22 +5489,22 @@
         <v>538</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="O45" s="1" t="s">
         <v>539</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="Q45" s="1" t="s">
         <v>537</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="S45" s="1" t="s">
         <v>38</v>
@@ -5555,22 +5555,22 @@
         <v>542</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="O46" s="1" t="s">
         <v>543</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q46" s="1" t="s">
         <v>541</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="S46" s="1" t="s">
         <v>41</v>
@@ -5624,7 +5624,7 @@
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>43</v>
@@ -5633,28 +5633,28 @@
         <v>498</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>579</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="M48" s="1" t="s">
         <v>44</v>
       </c>
       <c r="N48" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="O48" s="1" t="s">
         <v>917</v>
       </c>
-      <c r="O48" s="1" t="s">
+      <c r="P48" s="1" t="s">
         <v>918</v>
       </c>
-      <c r="P48" s="1" t="s">
+      <c r="Q48" s="1" t="s">
         <v>919</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>920</v>
       </c>
       <c r="R48" s="1" t="s">
         <v>44</v>
@@ -5861,7 +5861,7 @@
     </row>
     <row r="51" spans="1:27">
       <c r="A51" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B51">
         <v>61</v>
@@ -6064,7 +6064,7 @@
         <v>48</v>
       </c>
       <c r="I53" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
@@ -6101,7 +6101,7 @@
         <v>367</v>
       </c>
       <c r="H54" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I54" t="s">
         <v>51</v>
@@ -6163,7 +6163,7 @@
     </row>
     <row r="55" spans="1:27">
       <c r="A55" s="1" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B55">
         <v>10</v>
@@ -6228,7 +6228,7 @@
     </row>
     <row r="56" spans="1:27">
       <c r="A56" s="1" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B56">
         <v>887</v>
@@ -6311,7 +6311,7 @@
     </row>
     <row r="57" spans="1:27">
       <c r="A57" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B57" s="27">
         <f t="shared" ref="B57:P57" si="5">B56/B61</f>
@@ -6504,7 +6504,7 @@
     </row>
     <row r="59" spans="1:27">
       <c r="A59" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B59" s="3">
         <v>796.529</v>
@@ -6670,7 +6670,7 @@
     </row>
     <row r="61" spans="1:27">
       <c r="A61" s="1" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B61" s="3">
         <v>84</v>
@@ -7160,7 +7160,7 @@
         <v>333</v>
       </c>
       <c r="M66" s="22" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="N66" s="22" t="s">
         <v>22</v>
@@ -7175,7 +7175,7 @@
         <v>336</v>
       </c>
       <c r="R66" s="22" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="S66" s="22" t="s">
         <v>166</v>
@@ -7187,7 +7187,7 @@
         <v>333</v>
       </c>
       <c r="V66" s="22" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="W66" s="22" t="s">
         <v>21</v>
@@ -7207,169 +7207,169 @@
     </row>
     <row r="67" spans="1:27">
       <c r="A67" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="F67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="G67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="H67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="I67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="J67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="K67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="L67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="M67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="N67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="O67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="P67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="Q67" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="R67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="S67" s="22" t="s">
         <v>696</v>
       </c>
-      <c r="B67" s="22" t="s">
+      <c r="T67" s="22" t="s">
+        <v>696</v>
+      </c>
+      <c r="U67" s="22" t="s">
+        <v>696</v>
+      </c>
+      <c r="V67" s="22" t="s">
         <v>698</v>
       </c>
-      <c r="C67" s="22" t="s">
+      <c r="W67" s="22" t="s">
         <v>698</v>
       </c>
-      <c r="D67" s="22" t="s">
+      <c r="X67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y67" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="Z67" s="22" t="s">
         <v>698</v>
       </c>
-      <c r="E67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="F67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="G67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="H67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="I67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="J67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="K67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="L67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="M67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="N67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="O67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="P67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="Q67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="R67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="S67" s="22" t="s">
+      <c r="AA67" t="s">
         <v>697</v>
-      </c>
-      <c r="T67" s="22" t="s">
-        <v>697</v>
-      </c>
-      <c r="U67" s="22" t="s">
-        <v>697</v>
-      </c>
-      <c r="V67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="W67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="X67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="Y67" s="22" t="s">
-        <v>698</v>
-      </c>
-      <c r="Z67" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="AA67" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="68" spans="1:27">
       <c r="A68" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B68" s="22" t="s">
+        <v>699</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>699</v>
+      </c>
+      <c r="D68" s="22" t="s">
         <v>700</v>
       </c>
-      <c r="C68" s="22" t="s">
-        <v>700</v>
-      </c>
-      <c r="D68" s="22" t="s">
+      <c r="E68" s="22" t="s">
+        <v>699</v>
+      </c>
+      <c r="F68" s="22" t="s">
+        <v>699</v>
+      </c>
+      <c r="G68" s="22" t="s">
         <v>701</v>
       </c>
-      <c r="E68" s="22" t="s">
-        <v>700</v>
-      </c>
-      <c r="F68" s="22" t="s">
-        <v>700</v>
-      </c>
-      <c r="G68" s="22" t="s">
-        <v>702</v>
-      </c>
       <c r="H68" s="22" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="I68" s="22"/>
       <c r="J68" s="22"/>
       <c r="K68" s="22" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="S68" s="22" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="T68" s="22" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U68" s="22" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="69" spans="1:27">
       <c r="A69" s="2" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B69" s="22" t="s">
+        <v>689</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>689</v>
+      </c>
+      <c r="D69" s="22" t="s">
         <v>690</v>
       </c>
-      <c r="C69" s="22" t="s">
+      <c r="E69" s="22" t="s">
+        <v>689</v>
+      </c>
+      <c r="F69" s="22" t="s">
+        <v>689</v>
+      </c>
+      <c r="G69" s="22" t="s">
+        <v>704</v>
+      </c>
+      <c r="H69" s="22" t="s">
         <v>690</v>
       </c>
-      <c r="D69" s="22" t="s">
-        <v>691</v>
-      </c>
-      <c r="E69" s="22" t="s">
-        <v>690</v>
-      </c>
-      <c r="F69" s="22" t="s">
-        <v>690</v>
-      </c>
-      <c r="G69" s="22" t="s">
+      <c r="I69" s="22" t="s">
+        <v>692</v>
+      </c>
+      <c r="J69" s="22" t="s">
         <v>705</v>
       </c>
-      <c r="H69" s="22" t="s">
-        <v>691</v>
-      </c>
-      <c r="I69" s="22" t="s">
-        <v>693</v>
-      </c>
-      <c r="J69" s="22" t="s">
-        <v>706</v>
-      </c>
       <c r="K69" s="22" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="S69" s="22" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="T69" s="22" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="U69" s="22" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="70" spans="1:27">
@@ -7380,22 +7380,22 @@
         <v>345</v>
       </c>
       <c r="C70" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D70" s="22" t="s">
         <v>348</v>
       </c>
       <c r="E70" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F70" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G70" s="22" t="s">
         <v>346</v>
       </c>
       <c r="H70" s="22" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="I70" s="22" t="s">
         <v>344</v>
@@ -7407,22 +7407,22 @@
         <v>580</v>
       </c>
       <c r="L70" t="s">
+        <v>871</v>
+      </c>
+      <c r="M70" s="22" t="s">
+        <v>876</v>
+      </c>
+      <c r="N70" s="22" t="s">
         <v>872</v>
       </c>
-      <c r="M70" s="22" t="s">
+      <c r="O70" s="22" t="s">
         <v>877</v>
       </c>
-      <c r="N70" s="22" t="s">
+      <c r="P70" t="s">
         <v>873</v>
       </c>
-      <c r="O70" s="22" t="s">
-        <v>878</v>
-      </c>
-      <c r="P70" t="s">
+      <c r="Q70" t="s">
         <v>874</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>875</v>
       </c>
       <c r="S70" s="22" t="s">
         <v>349</v>
@@ -7434,21 +7434,21 @@
         <v>492</v>
       </c>
       <c r="W70" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="X70" t="s">
+        <v>878</v>
+      </c>
+      <c r="Y70" t="s">
+        <v>875</v>
+      </c>
+      <c r="Z70" t="s">
         <v>879</v>
-      </c>
-      <c r="Y70" t="s">
-        <v>876</v>
-      </c>
-      <c r="Z70" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="71" spans="1:27">
       <c r="A71" s="1" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B71">
         <v>0.37862000000000001</v>
@@ -7522,7 +7522,7 @@
     </row>
     <row r="72" spans="1:27">
       <c r="A72" s="1" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B72">
         <v>1.5</v>
@@ -7605,7 +7605,7 @@
     </row>
     <row r="73" spans="1:27">
       <c r="A73" s="2" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B73">
         <v>1.804</v>
@@ -7658,7 +7658,7 @@
     </row>
     <row r="74" spans="1:27">
       <c r="A74" s="2" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B74">
         <v>0.36799999999999999</v>
@@ -7711,7 +7711,7 @@
     </row>
     <row r="75" spans="1:27">
       <c r="A75" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B75">
         <v>6.6000000000000003E-2</v>
@@ -7740,7 +7740,7 @@
     </row>
     <row r="76" spans="1:27">
       <c r="A76" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B76">
         <v>0.90300000000000002</v>
@@ -7769,7 +7769,7 @@
     </row>
     <row r="77" spans="1:27">
       <c r="A77" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D77">
         <f>240.49/D9</f>
@@ -7851,7 +7851,7 @@
         <v>435</v>
       </c>
       <c r="H79" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I79" t="s">
         <v>431</v>
@@ -7917,7 +7917,7 @@
         <v>372</v>
       </c>
       <c r="H82" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="I82" t="s">
         <v>379</v>
@@ -8007,7 +8007,7 @@
         <v>462</v>
       </c>
       <c r="E88" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F88" t="s">
         <v>141</v>
@@ -8048,7 +8048,7 @@
         <v>463</v>
       </c>
       <c r="E89" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F89" t="s">
         <v>142</v>
@@ -8089,7 +8089,7 @@
         <v>464</v>
       </c>
       <c r="E90" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F90" t="s">
         <v>143</v>
@@ -8130,7 +8130,7 @@
         <v>465</v>
       </c>
       <c r="E91" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F91" t="s">
         <v>144</v>
@@ -8171,7 +8171,7 @@
         <v>466</v>
       </c>
       <c r="E92" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F92" t="s">
         <v>145</v>
@@ -8206,7 +8206,7 @@
         <v>467</v>
       </c>
       <c r="E93" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F93" t="s">
         <v>146</v>
@@ -8232,7 +8232,7 @@
         <v>446</v>
       </c>
       <c r="E94" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="H94" t="s">
         <v>533</v>
@@ -8249,7 +8249,7 @@
         <v>116</v>
       </c>
       <c r="E95" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="H95" t="s">
         <v>534</v>
@@ -8263,7 +8263,7 @@
         <v>117</v>
       </c>
       <c r="E96" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I96" t="s">
         <v>140</v>
@@ -8274,7 +8274,7 @@
         <v>118</v>
       </c>
       <c r="E97" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I97" t="s">
         <v>470</v>
@@ -8309,7 +8309,7 @@
     </row>
     <row r="101" spans="1:23">
       <c r="A101" s="6" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B101" t="s">
         <v>370</v>
@@ -8339,7 +8339,7 @@
         <v>370</v>
       </c>
       <c r="N101" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="S101" t="s">
         <v>192</v>
@@ -8356,134 +8356,134 @@
         <v>185</v>
       </c>
       <c r="B102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="F102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="G102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="H102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="I102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="J102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="K102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="L102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="Q102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="S102" t="s">
         <v>186</v>
       </c>
       <c r="T102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="U102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="W102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="103" spans="1:23">
       <c r="A103" s="4" t="s">
+        <v>804</v>
+      </c>
+      <c r="B103" t="s">
         <v>805</v>
       </c>
-      <c r="B103" t="s">
-        <v>806</v>
-      </c>
       <c r="C103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="G103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="H103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="I103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="J103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="K103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="L103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="Q103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="S103" t="s">
         <v>188</v>
       </c>
       <c r="T103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="U103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="W103" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="104" spans="1:23">
       <c r="A104" s="4" t="s">
+        <v>806</v>
+      </c>
+      <c r="B104" t="s">
         <v>807</v>
       </c>
-      <c r="B104" t="s">
-        <v>808</v>
-      </c>
       <c r="C104" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D104" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E104" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F104" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="T104" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="U104" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="W104" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="105" spans="1:23">
@@ -8491,45 +8491,45 @@
         <v>190</v>
       </c>
       <c r="B105" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C105" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E105" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F105" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="L105" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="S105" t="s">
         <v>191</v>
       </c>
       <c r="T105" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="U105" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="W105" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="106" spans="1:23">
       <c r="A106" s="4" t="s">
+        <v>809</v>
+      </c>
+      <c r="D106" t="s">
         <v>810</v>
       </c>
-      <c r="D106" t="s">
+      <c r="H106" t="s">
+        <v>828</v>
+      </c>
+      <c r="K106" t="s">
         <v>811</v>
-      </c>
-      <c r="H106" t="s">
-        <v>829</v>
-      </c>
-      <c r="K106" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="107" spans="1:23">
@@ -8631,7 +8631,7 @@
         <v>503</v>
       </c>
       <c r="D115" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E115" t="s">
         <v>575</v>
@@ -8646,7 +8646,7 @@
         <v>502</v>
       </c>
       <c r="J115" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="K115" s="33" t="s">
         <v>517</v>
@@ -8666,7 +8666,7 @@
         <v>472</v>
       </c>
       <c r="C116" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D116" t="s">
         <v>514</v>
@@ -8678,7 +8678,7 @@
         <v>479</v>
       </c>
       <c r="H116" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I116" t="s">
         <v>471</v>
@@ -8764,7 +8764,7 @@
     </row>
     <row r="120" spans="1:24">
       <c r="A120" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B120">
         <v>6500</v>
@@ -8827,7 +8827,7 @@
     </row>
     <row r="124" spans="1:24">
       <c r="A124" s="6" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C124" t="s">
         <v>444</v>
@@ -8859,7 +8859,7 @@
     </row>
     <row r="125" spans="1:24">
       <c r="A125" s="6" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C125" t="s">
         <v>444</v>
@@ -8870,7 +8870,7 @@
     </row>
     <row r="126" spans="1:24">
       <c r="A126" s="6" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="S126" t="s">
         <v>444</v>
@@ -8884,223 +8884,223 @@
     </row>
     <row r="127" spans="1:24">
       <c r="A127" s="6" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B127" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C127" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D127" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E127" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F127" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G127" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H127" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I127" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J127" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="K127" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="128" spans="1:24">
       <c r="A128" s="6" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J128" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="K128" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="129" spans="1:11">
       <c r="A129" s="6" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B129" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C129" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D129" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E129" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F129" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G129" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H129" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I129" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J129" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="K129" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="130" spans="1:11">
       <c r="A130" s="6" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D130" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G130" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I130" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J130" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="K130" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="131" spans="1:11">
       <c r="A131" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="B131" t="s">
         <v>646</v>
       </c>
-      <c r="B131" t="s">
-        <v>647</v>
-      </c>
       <c r="D131" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F131" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G131" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H131" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I131" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J131" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="K131" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="132" spans="1:11">
       <c r="A132" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H132" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I132" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="133" spans="1:11">
       <c r="A133" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B133" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D133" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G133" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H133" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I133" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J133" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="K133" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="134" spans="1:11">
       <c r="A134" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="I134" t="s">
         <v>650</v>
       </c>
-      <c r="I134" t="s">
-        <v>651</v>
-      </c>
       <c r="J134" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="K134" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="135" spans="1:11">
       <c r="A135" s="6" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B135" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C135" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D135" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E135" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F135" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G135" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H135" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I135" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J135" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="K135" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="136" spans="1:11">
       <c r="A136" s="6" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B136" t="s">
         <v>293</v>
@@ -9127,15 +9127,15 @@
         <v>293</v>
       </c>
       <c r="J136" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="K136" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="137" spans="1:11">
       <c r="A137" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B137" t="s">
         <v>293</v>
@@ -9164,297 +9164,297 @@
     </row>
     <row r="138" spans="1:11">
       <c r="A138" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="I138" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J138" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="139" spans="1:11">
       <c r="A139" s="6" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I139" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="140" spans="1:11">
       <c r="A140" s="6" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I140" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J140" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="141" spans="1:11">
       <c r="A141" s="6" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="142" spans="1:11">
       <c r="A142" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I142" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="143" spans="1:11">
       <c r="A143" s="6" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H143" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="144" spans="1:11">
       <c r="A144" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="145" spans="1:11">
       <c r="A145" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B145" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D145" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H145" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I145" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="146" spans="1:11">
       <c r="A146" s="6" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="H146" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I146" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J146" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="K146" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="147" spans="1:11">
       <c r="A147" s="6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H147" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I147" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J147" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="K147" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="148" spans="1:11">
       <c r="A148" s="6" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B148" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C148" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D148" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E148" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F148" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G148" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H148" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I148" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J148" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="K148" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="149" spans="1:11">
       <c r="A149" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I149" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J149" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="K149" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="150" spans="1:11">
       <c r="A150" s="6" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B150" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D150" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G150" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H150" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="151" spans="1:11">
       <c r="A151" s="6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="K151" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="152" spans="1:11">
       <c r="A152" s="6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D152" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G152" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H152" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I152" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J152" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="K152" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="153" spans="1:11">
       <c r="A153" s="6" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I153" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="154" spans="1:11">
       <c r="A154" s="6" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G154" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H154" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I154" t="s">
         <v>293</v>
       </c>
       <c r="J154" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="K154" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="155" spans="1:11">
       <c r="A155" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="156" spans="1:11">
       <c r="A156" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="157" spans="1:11">
       <c r="A157" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="158" spans="1:11">
       <c r="A158" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B158" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D158" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G158" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H158" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I158" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J158" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="159" spans="1:11">
       <c r="A159" s="6" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H159" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="160" spans="1:11">
       <c r="A160" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="G160" s="1" t="s">
         <v>781</v>
       </c>
-      <c r="G160" s="1" t="s">
-        <v>782</v>
-      </c>
       <c r="H160" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="I160" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
   </sheetData>
@@ -9468,7 +9468,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9668,22 +9668,22 @@
         <v>214</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>248</v>
       </c>
       <c r="G13" s="40" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" thickBot="1">
@@ -9710,10 +9710,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="J14" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -9748,7 +9748,7 @@
         <v>248</v>
       </c>
       <c r="J15" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" thickBot="1">
@@ -9780,10 +9780,10 @@
         <v>2200</v>
       </c>
       <c r="I16" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="J16" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -9795,7 +9795,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
       <c r="J17" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" thickBot="1"/>
@@ -9804,10 +9804,10 @@
         <v>496</v>
       </c>
       <c r="B20" s="15" t="s">
+        <v>715</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>716</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>717</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
@@ -10267,33 +10267,33 @@
       <c r="G20" s="39"/>
       <c r="H20" s="36"/>
       <c r="K20" t="s">
+        <v>634</v>
+      </c>
+      <c r="L20" t="s">
         <v>635</v>
-      </c>
-      <c r="L20" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B21" s="23" t="s">
+        <v>636</v>
+      </c>
+      <c r="C21" s="23" t="s">
         <v>637</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="D21" s="23" t="s">
         <v>638</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="E21" s="23" t="s">
         <v>639</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="F21" s="24" t="s">
         <v>640</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="G21" s="40" t="s">
         <v>641</v>
-      </c>
-      <c r="G21" s="40" t="s">
-        <v>642</v>
       </c>
       <c r="H21" s="36"/>
     </row>
@@ -10650,28 +10650,28 @@
         <v>214</v>
       </c>
       <c r="B14" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>720</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="D14" s="23" t="s">
         <v>721</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="E14" s="23" t="s">
         <v>722</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="F14" s="24" t="s">
         <v>723</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="G14" s="40" t="s">
+        <v>621</v>
+      </c>
+      <c r="J14" t="s">
         <v>724</v>
       </c>
-      <c r="G14" s="40" t="s">
-        <v>622</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>725</v>
-      </c>
-      <c r="K14" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" thickBot="1">
@@ -10698,10 +10698,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
+        <v>726</v>
+      </c>
+      <c r="K15" t="s">
         <v>727</v>
-      </c>
-      <c r="K15" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -10733,10 +10733,10 @@
         <v>2001</v>
       </c>
       <c r="J16" t="s">
+        <v>728</v>
+      </c>
+      <c r="K16" t="s">
         <v>729</v>
-      </c>
-      <c r="K16" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -10768,10 +10768,10 @@
         <v>2200</v>
       </c>
       <c r="J17" t="s">
+        <v>730</v>
+      </c>
+      <c r="K17" t="s">
         <v>731</v>
-      </c>
-      <c r="K17" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -10783,15 +10783,15 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
       <c r="J18" t="s">
+        <v>732</v>
+      </c>
+      <c r="K18" t="s">
         <v>733</v>
-      </c>
-      <c r="K18" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="K19" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16" thickBot="1"/>
@@ -10824,10 +10824,10 @@
       </c>
       <c r="E24" s="10"/>
       <c r="F24" t="s">
+        <v>777</v>
+      </c>
+      <c r="G24" t="s">
         <v>778</v>
-      </c>
-      <c r="G24" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="16" thickBot="1">
@@ -10848,10 +10848,10 @@
       </c>
       <c r="E25" s="28"/>
       <c r="F25" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="44" thickBot="1">
@@ -10883,7 +10883,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:H25"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -11083,13 +11083,13 @@
         <v>214</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C14" s="23" t="s">
         <v>249</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>567</v>
@@ -11098,7 +11098,7 @@
         <v>573</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="16" thickBot="1">
@@ -11125,10 +11125,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
+        <v>737</v>
+      </c>
+      <c r="K15" t="s">
         <v>738</v>
-      </c>
-      <c r="K15" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -11160,10 +11160,10 @@
         <v>2000</v>
       </c>
       <c r="J16" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K16" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -11195,10 +11195,10 @@
         <v>2200</v>
       </c>
       <c r="J17" t="s">
+        <v>740</v>
+      </c>
+      <c r="K17" t="s">
         <v>741</v>
-      </c>
-      <c r="K17" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -11210,10 +11210,10 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
       <c r="J18" t="s">
+        <v>742</v>
+      </c>
+      <c r="K18" t="s">
         <v>743</v>
-      </c>
-      <c r="K18" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16" thickBot="1"/>
@@ -11246,10 +11246,10 @@
       </c>
       <c r="E23" s="10"/>
       <c r="F23" t="s">
+        <v>782</v>
+      </c>
+      <c r="G23" t="s">
         <v>783</v>
-      </c>
-      <c r="G23" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="16" thickBot="1">
@@ -11270,13 +11270,13 @@
       </c>
       <c r="E24" s="28"/>
       <c r="F24" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G24" t="s">
+        <v>784</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>785</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="44" thickBot="1">
@@ -11507,22 +11507,22 @@
         <v>214</v>
       </c>
       <c r="B13" s="23" t="s">
+        <v>744</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>745</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="D13" s="23" t="s">
         <v>746</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="E13" s="23" t="s">
         <v>747</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="F13" s="24" t="s">
         <v>748</v>
       </c>
-      <c r="F13" s="24" t="s">
-        <v>749</v>
-      </c>
       <c r="G13" s="40" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16" thickBot="1">
@@ -11549,10 +11549,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
+        <v>749</v>
+      </c>
+      <c r="J14" t="s">
         <v>750</v>
-      </c>
-      <c r="J14" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -11584,10 +11584,10 @@
         <v>2000</v>
       </c>
       <c r="I15" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="J15" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" thickBot="1">
@@ -11654,10 +11654,10 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
+        <v>752</v>
+      </c>
+      <c r="G20" t="s">
         <v>753</v>
-      </c>
-      <c r="G20" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="16" thickBot="1">
@@ -11694,13 +11694,13 @@
         <v>2200</v>
       </c>
       <c r="G22" t="s">
+        <v>755</v>
+      </c>
+      <c r="H22" t="s">
         <v>756</v>
       </c>
-      <c r="H22" t="s">
-        <v>757</v>
-      </c>
       <c r="I22" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -11708,10 +11708,10 @@
         <v>231</v>
       </c>
       <c r="G23" s="41" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="H23" s="41" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -11719,10 +11719,10 @@
     </row>
     <row r="24" spans="1:9">
       <c r="G24" s="41" t="s">
+        <v>758</v>
+      </c>
+      <c r="H24" s="41" t="s">
         <v>759</v>
-      </c>
-      <c r="H24" s="41" t="s">
-        <v>760</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -11730,10 +11730,10 @@
     </row>
     <row r="25" spans="1:9">
       <c r="G25" s="41" t="s">
+        <v>760</v>
+      </c>
+      <c r="H25" s="41" t="s">
         <v>761</v>
-      </c>
-      <c r="H25" s="41" t="s">
-        <v>762</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -11741,10 +11741,10 @@
     </row>
     <row r="26" spans="1:9">
       <c r="G26" t="s">
+        <v>762</v>
+      </c>
+      <c r="H26" t="s">
         <v>763</v>
-      </c>
-      <c r="H26" t="s">
-        <v>764</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -11752,7 +11752,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="G27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -11760,7 +11760,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="G28" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -11768,10 +11768,10 @@
     </row>
     <row r="29" spans="1:9">
       <c r="G29" t="s">
+        <v>766</v>
+      </c>
+      <c r="H29" t="s">
         <v>767</v>
-      </c>
-      <c r="H29" t="s">
-        <v>768</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -11779,10 +11779,10 @@
     </row>
     <row r="30" spans="1:9">
       <c r="G30" t="s">
+        <v>768</v>
+      </c>
+      <c r="H30" t="s">
         <v>769</v>
-      </c>
-      <c r="H30" t="s">
-        <v>770</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -11790,10 +11790,10 @@
     </row>
     <row r="31" spans="1:9">
       <c r="G31" t="s">
+        <v>770</v>
+      </c>
+      <c r="H31" t="s">
         <v>771</v>
-      </c>
-      <c r="H31" t="s">
-        <v>772</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -14781,10 +14781,10 @@
     </row>
     <row r="19" spans="1:11" ht="16">
       <c r="J19" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="K19" s="46" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="16" thickBot="1">
@@ -14795,7 +14795,7 @@
         <v>252</v>
       </c>
       <c r="C20" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D20" t="s">
         <v>594</v>
@@ -14840,10 +14840,10 @@
         <v>1999</v>
       </c>
       <c r="F22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G22" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" thickBot="1">
@@ -14867,10 +14867,10 @@
         <v>2200</v>
       </c>
       <c r="F23" t="s">
+        <v>774</v>
+      </c>
+      <c r="G23" s="18" t="s">
         <v>775</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -14890,8 +14890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -15200,7 +15200,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
       <c r="J17" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" thickBot="1">
@@ -15269,7 +15269,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="16" thickBot="1"/>
-    <row r="25" spans="1:10" ht="30" thickBot="1">
+    <row r="25" spans="1:10" ht="44" thickBot="1">
       <c r="A25" s="12" t="s">
         <v>496</v>
       </c>
@@ -15277,7 +15277,7 @@
         <v>594</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>595</v>
+        <v>940</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>252</v>
@@ -15344,7 +15344,7 @@
         <v>2200</v>
       </c>
       <c r="H28" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -15356,7 +15356,7 @@
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="H29" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
   </sheetData>
@@ -15368,7 +15368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -15569,7 +15569,7 @@
         <v>214</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>570</v>
@@ -15587,10 +15587,10 @@
         <v>573</v>
       </c>
       <c r="L13" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="M13" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" thickBot="1">
@@ -15621,7 +15621,7 @@
         <v>570</v>
       </c>
       <c r="M14" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="16" thickBot="1">
@@ -15629,7 +15629,7 @@
         <v>212</v>
       </c>
       <c r="B15" s="13">
-        <f t="shared" ref="B15:G15" si="2">ROUND(2000*B14,0)</f>
+        <f t="shared" ref="B15:F15" si="2">ROUND(2000*B14,0)</f>
         <v>454</v>
       </c>
       <c r="C15" s="13">
@@ -15657,7 +15657,7 @@
         <v>571</v>
       </c>
       <c r="M15" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" thickBot="1">
@@ -15665,7 +15665,7 @@
         <v>213</v>
       </c>
       <c r="B16" s="2">
-        <f t="shared" ref="B16:G16" si="3">ROUND(2200*B14,0)</f>
+        <f t="shared" ref="B16:F16" si="3">ROUND(2200*B14,0)</f>
         <v>499</v>
       </c>
       <c r="C16" s="2">
@@ -15693,7 +15693,7 @@
         <v>572</v>
       </c>
       <c r="M16" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -15713,10 +15713,10 @@
     </row>
     <row r="18" spans="1:13">
       <c r="L18" t="s">
+        <v>931</v>
+      </c>
+      <c r="M18" t="s">
         <v>932</v>
-      </c>
-      <c r="M18" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="16" thickBot="1"/>
@@ -15878,7 +15878,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -16090,22 +16090,22 @@
         <v>214</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>248</v>
       </c>
       <c r="E14" s="23" t="s">
+        <v>615</v>
+      </c>
+      <c r="F14" s="24" t="s">
         <v>616</v>
       </c>
-      <c r="F14" s="24" t="s">
-        <v>617</v>
-      </c>
       <c r="G14" s="40" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" thickBot="1">
@@ -16133,10 +16133,10 @@
       </c>
       <c r="H15" s="22"/>
       <c r="J15" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="K15" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -16169,10 +16169,10 @@
       </c>
       <c r="H16" s="3"/>
       <c r="J16" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="K16" t="s">
         <v>614</v>
-      </c>
-      <c r="K16" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -16208,7 +16208,7 @@
         <v>248</v>
       </c>
       <c r="K17" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -16220,10 +16220,10 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
       <c r="J18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="K18" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -16231,15 +16231,15 @@
         <v>566</v>
       </c>
       <c r="K19" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="J20" t="s">
+        <v>622</v>
+      </c>
+      <c r="K20" t="s">
         <v>623</v>
-      </c>
-      <c r="K20" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16" thickBot="1">
@@ -16318,7 +16318,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -16515,7 +16515,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="J13" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30" thickBot="1">
@@ -16523,25 +16523,25 @@
         <v>214</v>
       </c>
       <c r="B14" s="23" t="s">
+        <v>820</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>818</v>
+      </c>
+      <c r="D14" s="23" t="s">
         <v>821</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="E14" s="23" t="s">
         <v>819</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="F14" s="24" t="s">
         <v>822</v>
       </c>
-      <c r="E14" s="23" t="s">
-        <v>820</v>
-      </c>
-      <c r="F14" s="24" t="s">
+      <c r="J14" t="s">
         <v>823</v>
       </c>
-      <c r="J14" t="s">
-        <v>824</v>
-      </c>
       <c r="K14" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" thickBot="1">
@@ -16568,10 +16568,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="K15" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -16603,10 +16603,10 @@
         <v>1999</v>
       </c>
       <c r="J16" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="K16" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -16638,10 +16638,10 @@
         <v>2200</v>
       </c>
       <c r="J17" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="K17" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -16653,7 +16653,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
       <c r="J18" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="16" thickBot="1"/>
@@ -16664,11 +16664,11 @@
       <c r="B21" s="15" t="s">
         <v>592</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="15" t="s">
+        <v>591</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>593</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>591</v>
       </c>
       <c r="E21" s="15"/>
     </row>
@@ -16680,13 +16680,13 @@
         <v>0.17558260000000001</v>
       </c>
       <c r="C22" s="9">
+        <v>0.42319580000000001</v>
+      </c>
+      <c r="D22" s="9">
         <v>0.40122160000000001</v>
       </c>
-      <c r="D22" s="9">
-        <v>0.42319580000000001</v>
-      </c>
       <c r="E22" s="10">
-        <f>SUM(B22:D22)</f>
+        <f ca="1">SUM(B22:F22)</f>
         <v>1</v>
       </c>
     </row>
@@ -16699,11 +16699,11 @@
         <v>351</v>
       </c>
       <c r="C23" s="11">
-        <f t="shared" si="2"/>
+        <f>ROUND(2000*D22,0)</f>
         <v>802</v>
       </c>
       <c r="D23" s="11">
-        <f t="shared" si="2"/>
+        <f>ROUND(2000*C22,0)</f>
         <v>846</v>
       </c>
       <c r="E23" s="28">
@@ -16711,7 +16711,7 @@
         <v>1999</v>
       </c>
       <c r="H23" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="44" thickBot="1">
@@ -16723,11 +16723,11 @@
         <v>386</v>
       </c>
       <c r="C24" s="13">
-        <f t="shared" ref="C24:D24" si="4">ROUND(2200*C22,0)</f>
+        <f>ROUND(2200*D22,0)</f>
         <v>883</v>
       </c>
       <c r="D24" s="13">
-        <f t="shared" si="4"/>
+        <f>ROUND(2200*C22,0)</f>
         <v>931</v>
       </c>
       <c r="E24" s="28">
@@ -16735,7 +16735,7 @@
         <v>2200</v>
       </c>
       <c r="H24" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="25" spans="1:11">

</xml_diff>

<commit_message>
script UK + sources
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F5BDD6-C02A-6748-A3A6-A61554073BDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09039BE-E311-5A46-887C-5A53BC42FE52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5220" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="947">
   <si>
     <t>Country</t>
   </si>
@@ -2882,6 +2882,24 @@
   </si>
   <si>
     <t>Towns and Suburbs</t>
+  </si>
+  <si>
+    <t>https://www.atlanticcouncil.org/blogs/ukrainealert/climate-change-threatens-the-ukrainian-breadbasket/</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20200119174837/http://cgo-sreznevskyi.kiev.ua/index.php?lang=uk&amp;fn=news_full&amp;p=1&amp;f=news-cgo&amp;val=2020-01-02-09-24-36-45&amp;ko=</t>
+  </si>
+  <si>
+    <t>https://www.atlanticcouncil.org/blogs/ukrainealert/climate-change-may-prevent-ukraine-from-becoming-an-agricultural-superpower/</t>
+  </si>
+  <si>
+    <t>https://en.ecoaction.org.ua/wp-content/uploads/2019/04/water-is-coming-eng-short.pdf</t>
+  </si>
+  <si>
+    <t>https://climateknowledgeportal.worldbank.org/country/ukraine/vulnerability</t>
+  </si>
+  <si>
+    <t>https://www.mdpi.com/2071-1050/9/7/1152</t>
   </si>
 </sst>
 </file>
@@ -3425,9 +3443,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O44" sqref="O44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8027,6 +8045,9 @@
       <c r="K88" t="s">
         <v>448</v>
       </c>
+      <c r="N88" t="s">
+        <v>941</v>
+      </c>
       <c r="S88" t="s">
         <v>119</v>
       </c>
@@ -8068,6 +8089,9 @@
       <c r="K89" t="s">
         <v>450</v>
       </c>
+      <c r="N89" t="s">
+        <v>942</v>
+      </c>
       <c r="S89" t="s">
         <v>120</v>
       </c>
@@ -8109,6 +8133,9 @@
       <c r="K90" t="s">
         <v>452</v>
       </c>
+      <c r="N90" t="s">
+        <v>943</v>
+      </c>
       <c r="S90" t="s">
         <v>121</v>
       </c>
@@ -8150,6 +8177,9 @@
       <c r="K91" t="s">
         <v>454</v>
       </c>
+      <c r="N91" t="s">
+        <v>944</v>
+      </c>
       <c r="S91" s="7" t="s">
         <v>122</v>
       </c>
@@ -8191,6 +8221,9 @@
       <c r="K92" t="s">
         <v>456</v>
       </c>
+      <c r="N92" t="s">
+        <v>945</v>
+      </c>
       <c r="U92" t="s">
         <v>126</v>
       </c>
@@ -8219,6 +8252,9 @@
       </c>
       <c r="J93" t="s">
         <v>468</v>
+      </c>
+      <c r="N93" t="s">
+        <v>946</v>
       </c>
       <c r="U93" t="s">
         <v>127</v>
@@ -16317,7 +16353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -16695,7 +16731,7 @@
         <v>212</v>
       </c>
       <c r="B23" s="11">
-        <f t="shared" ref="B23:D23" si="2">ROUND(2000*B22,0)</f>
+        <f t="shared" ref="B23" si="2">ROUND(2000*B22,0)</f>
         <v>351</v>
       </c>
       <c r="C23" s="11">

</xml_diff>

<commit_message>
minor fix, own ref cell UK urban
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456337A9-FA64-AD47-867A-18D352B7A09E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
     <sheet name="quotas_MX" sheetId="17" r:id="rId16"/>
     <sheet name="quotas_SK" sheetId="18" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2907,7 +2908,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -3165,7 +3166,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3442,42 +3443,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.36328125" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" customWidth="1"/>
-    <col min="6" max="6" width="6.453125" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" customWidth="1"/>
-    <col min="9" max="9" width="8.36328125" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" customWidth="1"/>
-    <col min="12" max="12" width="7.36328125" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="6.5" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" customWidth="1"/>
+    <col min="11" max="11" width="9.5" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" customWidth="1"/>
     <col min="13" max="14" width="8" customWidth="1"/>
-    <col min="15" max="15" width="8.453125" customWidth="1"/>
-    <col min="16" max="16" width="8.81640625" customWidth="1"/>
-    <col min="17" max="17" width="6.81640625" customWidth="1"/>
-    <col min="18" max="18" width="8.36328125" customWidth="1"/>
-    <col min="19" max="19" width="7.453125" customWidth="1"/>
-    <col min="20" max="20" width="8.36328125" customWidth="1"/>
-    <col min="21" max="21" width="6.453125" customWidth="1"/>
-    <col min="22" max="22" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" customWidth="1"/>
+    <col min="17" max="17" width="6.83203125" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" customWidth="1"/>
+    <col min="19" max="19" width="7.5" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" customWidth="1"/>
+    <col min="21" max="21" width="6.5" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -9514,16 +9515,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -9537,7 +9538,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -9558,7 +9559,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -9579,7 +9580,7 @@
         <v>0.92622883301508352</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -9598,8 +9599,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -9620,7 +9621,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -9644,7 +9645,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -9673,7 +9674,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -9713,7 +9714,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1">
+    <row r="13" spans="1:10" ht="16" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -9736,7 +9737,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -9766,7 +9767,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -9801,7 +9802,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -9848,8 +9849,8 @@
         <v>799</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1"/>
-    <row r="20" spans="1:10" ht="26.5" thickBot="1">
+    <row r="19" spans="1:10" ht="16" thickBot="1"/>
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>496</v>
       </c>
@@ -9862,7 +9863,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:10" ht="26.5" thickBot="1">
+    <row r="21" spans="1:10" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>211</v>
       </c>
@@ -9878,7 +9879,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -9896,7 +9897,7 @@
       </c>
       <c r="E22" s="28"/>
     </row>
-    <row r="23" spans="1:10" ht="39" thickBot="1">
+    <row r="23" spans="1:10" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>501</v>
       </c>
@@ -9920,19 +9921,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -9947,7 +9948,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -9969,7 +9970,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -9991,7 +9992,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -10032,7 +10033,7 @@
       <c r="G6" s="35"/>
       <c r="H6" s="36"/>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -10042,7 +10043,7 @@
       <c r="G7" s="35"/>
       <c r="H7" s="36"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>218</v>
       </c>
@@ -10064,7 +10065,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="36"/>
     </row>
-    <row r="9" spans="1:11" ht="26.5" thickBot="1">
+    <row r="9" spans="1:11" ht="30" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -10089,7 +10090,7 @@
       </c>
       <c r="H9" s="36"/>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1">
+    <row r="10" spans="1:11" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -10119,7 +10120,7 @@
       </c>
       <c r="H10" s="36"/>
     </row>
-    <row r="11" spans="1:11" ht="26.5" thickBot="1">
+    <row r="11" spans="1:11" ht="30" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>213</v>
       </c>
@@ -10164,7 +10165,7 @@
     <row r="13" spans="1:11">
       <c r="H13" s="36"/>
     </row>
-    <row r="14" spans="1:11" ht="39" thickBot="1">
+    <row r="14" spans="1:11" ht="44" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -10188,7 +10189,7 @@
       </c>
       <c r="H14" s="36"/>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -10215,7 +10216,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -10251,7 +10252,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="26.5" thickBot="1">
+    <row r="17" spans="1:12" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -10323,7 +10324,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="26.5" thickBot="1">
+    <row r="21" spans="1:12" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>784</v>
       </c>
@@ -10347,7 +10348,7 @@
       </c>
       <c r="H21" s="36"/>
     </row>
-    <row r="22" spans="1:12" ht="26.5" thickBot="1">
+    <row r="22" spans="1:12" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>211</v>
       </c>
@@ -10374,7 +10375,7 @@
         <v>0.99989215000000009</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>212</v>
       </c>
@@ -10407,7 +10408,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="26.5" thickBot="1">
+    <row r="24" spans="1:12" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>213</v>
       </c>
@@ -10496,16 +10497,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -10519,7 +10520,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -10540,7 +10541,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -10561,7 +10562,7 @@
         <v>0.99992877771181621</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -10580,8 +10581,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -10602,7 +10603,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -10626,7 +10627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -10655,7 +10656,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -10695,7 +10696,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -10724,7 +10725,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -10754,7 +10755,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -10789,7 +10790,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -10844,8 +10845,8 @@
         <v>732</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1"/>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1"/>
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="12" t="s">
         <v>496</v>
       </c>
@@ -10858,7 +10859,7 @@
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>211</v>
       </c>
@@ -10880,7 +10881,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1">
+    <row r="25" spans="1:11" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>212</v>
       </c>
@@ -10904,7 +10905,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="39" thickBot="1">
+    <row r="26" spans="1:11" ht="44" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>501</v>
       </c>
@@ -10929,16 +10930,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -10952,7 +10953,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1">
+    <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -10973,7 +10974,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -10994,7 +10995,7 @@
         <v>0.97760081385085629</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -11013,8 +11014,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -11035,7 +11036,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -11059,7 +11060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -11088,7 +11089,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -11128,7 +11129,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -11151,7 +11152,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -11181,7 +11182,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -11216,7 +11217,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -11266,8 +11267,8 @@
         <v>741</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1"/>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1"/>
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="12" t="s">
         <v>496</v>
       </c>
@@ -11280,7 +11281,7 @@
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>211</v>
       </c>
@@ -11302,7 +11303,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1">
+    <row r="24" spans="1:11" ht="16" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>212</v>
       </c>
@@ -11329,7 +11330,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="39" thickBot="1">
+    <row r="25" spans="1:11" ht="44" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>501</v>
       </c>
@@ -11353,16 +11354,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -11376,7 +11377,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -11397,7 +11398,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -11418,7 +11419,7 @@
         <v>1.0341140064832992</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -11437,8 +11438,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -11459,7 +11460,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -11483,7 +11484,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -11512,7 +11513,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -11552,7 +11553,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="39" thickBot="1">
+    <row r="13" spans="1:10" ht="44" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -11575,7 +11576,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -11605,7 +11606,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -11640,7 +11641,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -11678,7 +11679,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1">
+    <row r="19" spans="1:9" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>330</v>
       </c>
@@ -11689,7 +11690,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1">
+    <row r="20" spans="1:9" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>211</v>
       </c>
@@ -11710,7 +11711,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1">
+    <row r="21" spans="1:9" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>212</v>
       </c>
@@ -11727,7 +11728,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="26.5" thickBot="1">
+    <row r="22" spans="1:9" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>213</v>
       </c>
@@ -11855,16 +11856,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -11878,7 +11879,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -11899,7 +11900,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -11920,7 +11921,7 @@
         <v>0.95217958067188335</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -11939,8 +11940,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -11961,7 +11962,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -11985,7 +11986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -12014,7 +12015,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -12060,16 +12061,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -12083,7 +12084,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -12104,7 +12105,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -12125,7 +12126,7 @@
         <v>0.92970833595125124</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -12144,8 +12145,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -12166,7 +12167,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -12190,7 +12191,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -12219,7 +12220,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -12265,16 +12266,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -12288,7 +12289,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -12309,7 +12310,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -12330,7 +12331,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -12349,8 +12350,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -12371,7 +12372,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -12395,7 +12396,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -12424,7 +12425,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -12470,14 +12471,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -12966,30 +12967,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -13004,7 +13005,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -13022,7 +13023,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -13042,7 +13043,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -13073,7 +13074,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -13082,7 +13083,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -13103,7 +13104,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -13127,7 +13128,7 @@
         <v>1.0001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -13156,7 +13157,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -13185,8 +13186,8 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1"/>
-    <row r="12" spans="1:7" ht="15" thickBot="1">
+    <row r="11" spans="1:7" ht="16" thickBot="1"/>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>230</v>
       </c>
@@ -13204,7 +13205,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="8" t="s">
         <v>229</v>
       </c>
@@ -13224,7 +13225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>212</v>
       </c>
@@ -13249,7 +13250,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>213</v>
       </c>
@@ -13279,7 +13280,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="12" t="s">
         <v>214</v>
       </c>
@@ -13299,7 +13300,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="8" t="s">
         <v>211</v>
       </c>
@@ -13323,7 +13324,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>212</v>
       </c>
@@ -13352,7 +13353,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>213</v>
       </c>
@@ -13390,7 +13391,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="16" t="s">
         <v>330</v>
       </c>
@@ -13401,7 +13402,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>211</v>
       </c>
@@ -13416,7 +13417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>212</v>
       </c>
@@ -13433,7 +13434,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>213</v>
       </c>
@@ -13461,22 +13462,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>272</v>
       </c>
@@ -13502,7 +13503,7 @@
       <c r="K1" s="13"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -13535,7 +13536,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -13569,7 +13570,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1">
+    <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -13633,14 +13634,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>215</v>
       </c>
@@ -13660,7 +13661,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -13683,7 +13684,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -13708,7 +13709,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>213</v>
       </c>
@@ -13749,7 +13750,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -13763,7 +13764,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>218</v>
       </c>
@@ -13789,7 +13790,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -13818,7 +13819,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -13852,7 +13853,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -13902,7 +13903,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -13916,7 +13917,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="26.5" thickBot="1">
+    <row r="20" spans="1:12" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>224</v>
       </c>
@@ -13940,7 +13941,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>229</v>
       </c>
@@ -13966,7 +13967,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -13997,7 +13998,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>213</v>
       </c>
@@ -14028,7 +14029,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>231</v>
       </c>
@@ -14038,7 +14039,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -14063,7 +14064,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1">
+    <row r="27" spans="1:12" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>211</v>
       </c>
@@ -14082,7 +14083,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1">
+    <row r="28" spans="1:12" ht="16" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>212</v>
       </c>
@@ -14104,7 +14105,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1">
+    <row r="29" spans="1:12" ht="16" thickBot="1">
       <c r="A29" s="8" t="s">
         <v>500</v>
       </c>
@@ -14123,7 +14124,7 @@
       </c>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>499</v>
       </c>
@@ -14145,7 +14146,7 @@
       </c>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:12" ht="26.5" thickBot="1">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>501</v>
       </c>
@@ -14178,12 +14179,12 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
-    <row r="36" spans="1:10" ht="15" thickBot="1">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26.5" thickBot="1">
+    <row r="37" spans="1:10" ht="30" thickBot="1">
       <c r="A37" s="8" t="s">
         <v>202</v>
       </c>
@@ -14213,7 +14214,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="8" t="s">
         <v>211</v>
       </c>
@@ -14246,7 +14247,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="8" t="s">
         <v>212</v>
       </c>
@@ -14287,7 +14288,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" thickBot="1">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="8" t="s">
         <v>213</v>
       </c>
@@ -14354,12 +14355,12 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="15" thickBot="1">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" thickBot="1">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>277</v>
       </c>
@@ -14380,7 +14381,7 @@
       </c>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="15" thickBot="1">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="8" t="s">
         <v>211</v>
       </c>
@@ -14404,7 +14405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" thickBot="1">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="8" t="s">
         <v>212</v>
       </c>
@@ -14433,7 +14434,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="8" t="s">
         <v>213</v>
       </c>
@@ -14489,16 +14490,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -14512,7 +14513,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -14533,7 +14534,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -14554,7 +14555,7 @@
         <v>0.95277529961698948</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -14573,8 +14574,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -14595,7 +14596,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -14619,7 +14620,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -14648,7 +14649,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -14688,7 +14689,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="26.5" thickBot="1">
+    <row r="13" spans="1:11" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -14714,7 +14715,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -14744,7 +14745,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -14779,7 +14780,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.5" thickBot="1">
+    <row r="16" spans="1:11" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -14829,7 +14830,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.5">
+    <row r="19" spans="1:11" ht="16">
       <c r="J19" t="s">
         <v>927</v>
       </c>
@@ -14837,7 +14838,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1">
+    <row r="20" spans="1:11" ht="16" thickBot="1">
       <c r="A20" s="16" t="s">
         <v>330</v>
       </c>
@@ -14851,7 +14852,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="26.5" thickBot="1">
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>211</v>
       </c>
@@ -14869,7 +14870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -14896,7 +14897,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1">
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>213</v>
       </c>
@@ -14930,23 +14931,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G23" r:id="rId1"/>
+    <hyperlink ref="G23" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -14960,7 +14961,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -14981,7 +14982,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -15002,7 +15003,7 @@
         <v>0.90805800128462044</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -15021,8 +15022,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -15043,7 +15044,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -15067,7 +15068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -15096,7 +15097,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -15136,7 +15137,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="26.5" thickBot="1">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -15156,7 +15157,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -15180,7 +15181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -15209,7 +15210,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -15253,7 +15254,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1">
+    <row r="19" spans="1:10" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>330</v>
       </c>
@@ -15264,7 +15265,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="26.5" thickBot="1">
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>211</v>
       </c>
@@ -15279,7 +15280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1">
+    <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>212</v>
       </c>
@@ -15296,7 +15297,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="26.5" thickBot="1">
+    <row r="22" spans="1:10" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>213</v>
       </c>
@@ -15318,8 +15319,8 @@
         <v>231</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1"/>
-    <row r="25" spans="1:10" ht="39" thickBot="1">
+    <row r="24" spans="1:10" ht="16" thickBot="1"/>
+    <row r="25" spans="1:10" ht="44" thickBot="1">
       <c r="A25" s="12" t="s">
         <v>496</v>
       </c>
@@ -15334,7 +15335,7 @@
       </c>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:10" ht="26.5" thickBot="1">
+    <row r="26" spans="1:10" ht="30" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>211</v>
       </c>
@@ -15352,7 +15353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1">
+    <row r="27" spans="1:10" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>212</v>
       </c>
@@ -15373,7 +15374,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="39" thickBot="1">
+    <row r="28" spans="1:10" ht="44" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>501</v>
       </c>
@@ -15415,16 +15416,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1">
+    <row r="1" spans="1:13" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -15438,7 +15439,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:13" ht="26.5" thickBot="1">
+    <row r="2" spans="1:13" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -15459,7 +15460,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -15480,7 +15481,7 @@
         <v>0.9267197256851698</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="26.5" thickBot="1">
+    <row r="4" spans="1:13" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -15499,8 +15500,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1"/>
-    <row r="7" spans="1:13" ht="15" thickBot="1">
+    <row r="6" spans="1:13" ht="16" thickBot="1"/>
+    <row r="7" spans="1:13" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -15521,7 +15522,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="26.5" thickBot="1">
+    <row r="8" spans="1:13" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -15545,7 +15546,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1">
+    <row r="9" spans="1:13" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -15574,7 +15575,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.5" thickBot="1">
+    <row r="10" spans="1:13" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -15614,7 +15615,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:13" ht="26.5" thickBot="1">
+    <row r="13" spans="1:13" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -15643,7 +15644,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="26.5" thickBot="1">
+    <row r="14" spans="1:13" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -15674,7 +15675,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1">
+    <row r="15" spans="1:13" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -15710,7 +15711,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="26.5" thickBot="1">
+    <row r="16" spans="1:13" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -15769,8 +15770,8 @@
         <v>928</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" thickBot="1"/>
-    <row r="20" spans="1:13" ht="26.5" thickBot="1">
+    <row r="19" spans="1:13" ht="16" thickBot="1"/>
+    <row r="20" spans="1:13" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>496</v>
       </c>
@@ -15782,7 +15783,7 @@
       </c>
       <c r="D20" s="15"/>
     </row>
-    <row r="21" spans="1:13" ht="26.5" thickBot="1">
+    <row r="21" spans="1:13" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>211</v>
       </c>
@@ -15797,7 +15798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15" thickBot="1">
+    <row r="22" spans="1:13" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -15814,7 +15815,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="39" thickBot="1">
+    <row r="23" spans="1:13" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>501</v>
       </c>
@@ -15839,12 +15840,12 @@
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
     </row>
-    <row r="28" spans="1:13" ht="15" thickBot="1">
+    <row r="28" spans="1:13" ht="16" thickBot="1">
       <c r="A28" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="26.5" thickBot="1">
+    <row r="29" spans="1:13" ht="30" thickBot="1">
       <c r="A29" s="12" t="s">
         <v>496</v>
       </c>
@@ -15857,7 +15858,7 @@
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="1:13" ht="26.5" thickBot="1">
+    <row r="30" spans="1:13" ht="30" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>211</v>
       </c>
@@ -15873,7 +15874,7 @@
       </c>
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="1:13" ht="15" thickBot="1">
+    <row r="31" spans="1:13" ht="16" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>212</v>
       </c>
@@ -15891,7 +15892,7 @@
       </c>
       <c r="E31" s="28"/>
     </row>
-    <row r="32" spans="1:13" ht="39" thickBot="1">
+    <row r="32" spans="1:13" ht="44" thickBot="1">
       <c r="A32" s="8" t="s">
         <v>501</v>
       </c>
@@ -15924,19 +15925,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -15950,7 +15951,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -15971,7 +15972,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -15992,7 +15993,7 @@
         <v>0.97448244785232785</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -16011,8 +16012,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -16033,7 +16034,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -16057,7 +16058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -16086,7 +16087,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -16135,7 +16136,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="40"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -16158,7 +16159,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -16189,7 +16190,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -16225,7 +16226,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -16292,7 +16293,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1">
       <c r="A21" s="16" t="s">
         <v>330</v>
       </c>
@@ -16303,7 +16304,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1">
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>211</v>
       </c>
@@ -16318,7 +16319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>212</v>
       </c>
@@ -16335,7 +16336,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>213</v>
       </c>
@@ -16364,16 +16365,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -16387,7 +16388,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -16408,7 +16409,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -16429,7 +16430,7 @@
         <v>0.98351979013457747</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -16448,8 +16449,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -16470,7 +16471,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -16494,7 +16495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -16523,7 +16524,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -16568,7 +16569,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -16594,7 +16595,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -16624,7 +16625,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -16659,7 +16660,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -16706,8 +16707,8 @@
         <v>825</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1"/>
-    <row r="21" spans="1:11" ht="26.5" thickBot="1">
+    <row r="20" spans="1:11" ht="16" thickBot="1"/>
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>496</v>
       </c>
@@ -16722,7 +16723,7 @@
       </c>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1">
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>211</v>
       </c>
@@ -16736,11 +16737,11 @@
         <v>0.40122160000000001</v>
       </c>
       <c r="E22" s="10">
-        <f ca="1">SUM(B22:F22)</f>
+        <f>SUM(B22:D22)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>212</v>
       </c>
@@ -16764,7 +16765,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="39" thickBot="1">
+    <row r="24" spans="1:11" ht="44" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>501</v>
       </c>

</xml_diff>

<commit_message>
Wrong place sources CAN
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A3F276-9373-3A43-969D-D7F90508B657}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0217B644-2A8E-AD4F-B774-E75A7076A895}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3468,8 +3468,8 @@
   <dimension ref="A1:AA161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M107" sqref="M107"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L100" sqref="L100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8073,6 +8073,9 @@
       <c r="K88" t="s">
         <v>448</v>
       </c>
+      <c r="M88" t="s">
+        <v>948</v>
+      </c>
       <c r="N88" t="s">
         <v>937</v>
       </c>
@@ -8117,6 +8120,9 @@
       <c r="K89" t="s">
         <v>450</v>
       </c>
+      <c r="M89" t="s">
+        <v>949</v>
+      </c>
       <c r="N89" t="s">
         <v>938</v>
       </c>
@@ -8161,6 +8167,9 @@
       <c r="K90" t="s">
         <v>452</v>
       </c>
+      <c r="M90" t="s">
+        <v>950</v>
+      </c>
       <c r="N90" t="s">
         <v>939</v>
       </c>
@@ -8205,6 +8214,9 @@
       <c r="K91" t="s">
         <v>454</v>
       </c>
+      <c r="M91" t="s">
+        <v>951</v>
+      </c>
       <c r="N91" t="s">
         <v>940</v>
       </c>
@@ -8249,6 +8261,9 @@
       <c r="K92" t="s">
         <v>456</v>
       </c>
+      <c r="M92" t="s">
+        <v>952</v>
+      </c>
       <c r="N92" t="s">
         <v>941</v>
       </c>
@@ -8281,6 +8296,9 @@
       <c r="J93" t="s">
         <v>468</v>
       </c>
+      <c r="M93" t="s">
+        <v>953</v>
+      </c>
       <c r="N93" t="s">
         <v>942</v>
       </c>
@@ -8307,6 +8325,9 @@
       <c r="J94" t="s">
         <v>469</v>
       </c>
+      <c r="M94" t="s">
+        <v>954</v>
+      </c>
     </row>
     <row r="95" spans="1:21">
       <c r="A95" s="6" t="s">
@@ -8402,9 +8423,6 @@
       <c r="K101" t="s">
         <v>370</v>
       </c>
-      <c r="M101" t="s">
-        <v>948</v>
-      </c>
       <c r="N101" t="s">
         <v>877</v>
       </c>
@@ -8455,9 +8473,6 @@
       <c r="L102" t="s">
         <v>801</v>
       </c>
-      <c r="M102" t="s">
-        <v>949</v>
-      </c>
       <c r="Q102" t="s">
         <v>801</v>
       </c>
@@ -8511,9 +8526,6 @@
       <c r="L103" t="s">
         <v>803</v>
       </c>
-      <c r="M103" t="s">
-        <v>950</v>
-      </c>
       <c r="Q103" t="s">
         <v>803</v>
       </c>
@@ -8549,9 +8561,6 @@
       <c r="F104" t="s">
         <v>805</v>
       </c>
-      <c r="M104" t="s">
-        <v>951</v>
-      </c>
       <c r="T104" t="s">
         <v>805</v>
       </c>
@@ -8581,9 +8590,6 @@
       <c r="L105" t="s">
         <v>806</v>
       </c>
-      <c r="M105" t="s">
-        <v>952</v>
-      </c>
       <c r="S105" t="s">
         <v>191</v>
       </c>
@@ -8610,16 +8616,10 @@
       <c r="K106" t="s">
         <v>809</v>
       </c>
-      <c r="M106" t="s">
-        <v>953</v>
-      </c>
     </row>
     <row r="107" spans="1:23">
       <c r="A107" s="6" t="s">
         <v>261</v>
-      </c>
-      <c r="M107" t="s">
-        <v>954</v>
       </c>
       <c r="S107" t="s">
         <v>291</v>

</xml_diff>

<commit_message>
Add gender, age quota AU, CA, TR, UA
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D407DF28-12A9-5F44-AE5C-2AEA63DB23FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BCD710-02FF-224A-A6B9-7705B9BB44AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1000" yWindow="-17620" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="9" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,10 @@
     <sheet name="quotas_BR" sheetId="16" r:id="rId15"/>
     <sheet name="quotas_MX" sheetId="17" r:id="rId16"/>
     <sheet name="quotas_SK" sheetId="18" r:id="rId17"/>
+    <sheet name="quota_AU" sheetId="19" r:id="rId18"/>
+    <sheet name="quota_CA" sheetId="20" r:id="rId19"/>
+    <sheet name="quota_TR" sheetId="21" r:id="rId20"/>
+    <sheet name="quota_UA" sheetId="22" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1963" uniqueCount="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="977">
   <si>
     <t>Country</t>
   </si>
@@ -3534,9 +3538,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R94" sqref="R94"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -11527,8 +11531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -12030,7 +12034,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:F8"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -12640,6 +12644,410 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05927DD8-3271-5F43-85F8-050E6B527F39}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16" thickBot="1">
+      <c r="A1" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" ht="16" thickBot="1">
+      <c r="A2" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="9">
+        <f>1-C2</f>
+        <v>0.5064562063085738</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.49354379369142626</v>
+      </c>
+      <c r="D2" s="10">
+        <f>SUM(B2:C2)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" thickBot="1">
+      <c r="A3" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" s="11">
+        <f>ROUND(2000*B2,0)</f>
+        <v>1013</v>
+      </c>
+      <c r="C3" s="11">
+        <f>ROUND(2000*C2,0)</f>
+        <v>987</v>
+      </c>
+      <c r="D3" s="11">
+        <f>ROUND(2000*D2,0)</f>
+        <v>2000</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" thickBot="1">
+      <c r="A4" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="11">
+        <f>ROUND(2200*B2,0)</f>
+        <v>1114</v>
+      </c>
+      <c r="C4" s="11">
+        <f>ROUND(2200*C2,0)</f>
+        <v>1086</v>
+      </c>
+      <c r="D4" s="11">
+        <f>ROUND(2200*D2,0)</f>
+        <v>2200</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
+      <c r="A7" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="16" thickBot="1">
+      <c r="A8" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.11192255877789467</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.18591237270266067</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.26180562458671341</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.23014443705193119</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.21021500688079983</v>
+      </c>
+      <c r="G8" s="10">
+        <f>SUM(B8:F8)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" thickBot="1">
+      <c r="A9" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="11">
+        <f t="shared" ref="B9:G9" si="0">ROUND(2000*B8,0)</f>
+        <v>224</v>
+      </c>
+      <c r="C9" s="11">
+        <f t="shared" si="0"/>
+        <v>372</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" si="0"/>
+        <v>524</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="0"/>
+        <v>460</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="0"/>
+        <v>420</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" thickBot="1">
+      <c r="A10" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="11">
+        <f t="shared" ref="B10:G10" si="1">ROUND(2200*B8,0)</f>
+        <v>246</v>
+      </c>
+      <c r="C10" s="11">
+        <f t="shared" si="1"/>
+        <v>409</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" si="1"/>
+        <v>576</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="1"/>
+        <v>506</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="1"/>
+        <v>462</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60273D31-897F-3C47-8830-44A1DA7FF7AC}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16" thickBot="1">
+      <c r="A1" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" ht="16" thickBot="1">
+      <c r="A2" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="9">
+        <f>1-C2</f>
+        <v>0.5072618222776264</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.4927381777223736</v>
+      </c>
+      <c r="D2" s="10">
+        <f>SUM(B2:C2)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" thickBot="1">
+      <c r="A3" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" s="11">
+        <f>ROUND(2000*B2,0)</f>
+        <v>1015</v>
+      </c>
+      <c r="C3" s="11">
+        <f>ROUND(2000*C2,0)</f>
+        <v>985</v>
+      </c>
+      <c r="D3" s="11">
+        <f>ROUND(2000*D2,0)</f>
+        <v>2000</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" thickBot="1">
+      <c r="A4" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="11">
+        <f>ROUND(2200*B2,0)</f>
+        <v>1116</v>
+      </c>
+      <c r="C4" s="11">
+        <f>ROUND(2200*C2,0)</f>
+        <v>1084</v>
+      </c>
+      <c r="D4" s="11">
+        <f>ROUND(2200*D2,0)</f>
+        <v>2200</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
+      <c r="A7" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="16" thickBot="1">
+      <c r="A8" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.10402815988780871</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.17502163559091188</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.24488811098766669</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.25292269475436224</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.22313939877924996</v>
+      </c>
+      <c r="G8" s="10">
+        <f>SUM(B8:F8)</f>
+        <v>0.99999999999999944</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" thickBot="1">
+      <c r="A9" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="11">
+        <f t="shared" ref="B9:G9" si="0">ROUND(2000*B8,0)</f>
+        <v>208</v>
+      </c>
+      <c r="C9" s="11">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" si="0"/>
+        <v>490</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="0"/>
+        <v>506</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="0"/>
+        <v>446</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" thickBot="1">
+      <c r="A10" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="11">
+        <f t="shared" ref="B10:G10" si="1">ROUND(2200*B8,0)</f>
+        <v>229</v>
+      </c>
+      <c r="C10" s="11">
+        <f t="shared" si="1"/>
+        <v>385</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" si="1"/>
+        <v>539</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="1"/>
+        <v>556</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="1"/>
+        <v>491</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
@@ -13140,6 +13548,410 @@
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCB4E59-7736-3846-8586-8D1EB1F35F4E}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16" thickBot="1">
+      <c r="A1" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" ht="16" thickBot="1">
+      <c r="A2" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="9">
+        <f>1-C2</f>
+        <v>0.51342426197866531</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.48657573802133475</v>
+      </c>
+      <c r="D2" s="10">
+        <f>SUM(B2:C2)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" thickBot="1">
+      <c r="A3" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" s="11">
+        <f>ROUND(2000*B2,0)</f>
+        <v>1027</v>
+      </c>
+      <c r="C3" s="11">
+        <f>ROUND(2000*C2,0)</f>
+        <v>973</v>
+      </c>
+      <c r="D3" s="11">
+        <f>ROUND(2000*D2,0)</f>
+        <v>2000</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" thickBot="1">
+      <c r="A4" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="11">
+        <f>ROUND(2200*B2,0)</f>
+        <v>1130</v>
+      </c>
+      <c r="C4" s="11">
+        <f>ROUND(2200*C2,0)</f>
+        <v>1070</v>
+      </c>
+      <c r="D4" s="11">
+        <f>ROUND(2200*D2,0)</f>
+        <v>2200</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
+      <c r="A7" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="16" thickBot="1">
+      <c r="A8" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.1582325601298683</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.2131137356790879</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.29681998391047659</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.20571250504618752</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.12612121523437902</v>
+      </c>
+      <c r="G8" s="10">
+        <f>SUM(B8:F8)</f>
+        <v>0.99999999999999933</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" thickBot="1">
+      <c r="A9" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="11">
+        <f t="shared" ref="B9:G9" si="0">ROUND(2000*B8,0)</f>
+        <v>316</v>
+      </c>
+      <c r="C9" s="11">
+        <f t="shared" si="0"/>
+        <v>426</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" si="0"/>
+        <v>594</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="0"/>
+        <v>411</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" thickBot="1">
+      <c r="A10" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="11">
+        <f t="shared" ref="B10:G10" si="1">ROUND(2200*B8,0)</f>
+        <v>348</v>
+      </c>
+      <c r="C10" s="11">
+        <f t="shared" si="1"/>
+        <v>469</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" si="1"/>
+        <v>653</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="1"/>
+        <v>453</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCCF8E2-273E-6A4C-A004-D29D9094C515}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16" thickBot="1">
+      <c r="A1" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" ht="16" thickBot="1">
+      <c r="A2" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="9">
+        <f>1-C2</f>
+        <v>0.54857404271562449</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.45142595728437557</v>
+      </c>
+      <c r="D2" s="10">
+        <f>SUM(B2:C2)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" thickBot="1">
+      <c r="A3" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" s="11">
+        <f>ROUND(2000*B2,0)</f>
+        <v>1097</v>
+      </c>
+      <c r="C3" s="11">
+        <f>ROUND(2000*C2,0)</f>
+        <v>903</v>
+      </c>
+      <c r="D3" s="11">
+        <f>ROUND(2000*D2,0)</f>
+        <v>2000</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" thickBot="1">
+      <c r="A4" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="11">
+        <f>ROUND(2200*B2,0)</f>
+        <v>1207</v>
+      </c>
+      <c r="C4" s="11">
+        <f>ROUND(2200*C2,0)</f>
+        <v>993</v>
+      </c>
+      <c r="D4" s="11">
+        <f>ROUND(2200*D2,0)</f>
+        <v>2200</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
+      <c r="A7" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="16" thickBot="1">
+      <c r="A8" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" s="9">
+        <v>8.2159805419933327E-2</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.17834324173209759</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.28227842928850105</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.24861654266018471</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.20860198089928325</v>
+      </c>
+      <c r="G8" s="10">
+        <f>SUM(B8:F8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" thickBot="1">
+      <c r="A9" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="11">
+        <f t="shared" ref="B9:G9" si="0">ROUND(2000*B8,0)</f>
+        <v>164</v>
+      </c>
+      <c r="C9" s="11">
+        <f t="shared" si="0"/>
+        <v>357</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" si="0"/>
+        <v>565</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="0"/>
+        <v>417</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" thickBot="1">
+      <c r="A10" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="11">
+        <f t="shared" ref="B10:G10" si="1">ROUND(2200*B8,0)</f>
+        <v>181</v>
+      </c>
+      <c r="C10" s="11">
+        <f t="shared" si="1"/>
+        <v>392</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" si="1"/>
+        <v>621</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="1"/>
+        <v>547</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="1"/>
+        <v>459</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add region quota KR (+ src MX, AU)
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F52EDB-31A0-CC4C-A3FE-F8267C455345}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1000" yWindow="-17620" windowWidth="25600" windowHeight="14480" tabRatio="923"/>
+    <workbookView xWindow="860" yWindow="-16920" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="7" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -34,7 +35,7 @@
     <sheet name="quota_TR" sheetId="21" r:id="rId20"/>
     <sheet name="quota_UA" sheetId="22" r:id="rId21"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2109" uniqueCount="998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2141" uniqueCount="1014">
   <si>
     <t>Country</t>
   </si>
@@ -3057,11 +3058,59 @@
   <si>
     <t>~ Warren</t>
   </si>
+  <si>
+    <t>Seoul</t>
+  </si>
+  <si>
+    <t>Gyeonggi, and Incheon, Gangwon</t>
+  </si>
+  <si>
+    <t>North Chungcheong, South Chungcheong, Daejeon, Sejong</t>
+  </si>
+  <si>
+    <t>North Jeolla, South Jeolla, Gwanggju, and Jeju</t>
+  </si>
+  <si>
+    <t>South Gyeongsang, North Gyeongsang, Daegu, Busan, and Ulsan</t>
+  </si>
+  <si>
+    <t>https://kosis.kr/eng/statisticsList/statisticsListIndex.do?menuId=M_01_01&amp;vwcd=MT_ETITLE&amp;parmTabId=M_01_01&amp;statId=1962001&amp;themaId=#SelectStatsBoxDiv</t>
+  </si>
+  <si>
+    <t>https://www.abs.gov.au/statistics/people/population/national-state-and-territory-population/latest-release</t>
+  </si>
+  <si>
+    <t>Northern Territory, Western Australia</t>
+  </si>
+  <si>
+    <t>Australian Capital Territory, New South Wales</t>
+  </si>
+  <si>
+    <t>Tasmania, Victoria</t>
+  </si>
+  <si>
+    <t>Aguascalientes, Colima, Jalisco, Guanajuato, Michoacan, Nayarit, San Luis Potosi, Zacatecas</t>
+  </si>
+  <si>
+    <t>Federal District, Hidalgo, Mexico, Morelos, Puebla, Queretaro, Tlaxcala,</t>
+  </si>
+  <si>
+    <t>Coahuila, Nuevo Leon, Tamaulipas</t>
+  </si>
+  <si>
+    <t>Baja California; Baja California Sur; Chihuahua; Durango; Sinaloa; Sonora</t>
+  </si>
+  <si>
+    <t>Campeche, Chiapas, Guerrero, Oaxaca, Quintana Roo, Tabasco, Varacruz, Yucatan</t>
+  </si>
+  <si>
+    <t>https://www.inegi.org.mx/default.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -3319,7 +3368,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3596,42 +3645,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M2" sqref="M2:R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.36328125" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" customWidth="1"/>
-    <col min="6" max="6" width="6.453125" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" customWidth="1"/>
-    <col min="9" max="9" width="8.36328125" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" customWidth="1"/>
-    <col min="12" max="12" width="7.36328125" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="6.5" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" customWidth="1"/>
+    <col min="11" max="11" width="9.5" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" customWidth="1"/>
     <col min="13" max="14" width="8" customWidth="1"/>
-    <col min="15" max="15" width="8.453125" customWidth="1"/>
-    <col min="16" max="16" width="8.81640625" customWidth="1"/>
-    <col min="17" max="17" width="6.81640625" customWidth="1"/>
-    <col min="18" max="18" width="8.36328125" customWidth="1"/>
-    <col min="19" max="19" width="7.453125" customWidth="1"/>
-    <col min="20" max="20" width="8.36328125" customWidth="1"/>
-    <col min="21" max="21" width="6.453125" customWidth="1"/>
-    <col min="22" max="22" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" customWidth="1"/>
+    <col min="17" max="17" width="6.83203125" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" customWidth="1"/>
+    <col min="19" max="19" width="7.5" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" customWidth="1"/>
+    <col min="21" max="21" width="6.5" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -9785,16 +9834,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -9808,7 +9857,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -9829,7 +9878,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -9850,7 +9899,7 @@
         <v>0.92622883301508352</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -9869,8 +9918,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -9891,7 +9940,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -9915,7 +9964,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -9944,7 +9993,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -9984,7 +10033,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1">
+    <row r="13" spans="1:10" ht="16" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -10007,7 +10056,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -10037,7 +10086,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -10072,7 +10121,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -10119,8 +10168,8 @@
         <v>796</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1"/>
-    <row r="20" spans="1:10" ht="26.5" thickBot="1">
+    <row r="19" spans="1:10" ht="16" thickBot="1"/>
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>495</v>
       </c>
@@ -10133,7 +10182,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:10" ht="26.5" thickBot="1">
+    <row r="21" spans="1:10" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>211</v>
       </c>
@@ -10149,7 +10198,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -10167,7 +10216,7 @@
       </c>
       <c r="E22" s="28"/>
     </row>
-    <row r="23" spans="1:10" ht="39" thickBot="1">
+    <row r="23" spans="1:10" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>500</v>
       </c>
@@ -10191,19 +10240,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -10218,7 +10267,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -10240,7 +10289,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -10262,7 +10311,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -10303,7 +10352,7 @@
       <c r="G6" s="35"/>
       <c r="H6" s="36"/>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -10313,7 +10362,7 @@
       <c r="G7" s="35"/>
       <c r="H7" s="36"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>218</v>
       </c>
@@ -10335,7 +10384,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="36"/>
     </row>
-    <row r="9" spans="1:11" ht="26.5" thickBot="1">
+    <row r="9" spans="1:11" ht="30" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -10360,7 +10409,7 @@
       </c>
       <c r="H9" s="36"/>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1">
+    <row r="10" spans="1:11" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -10390,7 +10439,7 @@
       </c>
       <c r="H10" s="36"/>
     </row>
-    <row r="11" spans="1:11" ht="26.5" thickBot="1">
+    <row r="11" spans="1:11" ht="30" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>213</v>
       </c>
@@ -10435,7 +10484,7 @@
     <row r="13" spans="1:11">
       <c r="H13" s="36"/>
     </row>
-    <row r="14" spans="1:11" ht="39" thickBot="1">
+    <row r="14" spans="1:11" ht="44" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -10459,7 +10508,7 @@
       </c>
       <c r="H14" s="36"/>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -10486,7 +10535,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -10522,7 +10571,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="26.5" thickBot="1">
+    <row r="17" spans="1:12" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -10594,7 +10643,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="26.5" thickBot="1">
+    <row r="21" spans="1:12" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>781</v>
       </c>
@@ -10618,7 +10667,7 @@
       </c>
       <c r="H21" s="36"/>
     </row>
-    <row r="22" spans="1:12" ht="26.5" thickBot="1">
+    <row r="22" spans="1:12" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>211</v>
       </c>
@@ -10645,7 +10694,7 @@
         <v>0.99989215000000009</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>212</v>
       </c>
@@ -10678,7 +10727,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="26.5" thickBot="1">
+    <row r="24" spans="1:12" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>213</v>
       </c>
@@ -10767,16 +10816,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -10790,7 +10839,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -10811,7 +10860,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -10832,7 +10881,7 @@
         <v>0.99992877771181621</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -10851,8 +10900,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -10873,7 +10922,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -10897,7 +10946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -10926,7 +10975,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -10966,7 +11015,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -10995,7 +11044,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -11025,7 +11074,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -11060,7 +11109,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -11115,8 +11164,8 @@
         <v>729</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1"/>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1"/>
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="12" t="s">
         <v>495</v>
       </c>
@@ -11129,7 +11178,7 @@
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>211</v>
       </c>
@@ -11151,7 +11200,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1">
+    <row r="25" spans="1:11" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>212</v>
       </c>
@@ -11175,7 +11224,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="39" thickBot="1">
+    <row r="26" spans="1:11" ht="44" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>500</v>
       </c>
@@ -11200,16 +11249,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -11223,7 +11272,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1">
+    <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -11244,7 +11293,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -11265,7 +11314,7 @@
         <v>0.97760081385085629</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -11284,8 +11333,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -11306,7 +11355,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -11330,7 +11379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -11359,7 +11408,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -11399,7 +11448,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -11422,7 +11471,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -11452,7 +11501,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -11487,7 +11536,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -11537,8 +11586,8 @@
         <v>738</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1"/>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1"/>
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="12" t="s">
         <v>495</v>
       </c>
@@ -11551,7 +11600,7 @@
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>211</v>
       </c>
@@ -11573,7 +11622,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1">
+    <row r="24" spans="1:11" ht="16" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>212</v>
       </c>
@@ -11600,7 +11649,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="39" thickBot="1">
+    <row r="25" spans="1:11" ht="44" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>500</v>
       </c>
@@ -11624,16 +11673,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -11647,7 +11696,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -11668,7 +11717,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -11689,7 +11738,7 @@
         <v>1.0341140064832992</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -11708,8 +11757,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -11730,7 +11779,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -11754,7 +11803,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -11783,7 +11832,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -11823,7 +11872,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="39" thickBot="1">
+    <row r="13" spans="1:10" ht="44" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -11846,7 +11895,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -11876,7 +11925,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -11911,7 +11960,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -11949,7 +11998,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1">
+    <row r="19" spans="1:9" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>330</v>
       </c>
@@ -11960,7 +12009,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1">
+    <row r="20" spans="1:9" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>211</v>
       </c>
@@ -11981,7 +12030,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1">
+    <row r="21" spans="1:9" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>212</v>
       </c>
@@ -11998,7 +12047,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="26.5" thickBot="1">
+    <row r="22" spans="1:9" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>213</v>
       </c>
@@ -12126,16 +12175,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -12149,7 +12198,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -12170,7 +12219,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -12191,7 +12240,7 @@
         <v>0.95217958067188335</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -12210,8 +12259,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -12232,7 +12281,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -12256,7 +12305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -12285,7 +12334,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -12325,7 +12374,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -12348,7 +12397,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -12372,7 +12421,7 @@
         <v>0.99999999999999933</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1">
+    <row r="16" spans="1:7" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -12401,7 +12450,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="26.5" thickBot="1">
+    <row r="17" spans="1:9" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -12448,16 +12497,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:I19"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -12471,7 +12520,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -12492,7 +12541,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -12513,7 +12562,7 @@
         <v>0.92970833595125124</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -12532,8 +12581,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1"/>
-    <row r="7" spans="1:9" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -12554,7 +12603,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -12578,7 +12627,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -12607,7 +12656,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -12636,7 +12685,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>231</v>
       </c>
@@ -12647,7 +12696,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -12672,8 +12721,11 @@
       <c r="I14" s="40" t="s">
         <v>981</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1">
+      <c r="J14" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -12699,8 +12751,11 @@
       <c r="I15" t="s">
         <v>980</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1">
+      <c r="J15" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -12731,8 +12786,11 @@
       <c r="I16" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="26.5" thickBot="1">
+      <c r="J16" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -12763,8 +12821,11 @@
       <c r="I17" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="12" t="s">
         <v>231</v>
       </c>
@@ -12775,10 +12836,16 @@
       <c r="I18" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="I19" t="s">
         <v>924</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1013</v>
       </c>
     </row>
   </sheetData>
@@ -12787,16 +12854,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:F8"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -12810,7 +12877,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -12831,7 +12898,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -12852,7 +12919,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -12871,8 +12938,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -12893,7 +12960,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -12917,7 +12984,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -12946,7 +13013,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -12975,7 +13042,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>231</v>
       </c>
@@ -12986,22 +13053,171 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
+    <row r="14" spans="1:10" ht="30" thickBot="1">
+      <c r="A14" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>998</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>611</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>978</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>568</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>990</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>617</v>
+      </c>
+      <c r="I14" s="40" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16" thickBot="1">
+      <c r="A15" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B15" s="42">
+        <v>0.18616626833750199</v>
+      </c>
+      <c r="C15" s="42">
+        <v>0.343251015277311</v>
+      </c>
+      <c r="D15" s="42">
+        <v>0.10921309468591101</v>
+      </c>
+      <c r="E15" s="42">
+        <v>0.111043501384137</v>
+      </c>
+      <c r="F15" s="42">
+        <v>0.25032612031513901</v>
+      </c>
+      <c r="G15" s="22">
+        <f>SUM(B15:F15)</f>
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>611</v>
+      </c>
+      <c r="J15" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16" thickBot="1">
+      <c r="A16" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" s="13">
+        <f>ROUND(2000*B15,0)</f>
+        <v>372</v>
+      </c>
+      <c r="C16" s="13">
+        <f>ROUND(2000*C15,0)</f>
+        <v>687</v>
+      </c>
+      <c r="D16" s="13">
+        <f>ROUND(2000*D15,0)</f>
+        <v>218</v>
+      </c>
+      <c r="E16" s="13">
+        <f>ROUND(2000*E15,0)</f>
+        <v>222</v>
+      </c>
+      <c r="F16" s="13">
+        <f>ROUND(2000*F15,0)</f>
+        <v>501</v>
+      </c>
+      <c r="G16" s="3">
+        <f>SUM(B16:F16)</f>
+        <v>2000</v>
+      </c>
+      <c r="I16" t="s">
+        <v>978</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" thickBot="1">
+      <c r="A17" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" s="2">
+        <f>ROUND(2200*B15,0)</f>
+        <v>410</v>
+      </c>
+      <c r="C17" s="2">
+        <f>ROUND(2200*C15,0)</f>
+        <v>755</v>
+      </c>
+      <c r="D17" s="2">
+        <f>ROUND(2200*D15,0)</f>
+        <v>240</v>
+      </c>
+      <c r="E17" s="2">
+        <f>ROUND(2200*E15,0)</f>
+        <v>244</v>
+      </c>
+      <c r="F17" s="2">
+        <f>ROUND(2200*F15,0)</f>
+        <v>551</v>
+      </c>
+      <c r="G17" s="3">
+        <f>SUM(B17:F17)</f>
+        <v>2200</v>
+      </c>
+      <c r="I17" t="s">
+        <v>568</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="14"/>
+      <c r="I18" t="s">
+        <v>990</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="I19" t="s">
+        <v>924</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:I19"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -13015,7 +13231,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -13035,7 +13251,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -13054,7 +13270,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -13073,8 +13289,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1"/>
-    <row r="7" spans="1:9" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -13095,7 +13311,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -13119,7 +13335,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -13148,7 +13364,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -13177,7 +13393,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>231</v>
       </c>
@@ -13188,7 +13404,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -13213,8 +13429,11 @@
       <c r="I14" t="s">
         <v>987</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1">
+      <c r="J14" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -13241,7 +13460,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -13272,8 +13491,11 @@
       <c r="I16" s="40" t="s">
         <v>984</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="26.5" thickBot="1">
+      <c r="J16" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -13305,7 +13527,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18" s="12" t="s">
         <v>231</v>
       </c>
@@ -13316,10 +13538,16 @@
       <c r="I18" t="s">
         <v>986</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="I19" t="s">
         <v>924</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1004</v>
       </c>
     </row>
   </sheetData>
@@ -13328,16 +13556,16 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -13351,7 +13579,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -13371,7 +13599,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -13390,7 +13618,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -13409,8 +13637,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -13431,7 +13659,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -13455,7 +13683,7 @@
         <v>0.99999999999999944</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -13484,7 +13712,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -13524,7 +13752,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -13553,7 +13781,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -13583,7 +13811,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -13615,7 +13843,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="26.5" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -13676,14 +13904,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -14172,24 +14400,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -14203,7 +14431,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -14223,7 +14451,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -14242,7 +14470,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -14261,8 +14489,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -14283,7 +14511,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -14307,7 +14535,7 @@
         <v>0.99999999999999933</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -14336,7 +14564,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -14382,16 +14610,16 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -14405,7 +14633,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -14425,7 +14653,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -14444,7 +14672,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -14463,8 +14691,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -14485,7 +14713,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -14509,7 +14737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -14538,7 +14766,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -14584,22 +14812,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -14614,7 +14842,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -14632,7 +14860,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -14652,7 +14880,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -14683,7 +14911,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -14692,7 +14920,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -14713,7 +14941,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -14737,7 +14965,7 @@
         <v>1.0001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -14766,7 +14994,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -14795,8 +15023,8 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1"/>
-    <row r="12" spans="1:7" ht="15" thickBot="1">
+    <row r="11" spans="1:7" ht="16" thickBot="1"/>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>230</v>
       </c>
@@ -14814,7 +15042,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="8" t="s">
         <v>229</v>
       </c>
@@ -14834,7 +15062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>212</v>
       </c>
@@ -14859,7 +15087,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>213</v>
       </c>
@@ -14889,7 +15117,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="12" t="s">
         <v>214</v>
       </c>
@@ -14909,7 +15137,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="8" t="s">
         <v>211</v>
       </c>
@@ -14933,7 +15161,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>212</v>
       </c>
@@ -14962,7 +15190,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>213</v>
       </c>
@@ -15000,7 +15228,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="16" t="s">
         <v>330</v>
       </c>
@@ -15011,7 +15239,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>211</v>
       </c>
@@ -15026,7 +15254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>212</v>
       </c>
@@ -15043,7 +15271,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>213</v>
       </c>
@@ -15071,22 +15299,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>272</v>
       </c>
@@ -15112,7 +15340,7 @@
       <c r="K1" s="13"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -15145,7 +15373,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -15179,7 +15407,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1">
+    <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -15243,14 +15471,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>215</v>
       </c>
@@ -15270,7 +15498,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -15293,7 +15521,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -15318,7 +15546,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>213</v>
       </c>
@@ -15359,7 +15587,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -15373,7 +15601,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>218</v>
       </c>
@@ -15399,7 +15627,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -15428,7 +15656,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -15462,7 +15690,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -15512,7 +15740,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -15526,7 +15754,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="26.5" thickBot="1">
+    <row r="20" spans="1:12" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>224</v>
       </c>
@@ -15550,7 +15778,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>229</v>
       </c>
@@ -15576,7 +15804,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -15607,7 +15835,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>213</v>
       </c>
@@ -15638,7 +15866,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>231</v>
       </c>
@@ -15648,7 +15876,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -15673,7 +15901,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1">
+    <row r="27" spans="1:12" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>211</v>
       </c>
@@ -15692,7 +15920,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1">
+    <row r="28" spans="1:12" ht="16" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>212</v>
       </c>
@@ -15714,7 +15942,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1">
+    <row r="29" spans="1:12" ht="16" thickBot="1">
       <c r="A29" s="8" t="s">
         <v>499</v>
       </c>
@@ -15733,7 +15961,7 @@
       </c>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>498</v>
       </c>
@@ -15755,7 +15983,7 @@
       </c>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:12" ht="26.5" thickBot="1">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>500</v>
       </c>
@@ -15788,12 +16016,12 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
-    <row r="36" spans="1:10" ht="15" thickBot="1">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26.5" thickBot="1">
+    <row r="37" spans="1:10" ht="30" thickBot="1">
       <c r="A37" s="8" t="s">
         <v>202</v>
       </c>
@@ -15823,7 +16051,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="8" t="s">
         <v>211</v>
       </c>
@@ -15856,7 +16084,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="8" t="s">
         <v>212</v>
       </c>
@@ -15897,7 +16125,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" thickBot="1">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="8" t="s">
         <v>213</v>
       </c>
@@ -15964,12 +16192,12 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="15" thickBot="1">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" thickBot="1">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>277</v>
       </c>
@@ -15990,7 +16218,7 @@
       </c>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="15" thickBot="1">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="8" t="s">
         <v>211</v>
       </c>
@@ -16014,7 +16242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" thickBot="1">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="8" t="s">
         <v>212</v>
       </c>
@@ -16043,7 +16271,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="8" t="s">
         <v>213</v>
       </c>
@@ -16099,16 +16327,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -16122,7 +16350,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -16143,7 +16371,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -16164,7 +16392,7 @@
         <v>0.95277529961698948</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -16183,8 +16411,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -16205,7 +16433,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -16229,7 +16457,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -16258,7 +16486,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -16298,7 +16526,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="26.5" thickBot="1">
+    <row r="13" spans="1:11" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -16324,7 +16552,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -16354,7 +16582,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -16389,7 +16617,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.5" thickBot="1">
+    <row r="16" spans="1:11" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -16439,7 +16667,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.5">
+    <row r="19" spans="1:11" ht="16">
       <c r="J19" t="s">
         <v>924</v>
       </c>
@@ -16447,7 +16675,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1">
+    <row r="20" spans="1:11" ht="16" thickBot="1">
       <c r="A20" s="16" t="s">
         <v>330</v>
       </c>
@@ -16461,7 +16689,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="26.5" thickBot="1">
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>211</v>
       </c>
@@ -16479,7 +16707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -16506,7 +16734,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1">
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>213</v>
       </c>
@@ -16540,23 +16768,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G23" r:id="rId1"/>
+    <hyperlink ref="G23" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -16570,7 +16798,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -16591,7 +16819,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -16612,7 +16840,7 @@
         <v>0.90805800128462044</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -16631,8 +16859,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -16653,7 +16881,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -16677,7 +16905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -16706,7 +16934,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -16746,7 +16974,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="26.5" thickBot="1">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -16766,7 +16994,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -16790,7 +17018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -16819,7 +17047,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -16863,7 +17091,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1">
+    <row r="19" spans="1:10" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>330</v>
       </c>
@@ -16874,7 +17102,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="26.5" thickBot="1">
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>211</v>
       </c>
@@ -16889,7 +17117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1">
+    <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>212</v>
       </c>
@@ -16906,7 +17134,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="26.5" thickBot="1">
+    <row r="22" spans="1:10" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>213</v>
       </c>
@@ -16928,8 +17156,8 @@
         <v>231</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1"/>
-    <row r="25" spans="1:10" ht="39" thickBot="1">
+    <row r="24" spans="1:10" ht="16" thickBot="1"/>
+    <row r="25" spans="1:10" ht="44" thickBot="1">
       <c r="A25" s="12" t="s">
         <v>495</v>
       </c>
@@ -16944,7 +17172,7 @@
       </c>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:10" ht="26.5" thickBot="1">
+    <row r="26" spans="1:10" ht="30" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>211</v>
       </c>
@@ -16962,7 +17190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1">
+    <row r="27" spans="1:10" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>212</v>
       </c>
@@ -16983,7 +17211,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="39" thickBot="1">
+    <row r="28" spans="1:10" ht="44" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>500</v>
       </c>
@@ -17025,16 +17253,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1">
+    <row r="1" spans="1:13" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -17048,7 +17276,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:13" ht="26.5" thickBot="1">
+    <row r="2" spans="1:13" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -17069,7 +17297,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -17090,7 +17318,7 @@
         <v>0.9267197256851698</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="26.5" thickBot="1">
+    <row r="4" spans="1:13" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -17109,8 +17337,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1"/>
-    <row r="7" spans="1:13" ht="15" thickBot="1">
+    <row r="6" spans="1:13" ht="16" thickBot="1"/>
+    <row r="7" spans="1:13" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -17131,7 +17359,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="26.5" thickBot="1">
+    <row r="8" spans="1:13" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -17155,7 +17383,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1">
+    <row r="9" spans="1:13" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -17184,7 +17412,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.5" thickBot="1">
+    <row r="10" spans="1:13" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -17224,7 +17452,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:13" ht="26.5" thickBot="1">
+    <row r="13" spans="1:13" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>214</v>
       </c>
@@ -17253,7 +17481,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="26.5" thickBot="1">
+    <row r="14" spans="1:13" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -17284,7 +17512,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1">
+    <row r="15" spans="1:13" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -17320,7 +17548,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="26.5" thickBot="1">
+    <row r="16" spans="1:13" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>213</v>
       </c>
@@ -17379,8 +17607,8 @@
         <v>925</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" thickBot="1"/>
-    <row r="20" spans="1:13" ht="26.5" thickBot="1">
+    <row r="19" spans="1:13" ht="16" thickBot="1"/>
+    <row r="20" spans="1:13" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>495</v>
       </c>
@@ -17392,7 +17620,7 @@
       </c>
       <c r="D20" s="15"/>
     </row>
-    <row r="21" spans="1:13" ht="26.5" thickBot="1">
+    <row r="21" spans="1:13" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>211</v>
       </c>
@@ -17407,7 +17635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15" thickBot="1">
+    <row r="22" spans="1:13" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -17424,7 +17652,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="39" thickBot="1">
+    <row r="23" spans="1:13" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>500</v>
       </c>
@@ -17449,12 +17677,12 @@
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
     </row>
-    <row r="28" spans="1:13" ht="15" thickBot="1">
+    <row r="28" spans="1:13" ht="16" thickBot="1">
       <c r="A28" s="1" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="26.5" thickBot="1">
+    <row r="29" spans="1:13" ht="30" thickBot="1">
       <c r="A29" s="12" t="s">
         <v>495</v>
       </c>
@@ -17467,7 +17695,7 @@
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="1:13" ht="26.5" thickBot="1">
+    <row r="30" spans="1:13" ht="30" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>211</v>
       </c>
@@ -17483,7 +17711,7 @@
       </c>
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="1:13" ht="15" thickBot="1">
+    <row r="31" spans="1:13" ht="16" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>212</v>
       </c>
@@ -17501,7 +17729,7 @@
       </c>
       <c r="E31" s="28"/>
     </row>
-    <row r="32" spans="1:13" ht="39" thickBot="1">
+    <row r="32" spans="1:13" ht="44" thickBot="1">
       <c r="A32" s="8" t="s">
         <v>500</v>
       </c>
@@ -17534,19 +17762,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -17560,7 +17788,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -17581,7 +17809,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -17602,7 +17830,7 @@
         <v>0.97448244785232785</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -17621,8 +17849,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -17643,7 +17871,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -17667,7 +17895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -17696,7 +17924,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -17745,7 +17973,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="40"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -17768,7 +17996,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -17799,7 +18027,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -17835,7 +18063,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -17902,7 +18130,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1">
       <c r="A21" s="16" t="s">
         <v>330</v>
       </c>
@@ -17913,7 +18141,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1">
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>211</v>
       </c>
@@ -17928,7 +18156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>212</v>
       </c>
@@ -17945,7 +18173,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>213</v>
       </c>
@@ -17974,16 +18202,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>215</v>
       </c>
@@ -17997,7 +18225,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>211</v>
       </c>
@@ -18018,7 +18246,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>212</v>
       </c>
@@ -18039,7 +18267,7 @@
         <v>0.98351979013457747</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>213</v>
       </c>
@@ -18058,8 +18286,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>218</v>
       </c>
@@ -18080,7 +18308,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>211</v>
       </c>
@@ -18104,7 +18332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>212</v>
       </c>
@@ -18133,7 +18361,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>213</v>
       </c>
@@ -18178,7 +18406,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>214</v>
       </c>
@@ -18204,7 +18432,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -18234,7 +18462,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -18269,7 +18497,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -18316,8 +18544,8 @@
         <v>822</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1"/>
-    <row r="21" spans="1:11" ht="26.5" thickBot="1">
+    <row r="20" spans="1:11" ht="16" thickBot="1"/>
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>495</v>
       </c>
@@ -18332,7 +18560,7 @@
       </c>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1">
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>211</v>
       </c>
@@ -18350,7 +18578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>212</v>
       </c>
@@ -18374,7 +18602,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="39" thickBot="1">
+    <row r="24" spans="1:11" ht="44" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>500</v>
       </c>

</xml_diff>

<commit_message>
Add source region BR
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B410EBA7-96DB-D240-8DC0-7A431359AFF5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E0EABE-7EC2-3C46-9A0C-A6D42F292173}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="9" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="1032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="1033">
   <si>
     <t>Country</t>
   </si>
@@ -3159,6 +3159,9 @@
   </si>
   <si>
     <t>(Table 7)</t>
+  </si>
+  <si>
+    <t>https://ftp.ibge.gov.br/Estimativas_de_Populacao/Estimativas_2020/estimativa_dou_2020.pdf</t>
   </si>
 </sst>
 </file>
@@ -12230,10 +12233,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -12504,7 +12507,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>213</v>
       </c>
@@ -12535,8 +12538,11 @@
       <c r="I17" t="s">
         <v>923</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="12" t="s">
         <v>231</v>
       </c>
@@ -14795,7 +14801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add zip codes AU + quota in xlsx
</commit_message>
<xml_diff>
--- a/questionnaires/countries_specificities.xlsx
+++ b/questionnaires/countries_specificities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDE32C6-F70D-FC41-94DE-591FEB44853F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="7" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specificities" sheetId="1" r:id="rId1"/>
@@ -34,7 +35,7 @@
     <sheet name="quota_TR" sheetId="21" r:id="rId20"/>
     <sheet name="quota_UA" sheetId="22" r:id="rId21"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3711" uniqueCount="1084">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2322" uniqueCount="1088">
   <si>
     <t>Country</t>
   </si>
@@ -3315,11 +3316,23 @@
   <si>
     <t>Amazonia  Salazar et al. (2007) 10.1029/2007GL029695</t>
   </si>
+  <si>
+    <t>Main remote area of the Postal area is "Major City"</t>
+  </si>
+  <si>
+    <t>Remoteness Area (RA)ASGS Ed 2016 in .csv format) https://www.abs.gov.au/AUSSTATS/abs@.nsf/DetailsPage/1270.0.55.005July%202016?OpenDocument</t>
+  </si>
+  <si>
+    <t>POAs (Postal Areas ASGS Edition 2016 in .csv Format ): https://www.abs.gov.au/AUSSTATS/abs@.nsf/DetailsPage/1270.0.55.003July%202016?OpenDocument</t>
+  </si>
+  <si>
+    <t>census: https://www.abs.gov.au/AUSSTATS/abs@.nsf/DetailsPage/2074.02016?OpenDocument</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -3586,7 +3599,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3863,42 +3876,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q93" sqref="Q93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.36328125" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" customWidth="1"/>
-    <col min="6" max="6" width="6.453125" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" customWidth="1"/>
-    <col min="9" max="9" width="8.36328125" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" customWidth="1"/>
-    <col min="12" max="12" width="7.36328125" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="6.5" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" customWidth="1"/>
+    <col min="11" max="11" width="9.5" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" customWidth="1"/>
     <col min="13" max="14" width="8" customWidth="1"/>
-    <col min="15" max="15" width="8.453125" customWidth="1"/>
-    <col min="16" max="16" width="8.81640625" customWidth="1"/>
-    <col min="17" max="17" width="6.81640625" customWidth="1"/>
-    <col min="18" max="18" width="8.36328125" customWidth="1"/>
-    <col min="19" max="19" width="7.453125" customWidth="1"/>
-    <col min="20" max="20" width="8.36328125" customWidth="1"/>
-    <col min="21" max="21" width="6.453125" customWidth="1"/>
-    <col min="22" max="22" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" customWidth="1"/>
+    <col min="17" max="17" width="6.83203125" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" customWidth="1"/>
+    <col min="19" max="19" width="7.5" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" customWidth="1"/>
+    <col min="21" max="21" width="6.5" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -10592,16 +10605,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -10615,7 +10628,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -10636,7 +10649,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -10657,7 +10670,7 @@
         <v>0.92622883301508352</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -10676,8 +10689,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -10698,7 +10711,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -10722,7 +10735,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -10751,7 +10764,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -10791,7 +10804,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1">
+    <row r="13" spans="1:10" ht="16" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>213</v>
       </c>
@@ -10814,7 +10827,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>210</v>
       </c>
@@ -10844,7 +10857,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -10879,7 +10892,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -10926,8 +10939,8 @@
         <v>790</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1"/>
-    <row r="20" spans="1:10" ht="26.5" thickBot="1">
+    <row r="19" spans="1:10" ht="16" thickBot="1"/>
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>491</v>
       </c>
@@ -10940,7 +10953,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:10" ht="26.5" thickBot="1">
+    <row r="21" spans="1:10" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>210</v>
       </c>
@@ -10956,7 +10969,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>211</v>
       </c>
@@ -10974,7 +10987,7 @@
       </c>
       <c r="E22" s="28"/>
     </row>
-    <row r="23" spans="1:10" ht="39" thickBot="1">
+    <row r="23" spans="1:10" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>496</v>
       </c>
@@ -10998,19 +11011,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -11025,7 +11038,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -11047,7 +11060,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -11069,7 +11082,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -11110,7 +11123,7 @@
       <c r="G6" s="35"/>
       <c r="H6" s="36"/>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -11120,7 +11133,7 @@
       <c r="G7" s="35"/>
       <c r="H7" s="36"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>217</v>
       </c>
@@ -11142,7 +11155,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="36"/>
     </row>
-    <row r="9" spans="1:11" ht="26.5" thickBot="1">
+    <row r="9" spans="1:11" ht="30" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>210</v>
       </c>
@@ -11167,7 +11180,7 @@
       </c>
       <c r="H9" s="36"/>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1">
+    <row r="10" spans="1:11" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>211</v>
       </c>
@@ -11197,7 +11210,7 @@
       </c>
       <c r="H10" s="36"/>
     </row>
-    <row r="11" spans="1:11" ht="26.5" thickBot="1">
+    <row r="11" spans="1:11" ht="30" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>212</v>
       </c>
@@ -11242,7 +11255,7 @@
     <row r="13" spans="1:11">
       <c r="H13" s="36"/>
     </row>
-    <row r="14" spans="1:11" ht="39" thickBot="1">
+    <row r="14" spans="1:11" ht="44" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>213</v>
       </c>
@@ -11266,7 +11279,7 @@
       </c>
       <c r="H14" s="36"/>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>210</v>
       </c>
@@ -11293,7 +11306,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
@@ -11329,7 +11342,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="26.5" thickBot="1">
+    <row r="17" spans="1:12" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
@@ -11401,7 +11414,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="26.5" thickBot="1">
+    <row r="21" spans="1:12" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>775</v>
       </c>
@@ -11425,7 +11438,7 @@
       </c>
       <c r="H21" s="36"/>
     </row>
-    <row r="22" spans="1:12" ht="26.5" thickBot="1">
+    <row r="22" spans="1:12" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>210</v>
       </c>
@@ -11452,7 +11465,7 @@
         <v>0.99989215000000009</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>211</v>
       </c>
@@ -11485,7 +11498,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="26.5" thickBot="1">
+    <row r="24" spans="1:12" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>212</v>
       </c>
@@ -11574,16 +11587,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -11597,7 +11610,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -11618,7 +11631,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -11639,7 +11652,7 @@
         <v>0.99992877771181621</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -11658,8 +11671,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -11680,7 +11693,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -11704,7 +11717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -11733,7 +11746,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -11773,7 +11786,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>213</v>
       </c>
@@ -11802,7 +11815,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>210</v>
       </c>
@@ -11832,7 +11845,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
@@ -11867,7 +11880,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
@@ -11922,8 +11935,8 @@
         <v>723</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1"/>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1"/>
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="12" t="s">
         <v>491</v>
       </c>
@@ -11936,7 +11949,7 @@
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>210</v>
       </c>
@@ -11958,7 +11971,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1">
+    <row r="25" spans="1:11" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>211</v>
       </c>
@@ -11982,7 +11995,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="39" thickBot="1">
+    <row r="26" spans="1:11" ht="44" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>496</v>
       </c>
@@ -12007,16 +12020,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -12030,7 +12043,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1">
+    <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -12051,7 +12064,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -12072,7 +12085,7 @@
         <v>0.97760081385085629</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -12091,8 +12104,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -12113,7 +12126,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -12137,7 +12150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -12166,7 +12179,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -12206,7 +12219,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>213</v>
       </c>
@@ -12229,7 +12242,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>210</v>
       </c>
@@ -12259,7 +12272,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
@@ -12294,7 +12307,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
@@ -12344,8 +12357,8 @@
         <v>732</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1"/>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1"/>
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="12" t="s">
         <v>491</v>
       </c>
@@ -12358,7 +12371,7 @@
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>210</v>
       </c>
@@ -12380,7 +12393,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1">
+    <row r="24" spans="1:11" ht="16" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>211</v>
       </c>
@@ -12407,7 +12420,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="39" thickBot="1">
+    <row r="25" spans="1:11" ht="44" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>496</v>
       </c>
@@ -12431,16 +12444,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -12454,7 +12467,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -12475,7 +12488,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -12496,7 +12509,7 @@
         <v>1.0341140064832992</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -12515,8 +12528,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -12537,7 +12550,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -12561,7 +12574,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -12590,7 +12603,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -12630,7 +12643,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="39" thickBot="1">
+    <row r="13" spans="1:10" ht="44" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>213</v>
       </c>
@@ -12653,7 +12666,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>210</v>
       </c>
@@ -12683,7 +12696,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -12718,7 +12731,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -12756,7 +12769,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1">
+    <row r="19" spans="1:9" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>329</v>
       </c>
@@ -12767,7 +12780,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1">
+    <row r="20" spans="1:9" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>210</v>
       </c>
@@ -12788,7 +12801,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1">
+    <row r="21" spans="1:9" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>211</v>
       </c>
@@ -12805,7 +12818,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="26.5" thickBot="1">
+    <row r="22" spans="1:9" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -12933,16 +12946,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -12956,7 +12969,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -12977,7 +12990,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -12998,7 +13011,7 @@
         <v>0.95217958067188335</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -13017,8 +13030,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -13039,7 +13052,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -13063,7 +13076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -13092,7 +13105,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -13132,7 +13145,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>213</v>
       </c>
@@ -13155,7 +13168,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>210</v>
       </c>
@@ -13179,7 +13192,7 @@
         <v>0.99999999999999933</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1">
+    <row r="16" spans="1:7" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
@@ -13208,7 +13221,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="26.5" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
@@ -13258,16 +13271,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -13281,7 +13294,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -13302,7 +13315,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -13323,7 +13336,7 @@
         <v>0.92970833595125124</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -13342,8 +13355,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -13364,7 +13377,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -13388,7 +13401,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -13417,7 +13430,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -13457,7 +13470,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>213</v>
       </c>
@@ -13486,7 +13499,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>210</v>
       </c>
@@ -13516,7 +13529,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
@@ -13551,7 +13564,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="26.5" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
@@ -13615,16 +13628,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -13638,7 +13651,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -13659,7 +13672,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -13680,7 +13693,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -13699,8 +13712,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -13721,7 +13734,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -13745,7 +13758,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -13774,7 +13787,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -13814,7 +13827,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>213</v>
       </c>
@@ -13840,7 +13853,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>210</v>
       </c>
@@ -13870,7 +13883,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
@@ -13905,7 +13918,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="26.5" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
@@ -13969,16 +13982,16 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -13992,7 +14005,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -14012,7 +14025,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -14031,7 +14044,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -14050,8 +14063,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -14072,7 +14085,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -14096,7 +14109,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -14125,7 +14138,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -14165,7 +14178,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>213</v>
       </c>
@@ -14194,7 +14207,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>210</v>
       </c>
@@ -14221,7 +14234,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
@@ -14256,7 +14269,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="26.5" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
@@ -14311,22 +14324,108 @@
         <v>986</v>
       </c>
     </row>
+    <row r="22" spans="1:10" ht="16" thickBot="1"/>
+    <row r="23" spans="1:10" ht="30" thickBot="1">
+      <c r="A23" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:10" ht="16" thickBot="1">
+      <c r="A24" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0.28301939999999998</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.71698059999999997</v>
+      </c>
+      <c r="D24" s="9">
+        <f>SUM(B24:C24)</f>
+        <v>1</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" t="s">
+        <v>766</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="16" thickBot="1">
+      <c r="A25" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B25" s="11">
+        <f t="shared" ref="B25:C25" si="2">ROUND(2000*B24,0)</f>
+        <v>566</v>
+      </c>
+      <c r="C25" s="11">
+        <f t="shared" si="2"/>
+        <v>1434</v>
+      </c>
+      <c r="D25" s="11">
+        <f>SUM(B25:C25)</f>
+        <v>2000</v>
+      </c>
+      <c r="E25" s="28"/>
+      <c r="F25" t="s">
+        <v>721</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="44" thickBot="1">
+      <c r="A26" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="B26" s="13">
+        <f>ROUND(2200*B24,0)</f>
+        <v>623</v>
+      </c>
+      <c r="C26" s="13">
+        <f t="shared" ref="C26" si="3">ROUND(2200*C24,0)</f>
+        <v>1577</v>
+      </c>
+      <c r="D26" s="13">
+        <f>SUM(B26:C26)</f>
+        <v>2200</v>
+      </c>
+      <c r="E26" s="28"/>
+      <c r="G26" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="G27" t="s">
+        <v>1087</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -14340,7 +14439,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -14360,7 +14459,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -14379,7 +14478,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -14398,8 +14497,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -14420,7 +14519,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -14444,7 +14543,7 @@
         <v>0.99999999999999944</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -14473,7 +14572,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -14513,7 +14612,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>213</v>
       </c>
@@ -14542,7 +14641,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>210</v>
       </c>
@@ -14572,7 +14671,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
@@ -14604,7 +14703,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="26.5" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
@@ -14665,14 +14764,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -15161,24 +15260,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -15192,7 +15291,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -15212,7 +15311,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -15231,7 +15330,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -15250,8 +15349,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -15272,7 +15371,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -15296,7 +15395,7 @@
         <v>0.99999999999999933</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -15325,7 +15424,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -15365,7 +15464,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="76.5" thickBot="1">
+    <row r="14" spans="1:10" ht="86" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>213</v>
       </c>
@@ -15394,7 +15493,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>210</v>
       </c>
@@ -15418,7 +15517,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
@@ -15447,7 +15546,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="26.5" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
@@ -15499,16 +15598,16 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -15522,7 +15621,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -15542,7 +15641,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -15561,7 +15660,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -15580,8 +15679,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -15602,7 +15701,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -15626,7 +15725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -15655,7 +15754,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -15695,7 +15794,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>213</v>
       </c>
@@ -15724,7 +15823,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>210</v>
       </c>
@@ -15754,7 +15853,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
@@ -15789,7 +15888,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
@@ -15856,22 +15955,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -15886,7 +15985,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -15904,7 +16003,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -15924,7 +16023,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -15955,7 +16054,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -15964,7 +16063,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -15985,7 +16084,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -16009,7 +16108,7 @@
         <v>1.0001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -16038,7 +16137,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -16067,8 +16166,8 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1"/>
-    <row r="12" spans="1:7" ht="15" thickBot="1">
+    <row r="11" spans="1:7" ht="16" thickBot="1"/>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>229</v>
       </c>
@@ -16086,7 +16185,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="8" t="s">
         <v>228</v>
       </c>
@@ -16106,7 +16205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>211</v>
       </c>
@@ -16131,7 +16230,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>212</v>
       </c>
@@ -16161,7 +16260,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="12" t="s">
         <v>213</v>
       </c>
@@ -16181,7 +16280,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="8" t="s">
         <v>210</v>
       </c>
@@ -16205,7 +16304,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>211</v>
       </c>
@@ -16234,7 +16333,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>212</v>
       </c>
@@ -16272,7 +16371,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="16" t="s">
         <v>329</v>
       </c>
@@ -16283,7 +16382,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="8" t="s">
         <v>210</v>
       </c>
@@ -16298,7 +16397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>211</v>
       </c>
@@ -16315,7 +16414,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>212</v>
       </c>
@@ -16343,22 +16442,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>271</v>
       </c>
@@ -16384,7 +16483,7 @@
       <c r="K1" s="13"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -16417,7 +16516,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -16451,7 +16550,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1">
+    <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -16515,14 +16614,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>214</v>
       </c>
@@ -16542,7 +16641,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>210</v>
       </c>
@@ -16565,7 +16664,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>211</v>
       </c>
@@ -16590,7 +16689,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>212</v>
       </c>
@@ -16631,7 +16730,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -16645,7 +16744,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>217</v>
       </c>
@@ -16671,7 +16770,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>210</v>
       </c>
@@ -16700,7 +16799,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
@@ -16734,7 +16833,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
@@ -16784,7 +16883,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -16798,7 +16897,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="26.5" thickBot="1">
+    <row r="20" spans="1:12" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>223</v>
       </c>
@@ -16822,7 +16921,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>228</v>
       </c>
@@ -16848,7 +16947,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>211</v>
       </c>
@@ -16879,7 +16978,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>212</v>
       </c>
@@ -16910,7 +17009,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>230</v>
       </c>
@@ -16920,7 +17019,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -16945,7 +17044,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1">
+    <row r="27" spans="1:12" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>210</v>
       </c>
@@ -16964,7 +17063,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1">
+    <row r="28" spans="1:12" ht="16" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>211</v>
       </c>
@@ -16986,7 +17085,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1">
+    <row r="29" spans="1:12" ht="16" thickBot="1">
       <c r="A29" s="8" t="s">
         <v>495</v>
       </c>
@@ -17005,7 +17104,7 @@
       </c>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>494</v>
       </c>
@@ -17027,7 +17126,7 @@
       </c>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:12" ht="26.5" thickBot="1">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>496</v>
       </c>
@@ -17060,12 +17159,12 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
-    <row r="36" spans="1:10" ht="15" thickBot="1">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26.5" thickBot="1">
+    <row r="37" spans="1:10" ht="30" thickBot="1">
       <c r="A37" s="8" t="s">
         <v>201</v>
       </c>
@@ -17095,7 +17194,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="8" t="s">
         <v>210</v>
       </c>
@@ -17128,7 +17227,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="8" t="s">
         <v>211</v>
       </c>
@@ -17169,7 +17268,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" thickBot="1">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="8" t="s">
         <v>212</v>
       </c>
@@ -17236,12 +17335,12 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="15" thickBot="1">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" thickBot="1">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>276</v>
       </c>
@@ -17262,7 +17361,7 @@
       </c>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="15" thickBot="1">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="8" t="s">
         <v>210</v>
       </c>
@@ -17286,7 +17385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" thickBot="1">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="8" t="s">
         <v>211</v>
       </c>
@@ -17315,7 +17414,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="8" t="s">
         <v>212</v>
       </c>
@@ -17371,16 +17470,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -17394,7 +17493,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -17415,7 +17514,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -17436,7 +17535,7 @@
         <v>0.95277529961698948</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -17455,8 +17554,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -17477,7 +17576,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -17501,7 +17600,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -17530,7 +17629,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -17570,7 +17669,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="26.5" thickBot="1">
+    <row r="13" spans="1:11" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>213</v>
       </c>
@@ -17596,7 +17695,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>210</v>
       </c>
@@ -17626,7 +17725,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -17661,7 +17760,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.5" thickBot="1">
+    <row r="16" spans="1:11" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -17711,7 +17810,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.5">
+    <row r="19" spans="1:11" ht="16">
       <c r="J19" t="s">
         <v>909</v>
       </c>
@@ -17719,7 +17818,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1">
+    <row r="20" spans="1:11" ht="16" thickBot="1">
       <c r="A20" s="16" t="s">
         <v>329</v>
       </c>
@@ -17733,7 +17832,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="26.5" thickBot="1">
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>210</v>
       </c>
@@ -17751,7 +17850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>211</v>
       </c>
@@ -17778,7 +17877,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="26.5" thickBot="1">
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>212</v>
       </c>
@@ -17812,23 +17911,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G23" r:id="rId1"/>
+    <hyperlink ref="G23" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -17842,7 +17941,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -17863,7 +17962,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -17884,7 +17983,7 @@
         <v>0.90805800128462044</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -17903,8 +18002,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -17925,7 +18024,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -17949,7 +18048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -17978,7 +18077,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -18018,7 +18117,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="26.5" thickBot="1">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>213</v>
       </c>
@@ -18038,7 +18137,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>210</v>
       </c>
@@ -18062,7 +18161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -18091,7 +18190,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -18135,7 +18234,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1">
+    <row r="19" spans="1:10" ht="16" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>329</v>
       </c>
@@ -18146,7 +18245,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="26.5" thickBot="1">
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="8" t="s">
         <v>210</v>
       </c>
@@ -18161,7 +18260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1">
+    <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>211</v>
       </c>
@@ -18178,7 +18277,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="26.5" thickBot="1">
+    <row r="22" spans="1:10" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>212</v>
       </c>
@@ -18200,8 +18299,8 @@
         <v>230</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1"/>
-    <row r="25" spans="1:10" ht="39" thickBot="1">
+    <row r="24" spans="1:10" ht="16" thickBot="1"/>
+    <row r="25" spans="1:10" ht="44" thickBot="1">
       <c r="A25" s="12" t="s">
         <v>491</v>
       </c>
@@ -18216,7 +18315,7 @@
       </c>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:10" ht="26.5" thickBot="1">
+    <row r="26" spans="1:10" ht="30" thickBot="1">
       <c r="A26" s="8" t="s">
         <v>210</v>
       </c>
@@ -18234,7 +18333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1">
+    <row r="27" spans="1:10" ht="16" thickBot="1">
       <c r="A27" s="8" t="s">
         <v>211</v>
       </c>
@@ -18255,7 +18354,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="39" thickBot="1">
+    <row r="28" spans="1:10" ht="44" thickBot="1">
       <c r="A28" s="8" t="s">
         <v>496</v>
       </c>
@@ -18297,16 +18396,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1">
+    <row r="1" spans="1:13" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -18320,7 +18419,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:13" ht="26.5" thickBot="1">
+    <row r="2" spans="1:13" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -18341,7 +18440,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -18362,7 +18461,7 @@
         <v>0.9267197256851698</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="26.5" thickBot="1">
+    <row r="4" spans="1:13" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -18381,8 +18480,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1"/>
-    <row r="7" spans="1:13" ht="15" thickBot="1">
+    <row r="6" spans="1:13" ht="16" thickBot="1"/>
+    <row r="7" spans="1:13" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -18403,7 +18502,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="26.5" thickBot="1">
+    <row r="8" spans="1:13" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -18427,7 +18526,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1">
+    <row r="9" spans="1:13" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -18456,7 +18555,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.5" thickBot="1">
+    <row r="10" spans="1:13" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -18496,7 +18595,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="13" spans="1:13" ht="26.5" thickBot="1">
+    <row r="13" spans="1:13" ht="30" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>213</v>
       </c>
@@ -18525,7 +18624,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="26.5" thickBot="1">
+    <row r="14" spans="1:13" ht="30" thickBot="1">
       <c r="A14" s="8" t="s">
         <v>210</v>
       </c>
@@ -18556,7 +18655,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1">
+    <row r="15" spans="1:13" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>211</v>
       </c>
@@ -18592,7 +18691,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="26.5" thickBot="1">
+    <row r="16" spans="1:13" ht="30" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>212</v>
       </c>
@@ -18651,8 +18750,8 @@
         <v>910</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" thickBot="1"/>
-    <row r="20" spans="1:13" ht="26.5" thickBot="1">
+    <row r="19" spans="1:13" ht="16" thickBot="1"/>
+    <row r="20" spans="1:13" ht="30" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>491</v>
       </c>
@@ -18664,7 +18763,7 @@
       </c>
       <c r="D20" s="15"/>
     </row>
-    <row r="21" spans="1:13" ht="26.5" thickBot="1">
+    <row r="21" spans="1:13" ht="30" thickBot="1">
       <c r="A21" s="8" t="s">
         <v>210</v>
       </c>
@@ -18679,7 +18778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15" thickBot="1">
+    <row r="22" spans="1:13" ht="16" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>211</v>
       </c>
@@ -18696,7 +18795,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="39" thickBot="1">
+    <row r="23" spans="1:13" ht="44" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>496</v>
       </c>
@@ -18721,12 +18820,12 @@
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
     </row>
-    <row r="28" spans="1:13" ht="15" thickBot="1">
+    <row r="28" spans="1:13" ht="16" thickBot="1">
       <c r="A28" s="1" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="26.5" thickBot="1">
+    <row r="29" spans="1:13" ht="30" thickBot="1">
       <c r="A29" s="12" t="s">
         <v>491</v>
       </c>
@@ -18739,7 +18838,7 @@
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="1:13" ht="26.5" thickBot="1">
+    <row r="30" spans="1:13" ht="30" thickBot="1">
       <c r="A30" s="8" t="s">
         <v>210</v>
       </c>
@@ -18755,7 +18854,7 @@
       </c>
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="1:13" ht="15" thickBot="1">
+    <row r="31" spans="1:13" ht="16" thickBot="1">
       <c r="A31" s="8" t="s">
         <v>211</v>
       </c>
@@ -18773,7 +18872,7 @@
       </c>
       <c r="E31" s="28"/>
     </row>
-    <row r="32" spans="1:13" ht="39" thickBot="1">
+    <row r="32" spans="1:13" ht="44" thickBot="1">
       <c r="A32" s="8" t="s">
         <v>496</v>
       </c>
@@ -18806,19 +18905,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -18832,7 +18931,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -18853,7 +18952,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -18874,7 +18973,7 @@
         <v>0.97448244785232785</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -18893,8 +18992,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -18915,7 +19014,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -18939,7 +19038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -18968,7 +19067,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -19017,7 +19116,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="40"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>213</v>
       </c>
@@ -19040,7 +19139,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>210</v>
       </c>
@@ -19071,7 +19170,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
@@ -19107,7 +19206,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
@@ -19174,7 +19273,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1">
       <c r="A21" s="16" t="s">
         <v>329</v>
       </c>
@@ -19185,7 +19284,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1">
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>210</v>
       </c>
@@ -19200,7 +19299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>211</v>
       </c>
@@ -19217,7 +19316,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="26.5" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>212</v>
       </c>
@@ -19246,16 +19345,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>214</v>
       </c>
@@ -19269,7 +19368,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="26.5" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>210</v>
       </c>
@@ -19290,7 +19389,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>211</v>
       </c>
@@ -19311,7 +19410,7 @@
         <v>0.98351979013457747</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.5" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>212</v>
       </c>
@@ -19330,8 +19429,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>217</v>
       </c>
@@ -19352,7 +19451,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="26.5" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>210</v>
       </c>
@@ -19376,7 +19475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -19405,7 +19504,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.5" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>212</v>
       </c>
@@ -19450,7 +19549,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>213</v>
       </c>
@@ -19476,7 +19575,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.5" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>210</v>
       </c>
@@ -19506,7 +19605,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
@@ -19541,7 +19640,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
@@ -19588,8 +19687,8 @@
         <v>816</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1"/>
-    <row r="21" spans="1:11" ht="26.5" thickBot="1">
+    <row r="20" spans="1:11" ht="16" thickBot="1"/>
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>491</v>
       </c>
@@ -19604,7 +19703,7 @@
       </c>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:11" ht="26.5" thickBot="1">
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="8" t="s">
         <v>210</v>
       </c>
@@ -19622,7 +19721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>211</v>
       </c>
@@ -19646,7 +19745,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="39" thickBot="1">
+    <row r="24" spans="1:11" ht="44" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>496</v>
       </c>

</xml_diff>